<commit_message>
Add Income Tables Meta-data Table (NOT Complete)
</commit_message>
<xml_diff>
--- a/Data/MetaData.xlsx
+++ b/Data/MetaData.xlsx
@@ -17,17 +17,18 @@
     <sheet name="EduCodes-A" sheetId="6" r:id="rId3"/>
     <sheet name="EduCodes-B" sheetId="4" r:id="rId4"/>
     <sheet name="EduCodes-C" sheetId="5" r:id="rId5"/>
-    <sheet name="FoodTables" sheetId="10" r:id="rId6"/>
-    <sheet name="LoanTables" sheetId="7" r:id="rId7"/>
-    <sheet name="HouseTables" sheetId="8" r:id="rId8"/>
-    <sheet name="RegionWeights" sheetId="9" r:id="rId9"/>
+    <sheet name="IncomeTables" sheetId="11" r:id="rId6"/>
+    <sheet name="FoodTables" sheetId="10" r:id="rId7"/>
+    <sheet name="LoanTables" sheetId="7" r:id="rId8"/>
+    <sheet name="HouseTables" sheetId="8" r:id="rId9"/>
+    <sheet name="RegionWeights" sheetId="9" r:id="rId10"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1260" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1266" uniqueCount="316">
   <si>
     <t>Year</t>
   </si>
@@ -960,6 +961,21 @@
   </si>
   <si>
     <t>PriceSystem</t>
+  </si>
+  <si>
+    <t>PubWageTable</t>
+  </si>
+  <si>
+    <t>PrvWageTable</t>
+  </si>
+  <si>
+    <t>AggrIncTable</t>
+  </si>
+  <si>
+    <t>BussIncTable</t>
+  </si>
+  <si>
+    <t>OthrIncTable</t>
   </si>
 </sst>
 </file>
@@ -2068,11 +2084,1763 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E123"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="F30" sqref="F30:F61"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="11.375" customWidth="1"/>
+    <col min="3" max="3" width="11.25" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>293</v>
+      </c>
+      <c r="C1" t="s">
+        <v>296</v>
+      </c>
+      <c r="D1" t="s">
+        <v>297</v>
+      </c>
+      <c r="E1" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>35</v>
+      </c>
+      <c r="B2" t="s">
+        <v>294</v>
+      </c>
+      <c r="C2">
+        <v>5876050</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>36</v>
+      </c>
+      <c r="B3" t="s">
+        <v>294</v>
+      </c>
+      <c r="C3">
+        <v>6196716</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>37</v>
+      </c>
+      <c r="B4" t="s">
+        <v>294</v>
+      </c>
+      <c r="C4">
+        <v>6531840</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>38</v>
+      </c>
+      <c r="B5" t="s">
+        <v>294</v>
+      </c>
+      <c r="C5">
+        <v>6881821</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>39</v>
+      </c>
+      <c r="B6" t="s">
+        <v>294</v>
+      </c>
+      <c r="C6">
+        <v>7247396.0000000009</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>40</v>
+      </c>
+      <c r="B7" t="s">
+        <v>294</v>
+      </c>
+      <c r="C7">
+        <v>7628985.0000000009</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>41</v>
+      </c>
+      <c r="B8" t="s">
+        <v>294</v>
+      </c>
+      <c r="C8">
+        <v>8027360.0000000019</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>42</v>
+      </c>
+      <c r="B9" t="s">
+        <v>294</v>
+      </c>
+      <c r="C9">
+        <v>8443321.0000000037</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>43</v>
+      </c>
+      <c r="B10" t="s">
+        <v>294</v>
+      </c>
+      <c r="C10">
+        <v>8877330.0000000037</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>44</v>
+      </c>
+      <c r="B11" t="s">
+        <v>294</v>
+      </c>
+      <c r="C11">
+        <v>9330222.0000000037</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>45</v>
+      </c>
+      <c r="B12" t="s">
+        <v>294</v>
+      </c>
+      <c r="C12">
+        <v>9799820</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>46</v>
+      </c>
+      <c r="B13" t="s">
+        <v>294</v>
+      </c>
+      <c r="C13">
+        <v>10303832</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>47</v>
+      </c>
+      <c r="B14" t="s">
+        <v>294</v>
+      </c>
+      <c r="C14">
+        <v>10827590</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>48</v>
+      </c>
+      <c r="B15" t="s">
+        <v>294</v>
+      </c>
+      <c r="C15">
+        <v>11372800.999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>49</v>
+      </c>
+      <c r="B16" t="s">
+        <v>294</v>
+      </c>
+      <c r="C16">
+        <v>11939199.999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>50</v>
+      </c>
+      <c r="B17" t="s">
+        <v>294</v>
+      </c>
+      <c r="C17">
+        <v>12528149.999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>51</v>
+      </c>
+      <c r="B18" t="s">
+        <v>294</v>
+      </c>
+      <c r="C18">
+        <v>13140217.999999998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>52</v>
+      </c>
+      <c r="B19" t="s">
+        <v>294</v>
+      </c>
+      <c r="C19">
+        <v>13775970.999999996</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>53</v>
+      </c>
+      <c r="B20" t="s">
+        <v>294</v>
+      </c>
+      <c r="C20">
+        <v>14436879.999999996</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>54</v>
+      </c>
+      <c r="B21" t="s">
+        <v>294</v>
+      </c>
+      <c r="C21">
+        <v>15123104.999999996</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>55</v>
+      </c>
+      <c r="B22" t="s">
+        <v>294</v>
+      </c>
+      <c r="C22">
+        <v>15843230</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>56</v>
+      </c>
+      <c r="B23" t="s">
+        <v>294</v>
+      </c>
+      <c r="C23">
+        <v>16707879.000000002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>57</v>
+      </c>
+      <c r="B24" t="s">
+        <v>294</v>
+      </c>
+      <c r="C24">
+        <v>17615664</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>58</v>
+      </c>
+      <c r="B25" t="s">
+        <v>294</v>
+      </c>
+      <c r="C25">
+        <v>18569129.000000004</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>59</v>
+      </c>
+      <c r="B26" t="s">
+        <v>294</v>
+      </c>
+      <c r="C26">
+        <v>19570404.000000004</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>60</v>
+      </c>
+      <c r="B27" t="s">
+        <v>294</v>
+      </c>
+      <c r="C27">
+        <v>20621675.000000004</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>61</v>
+      </c>
+      <c r="B28" t="s">
+        <v>294</v>
+      </c>
+      <c r="C28">
+        <v>21724672.000000007</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>62</v>
+      </c>
+      <c r="B29" t="s">
+        <v>294</v>
+      </c>
+      <c r="C29">
+        <v>22882710.000000007</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>63</v>
+      </c>
+      <c r="B30" t="s">
+        <v>294</v>
+      </c>
+      <c r="C30">
+        <v>24098164.000000007</v>
+      </c>
+      <c r="E30" s="1"/>
+    </row>
+    <row r="31" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>64</v>
+      </c>
+      <c r="B31" t="s">
+        <v>294</v>
+      </c>
+      <c r="C31">
+        <v>25373998.000000011</v>
+      </c>
+      <c r="E31" s="1"/>
+    </row>
+    <row r="32" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>65</v>
+      </c>
+      <c r="B32" t="s">
+        <v>294</v>
+      </c>
+      <c r="C32">
+        <v>26700300</v>
+      </c>
+      <c r="E32" s="1"/>
+    </row>
+    <row r="33" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>66</v>
+      </c>
+      <c r="B33" t="s">
+        <v>294</v>
+      </c>
+      <c r="C33">
+        <v>27711567</v>
+      </c>
+      <c r="E33" s="1"/>
+    </row>
+    <row r="34" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>67</v>
+      </c>
+      <c r="B34" t="s">
+        <v>294</v>
+      </c>
+      <c r="C34">
+        <v>28757032</v>
+      </c>
+      <c r="E34" s="1"/>
+    </row>
+    <row r="35" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>68</v>
+      </c>
+      <c r="B35" t="s">
+        <v>294</v>
+      </c>
+      <c r="C35">
+        <v>29836785.000000004</v>
+      </c>
+      <c r="E35" s="1"/>
+    </row>
+    <row r="36" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>69</v>
+      </c>
+      <c r="B36" t="s">
+        <v>294</v>
+      </c>
+      <c r="C36">
+        <v>30952024.000000007</v>
+      </c>
+      <c r="D36">
+        <v>46918</v>
+      </c>
+      <c r="E36" s="1">
+        <f t="shared" ref="E36:E61" si="0">C36/D36</f>
+        <v>659.70467624365926</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>70</v>
+      </c>
+      <c r="B37" t="s">
+        <v>294</v>
+      </c>
+      <c r="C37">
+        <v>32106275.000000007</v>
+      </c>
+      <c r="D37">
+        <v>47249</v>
+      </c>
+      <c r="E37" s="1">
+        <f t="shared" si="0"/>
+        <v>679.51226480983735</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>71</v>
+      </c>
+      <c r="B38" t="s">
+        <v>294</v>
+      </c>
+      <c r="C38">
+        <v>32974956.000000011</v>
+      </c>
+      <c r="D38">
+        <v>46102</v>
+      </c>
+      <c r="E38" s="1">
+        <f t="shared" si="0"/>
+        <v>715.26085636198025</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>72</v>
+      </c>
+      <c r="B39" t="s">
+        <v>294</v>
+      </c>
+      <c r="C39">
+        <v>33862199.000000015</v>
+      </c>
+      <c r="D39">
+        <v>33141</v>
+      </c>
+      <c r="E39" s="1">
+        <f t="shared" si="0"/>
+        <v>1021.7615340514775</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>73</v>
+      </c>
+      <c r="B40" t="s">
+        <v>294</v>
+      </c>
+      <c r="C40">
+        <v>34768256.000000015</v>
+      </c>
+      <c r="D40">
+        <v>60228</v>
+      </c>
+      <c r="E40" s="1">
+        <f t="shared" si="0"/>
+        <v>577.27727967058536</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>74</v>
+      </c>
+      <c r="B41" t="s">
+        <v>294</v>
+      </c>
+      <c r="C41">
+        <v>35693379.000000015</v>
+      </c>
+      <c r="D41">
+        <v>100804</v>
+      </c>
+      <c r="E41" s="1">
+        <f t="shared" si="0"/>
+        <v>354.08693107416389</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>75</v>
+      </c>
+      <c r="B42" t="s">
+        <v>294</v>
+      </c>
+      <c r="C42">
+        <v>36633550</v>
+      </c>
+      <c r="D42">
+        <v>52693</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="0"/>
+        <v>695.22612111665683</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>76</v>
+      </c>
+      <c r="B43" t="s">
+        <v>294</v>
+      </c>
+      <c r="C43">
+        <v>37680190</v>
+      </c>
+      <c r="D43">
+        <v>52096</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="0"/>
+        <v>723.2837453931204</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>77</v>
+      </c>
+      <c r="B44" t="s">
+        <v>294</v>
+      </c>
+      <c r="C44">
+        <v>38752272</v>
+      </c>
+      <c r="D44">
+        <v>39130</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="0"/>
+        <v>990.34684385382059</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>78</v>
+      </c>
+      <c r="B45" t="s">
+        <v>294</v>
+      </c>
+      <c r="C45">
+        <v>39848912.000000007</v>
+      </c>
+      <c r="D45">
+        <v>60658</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="0"/>
+        <v>656.94404695176252</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>79</v>
+      </c>
+      <c r="B46" t="s">
+        <v>294</v>
+      </c>
+      <c r="C46">
+        <v>40971722.000000007</v>
+      </c>
+      <c r="D46">
+        <v>55675</v>
+      </c>
+      <c r="E46">
+        <f t="shared" si="0"/>
+        <v>735.90879209699165</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>80</v>
+      </c>
+      <c r="B47" t="s">
+        <v>294</v>
+      </c>
+      <c r="C47">
+        <v>42119145.000000007</v>
+      </c>
+      <c r="D47">
+        <v>55178</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="0"/>
+        <v>763.33221573815661</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>81</v>
+      </c>
+      <c r="B48" t="s">
+        <v>294</v>
+      </c>
+      <c r="C48">
+        <v>43227600.000000007</v>
+      </c>
+      <c r="D48">
+        <v>66708</v>
+      </c>
+      <c r="E48">
+        <f t="shared" si="0"/>
+        <v>648.0122324159023</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>82</v>
+      </c>
+      <c r="B49" t="s">
+        <v>294</v>
+      </c>
+      <c r="C49">
+        <v>44360585.000000007</v>
+      </c>
+      <c r="D49">
+        <v>48180</v>
+      </c>
+      <c r="E49">
+        <f t="shared" si="0"/>
+        <v>920.72613117476146</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>83</v>
+      </c>
+      <c r="B50" t="s">
+        <v>294</v>
+      </c>
+      <c r="C50">
+        <v>45517770.000000015</v>
+      </c>
+      <c r="D50">
+        <v>49900</v>
+      </c>
+      <c r="E50">
+        <f t="shared" si="0"/>
+        <v>912.17975951903838</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>84</v>
+      </c>
+      <c r="B51" t="s">
+        <v>294</v>
+      </c>
+      <c r="C51">
+        <v>46699470.000000015</v>
+      </c>
+      <c r="D51">
+        <v>54278</v>
+      </c>
+      <c r="E51">
+        <f t="shared" si="0"/>
+        <v>860.375658646229</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>85</v>
+      </c>
+      <c r="B52" t="s">
+        <v>294</v>
+      </c>
+      <c r="C52">
+        <v>48260000</v>
+      </c>
+      <c r="D52">
+        <v>57986</v>
+      </c>
+      <c r="E52">
+        <f t="shared" si="0"/>
+        <v>832.26985824164456</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>86</v>
+      </c>
+      <c r="B53" t="s">
+        <v>294</v>
+      </c>
+      <c r="C53">
+        <v>49288000</v>
+      </c>
+      <c r="D53">
+        <v>60662</v>
+      </c>
+      <c r="E53">
+        <f t="shared" si="0"/>
+        <v>812.50206059806794</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>87</v>
+      </c>
+      <c r="B54" t="s">
+        <v>294</v>
+      </c>
+      <c r="C54">
+        <v>50340000</v>
+      </c>
+      <c r="D54">
+        <v>77271</v>
+      </c>
+      <c r="E54">
+        <f t="shared" si="0"/>
+        <v>651.47338587568424</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>88</v>
+      </c>
+      <c r="B55" t="s">
+        <v>294</v>
+      </c>
+      <c r="C55">
+        <v>51416000</v>
+      </c>
+      <c r="D55">
+        <v>74398</v>
+      </c>
+      <c r="E55">
+        <f t="shared" si="0"/>
+        <v>691.09384660877981</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>89</v>
+      </c>
+      <c r="B56" t="s">
+        <v>294</v>
+      </c>
+      <c r="C56">
+        <v>52519000</v>
+      </c>
+      <c r="D56">
+        <v>72441</v>
+      </c>
+      <c r="E56">
+        <f t="shared" si="0"/>
+        <v>724.98999185544096</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>90</v>
+      </c>
+      <c r="B57" t="s">
+        <v>294</v>
+      </c>
+      <c r="C57">
+        <v>53647000</v>
+      </c>
+      <c r="D57">
+        <v>71461</v>
+      </c>
+      <c r="E57">
+        <f t="shared" si="0"/>
+        <v>750.71717440282112</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>91</v>
+      </c>
+      <c r="B58" t="s">
+        <v>294</v>
+      </c>
+      <c r="C58">
+        <v>54607000</v>
+      </c>
+      <c r="D58">
+        <v>69567</v>
+      </c>
+      <c r="E58">
+        <f t="shared" si="0"/>
+        <v>784.9555105150431</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>92</v>
+      </c>
+      <c r="B59" t="s">
+        <v>294</v>
+      </c>
+      <c r="C59">
+        <v>55502000</v>
+      </c>
+      <c r="D59">
+        <v>68058</v>
+      </c>
+      <c r="E59">
+        <f t="shared" si="0"/>
+        <v>815.51030003820267</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>93</v>
+      </c>
+      <c r="B60" t="s">
+        <v>294</v>
+      </c>
+      <c r="C60">
+        <v>56408000</v>
+      </c>
+      <c r="D60">
+        <v>67482</v>
+      </c>
+      <c r="E60">
+        <f t="shared" si="0"/>
+        <v>835.89697993539016</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>94</v>
+      </c>
+      <c r="B61" t="s">
+        <v>294</v>
+      </c>
+      <c r="C61">
+        <v>57327000</v>
+      </c>
+      <c r="D61">
+        <v>67177</v>
+      </c>
+      <c r="E61">
+        <f t="shared" si="0"/>
+        <v>853.37243401759531</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>95</v>
+      </c>
+      <c r="B62" t="s">
+        <v>294</v>
+      </c>
+      <c r="C62">
+        <v>58220000</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>35</v>
+      </c>
+      <c r="B63" t="s">
+        <v>295</v>
+      </c>
+      <c r="C63">
+        <v>13078950</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>36</v>
+      </c>
+      <c r="B64" t="s">
+        <v>295</v>
+      </c>
+      <c r="C64">
+        <v>13351284</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>37</v>
+      </c>
+      <c r="B65" t="s">
+        <v>295</v>
+      </c>
+      <c r="C65">
+        <v>13628160</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>38</v>
+      </c>
+      <c r="B66" t="s">
+        <v>295</v>
+      </c>
+      <c r="C66">
+        <v>13909179</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>39</v>
+      </c>
+      <c r="B67" t="s">
+        <v>295</v>
+      </c>
+      <c r="C67">
+        <v>14194603.999999996</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>40</v>
+      </c>
+      <c r="B68" t="s">
+        <v>295</v>
+      </c>
+      <c r="C68">
+        <v>14484014.999999998</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>41</v>
+      </c>
+      <c r="B69" t="s">
+        <v>295</v>
+      </c>
+      <c r="C69">
+        <v>14777639.999999996</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>42</v>
+      </c>
+      <c r="B70" t="s">
+        <v>295</v>
+      </c>
+      <c r="C70">
+        <v>15075678.999999994</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>43</v>
+      </c>
+      <c r="B71" t="s">
+        <v>295</v>
+      </c>
+      <c r="C71">
+        <v>15377669.999999996</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <v>44</v>
+      </c>
+      <c r="B72" t="s">
+        <v>295</v>
+      </c>
+      <c r="C72">
+        <v>15683777.999999993</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A73">
+        <v>45</v>
+      </c>
+      <c r="B73" t="s">
+        <v>295</v>
+      </c>
+      <c r="C73">
+        <v>15989180</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A74">
+        <v>46</v>
+      </c>
+      <c r="B74" t="s">
+        <v>295</v>
+      </c>
+      <c r="C74">
+        <v>16184168</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A75">
+        <v>47</v>
+      </c>
+      <c r="B75" t="s">
+        <v>295</v>
+      </c>
+      <c r="C75">
+        <v>16377410</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A76">
+        <v>48</v>
+      </c>
+      <c r="B76" t="s">
+        <v>295</v>
+      </c>
+      <c r="C76">
+        <v>16570199.000000002</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A77">
+        <v>49</v>
+      </c>
+      <c r="B77" t="s">
+        <v>295</v>
+      </c>
+      <c r="C77">
+        <v>16760800.000000002</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A78">
+        <v>50</v>
+      </c>
+      <c r="B78" t="s">
+        <v>295</v>
+      </c>
+      <c r="C78">
+        <v>16949850.000000004</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A79">
+        <v>51</v>
+      </c>
+      <c r="B79" t="s">
+        <v>295</v>
+      </c>
+      <c r="C79">
+        <v>17136782</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A80">
+        <v>52</v>
+      </c>
+      <c r="B80" t="s">
+        <v>295</v>
+      </c>
+      <c r="C80">
+        <v>17321029.000000004</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A81">
+        <v>53</v>
+      </c>
+      <c r="B81" t="s">
+        <v>295</v>
+      </c>
+      <c r="C81">
+        <v>17503120.000000004</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A82">
+        <v>54</v>
+      </c>
+      <c r="B82" t="s">
+        <v>295</v>
+      </c>
+      <c r="C82">
+        <v>17681895.000000004</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A83">
+        <v>55</v>
+      </c>
+      <c r="B83" t="s">
+        <v>295</v>
+      </c>
+      <c r="C83">
+        <v>17865770</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A84">
+        <v>56</v>
+      </c>
+      <c r="B84" t="s">
+        <v>295</v>
+      </c>
+      <c r="C84">
+        <v>18319121</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A85">
+        <v>57</v>
+      </c>
+      <c r="B85" t="s">
+        <v>295</v>
+      </c>
+      <c r="C85">
+        <v>18780336</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A86">
+        <v>58</v>
+      </c>
+      <c r="B86" t="s">
+        <v>295</v>
+      </c>
+      <c r="C86">
+        <v>19249870.999999996</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A87">
+        <v>59</v>
+      </c>
+      <c r="B87" t="s">
+        <v>295</v>
+      </c>
+      <c r="C87">
+        <v>19727595.999999996</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A88">
+        <v>60</v>
+      </c>
+      <c r="B88" t="s">
+        <v>295</v>
+      </c>
+      <c r="C88">
+        <v>20213324.999999996</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A89">
+        <v>61</v>
+      </c>
+      <c r="B89" t="s">
+        <v>295</v>
+      </c>
+      <c r="C89">
+        <v>20706327.999999993</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A90">
+        <v>62</v>
+      </c>
+      <c r="B90" t="s">
+        <v>295</v>
+      </c>
+      <c r="C90">
+        <v>21207289.999999993</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A91">
+        <v>63</v>
+      </c>
+      <c r="B91" t="s">
+        <v>295</v>
+      </c>
+      <c r="C91">
+        <v>21715835.999999993</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A92">
+        <v>64</v>
+      </c>
+      <c r="B92" t="s">
+        <v>295</v>
+      </c>
+      <c r="C92">
+        <v>22232001.999999989</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A93">
+        <v>65</v>
+      </c>
+      <c r="B93" t="s">
+        <v>295</v>
+      </c>
+      <c r="C93">
+        <v>22744700</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A94">
+        <v>66</v>
+      </c>
+      <c r="B94" t="s">
+        <v>295</v>
+      </c>
+      <c r="C94">
+        <v>22949433</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A95">
+        <v>67</v>
+      </c>
+      <c r="B95" t="s">
+        <v>295</v>
+      </c>
+      <c r="C95">
+        <v>23150968</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A96">
+        <v>68</v>
+      </c>
+      <c r="B96" t="s">
+        <v>295</v>
+      </c>
+      <c r="C96">
+        <v>23348214.999999996</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A97">
+        <v>69</v>
+      </c>
+      <c r="B97" t="s">
+        <v>295</v>
+      </c>
+      <c r="C97">
+        <v>23540975.999999993</v>
+      </c>
+      <c r="D97">
+        <v>54653</v>
+      </c>
+      <c r="E97">
+        <f t="shared" ref="E97:E122" si="1">C97/D97</f>
+        <v>430.73529357949229</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A98">
+        <v>70</v>
+      </c>
+      <c r="B98" t="s">
+        <v>295</v>
+      </c>
+      <c r="C98">
+        <v>23730724.999999993</v>
+      </c>
+      <c r="D98">
+        <v>55664</v>
+      </c>
+      <c r="E98">
+        <f t="shared" si="1"/>
+        <v>426.32087165852244</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A99">
+        <v>71</v>
+      </c>
+      <c r="B99" t="s">
+        <v>295</v>
+      </c>
+      <c r="C99">
+        <v>23683043.999999989</v>
+      </c>
+      <c r="D99">
+        <v>53935</v>
+      </c>
+      <c r="E99">
+        <f t="shared" si="1"/>
+        <v>439.10343932511336</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A100">
+        <v>72</v>
+      </c>
+      <c r="B100" t="s">
+        <v>295</v>
+      </c>
+      <c r="C100">
+        <v>23628800.999999985</v>
+      </c>
+      <c r="D100">
+        <v>33099</v>
+      </c>
+      <c r="E100">
+        <f t="shared" si="1"/>
+        <v>713.88262485271412</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A101">
+        <v>73</v>
+      </c>
+      <c r="B101" t="s">
+        <v>295</v>
+      </c>
+      <c r="C101">
+        <v>23567743.999999985</v>
+      </c>
+      <c r="D101">
+        <v>44146</v>
+      </c>
+      <c r="E101">
+        <f t="shared" si="1"/>
+        <v>533.85910388257116</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A102">
+        <v>74</v>
+      </c>
+      <c r="B102" t="s">
+        <v>295</v>
+      </c>
+      <c r="C102">
+        <v>23499620.999999985</v>
+      </c>
+      <c r="D102">
+        <v>92800</v>
+      </c>
+      <c r="E102">
+        <f t="shared" si="1"/>
+        <v>253.22867456896535</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A103">
+        <v>75</v>
+      </c>
+      <c r="B103" t="s">
+        <v>295</v>
+      </c>
+      <c r="C103">
+        <v>23421450</v>
+      </c>
+      <c r="D103">
+        <v>61055</v>
+      </c>
+      <c r="E103">
+        <f t="shared" si="1"/>
+        <v>383.6123167635738</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A104">
+        <v>76</v>
+      </c>
+      <c r="B104" t="s">
+        <v>295</v>
+      </c>
+      <c r="C104">
+        <v>23389810</v>
+      </c>
+      <c r="D104">
+        <v>59639</v>
+      </c>
+      <c r="E104">
+        <f t="shared" si="1"/>
+        <v>392.18984221734098</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A105">
+        <v>77</v>
+      </c>
+      <c r="B105" t="s">
+        <v>295</v>
+      </c>
+      <c r="C105">
+        <v>23350728</v>
+      </c>
+      <c r="D105">
+        <v>49905</v>
+      </c>
+      <c r="E105">
+        <f t="shared" si="1"/>
+        <v>467.90357679591222</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A106">
+        <v>78</v>
+      </c>
+      <c r="B106" t="s">
+        <v>295</v>
+      </c>
+      <c r="C106">
+        <v>23303087.999999993</v>
+      </c>
+      <c r="D106">
+        <v>79183</v>
+      </c>
+      <c r="E106">
+        <f t="shared" si="1"/>
+        <v>294.294078274377</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A107">
+        <v>79</v>
+      </c>
+      <c r="B107" t="s">
+        <v>295</v>
+      </c>
+      <c r="C107">
+        <v>23247277.999999993</v>
+      </c>
+      <c r="D107">
+        <v>77033</v>
+      </c>
+      <c r="E107">
+        <f t="shared" si="1"/>
+        <v>301.78336557059953</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A108">
+        <v>80</v>
+      </c>
+      <c r="B108" t="s">
+        <v>295</v>
+      </c>
+      <c r="C108">
+        <v>23181854.999999993</v>
+      </c>
+      <c r="D108">
+        <v>75787</v>
+      </c>
+      <c r="E108">
+        <f t="shared" si="1"/>
+        <v>305.88168155488398</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A109">
+        <v>81</v>
+      </c>
+      <c r="B109" t="s">
+        <v>295</v>
+      </c>
+      <c r="C109">
+        <v>23072399.999999993</v>
+      </c>
+      <c r="D109">
+        <v>86406</v>
+      </c>
+      <c r="E109">
+        <f t="shared" si="1"/>
+        <v>267.02312339420865</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A110">
+        <v>82</v>
+      </c>
+      <c r="B110" t="s">
+        <v>295</v>
+      </c>
+      <c r="C110">
+        <v>22954414.999999985</v>
+      </c>
+      <c r="D110">
+        <v>59940</v>
+      </c>
+      <c r="E110">
+        <f t="shared" si="1"/>
+        <v>382.95653987320628</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A111">
+        <v>83</v>
+      </c>
+      <c r="B111" t="s">
+        <v>295</v>
+      </c>
+      <c r="C111">
+        <v>22827229.999999985</v>
+      </c>
+      <c r="D111">
+        <v>62874</v>
+      </c>
+      <c r="E111">
+        <f t="shared" si="1"/>
+        <v>363.06311034767924</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A112">
+        <v>84</v>
+      </c>
+      <c r="B112" t="s">
+        <v>295</v>
+      </c>
+      <c r="C112">
+        <v>22690529.999999981</v>
+      </c>
+      <c r="D112">
+        <v>66361</v>
+      </c>
+      <c r="E112">
+        <f t="shared" si="1"/>
+        <v>341.92567923931199</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A113">
+        <v>85</v>
+      </c>
+      <c r="B113" t="s">
+        <v>295</v>
+      </c>
+      <c r="C113">
+        <v>22236000</v>
+      </c>
+      <c r="D113">
+        <v>77284</v>
+      </c>
+      <c r="E113">
+        <f t="shared" si="1"/>
+        <v>287.71802701723516</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A114">
+        <v>86</v>
+      </c>
+      <c r="B114" t="s">
+        <v>295</v>
+      </c>
+      <c r="C114">
+        <v>22078000</v>
+      </c>
+      <c r="D114">
+        <v>72814</v>
+      </c>
+      <c r="E114">
+        <f t="shared" si="1"/>
+        <v>303.21092097673522</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A115">
+        <v>87</v>
+      </c>
+      <c r="B115" t="s">
+        <v>295</v>
+      </c>
+      <c r="C115">
+        <v>21926000</v>
+      </c>
+      <c r="D115">
+        <v>83979</v>
+      </c>
+      <c r="E115">
+        <f t="shared" si="1"/>
+        <v>261.08908179425811</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A116">
+        <v>88</v>
+      </c>
+      <c r="B116" t="s">
+        <v>295</v>
+      </c>
+      <c r="C116">
+        <v>21780000</v>
+      </c>
+      <c r="D116">
+        <v>76072</v>
+      </c>
+      <c r="E116">
+        <f t="shared" si="1"/>
+        <v>286.30770848669681</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A117">
+        <v>89</v>
+      </c>
+      <c r="B117" t="s">
+        <v>295</v>
+      </c>
+      <c r="C117">
+        <v>21639000</v>
+      </c>
+      <c r="D117">
+        <v>79850</v>
+      </c>
+      <c r="E117">
+        <f t="shared" si="1"/>
+        <v>270.99561678146523</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A118">
+        <v>90</v>
+      </c>
+      <c r="B118" t="s">
+        <v>295</v>
+      </c>
+      <c r="C118">
+        <v>21503000</v>
+      </c>
+      <c r="D118">
+        <v>79079</v>
+      </c>
+      <c r="E118">
+        <f t="shared" si="1"/>
+        <v>271.91795546225927</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A119">
+        <v>91</v>
+      </c>
+      <c r="B119" t="s">
+        <v>295</v>
+      </c>
+      <c r="C119">
+        <v>21430000</v>
+      </c>
+      <c r="D119">
+        <v>76496</v>
+      </c>
+      <c r="E119">
+        <f t="shared" si="1"/>
+        <v>280.14536707801716</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A120">
+        <v>92</v>
+      </c>
+      <c r="B120" t="s">
+        <v>295</v>
+      </c>
+      <c r="C120">
+        <v>21441000</v>
+      </c>
+      <c r="D120">
+        <v>72301</v>
+      </c>
+      <c r="E120">
+        <f t="shared" si="1"/>
+        <v>296.55191491127368</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A121">
+        <v>93</v>
+      </c>
+      <c r="B121" t="s">
+        <v>295</v>
+      </c>
+      <c r="C121">
+        <v>21448000</v>
+      </c>
+      <c r="D121">
+        <v>71551</v>
+      </c>
+      <c r="E121">
+        <f t="shared" si="1"/>
+        <v>299.75821442048328</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A122">
+        <v>94</v>
+      </c>
+      <c r="B122" t="s">
+        <v>295</v>
+      </c>
+      <c r="C122">
+        <v>21446000</v>
+      </c>
+      <c r="D122">
+        <v>70439</v>
+      </c>
+      <c r="E122">
+        <f t="shared" si="1"/>
+        <v>304.46201678047674</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A123">
+        <v>95</v>
+      </c>
+      <c r="B123" t="s">
+        <v>295</v>
+      </c>
+      <c r="C123">
+        <v>21438000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R33"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
@@ -5371,9 +7139,210 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="13.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>311</v>
+      </c>
+      <c r="C1" t="s">
+        <v>312</v>
+      </c>
+      <c r="D1" t="s">
+        <v>313</v>
+      </c>
+      <c r="E1" t="s">
+        <v>314</v>
+      </c>
+      <c r="F1" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>94</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K9" sqref="K9:K10"/>
     </sheetView>
   </sheetViews>
@@ -6227,13 +8196,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="A1:I33"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -6977,7 +8944,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G33"/>
   <sheetViews>
@@ -7731,1756 +9698,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E123"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B40" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B70" sqref="B70"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="2" width="11.375" customWidth="1"/>
-    <col min="3" max="3" width="11.25" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>293</v>
-      </c>
-      <c r="C1" t="s">
-        <v>296</v>
-      </c>
-      <c r="D1" t="s">
-        <v>297</v>
-      </c>
-      <c r="E1" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>35</v>
-      </c>
-      <c r="B2" t="s">
-        <v>294</v>
-      </c>
-      <c r="C2">
-        <v>5876050</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>36</v>
-      </c>
-      <c r="B3" t="s">
-        <v>294</v>
-      </c>
-      <c r="C3">
-        <v>6196716</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>37</v>
-      </c>
-      <c r="B4" t="s">
-        <v>294</v>
-      </c>
-      <c r="C4">
-        <v>6531840</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>38</v>
-      </c>
-      <c r="B5" t="s">
-        <v>294</v>
-      </c>
-      <c r="C5">
-        <v>6881821</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>39</v>
-      </c>
-      <c r="B6" t="s">
-        <v>294</v>
-      </c>
-      <c r="C6">
-        <v>7247396.0000000009</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>40</v>
-      </c>
-      <c r="B7" t="s">
-        <v>294</v>
-      </c>
-      <c r="C7">
-        <v>7628985.0000000009</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>41</v>
-      </c>
-      <c r="B8" t="s">
-        <v>294</v>
-      </c>
-      <c r="C8">
-        <v>8027360.0000000019</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>42</v>
-      </c>
-      <c r="B9" t="s">
-        <v>294</v>
-      </c>
-      <c r="C9">
-        <v>8443321.0000000037</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>43</v>
-      </c>
-      <c r="B10" t="s">
-        <v>294</v>
-      </c>
-      <c r="C10">
-        <v>8877330.0000000037</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>44</v>
-      </c>
-      <c r="B11" t="s">
-        <v>294</v>
-      </c>
-      <c r="C11">
-        <v>9330222.0000000037</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>45</v>
-      </c>
-      <c r="B12" t="s">
-        <v>294</v>
-      </c>
-      <c r="C12">
-        <v>9799820</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>46</v>
-      </c>
-      <c r="B13" t="s">
-        <v>294</v>
-      </c>
-      <c r="C13">
-        <v>10303832</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>47</v>
-      </c>
-      <c r="B14" t="s">
-        <v>294</v>
-      </c>
-      <c r="C14">
-        <v>10827590</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>48</v>
-      </c>
-      <c r="B15" t="s">
-        <v>294</v>
-      </c>
-      <c r="C15">
-        <v>11372800.999999998</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>49</v>
-      </c>
-      <c r="B16" t="s">
-        <v>294</v>
-      </c>
-      <c r="C16">
-        <v>11939199.999999998</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>50</v>
-      </c>
-      <c r="B17" t="s">
-        <v>294</v>
-      </c>
-      <c r="C17">
-        <v>12528149.999999998</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>51</v>
-      </c>
-      <c r="B18" t="s">
-        <v>294</v>
-      </c>
-      <c r="C18">
-        <v>13140217.999999998</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>52</v>
-      </c>
-      <c r="B19" t="s">
-        <v>294</v>
-      </c>
-      <c r="C19">
-        <v>13775970.999999996</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>53</v>
-      </c>
-      <c r="B20" t="s">
-        <v>294</v>
-      </c>
-      <c r="C20">
-        <v>14436879.999999996</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <v>54</v>
-      </c>
-      <c r="B21" t="s">
-        <v>294</v>
-      </c>
-      <c r="C21">
-        <v>15123104.999999996</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22">
-        <v>55</v>
-      </c>
-      <c r="B22" t="s">
-        <v>294</v>
-      </c>
-      <c r="C22">
-        <v>15843230</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23">
-        <v>56</v>
-      </c>
-      <c r="B23" t="s">
-        <v>294</v>
-      </c>
-      <c r="C23">
-        <v>16707879.000000002</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24">
-        <v>57</v>
-      </c>
-      <c r="B24" t="s">
-        <v>294</v>
-      </c>
-      <c r="C24">
-        <v>17615664</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25">
-        <v>58</v>
-      </c>
-      <c r="B25" t="s">
-        <v>294</v>
-      </c>
-      <c r="C25">
-        <v>18569129.000000004</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26">
-        <v>59</v>
-      </c>
-      <c r="B26" t="s">
-        <v>294</v>
-      </c>
-      <c r="C26">
-        <v>19570404.000000004</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27">
-        <v>60</v>
-      </c>
-      <c r="B27" t="s">
-        <v>294</v>
-      </c>
-      <c r="C27">
-        <v>20621675.000000004</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28">
-        <v>61</v>
-      </c>
-      <c r="B28" t="s">
-        <v>294</v>
-      </c>
-      <c r="C28">
-        <v>21724672.000000007</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29">
-        <v>62</v>
-      </c>
-      <c r="B29" t="s">
-        <v>294</v>
-      </c>
-      <c r="C29">
-        <v>22882710.000000007</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>63</v>
-      </c>
-      <c r="B30" t="s">
-        <v>294</v>
-      </c>
-      <c r="C30">
-        <v>24098164.000000007</v>
-      </c>
-      <c r="E30" s="1"/>
-    </row>
-    <row r="31" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>64</v>
-      </c>
-      <c r="B31" t="s">
-        <v>294</v>
-      </c>
-      <c r="C31">
-        <v>25373998.000000011</v>
-      </c>
-      <c r="E31" s="1"/>
-    </row>
-    <row r="32" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>65</v>
-      </c>
-      <c r="B32" t="s">
-        <v>294</v>
-      </c>
-      <c r="C32">
-        <v>26700300</v>
-      </c>
-      <c r="E32" s="1"/>
-    </row>
-    <row r="33" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>66</v>
-      </c>
-      <c r="B33" t="s">
-        <v>294</v>
-      </c>
-      <c r="C33">
-        <v>27711567</v>
-      </c>
-      <c r="E33" s="1"/>
-    </row>
-    <row r="34" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>67</v>
-      </c>
-      <c r="B34" t="s">
-        <v>294</v>
-      </c>
-      <c r="C34">
-        <v>28757032</v>
-      </c>
-      <c r="E34" s="1"/>
-    </row>
-    <row r="35" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>68</v>
-      </c>
-      <c r="B35" t="s">
-        <v>294</v>
-      </c>
-      <c r="C35">
-        <v>29836785.000000004</v>
-      </c>
-      <c r="E35" s="1"/>
-    </row>
-    <row r="36" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>69</v>
-      </c>
-      <c r="B36" t="s">
-        <v>294</v>
-      </c>
-      <c r="C36">
-        <v>30952024.000000007</v>
-      </c>
-      <c r="D36">
-        <v>46918</v>
-      </c>
-      <c r="E36" s="1">
-        <f t="shared" ref="E36:E61" si="0">C36/D36</f>
-        <v>659.70467624365926</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>70</v>
-      </c>
-      <c r="B37" t="s">
-        <v>294</v>
-      </c>
-      <c r="C37">
-        <v>32106275.000000007</v>
-      </c>
-      <c r="D37">
-        <v>47249</v>
-      </c>
-      <c r="E37" s="1">
-        <f t="shared" si="0"/>
-        <v>679.51226480983735</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>71</v>
-      </c>
-      <c r="B38" t="s">
-        <v>294</v>
-      </c>
-      <c r="C38">
-        <v>32974956.000000011</v>
-      </c>
-      <c r="D38">
-        <v>46102</v>
-      </c>
-      <c r="E38" s="1">
-        <f t="shared" si="0"/>
-        <v>715.26085636198025</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>72</v>
-      </c>
-      <c r="B39" t="s">
-        <v>294</v>
-      </c>
-      <c r="C39">
-        <v>33862199.000000015</v>
-      </c>
-      <c r="D39">
-        <v>33141</v>
-      </c>
-      <c r="E39" s="1">
-        <f t="shared" si="0"/>
-        <v>1021.7615340514775</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>73</v>
-      </c>
-      <c r="B40" t="s">
-        <v>294</v>
-      </c>
-      <c r="C40">
-        <v>34768256.000000015</v>
-      </c>
-      <c r="D40">
-        <v>60228</v>
-      </c>
-      <c r="E40" s="1">
-        <f t="shared" si="0"/>
-        <v>577.27727967058536</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>74</v>
-      </c>
-      <c r="B41" t="s">
-        <v>294</v>
-      </c>
-      <c r="C41">
-        <v>35693379.000000015</v>
-      </c>
-      <c r="D41">
-        <v>100804</v>
-      </c>
-      <c r="E41" s="1">
-        <f t="shared" si="0"/>
-        <v>354.08693107416389</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42">
-        <v>75</v>
-      </c>
-      <c r="B42" t="s">
-        <v>294</v>
-      </c>
-      <c r="C42">
-        <v>36633550</v>
-      </c>
-      <c r="D42">
-        <v>52693</v>
-      </c>
-      <c r="E42">
-        <f t="shared" si="0"/>
-        <v>695.22612111665683</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A43">
-        <v>76</v>
-      </c>
-      <c r="B43" t="s">
-        <v>294</v>
-      </c>
-      <c r="C43">
-        <v>37680190</v>
-      </c>
-      <c r="D43">
-        <v>52096</v>
-      </c>
-      <c r="E43">
-        <f t="shared" si="0"/>
-        <v>723.2837453931204</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A44">
-        <v>77</v>
-      </c>
-      <c r="B44" t="s">
-        <v>294</v>
-      </c>
-      <c r="C44">
-        <v>38752272</v>
-      </c>
-      <c r="D44">
-        <v>39130</v>
-      </c>
-      <c r="E44">
-        <f t="shared" si="0"/>
-        <v>990.34684385382059</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A45">
-        <v>78</v>
-      </c>
-      <c r="B45" t="s">
-        <v>294</v>
-      </c>
-      <c r="C45">
-        <v>39848912.000000007</v>
-      </c>
-      <c r="D45">
-        <v>60658</v>
-      </c>
-      <c r="E45">
-        <f t="shared" si="0"/>
-        <v>656.94404695176252</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A46">
-        <v>79</v>
-      </c>
-      <c r="B46" t="s">
-        <v>294</v>
-      </c>
-      <c r="C46">
-        <v>40971722.000000007</v>
-      </c>
-      <c r="D46">
-        <v>55675</v>
-      </c>
-      <c r="E46">
-        <f t="shared" si="0"/>
-        <v>735.90879209699165</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A47">
-        <v>80</v>
-      </c>
-      <c r="B47" t="s">
-        <v>294</v>
-      </c>
-      <c r="C47">
-        <v>42119145.000000007</v>
-      </c>
-      <c r="D47">
-        <v>55178</v>
-      </c>
-      <c r="E47">
-        <f t="shared" si="0"/>
-        <v>763.33221573815661</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A48">
-        <v>81</v>
-      </c>
-      <c r="B48" t="s">
-        <v>294</v>
-      </c>
-      <c r="C48">
-        <v>43227600.000000007</v>
-      </c>
-      <c r="D48">
-        <v>66708</v>
-      </c>
-      <c r="E48">
-        <f t="shared" si="0"/>
-        <v>648.0122324159023</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A49">
-        <v>82</v>
-      </c>
-      <c r="B49" t="s">
-        <v>294</v>
-      </c>
-      <c r="C49">
-        <v>44360585.000000007</v>
-      </c>
-      <c r="D49">
-        <v>48180</v>
-      </c>
-      <c r="E49">
-        <f t="shared" si="0"/>
-        <v>920.72613117476146</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A50">
-        <v>83</v>
-      </c>
-      <c r="B50" t="s">
-        <v>294</v>
-      </c>
-      <c r="C50">
-        <v>45517770.000000015</v>
-      </c>
-      <c r="D50">
-        <v>49900</v>
-      </c>
-      <c r="E50">
-        <f t="shared" si="0"/>
-        <v>912.17975951903838</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A51">
-        <v>84</v>
-      </c>
-      <c r="B51" t="s">
-        <v>294</v>
-      </c>
-      <c r="C51">
-        <v>46699470.000000015</v>
-      </c>
-      <c r="D51">
-        <v>54278</v>
-      </c>
-      <c r="E51">
-        <f t="shared" si="0"/>
-        <v>860.375658646229</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A52">
-        <v>85</v>
-      </c>
-      <c r="B52" t="s">
-        <v>294</v>
-      </c>
-      <c r="C52">
-        <v>48260000</v>
-      </c>
-      <c r="D52">
-        <v>57986</v>
-      </c>
-      <c r="E52">
-        <f t="shared" si="0"/>
-        <v>832.26985824164456</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A53">
-        <v>86</v>
-      </c>
-      <c r="B53" t="s">
-        <v>294</v>
-      </c>
-      <c r="C53">
-        <v>49288000</v>
-      </c>
-      <c r="D53">
-        <v>60662</v>
-      </c>
-      <c r="E53">
-        <f t="shared" si="0"/>
-        <v>812.50206059806794</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A54">
-        <v>87</v>
-      </c>
-      <c r="B54" t="s">
-        <v>294</v>
-      </c>
-      <c r="C54">
-        <v>50340000</v>
-      </c>
-      <c r="D54">
-        <v>77271</v>
-      </c>
-      <c r="E54">
-        <f t="shared" si="0"/>
-        <v>651.47338587568424</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A55">
-        <v>88</v>
-      </c>
-      <c r="B55" t="s">
-        <v>294</v>
-      </c>
-      <c r="C55">
-        <v>51416000</v>
-      </c>
-      <c r="D55">
-        <v>74398</v>
-      </c>
-      <c r="E55">
-        <f t="shared" si="0"/>
-        <v>691.09384660877981</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A56">
-        <v>89</v>
-      </c>
-      <c r="B56" t="s">
-        <v>294</v>
-      </c>
-      <c r="C56">
-        <v>52519000</v>
-      </c>
-      <c r="D56">
-        <v>72441</v>
-      </c>
-      <c r="E56">
-        <f t="shared" si="0"/>
-        <v>724.98999185544096</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A57">
-        <v>90</v>
-      </c>
-      <c r="B57" t="s">
-        <v>294</v>
-      </c>
-      <c r="C57">
-        <v>53647000</v>
-      </c>
-      <c r="D57">
-        <v>71461</v>
-      </c>
-      <c r="E57">
-        <f t="shared" si="0"/>
-        <v>750.71717440282112</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A58">
-        <v>91</v>
-      </c>
-      <c r="B58" t="s">
-        <v>294</v>
-      </c>
-      <c r="C58">
-        <v>54607000</v>
-      </c>
-      <c r="D58">
-        <v>69567</v>
-      </c>
-      <c r="E58">
-        <f t="shared" si="0"/>
-        <v>784.9555105150431</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A59">
-        <v>92</v>
-      </c>
-      <c r="B59" t="s">
-        <v>294</v>
-      </c>
-      <c r="C59">
-        <v>55502000</v>
-      </c>
-      <c r="D59">
-        <v>68058</v>
-      </c>
-      <c r="E59">
-        <f t="shared" si="0"/>
-        <v>815.51030003820267</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A60">
-        <v>93</v>
-      </c>
-      <c r="B60" t="s">
-        <v>294</v>
-      </c>
-      <c r="C60">
-        <v>56408000</v>
-      </c>
-      <c r="D60">
-        <v>67482</v>
-      </c>
-      <c r="E60">
-        <f t="shared" si="0"/>
-        <v>835.89697993539016</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A61">
-        <v>94</v>
-      </c>
-      <c r="B61" t="s">
-        <v>294</v>
-      </c>
-      <c r="C61">
-        <v>57327000</v>
-      </c>
-      <c r="D61">
-        <v>67177</v>
-      </c>
-      <c r="E61">
-        <f t="shared" si="0"/>
-        <v>853.37243401759531</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A62">
-        <v>95</v>
-      </c>
-      <c r="B62" t="s">
-        <v>294</v>
-      </c>
-      <c r="C62">
-        <v>58220000</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A63">
-        <v>35</v>
-      </c>
-      <c r="B63" t="s">
-        <v>295</v>
-      </c>
-      <c r="C63">
-        <v>13078950</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A64">
-        <v>36</v>
-      </c>
-      <c r="B64" t="s">
-        <v>295</v>
-      </c>
-      <c r="C64">
-        <v>13351284</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A65">
-        <v>37</v>
-      </c>
-      <c r="B65" t="s">
-        <v>295</v>
-      </c>
-      <c r="C65">
-        <v>13628160</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A66">
-        <v>38</v>
-      </c>
-      <c r="B66" t="s">
-        <v>295</v>
-      </c>
-      <c r="C66">
-        <v>13909179</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A67">
-        <v>39</v>
-      </c>
-      <c r="B67" t="s">
-        <v>295</v>
-      </c>
-      <c r="C67">
-        <v>14194603.999999996</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A68">
-        <v>40</v>
-      </c>
-      <c r="B68" t="s">
-        <v>295</v>
-      </c>
-      <c r="C68">
-        <v>14484014.999999998</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A69">
-        <v>41</v>
-      </c>
-      <c r="B69" t="s">
-        <v>295</v>
-      </c>
-      <c r="C69">
-        <v>14777639.999999996</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A70">
-        <v>42</v>
-      </c>
-      <c r="B70" t="s">
-        <v>295</v>
-      </c>
-      <c r="C70">
-        <v>15075678.999999994</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A71">
-        <v>43</v>
-      </c>
-      <c r="B71" t="s">
-        <v>295</v>
-      </c>
-      <c r="C71">
-        <v>15377669.999999996</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A72">
-        <v>44</v>
-      </c>
-      <c r="B72" t="s">
-        <v>295</v>
-      </c>
-      <c r="C72">
-        <v>15683777.999999993</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A73">
-        <v>45</v>
-      </c>
-      <c r="B73" t="s">
-        <v>295</v>
-      </c>
-      <c r="C73">
-        <v>15989180</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A74">
-        <v>46</v>
-      </c>
-      <c r="B74" t="s">
-        <v>295</v>
-      </c>
-      <c r="C74">
-        <v>16184168</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A75">
-        <v>47</v>
-      </c>
-      <c r="B75" t="s">
-        <v>295</v>
-      </c>
-      <c r="C75">
-        <v>16377410</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A76">
-        <v>48</v>
-      </c>
-      <c r="B76" t="s">
-        <v>295</v>
-      </c>
-      <c r="C76">
-        <v>16570199.000000002</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A77">
-        <v>49</v>
-      </c>
-      <c r="B77" t="s">
-        <v>295</v>
-      </c>
-      <c r="C77">
-        <v>16760800.000000002</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A78">
-        <v>50</v>
-      </c>
-      <c r="B78" t="s">
-        <v>295</v>
-      </c>
-      <c r="C78">
-        <v>16949850.000000004</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A79">
-        <v>51</v>
-      </c>
-      <c r="B79" t="s">
-        <v>295</v>
-      </c>
-      <c r="C79">
-        <v>17136782</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A80">
-        <v>52</v>
-      </c>
-      <c r="B80" t="s">
-        <v>295</v>
-      </c>
-      <c r="C80">
-        <v>17321029.000000004</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A81">
-        <v>53</v>
-      </c>
-      <c r="B81" t="s">
-        <v>295</v>
-      </c>
-      <c r="C81">
-        <v>17503120.000000004</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A82">
-        <v>54</v>
-      </c>
-      <c r="B82" t="s">
-        <v>295</v>
-      </c>
-      <c r="C82">
-        <v>17681895.000000004</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A83">
-        <v>55</v>
-      </c>
-      <c r="B83" t="s">
-        <v>295</v>
-      </c>
-      <c r="C83">
-        <v>17865770</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A84">
-        <v>56</v>
-      </c>
-      <c r="B84" t="s">
-        <v>295</v>
-      </c>
-      <c r="C84">
-        <v>18319121</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A85">
-        <v>57</v>
-      </c>
-      <c r="B85" t="s">
-        <v>295</v>
-      </c>
-      <c r="C85">
-        <v>18780336</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A86">
-        <v>58</v>
-      </c>
-      <c r="B86" t="s">
-        <v>295</v>
-      </c>
-      <c r="C86">
-        <v>19249870.999999996</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A87">
-        <v>59</v>
-      </c>
-      <c r="B87" t="s">
-        <v>295</v>
-      </c>
-      <c r="C87">
-        <v>19727595.999999996</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A88">
-        <v>60</v>
-      </c>
-      <c r="B88" t="s">
-        <v>295</v>
-      </c>
-      <c r="C88">
-        <v>20213324.999999996</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A89">
-        <v>61</v>
-      </c>
-      <c r="B89" t="s">
-        <v>295</v>
-      </c>
-      <c r="C89">
-        <v>20706327.999999993</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A90">
-        <v>62</v>
-      </c>
-      <c r="B90" t="s">
-        <v>295</v>
-      </c>
-      <c r="C90">
-        <v>21207289.999999993</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A91">
-        <v>63</v>
-      </c>
-      <c r="B91" t="s">
-        <v>295</v>
-      </c>
-      <c r="C91">
-        <v>21715835.999999993</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A92">
-        <v>64</v>
-      </c>
-      <c r="B92" t="s">
-        <v>295</v>
-      </c>
-      <c r="C92">
-        <v>22232001.999999989</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A93">
-        <v>65</v>
-      </c>
-      <c r="B93" t="s">
-        <v>295</v>
-      </c>
-      <c r="C93">
-        <v>22744700</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A94">
-        <v>66</v>
-      </c>
-      <c r="B94" t="s">
-        <v>295</v>
-      </c>
-      <c r="C94">
-        <v>22949433</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A95">
-        <v>67</v>
-      </c>
-      <c r="B95" t="s">
-        <v>295</v>
-      </c>
-      <c r="C95">
-        <v>23150968</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A96">
-        <v>68</v>
-      </c>
-      <c r="B96" t="s">
-        <v>295</v>
-      </c>
-      <c r="C96">
-        <v>23348214.999999996</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A97">
-        <v>69</v>
-      </c>
-      <c r="B97" t="s">
-        <v>295</v>
-      </c>
-      <c r="C97">
-        <v>23540975.999999993</v>
-      </c>
-      <c r="D97">
-        <v>54653</v>
-      </c>
-      <c r="E97">
-        <f t="shared" ref="E97:E122" si="1">C97/D97</f>
-        <v>430.73529357949229</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A98">
-        <v>70</v>
-      </c>
-      <c r="B98" t="s">
-        <v>295</v>
-      </c>
-      <c r="C98">
-        <v>23730724.999999993</v>
-      </c>
-      <c r="D98">
-        <v>55664</v>
-      </c>
-      <c r="E98">
-        <f t="shared" si="1"/>
-        <v>426.32087165852244</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A99">
-        <v>71</v>
-      </c>
-      <c r="B99" t="s">
-        <v>295</v>
-      </c>
-      <c r="C99">
-        <v>23683043.999999989</v>
-      </c>
-      <c r="D99">
-        <v>53935</v>
-      </c>
-      <c r="E99">
-        <f t="shared" si="1"/>
-        <v>439.10343932511336</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A100">
-        <v>72</v>
-      </c>
-      <c r="B100" t="s">
-        <v>295</v>
-      </c>
-      <c r="C100">
-        <v>23628800.999999985</v>
-      </c>
-      <c r="D100">
-        <v>33099</v>
-      </c>
-      <c r="E100">
-        <f t="shared" si="1"/>
-        <v>713.88262485271412</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A101">
-        <v>73</v>
-      </c>
-      <c r="B101" t="s">
-        <v>295</v>
-      </c>
-      <c r="C101">
-        <v>23567743.999999985</v>
-      </c>
-      <c r="D101">
-        <v>44146</v>
-      </c>
-      <c r="E101">
-        <f t="shared" si="1"/>
-        <v>533.85910388257116</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A102">
-        <v>74</v>
-      </c>
-      <c r="B102" t="s">
-        <v>295</v>
-      </c>
-      <c r="C102">
-        <v>23499620.999999985</v>
-      </c>
-      <c r="D102">
-        <v>92800</v>
-      </c>
-      <c r="E102">
-        <f t="shared" si="1"/>
-        <v>253.22867456896535</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A103">
-        <v>75</v>
-      </c>
-      <c r="B103" t="s">
-        <v>295</v>
-      </c>
-      <c r="C103">
-        <v>23421450</v>
-      </c>
-      <c r="D103">
-        <v>61055</v>
-      </c>
-      <c r="E103">
-        <f t="shared" si="1"/>
-        <v>383.6123167635738</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A104">
-        <v>76</v>
-      </c>
-      <c r="B104" t="s">
-        <v>295</v>
-      </c>
-      <c r="C104">
-        <v>23389810</v>
-      </c>
-      <c r="D104">
-        <v>59639</v>
-      </c>
-      <c r="E104">
-        <f t="shared" si="1"/>
-        <v>392.18984221734098</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A105">
-        <v>77</v>
-      </c>
-      <c r="B105" t="s">
-        <v>295</v>
-      </c>
-      <c r="C105">
-        <v>23350728</v>
-      </c>
-      <c r="D105">
-        <v>49905</v>
-      </c>
-      <c r="E105">
-        <f t="shared" si="1"/>
-        <v>467.90357679591222</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A106">
-        <v>78</v>
-      </c>
-      <c r="B106" t="s">
-        <v>295</v>
-      </c>
-      <c r="C106">
-        <v>23303087.999999993</v>
-      </c>
-      <c r="D106">
-        <v>79183</v>
-      </c>
-      <c r="E106">
-        <f t="shared" si="1"/>
-        <v>294.294078274377</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A107">
-        <v>79</v>
-      </c>
-      <c r="B107" t="s">
-        <v>295</v>
-      </c>
-      <c r="C107">
-        <v>23247277.999999993</v>
-      </c>
-      <c r="D107">
-        <v>77033</v>
-      </c>
-      <c r="E107">
-        <f t="shared" si="1"/>
-        <v>301.78336557059953</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A108">
-        <v>80</v>
-      </c>
-      <c r="B108" t="s">
-        <v>295</v>
-      </c>
-      <c r="C108">
-        <v>23181854.999999993</v>
-      </c>
-      <c r="D108">
-        <v>75787</v>
-      </c>
-      <c r="E108">
-        <f t="shared" si="1"/>
-        <v>305.88168155488398</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A109">
-        <v>81</v>
-      </c>
-      <c r="B109" t="s">
-        <v>295</v>
-      </c>
-      <c r="C109">
-        <v>23072399.999999993</v>
-      </c>
-      <c r="D109">
-        <v>86406</v>
-      </c>
-      <c r="E109">
-        <f t="shared" si="1"/>
-        <v>267.02312339420865</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A110">
-        <v>82</v>
-      </c>
-      <c r="B110" t="s">
-        <v>295</v>
-      </c>
-      <c r="C110">
-        <v>22954414.999999985</v>
-      </c>
-      <c r="D110">
-        <v>59940</v>
-      </c>
-      <c r="E110">
-        <f t="shared" si="1"/>
-        <v>382.95653987320628</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A111">
-        <v>83</v>
-      </c>
-      <c r="B111" t="s">
-        <v>295</v>
-      </c>
-      <c r="C111">
-        <v>22827229.999999985</v>
-      </c>
-      <c r="D111">
-        <v>62874</v>
-      </c>
-      <c r="E111">
-        <f t="shared" si="1"/>
-        <v>363.06311034767924</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A112">
-        <v>84</v>
-      </c>
-      <c r="B112" t="s">
-        <v>295</v>
-      </c>
-      <c r="C112">
-        <v>22690529.999999981</v>
-      </c>
-      <c r="D112">
-        <v>66361</v>
-      </c>
-      <c r="E112">
-        <f t="shared" si="1"/>
-        <v>341.92567923931199</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A113">
-        <v>85</v>
-      </c>
-      <c r="B113" t="s">
-        <v>295</v>
-      </c>
-      <c r="C113">
-        <v>22236000</v>
-      </c>
-      <c r="D113">
-        <v>77284</v>
-      </c>
-      <c r="E113">
-        <f t="shared" si="1"/>
-        <v>287.71802701723516</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A114">
-        <v>86</v>
-      </c>
-      <c r="B114" t="s">
-        <v>295</v>
-      </c>
-      <c r="C114">
-        <v>22078000</v>
-      </c>
-      <c r="D114">
-        <v>72814</v>
-      </c>
-      <c r="E114">
-        <f t="shared" si="1"/>
-        <v>303.21092097673522</v>
-      </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A115">
-        <v>87</v>
-      </c>
-      <c r="B115" t="s">
-        <v>295</v>
-      </c>
-      <c r="C115">
-        <v>21926000</v>
-      </c>
-      <c r="D115">
-        <v>83979</v>
-      </c>
-      <c r="E115">
-        <f t="shared" si="1"/>
-        <v>261.08908179425811</v>
-      </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A116">
-        <v>88</v>
-      </c>
-      <c r="B116" t="s">
-        <v>295</v>
-      </c>
-      <c r="C116">
-        <v>21780000</v>
-      </c>
-      <c r="D116">
-        <v>76072</v>
-      </c>
-      <c r="E116">
-        <f t="shared" si="1"/>
-        <v>286.30770848669681</v>
-      </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A117">
-        <v>89</v>
-      </c>
-      <c r="B117" t="s">
-        <v>295</v>
-      </c>
-      <c r="C117">
-        <v>21639000</v>
-      </c>
-      <c r="D117">
-        <v>79850</v>
-      </c>
-      <c r="E117">
-        <f t="shared" si="1"/>
-        <v>270.99561678146523</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A118">
-        <v>90</v>
-      </c>
-      <c r="B118" t="s">
-        <v>295</v>
-      </c>
-      <c r="C118">
-        <v>21503000</v>
-      </c>
-      <c r="D118">
-        <v>79079</v>
-      </c>
-      <c r="E118">
-        <f t="shared" si="1"/>
-        <v>271.91795546225927</v>
-      </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A119">
-        <v>91</v>
-      </c>
-      <c r="B119" t="s">
-        <v>295</v>
-      </c>
-      <c r="C119">
-        <v>21430000</v>
-      </c>
-      <c r="D119">
-        <v>76496</v>
-      </c>
-      <c r="E119">
-        <f t="shared" si="1"/>
-        <v>280.14536707801716</v>
-      </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A120">
-        <v>92</v>
-      </c>
-      <c r="B120" t="s">
-        <v>295</v>
-      </c>
-      <c r="C120">
-        <v>21441000</v>
-      </c>
-      <c r="D120">
-        <v>72301</v>
-      </c>
-      <c r="E120">
-        <f t="shared" si="1"/>
-        <v>296.55191491127368</v>
-      </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A121">
-        <v>93</v>
-      </c>
-      <c r="B121" t="s">
-        <v>295</v>
-      </c>
-      <c r="C121">
-        <v>21448000</v>
-      </c>
-      <c r="D121">
-        <v>71551</v>
-      </c>
-      <c r="E121">
-        <f t="shared" si="1"/>
-        <v>299.75821442048328</v>
-      </c>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A122">
-        <v>94</v>
-      </c>
-      <c r="B122" t="s">
-        <v>295</v>
-      </c>
-      <c r="C122">
-        <v>21446000</v>
-      </c>
-      <c r="D122">
-        <v>70439</v>
-      </c>
-      <c r="E122">
-        <f t="shared" si="1"/>
-        <v>304.46201678047674</v>
-      </c>
-    </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A123">
-        <v>95</v>
-      </c>
-      <c r="B123" t="s">
-        <v>295</v>
-      </c>
-      <c r="C123">
-        <v>21438000</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Added rough weights for 63-68
</commit_message>
<xml_diff>
--- a/Data/MetaData.xlsx
+++ b/Data/MetaData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="6150" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="6150" firstSheet="3" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="CompressedFileNames" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1266" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1294" uniqueCount="320">
   <si>
     <t>Year</t>
   </si>
@@ -976,6 +976,18 @@
   </si>
   <si>
     <t>OthrIncTable</t>
+  </si>
+  <si>
+    <t>P4S1</t>
+  </si>
+  <si>
+    <t>P4S2</t>
+  </si>
+  <si>
+    <t>P4S3</t>
+  </si>
+  <si>
+    <t>P4S4</t>
   </si>
 </sst>
 </file>
@@ -1136,7 +1148,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -1485,8 +1496,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
@@ -2088,11 +2100,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E123"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B50" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F30" sqref="F30:F61"/>
+      <selection pane="bottomRight" activeCell="E30" sqref="E30:E61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2426,7 +2438,7 @@
         <v>22882710.000000007</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>63</v>
       </c>
@@ -2436,9 +2448,15 @@
       <c r="C30">
         <v>24098164.000000007</v>
       </c>
-      <c r="E30" s="1"/>
-    </row>
-    <row r="31" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="D30">
+        <v>73892</v>
+      </c>
+      <c r="E30" s="2">
+        <f t="shared" ref="E30:E61" si="0">C30/D30</f>
+        <v>326.12683375737572</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>64</v>
       </c>
@@ -2448,9 +2466,15 @@
       <c r="C31">
         <v>25373998.000000011</v>
       </c>
-      <c r="E31" s="1"/>
-    </row>
-    <row r="32" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="D31">
+        <v>70684</v>
+      </c>
+      <c r="E31" s="2">
+        <f t="shared" si="0"/>
+        <v>358.97795823665911</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>65</v>
       </c>
@@ -2460,9 +2484,15 @@
       <c r="C32">
         <v>26700300</v>
       </c>
-      <c r="E32" s="1"/>
-    </row>
-    <row r="33" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="D32">
+        <v>13788</v>
+      </c>
+      <c r="E32" s="2">
+        <f t="shared" si="0"/>
+        <v>1936.4882506527415</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>66</v>
       </c>
@@ -2472,9 +2502,15 @@
       <c r="C33">
         <v>27711567</v>
       </c>
-      <c r="E33" s="1"/>
-    </row>
-    <row r="34" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="D33">
+        <v>13984</v>
+      </c>
+      <c r="E33" s="2">
+        <f t="shared" si="0"/>
+        <v>1981.6623998855835</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>67</v>
       </c>
@@ -2484,9 +2520,15 @@
       <c r="C34">
         <v>28757032</v>
       </c>
-      <c r="E34" s="1"/>
-    </row>
-    <row r="35" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="D34">
+        <v>20590</v>
+      </c>
+      <c r="E34" s="2">
+        <f t="shared" si="0"/>
+        <v>1396.6504128217582</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>68</v>
       </c>
@@ -2496,9 +2538,15 @@
       <c r="C35">
         <v>29836785.000000004</v>
       </c>
-      <c r="E35" s="1"/>
-    </row>
-    <row r="36" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="D35">
+        <v>28136</v>
+      </c>
+      <c r="E35" s="2">
+        <f t="shared" si="0"/>
+        <v>1060.4487133920957</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>69</v>
       </c>
@@ -2509,14 +2557,14 @@
         <v>30952024.000000007</v>
       </c>
       <c r="D36">
-        <v>46918</v>
-      </c>
-      <c r="E36" s="1">
-        <f t="shared" ref="E36:E61" si="0">C36/D36</f>
-        <v>659.70467624365926</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+        <v>46930</v>
+      </c>
+      <c r="E36" s="2">
+        <f t="shared" si="0"/>
+        <v>659.53598977200102</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>70</v>
       </c>
@@ -2527,14 +2575,14 @@
         <v>32106275.000000007</v>
       </c>
       <c r="D37">
-        <v>47249</v>
-      </c>
-      <c r="E37" s="1">
+        <v>47255</v>
+      </c>
+      <c r="E37" s="2">
         <f t="shared" si="0"/>
-        <v>679.51226480983735</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+        <v>679.4259866680776</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>71</v>
       </c>
@@ -2545,14 +2593,14 @@
         <v>32974956.000000011</v>
       </c>
       <c r="D38">
-        <v>46102</v>
-      </c>
-      <c r="E38" s="1">
+        <v>46095</v>
+      </c>
+      <c r="E38" s="2">
         <f t="shared" si="0"/>
-        <v>715.26085636198025</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+        <v>715.36947608200478</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>72</v>
       </c>
@@ -2565,12 +2613,12 @@
       <c r="D39">
         <v>33141</v>
       </c>
-      <c r="E39" s="1">
+      <c r="E39" s="2">
         <f t="shared" si="0"/>
         <v>1021.7615340514775</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>73</v>
       </c>
@@ -2583,12 +2631,12 @@
       <c r="D40">
         <v>60228</v>
       </c>
-      <c r="E40" s="1">
+      <c r="E40" s="2">
         <f t="shared" si="0"/>
         <v>577.27727967058536</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>74</v>
       </c>
@@ -2599,11 +2647,11 @@
         <v>35693379.000000015</v>
       </c>
       <c r="D41">
-        <v>100804</v>
-      </c>
-      <c r="E41" s="1">
+        <v>100785</v>
+      </c>
+      <c r="E41" s="2">
         <f t="shared" si="0"/>
-        <v>354.08693107416389</v>
+        <v>354.15368358386678</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
@@ -2619,7 +2667,7 @@
       <c r="D42">
         <v>52693</v>
       </c>
-      <c r="E42">
+      <c r="E42" s="2">
         <f t="shared" si="0"/>
         <v>695.22612111665683</v>
       </c>
@@ -2637,7 +2685,7 @@
       <c r="D43">
         <v>52096</v>
       </c>
-      <c r="E43">
+      <c r="E43" s="2">
         <f t="shared" si="0"/>
         <v>723.2837453931204</v>
       </c>
@@ -2655,7 +2703,7 @@
       <c r="D44">
         <v>39130</v>
       </c>
-      <c r="E44">
+      <c r="E44" s="2">
         <f t="shared" si="0"/>
         <v>990.34684385382059</v>
       </c>
@@ -2673,7 +2721,7 @@
       <c r="D45">
         <v>60658</v>
       </c>
-      <c r="E45">
+      <c r="E45" s="2">
         <f t="shared" si="0"/>
         <v>656.94404695176252</v>
       </c>
@@ -2691,7 +2739,7 @@
       <c r="D46">
         <v>55675</v>
       </c>
-      <c r="E46">
+      <c r="E46" s="2">
         <f t="shared" si="0"/>
         <v>735.90879209699165</v>
       </c>
@@ -2709,7 +2757,7 @@
       <c r="D47">
         <v>55178</v>
       </c>
-      <c r="E47">
+      <c r="E47" s="2">
         <f t="shared" si="0"/>
         <v>763.33221573815661</v>
       </c>
@@ -2727,7 +2775,7 @@
       <c r="D48">
         <v>66708</v>
       </c>
-      <c r="E48">
+      <c r="E48" s="2">
         <f t="shared" si="0"/>
         <v>648.0122324159023</v>
       </c>
@@ -2745,7 +2793,7 @@
       <c r="D49">
         <v>48180</v>
       </c>
-      <c r="E49">
+      <c r="E49" s="2">
         <f t="shared" si="0"/>
         <v>920.72613117476146</v>
       </c>
@@ -2763,7 +2811,7 @@
       <c r="D50">
         <v>49900</v>
       </c>
-      <c r="E50">
+      <c r="E50" s="2">
         <f t="shared" si="0"/>
         <v>912.17975951903838</v>
       </c>
@@ -2781,7 +2829,7 @@
       <c r="D51">
         <v>54278</v>
       </c>
-      <c r="E51">
+      <c r="E51" s="2">
         <f t="shared" si="0"/>
         <v>860.375658646229</v>
       </c>
@@ -2799,7 +2847,7 @@
       <c r="D52">
         <v>57986</v>
       </c>
-      <c r="E52">
+      <c r="E52" s="2">
         <f t="shared" si="0"/>
         <v>832.26985824164456</v>
       </c>
@@ -2817,7 +2865,7 @@
       <c r="D53">
         <v>60662</v>
       </c>
-      <c r="E53">
+      <c r="E53" s="2">
         <f t="shared" si="0"/>
         <v>812.50206059806794</v>
       </c>
@@ -2835,7 +2883,7 @@
       <c r="D54">
         <v>77271</v>
       </c>
-      <c r="E54">
+      <c r="E54" s="2">
         <f t="shared" si="0"/>
         <v>651.47338587568424</v>
       </c>
@@ -2853,7 +2901,7 @@
       <c r="D55">
         <v>74398</v>
       </c>
-      <c r="E55">
+      <c r="E55" s="2">
         <f t="shared" si="0"/>
         <v>691.09384660877981</v>
       </c>
@@ -2871,7 +2919,7 @@
       <c r="D56">
         <v>72441</v>
       </c>
-      <c r="E56">
+      <c r="E56" s="2">
         <f t="shared" si="0"/>
         <v>724.98999185544096</v>
       </c>
@@ -2889,7 +2937,7 @@
       <c r="D57">
         <v>71461</v>
       </c>
-      <c r="E57">
+      <c r="E57" s="2">
         <f t="shared" si="0"/>
         <v>750.71717440282112</v>
       </c>
@@ -2907,7 +2955,7 @@
       <c r="D58">
         <v>69567</v>
       </c>
-      <c r="E58">
+      <c r="E58" s="2">
         <f t="shared" si="0"/>
         <v>784.9555105150431</v>
       </c>
@@ -2925,7 +2973,7 @@
       <c r="D59">
         <v>68058</v>
       </c>
-      <c r="E59">
+      <c r="E59" s="2">
         <f t="shared" si="0"/>
         <v>815.51030003820267</v>
       </c>
@@ -2943,7 +2991,7 @@
       <c r="D60">
         <v>67482</v>
       </c>
-      <c r="E60">
+      <c r="E60" s="2">
         <f t="shared" si="0"/>
         <v>835.89697993539016</v>
       </c>
@@ -2961,7 +3009,7 @@
       <c r="D61">
         <v>67177</v>
       </c>
-      <c r="E61">
+      <c r="E61" s="2">
         <f t="shared" si="0"/>
         <v>853.37243401759531</v>
       </c>
@@ -3175,7 +3223,7 @@
         <v>17321029.000000004</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>53</v>
       </c>
@@ -3186,7 +3234,7 @@
         <v>17503120.000000004</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>54</v>
       </c>
@@ -3197,7 +3245,7 @@
         <v>17681895.000000004</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>55</v>
       </c>
@@ -3208,7 +3256,7 @@
         <v>17865770</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>56</v>
       </c>
@@ -3219,7 +3267,7 @@
         <v>18319121</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>57</v>
       </c>
@@ -3230,7 +3278,7 @@
         <v>18780336</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>58</v>
       </c>
@@ -3241,7 +3289,7 @@
         <v>19249870.999999996</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>59</v>
       </c>
@@ -3252,7 +3300,7 @@
         <v>19727595.999999996</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>60</v>
       </c>
@@ -3263,7 +3311,7 @@
         <v>20213324.999999996</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>61</v>
       </c>
@@ -3274,7 +3322,7 @@
         <v>20706327.999999993</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>62</v>
       </c>
@@ -3285,7 +3333,7 @@
         <v>21207289.999999993</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>63</v>
       </c>
@@ -3295,8 +3343,15 @@
       <c r="C91">
         <v>21715835.999999993</v>
       </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D91">
+        <v>70169</v>
+      </c>
+      <c r="E91">
+        <f t="shared" ref="E91:E96" si="1">C91/D91</f>
+        <v>309.47905770354419</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>64</v>
       </c>
@@ -3306,8 +3361,15 @@
       <c r="C92">
         <v>22232001.999999989</v>
       </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D92">
+        <v>74852</v>
+      </c>
+      <c r="E92">
+        <f t="shared" si="1"/>
+        <v>297.01279858921589</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>65</v>
       </c>
@@ -3317,8 +3379,15 @@
       <c r="C93">
         <v>22744700</v>
       </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D93">
+        <v>16758</v>
+      </c>
+      <c r="E93">
+        <f t="shared" si="1"/>
+        <v>1357.2443012292636</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>66</v>
       </c>
@@ -3328,8 +3397,15 @@
       <c r="C94">
         <v>22949433</v>
       </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D94">
+        <v>17347</v>
+      </c>
+      <c r="E94">
+        <f t="shared" si="1"/>
+        <v>1322.9626448377242</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>67</v>
       </c>
@@ -3339,8 +3415,15 @@
       <c r="C95">
         <v>23150968</v>
       </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D95">
+        <v>25138</v>
+      </c>
+      <c r="E95">
+        <f t="shared" si="1"/>
+        <v>920.95504813429864</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>68</v>
       </c>
@@ -3349,6 +3432,13 @@
       </c>
       <c r="C96">
         <v>23348214.999999996</v>
+      </c>
+      <c r="D96">
+        <v>35647</v>
+      </c>
+      <c r="E96">
+        <f t="shared" si="1"/>
+        <v>654.98400987460366</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.2">
@@ -3362,11 +3452,11 @@
         <v>23540975.999999993</v>
       </c>
       <c r="D97">
-        <v>54653</v>
+        <v>54789</v>
       </c>
       <c r="E97">
-        <f t="shared" ref="E97:E122" si="1">C97/D97</f>
-        <v>430.73529357949229</v>
+        <f>C97/D97</f>
+        <v>429.66610085966147</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.2">
@@ -3380,11 +3470,11 @@
         <v>23730724.999999993</v>
       </c>
       <c r="D98">
-        <v>55664</v>
+        <v>55650</v>
       </c>
       <c r="E98">
-        <f t="shared" si="1"/>
-        <v>426.32087165852244</v>
+        <f t="shared" ref="E98:E122" si="2">C98/D98</f>
+        <v>426.42812219227301</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.2">
@@ -3398,11 +3488,11 @@
         <v>23683043.999999989</v>
       </c>
       <c r="D99">
-        <v>53935</v>
+        <v>53936</v>
       </c>
       <c r="E99">
-        <f t="shared" si="1"/>
-        <v>439.10343932511336</v>
+        <f t="shared" si="2"/>
+        <v>439.09529813111817</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.2">
@@ -3416,11 +3506,11 @@
         <v>23628800.999999985</v>
       </c>
       <c r="D100">
-        <v>33099</v>
+        <v>33117</v>
       </c>
       <c r="E100">
-        <f t="shared" si="1"/>
-        <v>713.88262485271412</v>
+        <f t="shared" si="2"/>
+        <v>713.49461001902296</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.2">
@@ -3437,7 +3527,7 @@
         <v>44146</v>
       </c>
       <c r="E101">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>533.85910388257116</v>
       </c>
     </row>
@@ -3455,7 +3545,7 @@
         <v>92800</v>
       </c>
       <c r="E102">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>253.22867456896535</v>
       </c>
     </row>
@@ -3473,7 +3563,7 @@
         <v>61055</v>
       </c>
       <c r="E103">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>383.6123167635738</v>
       </c>
     </row>
@@ -3491,7 +3581,7 @@
         <v>59639</v>
       </c>
       <c r="E104">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>392.18984221734098</v>
       </c>
     </row>
@@ -3509,7 +3599,7 @@
         <v>49905</v>
       </c>
       <c r="E105">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>467.90357679591222</v>
       </c>
     </row>
@@ -3527,7 +3617,7 @@
         <v>79183</v>
       </c>
       <c r="E106">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>294.294078274377</v>
       </c>
     </row>
@@ -3545,7 +3635,7 @@
         <v>77033</v>
       </c>
       <c r="E107">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>301.78336557059953</v>
       </c>
     </row>
@@ -3563,7 +3653,7 @@
         <v>75787</v>
       </c>
       <c r="E108">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>305.88168155488398</v>
       </c>
     </row>
@@ -3581,7 +3671,7 @@
         <v>86406</v>
       </c>
       <c r="E109">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>267.02312339420865</v>
       </c>
     </row>
@@ -3599,7 +3689,7 @@
         <v>59940</v>
       </c>
       <c r="E110">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>382.95653987320628</v>
       </c>
     </row>
@@ -3617,7 +3707,7 @@
         <v>62874</v>
       </c>
       <c r="E111">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>363.06311034767924</v>
       </c>
     </row>
@@ -3635,7 +3725,7 @@
         <v>66361</v>
       </c>
       <c r="E112">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>341.92567923931199</v>
       </c>
     </row>
@@ -3653,7 +3743,7 @@
         <v>77284</v>
       </c>
       <c r="E113">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>287.71802701723516</v>
       </c>
     </row>
@@ -3671,7 +3761,7 @@
         <v>72814</v>
       </c>
       <c r="E114">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>303.21092097673522</v>
       </c>
     </row>
@@ -3689,7 +3779,7 @@
         <v>83979</v>
       </c>
       <c r="E115">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>261.08908179425811</v>
       </c>
     </row>
@@ -3707,7 +3797,7 @@
         <v>76072</v>
       </c>
       <c r="E116">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>286.30770848669681</v>
       </c>
     </row>
@@ -3725,7 +3815,7 @@
         <v>79850</v>
       </c>
       <c r="E117">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>270.99561678146523</v>
       </c>
     </row>
@@ -3743,7 +3833,7 @@
         <v>79079</v>
       </c>
       <c r="E118">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>271.91795546225927</v>
       </c>
     </row>
@@ -3761,7 +3851,7 @@
         <v>76496</v>
       </c>
       <c r="E119">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>280.14536707801716</v>
       </c>
     </row>
@@ -3779,7 +3869,7 @@
         <v>72301</v>
       </c>
       <c r="E120">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>296.55191491127368</v>
       </c>
     </row>
@@ -3797,7 +3887,7 @@
         <v>71551</v>
       </c>
       <c r="E121">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>299.75821442048328</v>
       </c>
     </row>
@@ -3815,7 +3905,7 @@
         <v>70439</v>
       </c>
       <c r="E122">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>304.46201678047674</v>
       </c>
     </row>
@@ -7141,8 +7231,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -7177,36 +7267,120 @@
       <c r="A2">
         <v>63</v>
       </c>
+      <c r="B2" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>319</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>64</v>
       </c>
+      <c r="B3" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>319</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>65</v>
       </c>
+      <c r="B4" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>319</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>66</v>
       </c>
+      <c r="B5" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>319</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>67</v>
       </c>
+      <c r="B6" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>319</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>68</v>
       </c>
+      <c r="B7" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>319</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>69</v>
       </c>
+      <c r="B8" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>319</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
@@ -7335,6 +7509,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updated for Insurance Tables
</commit_message>
<xml_diff>
--- a/Data/MetaData.xlsx
+++ b/Data/MetaData.xlsx
@@ -21,14 +21,15 @@
     <sheet name="FoodTables" sheetId="10" r:id="rId7"/>
     <sheet name="LoanTables" sheetId="7" r:id="rId8"/>
     <sheet name="HouseTables" sheetId="8" r:id="rId9"/>
-    <sheet name="RegionWeights" sheetId="9" r:id="rId10"/>
+    <sheet name="InsuranceTables" sheetId="12" r:id="rId10"/>
+    <sheet name="RegionWeights" sheetId="9" r:id="rId11"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1294" uniqueCount="320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1330" uniqueCount="325">
   <si>
     <t>Year</t>
   </si>
@@ -988,6 +989,21 @@
   </si>
   <si>
     <t>P4S4</t>
+  </si>
+  <si>
+    <t>InsuredCount</t>
+  </si>
+  <si>
+    <t>InsuranceCosts</t>
+  </si>
+  <si>
+    <t>GovPaid</t>
+  </si>
+  <si>
+    <t>SS1</t>
+  </si>
+  <si>
+    <t>SS2</t>
   </si>
 </sst>
 </file>
@@ -2098,13 +2114,379 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="H33" sqref="H33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="8" max="8" width="13.875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>269</v>
+      </c>
+      <c r="C1" t="s">
+        <v>291</v>
+      </c>
+      <c r="D1" t="s">
+        <v>292</v>
+      </c>
+      <c r="E1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G1" t="s">
+        <v>320</v>
+      </c>
+      <c r="H1" t="s">
+        <v>321</v>
+      </c>
+      <c r="I1" t="s">
+        <v>322</v>
+      </c>
+      <c r="J1" t="s">
+        <v>323</v>
+      </c>
+      <c r="K1" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>90</v>
+      </c>
+      <c r="B29" t="s">
+        <v>276</v>
+      </c>
+      <c r="C29">
+        <v>125311</v>
+      </c>
+      <c r="D29">
+        <v>125317</v>
+      </c>
+      <c r="E29" t="s">
+        <v>66</v>
+      </c>
+      <c r="F29" t="s">
+        <v>67</v>
+      </c>
+      <c r="G29" t="s">
+        <v>277</v>
+      </c>
+      <c r="H29" t="s">
+        <v>70</v>
+      </c>
+      <c r="I29">
+        <v>125312</v>
+      </c>
+      <c r="J29">
+        <v>125313</v>
+      </c>
+      <c r="K29">
+        <v>125314</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>91</v>
+      </c>
+      <c r="B30" t="s">
+        <v>276</v>
+      </c>
+      <c r="C30">
+        <v>125311</v>
+      </c>
+      <c r="D30">
+        <v>125317</v>
+      </c>
+      <c r="E30" t="s">
+        <v>66</v>
+      </c>
+      <c r="F30" t="s">
+        <v>67</v>
+      </c>
+      <c r="G30" t="s">
+        <v>277</v>
+      </c>
+      <c r="H30" t="s">
+        <v>70</v>
+      </c>
+      <c r="I30">
+        <v>125312</v>
+      </c>
+      <c r="J30">
+        <v>125313</v>
+      </c>
+      <c r="K30">
+        <v>125314</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>92</v>
+      </c>
+      <c r="B31" t="s">
+        <v>276</v>
+      </c>
+      <c r="C31">
+        <v>125311</v>
+      </c>
+      <c r="D31">
+        <v>125317</v>
+      </c>
+      <c r="E31" t="s">
+        <v>66</v>
+      </c>
+      <c r="F31" t="s">
+        <v>67</v>
+      </c>
+      <c r="G31" t="s">
+        <v>277</v>
+      </c>
+      <c r="H31" t="s">
+        <v>70</v>
+      </c>
+      <c r="I31">
+        <v>125312</v>
+      </c>
+      <c r="J31">
+        <v>125313</v>
+      </c>
+      <c r="K31">
+        <v>125314</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>93</v>
+      </c>
+      <c r="B32" t="s">
+        <v>276</v>
+      </c>
+      <c r="C32">
+        <v>125311</v>
+      </c>
+      <c r="D32">
+        <v>125317</v>
+      </c>
+      <c r="E32" t="s">
+        <v>66</v>
+      </c>
+      <c r="F32" t="s">
+        <v>67</v>
+      </c>
+      <c r="G32" t="s">
+        <v>277</v>
+      </c>
+      <c r="H32" t="s">
+        <v>70</v>
+      </c>
+      <c r="I32">
+        <v>125312</v>
+      </c>
+      <c r="J32">
+        <v>125313</v>
+      </c>
+      <c r="K32">
+        <v>125314</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>94</v>
+      </c>
+      <c r="B33" t="s">
+        <v>276</v>
+      </c>
+      <c r="C33">
+        <v>125311</v>
+      </c>
+      <c r="D33">
+        <v>125317</v>
+      </c>
+      <c r="E33" t="s">
+        <v>66</v>
+      </c>
+      <c r="F33" t="s">
+        <v>67</v>
+      </c>
+      <c r="G33" t="s">
+        <v>277</v>
+      </c>
+      <c r="H33" t="s">
+        <v>70</v>
+      </c>
+      <c r="I33">
+        <v>125312</v>
+      </c>
+      <c r="J33">
+        <v>125313</v>
+      </c>
+      <c r="K33">
+        <v>125314</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E123"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B50" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B53" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E30" sqref="E30:E61"/>
+      <selection pane="bottomRight" activeCell="G113" sqref="G113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
add education and edit Metadata tables
</commit_message>
<xml_diff>
--- a/Data/MetaData.xlsx
+++ b/Data/MetaData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="6150" firstSheet="5" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="6150" firstSheet="6" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="CompressedFileNames" sheetId="1" r:id="rId1"/>
@@ -19,13 +19,14 @@
     <sheet name="HouseTables" sheetId="8" r:id="rId10"/>
     <sheet name="RegionWeights" sheetId="9" r:id="rId11"/>
     <sheet name="MedicalTables" sheetId="13" r:id="rId12"/>
+    <sheet name="EducationTables" sheetId="14" r:id="rId13"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2064" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2185" uniqueCount="354">
   <si>
     <t>Year</t>
   </si>
@@ -1078,6 +1079,15 @@
   </si>
   <si>
     <t>measure</t>
+  </si>
+  <si>
+    <t>P3S07</t>
+  </si>
+  <si>
+    <t>P3S08</t>
+  </si>
+  <si>
+    <t>EduExpenditure</t>
   </si>
 </sst>
 </file>
@@ -4788,8 +4798,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K37" sqref="K37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5487,6 +5497,699 @@
       </c>
       <c r="H33" t="s">
         <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="7" max="7" width="16.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>269</v>
+      </c>
+      <c r="C1" t="s">
+        <v>291</v>
+      </c>
+      <c r="D1" t="s">
+        <v>292</v>
+      </c>
+      <c r="E1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G1" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2">
+        <v>63</v>
+      </c>
+      <c r="B2" t="s">
+        <v>276</v>
+      </c>
+      <c r="E2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3">
+        <v>64</v>
+      </c>
+      <c r="B3" t="s">
+        <v>276</v>
+      </c>
+      <c r="E3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4">
+        <v>65</v>
+      </c>
+      <c r="B4" t="s">
+        <v>276</v>
+      </c>
+      <c r="E4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5">
+        <v>66</v>
+      </c>
+      <c r="B5" t="s">
+        <v>276</v>
+      </c>
+      <c r="E5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6">
+        <v>67</v>
+      </c>
+      <c r="B6" t="s">
+        <v>276</v>
+      </c>
+      <c r="E6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7">
+        <v>68</v>
+      </c>
+      <c r="B7" t="s">
+        <v>276</v>
+      </c>
+      <c r="E7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8">
+        <v>69</v>
+      </c>
+      <c r="B8" t="s">
+        <v>276</v>
+      </c>
+      <c r="E8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9">
+        <v>70</v>
+      </c>
+      <c r="B9" t="s">
+        <v>288</v>
+      </c>
+      <c r="C9">
+        <v>72114</v>
+      </c>
+      <c r="D9">
+        <v>72191</v>
+      </c>
+      <c r="E9" t="s">
+        <v>51</v>
+      </c>
+      <c r="F9" t="s">
+        <v>274</v>
+      </c>
+      <c r="G9" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10">
+        <v>71</v>
+      </c>
+      <c r="B10" t="s">
+        <v>287</v>
+      </c>
+      <c r="C10">
+        <v>72114</v>
+      </c>
+      <c r="D10">
+        <v>72191</v>
+      </c>
+      <c r="E10" t="s">
+        <v>51</v>
+      </c>
+      <c r="F10" t="s">
+        <v>274</v>
+      </c>
+      <c r="G10" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11">
+        <v>72</v>
+      </c>
+      <c r="B11" t="s">
+        <v>347</v>
+      </c>
+      <c r="C11">
+        <v>72114</v>
+      </c>
+      <c r="D11">
+        <v>72191</v>
+      </c>
+      <c r="E11" t="s">
+        <v>51</v>
+      </c>
+      <c r="F11" t="s">
+        <v>274</v>
+      </c>
+      <c r="G11" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12">
+        <v>73</v>
+      </c>
+      <c r="B12" t="s">
+        <v>346</v>
+      </c>
+      <c r="C12">
+        <v>72114</v>
+      </c>
+      <c r="D12">
+        <v>72191</v>
+      </c>
+      <c r="E12" t="s">
+        <v>51</v>
+      </c>
+      <c r="F12" t="s">
+        <v>274</v>
+      </c>
+      <c r="G12" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13">
+        <v>74</v>
+      </c>
+      <c r="B13" t="s">
+        <v>351</v>
+      </c>
+      <c r="C13">
+        <v>72114</v>
+      </c>
+      <c r="D13">
+        <v>72191</v>
+      </c>
+      <c r="E13" t="s">
+        <v>51</v>
+      </c>
+      <c r="F13" t="s">
+        <v>274</v>
+      </c>
+      <c r="G13" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14">
+        <v>75</v>
+      </c>
+      <c r="B14" t="s">
+        <v>352</v>
+      </c>
+      <c r="C14">
+        <v>72114</v>
+      </c>
+      <c r="D14">
+        <v>72191</v>
+      </c>
+      <c r="E14" t="s">
+        <v>51</v>
+      </c>
+      <c r="F14" t="s">
+        <v>274</v>
+      </c>
+      <c r="G14" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15">
+        <v>76</v>
+      </c>
+      <c r="B15" t="s">
+        <v>273</v>
+      </c>
+      <c r="C15">
+        <v>72114</v>
+      </c>
+      <c r="D15">
+        <v>72191</v>
+      </c>
+      <c r="E15" t="s">
+        <v>51</v>
+      </c>
+      <c r="F15" t="s">
+        <v>274</v>
+      </c>
+      <c r="G15" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16">
+        <v>77</v>
+      </c>
+      <c r="B16" t="s">
+        <v>273</v>
+      </c>
+      <c r="C16">
+        <v>72114</v>
+      </c>
+      <c r="D16">
+        <v>72191</v>
+      </c>
+      <c r="E16" t="s">
+        <v>51</v>
+      </c>
+      <c r="F16" t="s">
+        <v>274</v>
+      </c>
+      <c r="G16" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17">
+        <v>78</v>
+      </c>
+      <c r="B17" t="s">
+        <v>273</v>
+      </c>
+      <c r="C17">
+        <v>72114</v>
+      </c>
+      <c r="D17">
+        <v>72191</v>
+      </c>
+      <c r="E17" t="s">
+        <v>51</v>
+      </c>
+      <c r="F17" t="s">
+        <v>274</v>
+      </c>
+      <c r="G17" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18">
+        <v>79</v>
+      </c>
+      <c r="B18" t="s">
+        <v>273</v>
+      </c>
+      <c r="C18">
+        <v>72114</v>
+      </c>
+      <c r="D18">
+        <v>72191</v>
+      </c>
+      <c r="E18" t="s">
+        <v>51</v>
+      </c>
+      <c r="F18" t="s">
+        <v>274</v>
+      </c>
+      <c r="G18" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19">
+        <v>80</v>
+      </c>
+      <c r="B19" t="s">
+        <v>273</v>
+      </c>
+      <c r="C19">
+        <v>72114</v>
+      </c>
+      <c r="D19">
+        <v>72191</v>
+      </c>
+      <c r="E19" t="s">
+        <v>51</v>
+      </c>
+      <c r="F19" t="s">
+        <v>274</v>
+      </c>
+      <c r="G19" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20">
+        <v>81</v>
+      </c>
+      <c r="B20" t="s">
+        <v>273</v>
+      </c>
+      <c r="C20">
+        <v>72114</v>
+      </c>
+      <c r="D20">
+        <v>72191</v>
+      </c>
+      <c r="E20" t="s">
+        <v>51</v>
+      </c>
+      <c r="F20" t="s">
+        <v>274</v>
+      </c>
+      <c r="G20" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21">
+        <v>82</v>
+      </c>
+      <c r="B21" t="s">
+        <v>273</v>
+      </c>
+      <c r="C21">
+        <v>72114</v>
+      </c>
+      <c r="D21">
+        <v>72191</v>
+      </c>
+      <c r="E21" t="s">
+        <v>51</v>
+      </c>
+      <c r="F21" t="s">
+        <v>274</v>
+      </c>
+      <c r="G21" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22">
+        <v>83</v>
+      </c>
+      <c r="B22" t="s">
+        <v>273</v>
+      </c>
+      <c r="C22">
+        <v>72114</v>
+      </c>
+      <c r="D22">
+        <v>72191</v>
+      </c>
+      <c r="E22" t="s">
+        <v>51</v>
+      </c>
+      <c r="F22" t="s">
+        <v>274</v>
+      </c>
+      <c r="G22" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23">
+        <v>84</v>
+      </c>
+      <c r="B23" t="s">
+        <v>276</v>
+      </c>
+      <c r="C23">
+        <v>101111</v>
+      </c>
+      <c r="D23">
+        <v>105115</v>
+      </c>
+      <c r="E23" t="s">
+        <v>66</v>
+      </c>
+      <c r="F23" t="s">
+        <v>67</v>
+      </c>
+      <c r="G23" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24">
+        <v>85</v>
+      </c>
+      <c r="B24" t="s">
+        <v>276</v>
+      </c>
+      <c r="C24">
+        <v>101111</v>
+      </c>
+      <c r="D24">
+        <v>105115</v>
+      </c>
+      <c r="E24" t="s">
+        <v>51</v>
+      </c>
+      <c r="F24" t="s">
+        <v>67</v>
+      </c>
+      <c r="G24" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25">
+        <v>86</v>
+      </c>
+      <c r="B25" t="s">
+        <v>276</v>
+      </c>
+      <c r="C25">
+        <v>101111</v>
+      </c>
+      <c r="D25">
+        <v>105115</v>
+      </c>
+      <c r="E25" t="s">
+        <v>66</v>
+      </c>
+      <c r="F25" t="s">
+        <v>67</v>
+      </c>
+      <c r="G25" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26">
+        <v>87</v>
+      </c>
+      <c r="B26" t="s">
+        <v>276</v>
+      </c>
+      <c r="C26">
+        <v>101111</v>
+      </c>
+      <c r="D26">
+        <v>105115</v>
+      </c>
+      <c r="E26" t="s">
+        <v>66</v>
+      </c>
+      <c r="F26" t="s">
+        <v>67</v>
+      </c>
+      <c r="G26" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27">
+        <v>88</v>
+      </c>
+      <c r="B27" t="s">
+        <v>276</v>
+      </c>
+      <c r="C27">
+        <v>101111</v>
+      </c>
+      <c r="D27">
+        <v>105115</v>
+      </c>
+      <c r="E27" t="s">
+        <v>66</v>
+      </c>
+      <c r="F27" t="s">
+        <v>67</v>
+      </c>
+      <c r="G27" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28">
+        <v>89</v>
+      </c>
+      <c r="B28" t="s">
+        <v>276</v>
+      </c>
+      <c r="C28">
+        <v>101111</v>
+      </c>
+      <c r="D28">
+        <v>105115</v>
+      </c>
+      <c r="E28" t="s">
+        <v>284</v>
+      </c>
+      <c r="F28" t="s">
+        <v>278</v>
+      </c>
+      <c r="G28" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29">
+        <v>90</v>
+      </c>
+      <c r="B29" t="s">
+        <v>276</v>
+      </c>
+      <c r="C29">
+        <v>101111</v>
+      </c>
+      <c r="D29">
+        <v>105115</v>
+      </c>
+      <c r="E29" t="s">
+        <v>66</v>
+      </c>
+      <c r="F29" t="s">
+        <v>67</v>
+      </c>
+      <c r="G29" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30">
+        <v>91</v>
+      </c>
+      <c r="B30" t="s">
+        <v>276</v>
+      </c>
+      <c r="C30">
+        <v>101111</v>
+      </c>
+      <c r="D30">
+        <v>105115</v>
+      </c>
+      <c r="E30" t="s">
+        <v>66</v>
+      </c>
+      <c r="F30" t="s">
+        <v>67</v>
+      </c>
+      <c r="G30" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31">
+        <v>92</v>
+      </c>
+      <c r="B31" t="s">
+        <v>276</v>
+      </c>
+      <c r="C31">
+        <v>101111</v>
+      </c>
+      <c r="D31">
+        <v>105115</v>
+      </c>
+      <c r="E31" t="s">
+        <v>66</v>
+      </c>
+      <c r="F31" t="s">
+        <v>67</v>
+      </c>
+      <c r="G31" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32">
+        <v>93</v>
+      </c>
+      <c r="B32" t="s">
+        <v>276</v>
+      </c>
+      <c r="C32">
+        <v>101111</v>
+      </c>
+      <c r="D32">
+        <v>105115</v>
+      </c>
+      <c r="E32" t="s">
+        <v>66</v>
+      </c>
+      <c r="F32" t="s">
+        <v>67</v>
+      </c>
+      <c r="G32" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33">
+        <v>94</v>
+      </c>
+      <c r="B33" t="s">
+        <v>276</v>
+      </c>
+      <c r="C33">
+        <v>101111</v>
+      </c>
+      <c r="D33">
+        <v>105115</v>
+      </c>
+      <c r="E33" t="s">
+        <v>66</v>
+      </c>
+      <c r="F33" t="s">
+        <v>67</v>
+      </c>
+      <c r="G33" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -8800,7 +9503,7 @@
   <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N27" sqref="N27"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9327,7 +10030,7 @@
       <c r="D28" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="E28" s="2" t="s">
+      <c r="F28" s="2" t="s">
         <v>324</v>
       </c>
       <c r="G28" t="s">
@@ -9347,7 +10050,7 @@
       <c r="D29" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="E29" s="2" t="s">
+      <c r="F29" s="2" t="s">
         <v>324</v>
       </c>
       <c r="G29" t="s">
@@ -9367,7 +10070,7 @@
       <c r="D30" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="E30" s="2" t="s">
+      <c r="F30" s="2" t="s">
         <v>324</v>
       </c>
       <c r="G30" t="s">
@@ -9387,7 +10090,7 @@
       <c r="D31" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="E31" s="2" t="s">
+      <c r="F31" s="2" t="s">
         <v>324</v>
       </c>
       <c r="G31" t="s">
@@ -9407,7 +10110,7 @@
       <c r="D32" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="E32" s="2" t="s">
+      <c r="F32" s="2" t="s">
         <v>324</v>
       </c>
       <c r="G32" t="s">
@@ -9427,7 +10130,7 @@
       <c r="D33" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="E33" s="2" t="s">
+      <c r="F33" s="2" t="s">
         <v>324</v>
       </c>
       <c r="G33" t="s">
@@ -9445,7 +10148,7 @@
   <dimension ref="A1:R33"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11058,7 +11761,7 @@
   <dimension ref="A1:L33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="A1:L33"/>
+      <selection activeCell="G19" sqref="A1:L33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
edit metadata.xlsx & add 2 files & edit other files
</commit_message>
<xml_diff>
--- a/Data/MetaData.xlsx
+++ b/Data/MetaData.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2185" uniqueCount="354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2223" uniqueCount="352">
   <si>
     <t>Year</t>
   </si>
@@ -1079,12 +1079,6 @@
   </si>
   <si>
     <t>measure</t>
-  </si>
-  <si>
-    <t>P3S07</t>
-  </si>
-  <si>
-    <t>P3S08</t>
   </si>
   <si>
     <t>EduExpenditure</t>
@@ -1920,7 +1914,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2207,8 +2201,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2260,6 +2254,9 @@
       <c r="F2" t="s">
         <v>274</v>
       </c>
+      <c r="G2" t="s">
+        <v>275</v>
+      </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3">
@@ -2280,6 +2277,9 @@
       <c r="F3" t="s">
         <v>274</v>
       </c>
+      <c r="G3" t="s">
+        <v>275</v>
+      </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4">
@@ -2300,6 +2300,9 @@
       <c r="F4" t="s">
         <v>274</v>
       </c>
+      <c r="G4" t="s">
+        <v>275</v>
+      </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5">
@@ -2320,6 +2323,9 @@
       <c r="F5" t="s">
         <v>274</v>
       </c>
+      <c r="G5" t="s">
+        <v>275</v>
+      </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6">
@@ -2340,6 +2346,9 @@
       <c r="F6" t="s">
         <v>274</v>
       </c>
+      <c r="G6" t="s">
+        <v>275</v>
+      </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7">
@@ -2359,6 +2368,9 @@
       </c>
       <c r="F7" t="s">
         <v>274</v>
+      </c>
+      <c r="G7" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -5509,7 +5521,7 @@
   <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5537,7 +5549,7 @@
         <v>76</v>
       </c>
       <c r="G1" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -5545,10 +5557,22 @@
         <v>63</v>
       </c>
       <c r="B2" t="s">
-        <v>276</v>
+        <v>273</v>
+      </c>
+      <c r="C2">
+        <v>72114</v>
+      </c>
+      <c r="D2">
+        <v>72170</v>
       </c>
       <c r="E2" t="s">
         <v>51</v>
+      </c>
+      <c r="F2" t="s">
+        <v>274</v>
+      </c>
+      <c r="G2" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -5556,10 +5580,22 @@
         <v>64</v>
       </c>
       <c r="B3" t="s">
-        <v>276</v>
+        <v>273</v>
+      </c>
+      <c r="C3">
+        <v>72114</v>
+      </c>
+      <c r="D3">
+        <v>72170</v>
       </c>
       <c r="E3" t="s">
         <v>51</v>
+      </c>
+      <c r="F3" t="s">
+        <v>274</v>
+      </c>
+      <c r="G3" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -5567,10 +5603,22 @@
         <v>65</v>
       </c>
       <c r="B4" t="s">
-        <v>276</v>
+        <v>273</v>
+      </c>
+      <c r="C4">
+        <v>72114</v>
+      </c>
+      <c r="D4">
+        <v>72170</v>
       </c>
       <c r="E4" t="s">
         <v>51</v>
+      </c>
+      <c r="F4" t="s">
+        <v>274</v>
+      </c>
+      <c r="G4" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -5578,10 +5626,22 @@
         <v>66</v>
       </c>
       <c r="B5" t="s">
-        <v>276</v>
+        <v>273</v>
+      </c>
+      <c r="C5">
+        <v>72114</v>
+      </c>
+      <c r="D5">
+        <v>72170</v>
       </c>
       <c r="E5" t="s">
         <v>51</v>
+      </c>
+      <c r="F5" t="s">
+        <v>274</v>
+      </c>
+      <c r="G5" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -5589,10 +5649,22 @@
         <v>67</v>
       </c>
       <c r="B6" t="s">
-        <v>276</v>
+        <v>273</v>
+      </c>
+      <c r="C6">
+        <v>72114</v>
+      </c>
+      <c r="D6">
+        <v>72170</v>
       </c>
       <c r="E6" t="s">
         <v>51</v>
+      </c>
+      <c r="F6" t="s">
+        <v>274</v>
+      </c>
+      <c r="G6" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -5600,10 +5672,22 @@
         <v>68</v>
       </c>
       <c r="B7" t="s">
-        <v>276</v>
+        <v>273</v>
+      </c>
+      <c r="C7">
+        <v>72114</v>
+      </c>
+      <c r="D7">
+        <v>72170</v>
       </c>
       <c r="E7" t="s">
         <v>51</v>
+      </c>
+      <c r="F7" t="s">
+        <v>274</v>
+      </c>
+      <c r="G7" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -5611,10 +5695,22 @@
         <v>69</v>
       </c>
       <c r="B8" t="s">
-        <v>276</v>
+        <v>273</v>
+      </c>
+      <c r="C8">
+        <v>72114</v>
+      </c>
+      <c r="D8">
+        <v>72170</v>
       </c>
       <c r="E8" t="s">
         <v>51</v>
+      </c>
+      <c r="F8" t="s">
+        <v>274</v>
+      </c>
+      <c r="G8" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -5622,7 +5718,7 @@
         <v>70</v>
       </c>
       <c r="B9" t="s">
-        <v>288</v>
+        <v>273</v>
       </c>
       <c r="C9">
         <v>72114</v>
@@ -5645,7 +5741,7 @@
         <v>71</v>
       </c>
       <c r="B10" t="s">
-        <v>287</v>
+        <v>273</v>
       </c>
       <c r="C10">
         <v>72114</v>
@@ -5668,7 +5764,7 @@
         <v>72</v>
       </c>
       <c r="B11" t="s">
-        <v>347</v>
+        <v>273</v>
       </c>
       <c r="C11">
         <v>72114</v>
@@ -5691,7 +5787,7 @@
         <v>73</v>
       </c>
       <c r="B12" t="s">
-        <v>346</v>
+        <v>273</v>
       </c>
       <c r="C12">
         <v>72114</v>
@@ -5714,7 +5810,7 @@
         <v>74</v>
       </c>
       <c r="B13" t="s">
-        <v>351</v>
+        <v>273</v>
       </c>
       <c r="C13">
         <v>72114</v>
@@ -5737,7 +5833,7 @@
         <v>75</v>
       </c>
       <c r="B14" t="s">
-        <v>352</v>
+        <v>273</v>
       </c>
       <c r="C14">
         <v>72114</v>
@@ -10148,7 +10244,7 @@
   <dimension ref="A1:R33"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11761,7 +11857,7 @@
   <dimension ref="A1:L33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G19" sqref="A1:L33"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11833,6 +11929,15 @@
       <c r="F2" t="s">
         <v>274</v>
       </c>
+      <c r="G2" t="s">
+        <v>304</v>
+      </c>
+      <c r="J2" t="s">
+        <v>306</v>
+      </c>
+      <c r="L2" t="s">
+        <v>289</v>
+      </c>
     </row>
     <row r="3" spans="1:12">
       <c r="A3">
@@ -11853,6 +11958,15 @@
       <c r="F3" t="s">
         <v>274</v>
       </c>
+      <c r="G3" t="s">
+        <v>304</v>
+      </c>
+      <c r="J3" t="s">
+        <v>306</v>
+      </c>
+      <c r="L3" t="s">
+        <v>289</v>
+      </c>
     </row>
     <row r="4" spans="1:12">
       <c r="A4">
@@ -11873,6 +11987,15 @@
       <c r="F4" t="s">
         <v>274</v>
       </c>
+      <c r="G4" t="s">
+        <v>304</v>
+      </c>
+      <c r="J4" t="s">
+        <v>306</v>
+      </c>
+      <c r="L4" t="s">
+        <v>289</v>
+      </c>
     </row>
     <row r="5" spans="1:12">
       <c r="A5">
@@ -11893,6 +12016,15 @@
       <c r="F5" t="s">
         <v>274</v>
       </c>
+      <c r="G5" t="s">
+        <v>304</v>
+      </c>
+      <c r="J5" t="s">
+        <v>306</v>
+      </c>
+      <c r="L5" t="s">
+        <v>289</v>
+      </c>
     </row>
     <row r="6" spans="1:12">
       <c r="A6">
@@ -11913,6 +12045,15 @@
       <c r="F6" t="s">
         <v>274</v>
       </c>
+      <c r="G6" t="s">
+        <v>304</v>
+      </c>
+      <c r="J6" t="s">
+        <v>306</v>
+      </c>
+      <c r="L6" t="s">
+        <v>289</v>
+      </c>
     </row>
     <row r="7" spans="1:12">
       <c r="A7">
@@ -11932,6 +12073,15 @@
       </c>
       <c r="F7" t="s">
         <v>274</v>
+      </c>
+      <c r="G7" t="s">
+        <v>304</v>
+      </c>
+      <c r="J7" t="s">
+        <v>306</v>
+      </c>
+      <c r="L7" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="8" spans="1:12">

</xml_diff>

<commit_message>
Add sheets and edit in Metadata.xlsx
</commit_message>
<xml_diff>
--- a/Data/MetaData.xlsx
+++ b/Data/MetaData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="6150" firstSheet="5" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="6150" firstSheet="5" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="CompressedFileNames" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3804" uniqueCount="366">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4190" uniqueCount="379">
   <si>
     <t>Year</t>
   </si>
@@ -1129,6 +1129,45 @@
   </si>
   <si>
     <t>SubsidyTable</t>
+  </si>
+  <si>
+    <t>dimension</t>
+  </si>
+  <si>
+    <t>month_number</t>
+  </si>
+  <si>
+    <t>Subsidy</t>
+  </si>
+  <si>
+    <t>Dycol01</t>
+  </si>
+  <si>
+    <t>Dycol02</t>
+  </si>
+  <si>
+    <t>Dycol03</t>
+  </si>
+  <si>
+    <t>Dycol04</t>
+  </si>
+  <si>
+    <t>rent</t>
+  </si>
+  <si>
+    <t>interest</t>
+  </si>
+  <si>
+    <t>aid</t>
+  </si>
+  <si>
+    <t>homemade</t>
+  </si>
+  <si>
+    <t>intra</t>
+  </si>
+  <si>
+    <t>retirement</t>
   </si>
 </sst>
 </file>
@@ -1485,7 +1524,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1650,11 +1689,22 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1968,7 +2018,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2253,15 +2303,18 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q33"/>
+  <dimension ref="A1:R33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="17" max="17" width="13.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:18">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2313,254 +2366,257 @@
       <c r="Q1" t="s">
         <v>339</v>
       </c>
-    </row>
-    <row r="2" spans="1:17">
+      <c r="R1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
       <c r="A2">
         <v>63</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>318</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" t="s">
         <v>52</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3" t="s">
+      <c r="E2" t="s">
         <v>330</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" t="s">
         <v>53</v>
       </c>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3" t="s">
+      <c r="K2" t="s">
         <v>54</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="L2" t="s">
         <v>55</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="M2" t="s">
         <v>58</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="N2" t="s">
         <v>56</v>
       </c>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3" t="s">
+      <c r="O2" t="s">
         <v>57</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="P2" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="3" spans="1:17">
+      <c r="Q2" t="s">
+        <v>60</v>
+      </c>
+      <c r="R2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
       <c r="A3">
         <v>64</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>318</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" t="s">
         <v>52</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3" t="s">
+      <c r="E3" t="s">
         <v>330</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" t="s">
         <v>53</v>
       </c>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3" t="s">
+      <c r="K3" t="s">
         <v>54</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="L3" t="s">
         <v>55</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="M3" t="s">
         <v>58</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="N3" t="s">
         <v>56</v>
       </c>
-      <c r="O3" s="3"/>
-      <c r="P3" s="3" t="s">
+      <c r="O3" t="s">
         <v>57</v>
       </c>
-      <c r="Q3" s="3" t="s">
+      <c r="P3" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="4" spans="1:17">
+      <c r="Q3" t="s">
+        <v>60</v>
+      </c>
+      <c r="R3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
       <c r="A4">
         <v>65</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>318</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" t="s">
         <v>52</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3" t="s">
+      <c r="E4" t="s">
         <v>330</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" t="s">
         <v>53</v>
       </c>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3" t="s">
+      <c r="K4" t="s">
         <v>54</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="L4" t="s">
         <v>55</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="M4" t="s">
         <v>58</v>
       </c>
-      <c r="N4" s="3" t="s">
+      <c r="N4" t="s">
         <v>56</v>
       </c>
-      <c r="O4" s="3"/>
-      <c r="P4" s="3" t="s">
+      <c r="O4" t="s">
         <v>57</v>
       </c>
-      <c r="Q4" s="3" t="s">
+      <c r="P4" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="5" spans="1:17">
+      <c r="Q4" t="s">
+        <v>60</v>
+      </c>
+      <c r="R4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
       <c r="A5">
         <v>66</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>318</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" t="s">
         <v>52</v>
       </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3" t="s">
+      <c r="E5" t="s">
         <v>330</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" t="s">
         <v>53</v>
       </c>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3" t="s">
+      <c r="K5" t="s">
         <v>54</v>
       </c>
-      <c r="L5" s="3" t="s">
+      <c r="L5" t="s">
         <v>55</v>
       </c>
-      <c r="M5" s="3" t="s">
+      <c r="M5" t="s">
         <v>58</v>
       </c>
-      <c r="N5" s="3" t="s">
+      <c r="N5" t="s">
         <v>56</v>
       </c>
-      <c r="O5" s="3"/>
-      <c r="P5" s="3" t="s">
+      <c r="O5" t="s">
         <v>57</v>
       </c>
-      <c r="Q5" s="3" t="s">
+      <c r="P5" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="6" spans="1:17">
+      <c r="Q5" t="s">
+        <v>60</v>
+      </c>
+      <c r="R5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
       <c r="A6">
         <v>67</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>318</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" t="s">
         <v>52</v>
       </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3" t="s">
+      <c r="E6" t="s">
         <v>330</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" t="s">
         <v>53</v>
       </c>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3" t="s">
+      <c r="K6" t="s">
         <v>54</v>
       </c>
-      <c r="L6" s="3" t="s">
+      <c r="L6" t="s">
         <v>55</v>
       </c>
-      <c r="M6" s="3" t="s">
+      <c r="M6" t="s">
         <v>58</v>
       </c>
-      <c r="N6" s="3" t="s">
+      <c r="N6" t="s">
         <v>56</v>
       </c>
-      <c r="O6" s="3"/>
-      <c r="P6" s="3" t="s">
+      <c r="O6" t="s">
         <v>57</v>
       </c>
-      <c r="Q6" s="3" t="s">
+      <c r="P6" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="7" spans="1:17">
+      <c r="Q6" t="s">
+        <v>60</v>
+      </c>
+      <c r="R6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18">
       <c r="A7">
         <v>68</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>318</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" t="s">
         <v>52</v>
       </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3" t="s">
+      <c r="E7" t="s">
         <v>330</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" t="s">
         <v>53</v>
       </c>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3" t="s">
+      <c r="K7" t="s">
         <v>54</v>
       </c>
-      <c r="L7" s="3" t="s">
+      <c r="L7" t="s">
         <v>55</v>
       </c>
-      <c r="M7" s="3" t="s">
+      <c r="M7" t="s">
         <v>58</v>
       </c>
-      <c r="N7" s="3" t="s">
+      <c r="N7" t="s">
         <v>56</v>
       </c>
-      <c r="O7" s="3"/>
-      <c r="P7" s="3" t="s">
+      <c r="O7" t="s">
         <v>57</v>
       </c>
-      <c r="Q7" s="3" t="s">
+      <c r="P7" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="8" spans="1:17">
+      <c r="Q7" t="s">
+        <v>60</v>
+      </c>
+      <c r="R7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18">
       <c r="A8">
         <v>69</v>
       </c>
@@ -2603,8 +2659,11 @@
       <c r="Q8" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="9" spans="1:17">
+      <c r="R8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18">
       <c r="A9">
         <v>70</v>
       </c>
@@ -2647,8 +2706,11 @@
       <c r="Q9" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="10" spans="1:17">
+      <c r="R9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18">
       <c r="A10">
         <v>71</v>
       </c>
@@ -2691,8 +2753,11 @@
       <c r="Q10" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="11" spans="1:17">
+      <c r="R10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18">
       <c r="A11">
         <v>72</v>
       </c>
@@ -2735,8 +2800,11 @@
       <c r="Q11" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="12" spans="1:17">
+      <c r="R11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18">
       <c r="A12">
         <v>73</v>
       </c>
@@ -2779,8 +2847,11 @@
       <c r="Q12" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="13" spans="1:17">
+      <c r="R12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18">
       <c r="A13">
         <v>74</v>
       </c>
@@ -2826,8 +2897,11 @@
       <c r="Q13" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="14" spans="1:17">
+      <c r="R13" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18">
       <c r="A14">
         <v>75</v>
       </c>
@@ -2873,8 +2947,11 @@
       <c r="Q14" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="15" spans="1:17">
+      <c r="R14" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18">
       <c r="A15">
         <v>76</v>
       </c>
@@ -2920,8 +2997,11 @@
       <c r="Q15" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="16" spans="1:17">
+      <c r="R15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18">
       <c r="A16">
         <v>77</v>
       </c>
@@ -2967,8 +3047,11 @@
       <c r="Q16" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="17" spans="1:17">
+      <c r="R16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18">
       <c r="A17">
         <v>78</v>
       </c>
@@ -3014,8 +3097,11 @@
       <c r="Q17" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="18" spans="1:17">
+      <c r="R17" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18">
       <c r="A18">
         <v>79</v>
       </c>
@@ -3061,8 +3147,11 @@
       <c r="Q18" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="19" spans="1:17">
+      <c r="R18" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18">
       <c r="A19">
         <v>80</v>
       </c>
@@ -3108,8 +3197,11 @@
       <c r="Q19" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="20" spans="1:17">
+      <c r="R19" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18">
       <c r="A20">
         <v>81</v>
       </c>
@@ -3155,8 +3247,11 @@
       <c r="Q20" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="21" spans="1:17">
+      <c r="R20" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18">
       <c r="A21">
         <v>82</v>
       </c>
@@ -3202,8 +3297,11 @@
       <c r="Q21" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="22" spans="1:17">
+      <c r="R21" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18">
       <c r="A22">
         <v>83</v>
       </c>
@@ -3249,8 +3347,11 @@
       <c r="Q22" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="23" spans="1:17">
+      <c r="R22" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18">
       <c r="A23">
         <v>84</v>
       </c>
@@ -3302,8 +3403,11 @@
       <c r="Q23" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="24" spans="1:17">
+      <c r="R23" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18">
       <c r="A24">
         <v>85</v>
       </c>
@@ -3355,8 +3459,11 @@
       <c r="Q24" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="25" spans="1:17">
+      <c r="R24" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18">
       <c r="A25">
         <v>86</v>
       </c>
@@ -3408,8 +3515,11 @@
       <c r="Q25" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="26" spans="1:17">
+      <c r="R25" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18">
       <c r="A26">
         <v>87</v>
       </c>
@@ -3461,8 +3571,11 @@
       <c r="Q26" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="27" spans="1:17">
+      <c r="R26" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18">
       <c r="A27">
         <v>88</v>
       </c>
@@ -3514,8 +3627,11 @@
       <c r="Q27" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="28" spans="1:17">
+      <c r="R27" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18">
       <c r="A28">
         <v>89</v>
       </c>
@@ -3567,8 +3683,11 @@
       <c r="Q28" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="29" spans="1:17">
+      <c r="R28" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18">
       <c r="A29">
         <v>90</v>
       </c>
@@ -3620,8 +3739,11 @@
       <c r="Q29" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="30" spans="1:17">
+      <c r="R29" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18">
       <c r="A30">
         <v>91</v>
       </c>
@@ -3673,8 +3795,11 @@
       <c r="Q30" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="31" spans="1:17">
+      <c r="R30" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18">
       <c r="A31">
         <v>92</v>
       </c>
@@ -3726,8 +3851,11 @@
       <c r="Q31" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="32" spans="1:17">
+      <c r="R31" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18">
       <c r="A32">
         <v>93</v>
       </c>
@@ -3779,8 +3907,11 @@
       <c r="Q32" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="33" spans="1:17">
+      <c r="R32" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18">
       <c r="A33">
         <v>94</v>
       </c>
@@ -3831,6 +3962,9 @@
       </c>
       <c r="Q33" t="s">
         <v>329</v>
+      </c>
+      <c r="R33" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -3840,276 +3974,1030 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B33"/>
+  <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="3" width="9.140625" style="3"/>
+    <col min="4" max="4" width="10.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="9.140625" style="3"/>
+    <col min="8" max="8" width="11.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="3"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:10">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2">
+      <c r="C1" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>373</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>374</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>375</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>377</v>
+      </c>
+      <c r="J1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="6">
         <v>63</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="5" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3">
+      <c r="C2" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="J2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="6">
         <v>64</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="5" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4">
+      <c r="C3" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="J3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="6">
         <v>65</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="5" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5">
+      <c r="C4" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="J4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="6">
         <v>66</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="5" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6">
+      <c r="C5" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="J5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="6">
         <v>67</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="5" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7">
+      <c r="C6" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="J6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="6">
         <v>68</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="5" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8">
+      <c r="C7" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="J7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="3">
         <v>69</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="4" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9">
+      <c r="C8" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="3">
         <v>70</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="4" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10">
+      <c r="C9" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="3">
         <v>71</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="4" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11">
+      <c r="C10" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="3">
         <v>72</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="4" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12">
+      <c r="C11" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="3">
         <v>73</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="4" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13">
+      <c r="C12" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="3">
         <v>74</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="4" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14">
+      <c r="C13" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J13" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="3">
         <v>75</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="4" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15">
+      <c r="C14" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J14" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" s="3">
         <v>76</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="4" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16">
+      <c r="C15" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" s="3">
         <v>77</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="4" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17">
+      <c r="C16" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" s="3">
         <v>78</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="4" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18">
+      <c r="C17" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="J17" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="3">
         <v>79</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="4" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19">
+      <c r="C18" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="J18" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" s="3">
         <v>80</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="4" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20">
+      <c r="C19" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="J19" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="3">
         <v>81</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="4" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21">
+      <c r="C20" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="J20" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" s="3">
         <v>82</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="4" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22">
+      <c r="C21" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="J21" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" s="3">
         <v>83</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="4" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23">
+      <c r="C22" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="J22" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" s="3">
         <v>84</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="4" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24">
+      <c r="C23" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="J23" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" s="3">
         <v>85</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="4" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25">
+      <c r="C24" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="J24" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" s="3">
         <v>86</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="4" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26">
+      <c r="C25" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="J25" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" s="3">
         <v>87</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="4" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="A27">
+      <c r="C26" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="J26" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" s="3">
         <v>88</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="4" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="28" spans="1:2">
-      <c r="A28">
+      <c r="C27" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="J27" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28" s="3">
         <v>89</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="4" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="A29">
+      <c r="C28" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="J28" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29" s="3">
         <v>90</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="4" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="30" spans="1:2">
-      <c r="A30">
+      <c r="C29" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="I29" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="J29" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="A30" s="3">
         <v>91</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="4" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="31" spans="1:2">
-      <c r="A31">
+      <c r="C30" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="I30" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="J30" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="A31" s="3">
         <v>92</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" s="4" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="32" spans="1:2">
-      <c r="A32">
+      <c r="C31" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="H31" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="I31" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="J31" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="A32" s="3">
         <v>93</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B32" s="4" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="33" spans="1:2">
-      <c r="A33">
+      <c r="C32" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="H32" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="I32" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="J32" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
+      <c r="A33" s="3">
         <v>94</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B33" s="4" t="s">
         <v>323</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="I33" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="J33" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -4119,224 +5007,154 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B33"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" t="s">
+        <v>331</v>
+      </c>
+      <c r="D1" t="s">
+        <v>366</v>
+      </c>
+      <c r="E1" t="s">
+        <v>367</v>
+      </c>
+      <c r="F1" t="s">
+        <v>368</v>
+      </c>
+      <c r="G1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2">
-        <v>63</v>
-      </c>
-      <c r="B2" s="2"/>
-    </row>
-    <row r="3" spans="1:2">
+        <v>90</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="C2" t="s">
+        <v>369</v>
+      </c>
+      <c r="D2" t="s">
+        <v>370</v>
+      </c>
+      <c r="E2" t="s">
+        <v>371</v>
+      </c>
+      <c r="F2" t="s">
+        <v>372</v>
+      </c>
+      <c r="G2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3">
-        <v>64</v>
-      </c>
-      <c r="B3" s="2"/>
-    </row>
-    <row r="4" spans="1:2">
+        <v>91</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="C3" t="s">
+        <v>369</v>
+      </c>
+      <c r="D3" t="s">
+        <v>370</v>
+      </c>
+      <c r="E3" t="s">
+        <v>371</v>
+      </c>
+      <c r="F3" t="s">
+        <v>372</v>
+      </c>
+      <c r="G3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4">
-        <v>65</v>
-      </c>
-      <c r="B4" s="2"/>
-    </row>
-    <row r="5" spans="1:2">
+        <v>92</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="C4" t="s">
+        <v>369</v>
+      </c>
+      <c r="D4" t="s">
+        <v>370</v>
+      </c>
+      <c r="E4" t="s">
+        <v>371</v>
+      </c>
+      <c r="F4" t="s">
+        <v>372</v>
+      </c>
+      <c r="G4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5">
+        <v>93</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="C5" t="s">
+        <v>369</v>
+      </c>
+      <c r="D5" t="s">
+        <v>370</v>
+      </c>
+      <c r="E5" t="s">
+        <v>371</v>
+      </c>
+      <c r="F5" t="s">
+        <v>372</v>
+      </c>
+      <c r="G5" t="s">
         <v>66</v>
       </c>
-      <c r="B5" s="2"/>
-    </row>
-    <row r="6" spans="1:2">
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6">
-        <v>67</v>
-      </c>
-      <c r="B6" s="2"/>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7">
-        <v>68</v>
-      </c>
-      <c r="B7" s="2"/>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8">
-        <v>69</v>
-      </c>
-      <c r="B8" s="2"/>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9">
-        <v>70</v>
-      </c>
-      <c r="B9" s="2"/>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10">
-        <v>71</v>
-      </c>
-      <c r="B10" s="2"/>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11">
-        <v>72</v>
-      </c>
-      <c r="B11" s="2"/>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12">
-        <v>73</v>
-      </c>
-      <c r="B12" s="2"/>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13">
-        <v>74</v>
-      </c>
-      <c r="B13" s="2"/>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14">
-        <v>75</v>
-      </c>
-      <c r="B14" s="2"/>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15">
-        <v>76</v>
-      </c>
-      <c r="B15" s="2"/>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16">
-        <v>77</v>
-      </c>
-      <c r="B16" s="2"/>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17">
-        <v>78</v>
-      </c>
-      <c r="B17" s="2"/>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18">
-        <v>79</v>
-      </c>
-      <c r="B18" s="2"/>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19">
-        <v>80</v>
-      </c>
-      <c r="B19" s="2"/>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20">
-        <v>81</v>
-      </c>
-      <c r="B20" s="2"/>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21">
-        <v>82</v>
-      </c>
-      <c r="B21" s="2"/>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22">
-        <v>83</v>
-      </c>
-      <c r="B22" s="2"/>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23">
-        <v>84</v>
-      </c>
-      <c r="B23" s="2"/>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24">
-        <v>85</v>
-      </c>
-      <c r="B24" s="2"/>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25">
-        <v>86</v>
-      </c>
-      <c r="B25" s="2"/>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26">
-        <v>87</v>
-      </c>
-      <c r="B26" s="2"/>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="A27">
-        <v>88</v>
-      </c>
-      <c r="B27" s="2"/>
-    </row>
-    <row r="28" spans="1:2">
-      <c r="A28">
-        <v>89</v>
-      </c>
-      <c r="B28" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>324</v>
       </c>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="A29">
-        <v>90</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2">
-      <c r="A30">
-        <v>91</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
-      <c r="A31">
-        <v>92</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2">
-      <c r="A32">
-        <v>93</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2">
-      <c r="A33">
-        <v>94</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>324</v>
+      <c r="C6" t="s">
+        <v>369</v>
+      </c>
+      <c r="D6" t="s">
+        <v>370</v>
+      </c>
+      <c r="E6" t="s">
+        <v>371</v>
+      </c>
+      <c r="F6" t="s">
+        <v>372</v>
+      </c>
+      <c r="G6" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -4349,7 +5167,7 @@
   <dimension ref="A1:L33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="C1" sqref="C1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13904,8 +14722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G33"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -14731,10 +15549,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R33"/>
+  <dimension ref="A1:S33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S15" sqref="S15"/>
+    <sheetView topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S1" sqref="S1:S33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -14750,7 +15568,7 @@
     <col min="18" max="18" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:19">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -14805,8 +15623,11 @@
       <c r="R1" t="s">
         <v>339</v>
       </c>
-    </row>
-    <row r="2" spans="1:18">
+      <c r="S1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19">
       <c r="A2">
         <v>63</v>
       </c>
@@ -14825,20 +15646,11 @@
       <c r="H2" t="s">
         <v>53</v>
       </c>
-      <c r="K2" t="s">
-        <v>55</v>
-      </c>
-      <c r="M2" t="s">
-        <v>56</v>
-      </c>
-      <c r="O2" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18">
+      <c r="S2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19">
       <c r="A3">
         <v>64</v>
       </c>
@@ -14857,20 +15669,11 @@
       <c r="H3" t="s">
         <v>53</v>
       </c>
-      <c r="K3" t="s">
-        <v>55</v>
-      </c>
-      <c r="M3" t="s">
-        <v>56</v>
-      </c>
-      <c r="O3" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18">
+      <c r="S3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19">
       <c r="A4">
         <v>65</v>
       </c>
@@ -14889,20 +15692,11 @@
       <c r="H4" t="s">
         <v>53</v>
       </c>
-      <c r="K4" t="s">
-        <v>55</v>
-      </c>
-      <c r="M4" t="s">
-        <v>56</v>
-      </c>
-      <c r="O4" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18">
+      <c r="S4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19">
       <c r="A5">
         <v>66</v>
       </c>
@@ -14921,20 +15715,11 @@
       <c r="H5" t="s">
         <v>53</v>
       </c>
-      <c r="K5" t="s">
-        <v>55</v>
-      </c>
-      <c r="M5" t="s">
-        <v>56</v>
-      </c>
-      <c r="O5" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18">
+      <c r="S5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19">
       <c r="A6">
         <v>67</v>
       </c>
@@ -14953,20 +15738,11 @@
       <c r="H6" t="s">
         <v>53</v>
       </c>
-      <c r="K6" t="s">
-        <v>55</v>
-      </c>
-      <c r="M6" t="s">
-        <v>56</v>
-      </c>
-      <c r="O6" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18">
+      <c r="S6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19">
       <c r="A7">
         <v>68</v>
       </c>
@@ -14985,20 +15761,11 @@
       <c r="H7" t="s">
         <v>53</v>
       </c>
-      <c r="K7" t="s">
-        <v>55</v>
-      </c>
-      <c r="M7" t="s">
-        <v>56</v>
-      </c>
-      <c r="O7" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18">
+      <c r="S7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19">
       <c r="A8">
         <v>69</v>
       </c>
@@ -15032,8 +15799,11 @@
       <c r="R8" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="9" spans="1:18">
+      <c r="S8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19">
       <c r="A9">
         <v>70</v>
       </c>
@@ -15079,8 +15849,11 @@
       <c r="R9" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="10" spans="1:18">
+      <c r="S9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19">
       <c r="A10">
         <v>71</v>
       </c>
@@ -15126,8 +15899,11 @@
       <c r="R10" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="11" spans="1:18">
+      <c r="S10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19">
       <c r="A11">
         <v>72</v>
       </c>
@@ -15173,8 +15949,11 @@
       <c r="R11" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="12" spans="1:18">
+      <c r="S11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19">
       <c r="A12">
         <v>73</v>
       </c>
@@ -15220,8 +15999,11 @@
       <c r="R12" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="13" spans="1:18">
+      <c r="S12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19">
       <c r="A13">
         <v>74</v>
       </c>
@@ -15270,8 +16052,11 @@
       <c r="R13" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="14" spans="1:18">
+      <c r="S13" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19">
       <c r="A14">
         <v>75</v>
       </c>
@@ -15320,8 +16105,11 @@
       <c r="R14" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="15" spans="1:18">
+      <c r="S14" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19">
       <c r="A15">
         <v>76</v>
       </c>
@@ -15370,8 +16158,11 @@
       <c r="R15" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="16" spans="1:18">
+      <c r="S15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19">
       <c r="A16">
         <v>77</v>
       </c>
@@ -15420,8 +16211,11 @@
       <c r="R16" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="17" spans="1:18">
+      <c r="S16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19">
       <c r="A17">
         <v>78</v>
       </c>
@@ -15470,8 +16264,11 @@
       <c r="R17" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="18" spans="1:18">
+      <c r="S17" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19">
       <c r="A18">
         <v>79</v>
       </c>
@@ -15520,8 +16317,11 @@
       <c r="R18" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="19" spans="1:18">
+      <c r="S18" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19">
       <c r="A19">
         <v>80</v>
       </c>
@@ -15570,8 +16370,11 @@
       <c r="R19" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="20" spans="1:18">
+      <c r="S19" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19">
       <c r="A20">
         <v>81</v>
       </c>
@@ -15620,8 +16423,11 @@
       <c r="R20" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="21" spans="1:18">
+      <c r="S20" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19">
       <c r="A21">
         <v>82</v>
       </c>
@@ -15670,8 +16476,11 @@
       <c r="R21" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="22" spans="1:18">
+      <c r="S21" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19">
       <c r="A22">
         <v>83</v>
       </c>
@@ -15720,8 +16529,11 @@
       <c r="R22" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="23" spans="1:18">
+      <c r="S22" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19">
       <c r="A23">
         <v>84</v>
       </c>
@@ -15776,8 +16588,11 @@
       <c r="R23" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="24" spans="1:18">
+      <c r="S23" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19">
       <c r="A24">
         <v>85</v>
       </c>
@@ -15832,8 +16647,11 @@
       <c r="R24" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="25" spans="1:18">
+      <c r="S24" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19">
       <c r="A25">
         <v>86</v>
       </c>
@@ -15888,8 +16706,11 @@
       <c r="R25" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="26" spans="1:18">
+      <c r="S25" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19">
       <c r="A26">
         <v>87</v>
       </c>
@@ -15944,8 +16765,11 @@
       <c r="R26" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="27" spans="1:18">
+      <c r="S26" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19">
       <c r="A27">
         <v>88</v>
       </c>
@@ -16000,8 +16824,11 @@
       <c r="R27" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="28" spans="1:18">
+      <c r="S27" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19">
       <c r="A28">
         <v>89</v>
       </c>
@@ -16056,8 +16883,11 @@
       <c r="R28" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="29" spans="1:18">
+      <c r="S28" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19">
       <c r="A29">
         <v>90</v>
       </c>
@@ -16112,8 +16942,11 @@
       <c r="R29" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="30" spans="1:18">
+      <c r="S29" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19">
       <c r="A30">
         <v>91</v>
       </c>
@@ -16168,8 +17001,11 @@
       <c r="R30" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="31" spans="1:18">
+      <c r="S30" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19">
       <c r="A31">
         <v>92</v>
       </c>
@@ -16224,8 +17060,11 @@
       <c r="R31" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="32" spans="1:18">
+      <c r="S31" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19">
       <c r="A32">
         <v>93</v>
       </c>
@@ -16280,8 +17119,11 @@
       <c r="R32" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="33" spans="1:18">
+      <c r="S32" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19">
       <c r="A33">
         <v>94</v>
       </c>
@@ -16335,6 +17177,9 @@
       </c>
       <c r="R33" t="s">
         <v>329</v>
+      </c>
+      <c r="S33" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -16344,10 +17189,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R33"/>
+  <dimension ref="A1:S33"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="S21" sqref="S21"/>
+      <selection activeCell="S1" sqref="S1:S33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -16363,7 +17208,7 @@
     <col min="18" max="18" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:19">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -16418,248 +17263,203 @@
       <c r="R1" t="s">
         <v>339</v>
       </c>
-    </row>
-    <row r="2" spans="1:18">
+      <c r="S1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19">
       <c r="A2">
         <v>63</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D2" s="3" t="s">
+      <c r="C2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" t="s">
         <v>52</v>
       </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3" t="s">
+      <c r="F2" t="s">
         <v>330</v>
       </c>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3" t="s">
+      <c r="H2" t="s">
         <v>53</v>
       </c>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3" t="s">
+      <c r="N2" t="s">
         <v>55</v>
       </c>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3" t="s">
+      <c r="P2" t="s">
         <v>56</v>
       </c>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3" t="s">
+      <c r="R2" t="s">
         <v>59</v>
       </c>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="R2" s="3"/>
-    </row>
-    <row r="3" spans="1:18">
+      <c r="S2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19">
       <c r="A3">
         <v>64</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D3" s="3" t="s">
+      <c r="C3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" t="s">
         <v>52</v>
       </c>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3" t="s">
+      <c r="F3" t="s">
         <v>330</v>
       </c>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3" t="s">
+      <c r="H3" t="s">
         <v>53</v>
       </c>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3" t="s">
+      <c r="N3" t="s">
         <v>55</v>
       </c>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3" t="s">
+      <c r="P3" t="s">
         <v>56</v>
       </c>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3" t="s">
+      <c r="R3" t="s">
         <v>59</v>
       </c>
-      <c r="P3" s="3"/>
-      <c r="Q3" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="R3" s="3"/>
-    </row>
-    <row r="4" spans="1:18">
+      <c r="S3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19">
       <c r="A4">
         <v>65</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D4" s="3" t="s">
+      <c r="C4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" t="s">
         <v>52</v>
       </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3" t="s">
+      <c r="F4" t="s">
         <v>330</v>
       </c>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3" t="s">
+      <c r="H4" t="s">
         <v>53</v>
       </c>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3" t="s">
+      <c r="N4" t="s">
         <v>55</v>
       </c>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3" t="s">
+      <c r="P4" t="s">
         <v>56</v>
       </c>
-      <c r="N4" s="3"/>
-      <c r="O4" s="3" t="s">
+      <c r="R4" t="s">
         <v>59</v>
       </c>
-      <c r="P4" s="3"/>
-      <c r="Q4" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="R4" s="3"/>
-    </row>
-    <row r="5" spans="1:18">
+      <c r="S4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19">
       <c r="A5">
         <v>66</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D5" s="3" t="s">
+      <c r="C5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" t="s">
         <v>52</v>
       </c>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3" t="s">
+      <c r="F5" t="s">
         <v>330</v>
       </c>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3" t="s">
+      <c r="H5" t="s">
         <v>53</v>
       </c>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3" t="s">
+      <c r="N5" t="s">
         <v>55</v>
       </c>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3" t="s">
+      <c r="P5" t="s">
         <v>56</v>
       </c>
-      <c r="N5" s="3"/>
-      <c r="O5" s="3" t="s">
+      <c r="R5" t="s">
         <v>59</v>
       </c>
-      <c r="P5" s="3"/>
-      <c r="Q5" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="R5" s="3"/>
-    </row>
-    <row r="6" spans="1:18">
+      <c r="S5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19">
       <c r="A6">
         <v>67</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D6" s="3" t="s">
+      <c r="C6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" t="s">
         <v>52</v>
       </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3" t="s">
+      <c r="F6" t="s">
         <v>330</v>
       </c>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3" t="s">
+      <c r="H6" t="s">
         <v>53</v>
       </c>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3" t="s">
+      <c r="N6" t="s">
         <v>55</v>
       </c>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3" t="s">
+      <c r="P6" t="s">
         <v>56</v>
       </c>
-      <c r="N6" s="3"/>
-      <c r="O6" s="3" t="s">
+      <c r="R6" t="s">
         <v>59</v>
       </c>
-      <c r="P6" s="3"/>
-      <c r="Q6" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="R6" s="3"/>
-    </row>
-    <row r="7" spans="1:18">
+      <c r="S6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19">
       <c r="A7">
         <v>68</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D7" s="3" t="s">
+      <c r="C7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" t="s">
         <v>52</v>
       </c>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3" t="s">
+      <c r="F7" t="s">
         <v>330</v>
       </c>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3" t="s">
+      <c r="H7" t="s">
         <v>53</v>
       </c>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3" t="s">
+      <c r="N7" t="s">
         <v>55</v>
       </c>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3" t="s">
+      <c r="P7" t="s">
         <v>56</v>
       </c>
-      <c r="N7" s="3"/>
-      <c r="O7" s="3" t="s">
+      <c r="R7" t="s">
         <v>59</v>
       </c>
-      <c r="P7" s="3"/>
-      <c r="Q7" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="R7" s="3"/>
-    </row>
-    <row r="8" spans="1:18">
+      <c r="S7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19">
       <c r="A8">
         <v>69</v>
       </c>
@@ -16693,8 +17493,11 @@
       <c r="R8" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="9" spans="1:18">
+      <c r="S8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19">
       <c r="A9">
         <v>70</v>
       </c>
@@ -16740,8 +17543,11 @@
       <c r="R9" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="10" spans="1:18">
+      <c r="S9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19">
       <c r="A10">
         <v>71</v>
       </c>
@@ -16787,8 +17593,11 @@
       <c r="R10" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="11" spans="1:18">
+      <c r="S10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19">
       <c r="A11">
         <v>72</v>
       </c>
@@ -16834,8 +17643,11 @@
       <c r="R11" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="12" spans="1:18">
+      <c r="S11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19">
       <c r="A12">
         <v>73</v>
       </c>
@@ -16881,8 +17693,11 @@
       <c r="R12" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="13" spans="1:18">
+      <c r="S12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19">
       <c r="A13">
         <v>74</v>
       </c>
@@ -16931,8 +17746,11 @@
       <c r="R13" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="14" spans="1:18">
+      <c r="S13" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19">
       <c r="A14">
         <v>75</v>
       </c>
@@ -16981,8 +17799,11 @@
       <c r="R14" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="15" spans="1:18">
+      <c r="S14" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19">
       <c r="A15">
         <v>76</v>
       </c>
@@ -17031,8 +17852,11 @@
       <c r="R15" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="16" spans="1:18">
+      <c r="S15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19">
       <c r="A16">
         <v>77</v>
       </c>
@@ -17081,8 +17905,11 @@
       <c r="R16" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="17" spans="1:18">
+      <c r="S16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19">
       <c r="A17">
         <v>78</v>
       </c>
@@ -17131,8 +17958,11 @@
       <c r="R17" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="18" spans="1:18">
+      <c r="S17" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19">
       <c r="A18">
         <v>79</v>
       </c>
@@ -17181,8 +18011,11 @@
       <c r="R18" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="19" spans="1:18">
+      <c r="S18" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19">
       <c r="A19">
         <v>80</v>
       </c>
@@ -17231,8 +18064,11 @@
       <c r="R19" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="20" spans="1:18">
+      <c r="S19" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19">
       <c r="A20">
         <v>81</v>
       </c>
@@ -17281,8 +18117,11 @@
       <c r="R20" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="21" spans="1:18">
+      <c r="S20" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19">
       <c r="A21">
         <v>82</v>
       </c>
@@ -17331,8 +18170,11 @@
       <c r="R21" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="22" spans="1:18">
+      <c r="S21" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19">
       <c r="A22">
         <v>83</v>
       </c>
@@ -17381,8 +18223,11 @@
       <c r="R22" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="23" spans="1:18">
+      <c r="S22" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19">
       <c r="A23">
         <v>84</v>
       </c>
@@ -17437,8 +18282,11 @@
       <c r="R23" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="24" spans="1:18">
+      <c r="S23" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19">
       <c r="A24">
         <v>85</v>
       </c>
@@ -17493,8 +18341,11 @@
       <c r="R24" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="25" spans="1:18">
+      <c r="S24" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19">
       <c r="A25">
         <v>86</v>
       </c>
@@ -17549,8 +18400,11 @@
       <c r="R25" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="26" spans="1:18">
+      <c r="S25" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19">
       <c r="A26">
         <v>87</v>
       </c>
@@ -17605,8 +18459,11 @@
       <c r="R26" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="27" spans="1:18">
+      <c r="S26" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19">
       <c r="A27">
         <v>88</v>
       </c>
@@ -17661,8 +18518,11 @@
       <c r="R27" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="28" spans="1:18">
+      <c r="S27" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19">
       <c r="A28">
         <v>89</v>
       </c>
@@ -17717,8 +18577,11 @@
       <c r="R28" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="29" spans="1:18">
+      <c r="S28" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19">
       <c r="A29">
         <v>90</v>
       </c>
@@ -17773,8 +18636,11 @@
       <c r="R29" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="30" spans="1:18">
+      <c r="S29" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19">
       <c r="A30">
         <v>91</v>
       </c>
@@ -17829,8 +18695,11 @@
       <c r="R30" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="31" spans="1:18">
+      <c r="S30" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19">
       <c r="A31">
         <v>92</v>
       </c>
@@ -17885,8 +18754,11 @@
       <c r="R31" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="32" spans="1:18">
+      <c r="S31" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19">
       <c r="A32">
         <v>93</v>
       </c>
@@ -17941,8 +18813,11 @@
       <c r="R32" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="33" spans="1:18">
+      <c r="S32" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19">
       <c r="A33">
         <v>94</v>
       </c>
@@ -17996,6 +18871,9 @@
       </c>
       <c r="R33" t="s">
         <v>329</v>
+      </c>
+      <c r="S33" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -18005,15 +18883,19 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q33"/>
+  <dimension ref="A1:R33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="S10" sqref="S10"/>
+      <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="17" max="17" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:18">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -18065,8 +18947,11 @@
       <c r="Q1" t="s">
         <v>339</v>
       </c>
-    </row>
-    <row r="2" spans="1:17">
+      <c r="R1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
       <c r="A2">
         <v>63</v>
       </c>
@@ -18100,8 +18985,11 @@
       <c r="Q2" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="3" spans="1:17">
+      <c r="R2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
       <c r="A3">
         <v>64</v>
       </c>
@@ -18135,8 +19023,11 @@
       <c r="Q3" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="4" spans="1:17">
+      <c r="R3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
       <c r="A4">
         <v>65</v>
       </c>
@@ -18170,8 +19061,11 @@
       <c r="Q4" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="5" spans="1:17">
+      <c r="R4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
       <c r="A5">
         <v>66</v>
       </c>
@@ -18205,8 +19099,11 @@
       <c r="Q5" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="6" spans="1:17">
+      <c r="R5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
       <c r="A6">
         <v>67</v>
       </c>
@@ -18240,8 +19137,11 @@
       <c r="Q6" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="7" spans="1:17">
+      <c r="R6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18">
       <c r="A7">
         <v>68</v>
       </c>
@@ -18275,8 +19175,11 @@
       <c r="Q7" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="8" spans="1:17">
+      <c r="R7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18">
       <c r="A8">
         <v>69</v>
       </c>
@@ -18319,8 +19222,11 @@
       <c r="Q8" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="9" spans="1:17">
+      <c r="R8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18">
       <c r="A9">
         <v>70</v>
       </c>
@@ -18363,8 +19269,11 @@
       <c r="Q9" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="10" spans="1:17">
+      <c r="R9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18">
       <c r="A10">
         <v>71</v>
       </c>
@@ -18407,8 +19316,11 @@
       <c r="Q10" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="11" spans="1:17">
+      <c r="R10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18">
       <c r="A11">
         <v>72</v>
       </c>
@@ -18451,8 +19363,11 @@
       <c r="Q11" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="12" spans="1:17">
+      <c r="R11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18">
       <c r="A12">
         <v>73</v>
       </c>
@@ -18495,8 +19410,11 @@
       <c r="Q12" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="13" spans="1:17">
+      <c r="R12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18">
       <c r="A13">
         <v>74</v>
       </c>
@@ -18542,8 +19460,11 @@
       <c r="Q13" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="14" spans="1:17">
+      <c r="R13" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18">
       <c r="A14">
         <v>75</v>
       </c>
@@ -18589,8 +19510,11 @@
       <c r="Q14" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="15" spans="1:17">
+      <c r="R14" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18">
       <c r="A15">
         <v>76</v>
       </c>
@@ -18636,8 +19560,11 @@
       <c r="Q15" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="16" spans="1:17">
+      <c r="R15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18">
       <c r="A16">
         <v>77</v>
       </c>
@@ -18683,8 +19610,11 @@
       <c r="Q16" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="17" spans="1:17">
+      <c r="R16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18">
       <c r="A17">
         <v>78</v>
       </c>
@@ -18730,8 +19660,11 @@
       <c r="Q17" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="18" spans="1:17">
+      <c r="R17" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18">
       <c r="A18">
         <v>79</v>
       </c>
@@ -18777,8 +19710,11 @@
       <c r="Q18" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="19" spans="1:17">
+      <c r="R18" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18">
       <c r="A19">
         <v>80</v>
       </c>
@@ -18824,8 +19760,11 @@
       <c r="Q19" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="20" spans="1:17">
+      <c r="R19" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18">
       <c r="A20">
         <v>81</v>
       </c>
@@ -18871,8 +19810,11 @@
       <c r="Q20" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="21" spans="1:17">
+      <c r="R20" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18">
       <c r="A21">
         <v>82</v>
       </c>
@@ -18918,8 +19860,11 @@
       <c r="Q21" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="22" spans="1:17">
+      <c r="R21" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18">
       <c r="A22">
         <v>83</v>
       </c>
@@ -18965,8 +19910,11 @@
       <c r="Q22" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="23" spans="1:17">
+      <c r="R22" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18">
       <c r="A23">
         <v>84</v>
       </c>
@@ -19018,8 +19966,11 @@
       <c r="Q23" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="24" spans="1:17">
+      <c r="R23" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18">
       <c r="A24">
         <v>85</v>
       </c>
@@ -19071,8 +20022,11 @@
       <c r="Q24" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="25" spans="1:17">
+      <c r="R24" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18">
       <c r="A25">
         <v>86</v>
       </c>
@@ -19124,8 +20078,11 @@
       <c r="Q25" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="26" spans="1:17">
+      <c r="R25" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18">
       <c r="A26">
         <v>87</v>
       </c>
@@ -19177,8 +20134,11 @@
       <c r="Q26" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="27" spans="1:17">
+      <c r="R26" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18">
       <c r="A27">
         <v>88</v>
       </c>
@@ -19230,8 +20190,11 @@
       <c r="Q27" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="28" spans="1:17">
+      <c r="R27" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18">
       <c r="A28">
         <v>89</v>
       </c>
@@ -19283,8 +20246,11 @@
       <c r="Q28" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="29" spans="1:17">
+      <c r="R28" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18">
       <c r="A29">
         <v>90</v>
       </c>
@@ -19336,8 +20302,11 @@
       <c r="Q29" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="30" spans="1:17">
+      <c r="R29" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18">
       <c r="A30">
         <v>91</v>
       </c>
@@ -19389,8 +20358,11 @@
       <c r="Q30" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="31" spans="1:17">
+      <c r="R30" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18">
       <c r="A31">
         <v>92</v>
       </c>
@@ -19442,8 +20414,11 @@
       <c r="Q31" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="32" spans="1:17">
+      <c r="R31" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18">
       <c r="A32">
         <v>93</v>
       </c>
@@ -19495,8 +20470,11 @@
       <c r="Q32" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="33" spans="1:17">
+      <c r="R32" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18">
       <c r="A33">
         <v>94</v>
       </c>
@@ -19547,6 +20525,9 @@
       </c>
       <c r="Q33" t="s">
         <v>329</v>
+      </c>
+      <c r="R33" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add six files & edit Metadata.xlsx
</commit_message>
<xml_diff>
--- a/Data/MetaData.xlsx
+++ b/Data/MetaData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="6150" firstSheet="6" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="6150" firstSheet="16" activeTab="18"/>
   </bookViews>
   <sheets>
     <sheet name="CompressedFileNames" sheetId="1" r:id="rId1"/>
@@ -25,13 +25,17 @@
     <sheet name="RegionWeights" sheetId="9" r:id="rId16"/>
     <sheet name="MedicalTables" sheetId="13" r:id="rId17"/>
     <sheet name="EducationTables" sheetId="14" r:id="rId18"/>
+    <sheet name="Expenditure Tables" sheetId="20" r:id="rId19"/>
+    <sheet name="ClothTables" sheetId="21" r:id="rId20"/>
+    <sheet name="EnergyTables" sheetId="22" r:id="rId21"/>
+    <sheet name="FurnitureTables" sheetId="23" r:id="rId22"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4151" uniqueCount="380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5140" uniqueCount="404">
   <si>
     <t>Year</t>
   </si>
@@ -1171,6 +1175,78 @@
   </si>
   <si>
     <t>Dycol05</t>
+  </si>
+  <si>
+    <t>P3S02</t>
+  </si>
+  <si>
+    <t>P3S07</t>
+  </si>
+  <si>
+    <t>P3S08</t>
+  </si>
+  <si>
+    <t>P3S10</t>
+  </si>
+  <si>
+    <t>P3S11</t>
+  </si>
+  <si>
+    <t>P3S12</t>
+  </si>
+  <si>
+    <t>P3S14</t>
+  </si>
+  <si>
+    <t>food</t>
+  </si>
+  <si>
+    <t>cigar</t>
+  </si>
+  <si>
+    <t>furniture</t>
+  </si>
+  <si>
+    <t>medical</t>
+  </si>
+  <si>
+    <t>transportation</t>
+  </si>
+  <si>
+    <t>communiccation</t>
+  </si>
+  <si>
+    <t>amusement</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>badavam</t>
+  </si>
+  <si>
+    <t>investment</t>
+  </si>
+  <si>
+    <t>education</t>
+  </si>
+  <si>
+    <t>hotel</t>
+  </si>
+  <si>
+    <t>cloth</t>
+  </si>
+  <si>
+    <t>Cloth_Exp</t>
+  </si>
+  <si>
+    <t>home</t>
+  </si>
+  <si>
+    <t>Energy_Exp</t>
+  </si>
+  <si>
+    <t>Furniture_Exp</t>
   </si>
 </sst>
 </file>
@@ -2021,7 +2097,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3979,8 +4055,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7062,7 +7138,7 @@
   <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="F2" sqref="F2:G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9671,7 +9747,7 @@
   <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11438,6 +11514,1542 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="8" max="8" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.5703125" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="9.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1" t="s">
+        <v>388</v>
+      </c>
+      <c r="D1" t="s">
+        <v>399</v>
+      </c>
+      <c r="E1" t="s">
+        <v>401</v>
+      </c>
+      <c r="F1" t="s">
+        <v>389</v>
+      </c>
+      <c r="G1" t="s">
+        <v>390</v>
+      </c>
+      <c r="H1" t="s">
+        <v>391</v>
+      </c>
+      <c r="I1" t="s">
+        <v>392</v>
+      </c>
+      <c r="J1" t="s">
+        <v>393</v>
+      </c>
+      <c r="K1" t="s">
+        <v>397</v>
+      </c>
+      <c r="L1" t="s">
+        <v>398</v>
+      </c>
+      <c r="M1" t="s">
+        <v>394</v>
+      </c>
+      <c r="N1" t="s">
+        <v>395</v>
+      </c>
+      <c r="O1" t="s">
+        <v>396</v>
+      </c>
+      <c r="P1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
+      <c r="A2">
+        <v>63</v>
+      </c>
+      <c r="B2" t="s">
+        <v>299</v>
+      </c>
+      <c r="C2" t="s">
+        <v>299</v>
+      </c>
+      <c r="D2" t="s">
+        <v>380</v>
+      </c>
+      <c r="E2" t="s">
+        <v>288</v>
+      </c>
+      <c r="F2" t="s">
+        <v>287</v>
+      </c>
+      <c r="G2" t="s">
+        <v>347</v>
+      </c>
+      <c r="H2" t="s">
+        <v>346</v>
+      </c>
+      <c r="I2" t="s">
+        <v>346</v>
+      </c>
+      <c r="J2" t="s">
+        <v>381</v>
+      </c>
+      <c r="M2" t="s">
+        <v>382</v>
+      </c>
+      <c r="N2" t="s">
+        <v>273</v>
+      </c>
+      <c r="P2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
+      <c r="A3">
+        <v>64</v>
+      </c>
+      <c r="B3" t="s">
+        <v>299</v>
+      </c>
+      <c r="C3" t="s">
+        <v>299</v>
+      </c>
+      <c r="D3" t="s">
+        <v>380</v>
+      </c>
+      <c r="E3" t="s">
+        <v>288</v>
+      </c>
+      <c r="F3" t="s">
+        <v>287</v>
+      </c>
+      <c r="G3" t="s">
+        <v>347</v>
+      </c>
+      <c r="H3" t="s">
+        <v>346</v>
+      </c>
+      <c r="I3" t="s">
+        <v>346</v>
+      </c>
+      <c r="J3" t="s">
+        <v>381</v>
+      </c>
+      <c r="M3" t="s">
+        <v>382</v>
+      </c>
+      <c r="N3" t="s">
+        <v>273</v>
+      </c>
+      <c r="P3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
+      <c r="A4">
+        <v>65</v>
+      </c>
+      <c r="B4" t="s">
+        <v>299</v>
+      </c>
+      <c r="C4" t="s">
+        <v>299</v>
+      </c>
+      <c r="D4" t="s">
+        <v>380</v>
+      </c>
+      <c r="E4" t="s">
+        <v>288</v>
+      </c>
+      <c r="F4" t="s">
+        <v>287</v>
+      </c>
+      <c r="G4" t="s">
+        <v>347</v>
+      </c>
+      <c r="H4" t="s">
+        <v>346</v>
+      </c>
+      <c r="I4" t="s">
+        <v>346</v>
+      </c>
+      <c r="J4" t="s">
+        <v>381</v>
+      </c>
+      <c r="M4" t="s">
+        <v>382</v>
+      </c>
+      <c r="N4" t="s">
+        <v>273</v>
+      </c>
+      <c r="P4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
+      <c r="A5">
+        <v>66</v>
+      </c>
+      <c r="B5" t="s">
+        <v>299</v>
+      </c>
+      <c r="C5" t="s">
+        <v>299</v>
+      </c>
+      <c r="D5" t="s">
+        <v>380</v>
+      </c>
+      <c r="E5" t="s">
+        <v>288</v>
+      </c>
+      <c r="F5" t="s">
+        <v>287</v>
+      </c>
+      <c r="G5" t="s">
+        <v>347</v>
+      </c>
+      <c r="H5" t="s">
+        <v>346</v>
+      </c>
+      <c r="I5" t="s">
+        <v>346</v>
+      </c>
+      <c r="J5" t="s">
+        <v>381</v>
+      </c>
+      <c r="M5" t="s">
+        <v>382</v>
+      </c>
+      <c r="N5" t="s">
+        <v>273</v>
+      </c>
+      <c r="O5" t="s">
+        <v>383</v>
+      </c>
+      <c r="P5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
+      <c r="A6">
+        <v>67</v>
+      </c>
+      <c r="B6" t="s">
+        <v>299</v>
+      </c>
+      <c r="C6" t="s">
+        <v>299</v>
+      </c>
+      <c r="D6" t="s">
+        <v>380</v>
+      </c>
+      <c r="E6" t="s">
+        <v>288</v>
+      </c>
+      <c r="F6" t="s">
+        <v>287</v>
+      </c>
+      <c r="G6" t="s">
+        <v>347</v>
+      </c>
+      <c r="H6" t="s">
+        <v>346</v>
+      </c>
+      <c r="I6" t="s">
+        <v>346</v>
+      </c>
+      <c r="J6" t="s">
+        <v>381</v>
+      </c>
+      <c r="M6" t="s">
+        <v>382</v>
+      </c>
+      <c r="N6" t="s">
+        <v>273</v>
+      </c>
+      <c r="O6" t="s">
+        <v>383</v>
+      </c>
+      <c r="P6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16">
+      <c r="A7">
+        <v>68</v>
+      </c>
+      <c r="B7" t="s">
+        <v>299</v>
+      </c>
+      <c r="C7" t="s">
+        <v>299</v>
+      </c>
+      <c r="D7" t="s">
+        <v>380</v>
+      </c>
+      <c r="E7" t="s">
+        <v>288</v>
+      </c>
+      <c r="F7" t="s">
+        <v>287</v>
+      </c>
+      <c r="G7" t="s">
+        <v>347</v>
+      </c>
+      <c r="H7" t="s">
+        <v>346</v>
+      </c>
+      <c r="I7" t="s">
+        <v>346</v>
+      </c>
+      <c r="J7" t="s">
+        <v>381</v>
+      </c>
+      <c r="M7" t="s">
+        <v>382</v>
+      </c>
+      <c r="N7" t="s">
+        <v>273</v>
+      </c>
+      <c r="O7" t="s">
+        <v>383</v>
+      </c>
+      <c r="P7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16">
+      <c r="A8">
+        <v>69</v>
+      </c>
+      <c r="B8" t="s">
+        <v>299</v>
+      </c>
+      <c r="C8" t="s">
+        <v>299</v>
+      </c>
+      <c r="D8" t="s">
+        <v>380</v>
+      </c>
+      <c r="E8" t="s">
+        <v>288</v>
+      </c>
+      <c r="F8" t="s">
+        <v>287</v>
+      </c>
+      <c r="G8" t="s">
+        <v>347</v>
+      </c>
+      <c r="H8" t="s">
+        <v>346</v>
+      </c>
+      <c r="I8" t="s">
+        <v>346</v>
+      </c>
+      <c r="J8" t="s">
+        <v>381</v>
+      </c>
+      <c r="M8" t="s">
+        <v>382</v>
+      </c>
+      <c r="N8" t="s">
+        <v>273</v>
+      </c>
+      <c r="O8" t="s">
+        <v>383</v>
+      </c>
+      <c r="P8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
+      <c r="A9">
+        <v>70</v>
+      </c>
+      <c r="B9" t="s">
+        <v>299</v>
+      </c>
+      <c r="C9" t="s">
+        <v>299</v>
+      </c>
+      <c r="D9" t="s">
+        <v>380</v>
+      </c>
+      <c r="E9" t="s">
+        <v>288</v>
+      </c>
+      <c r="F9" t="s">
+        <v>287</v>
+      </c>
+      <c r="G9" t="s">
+        <v>347</v>
+      </c>
+      <c r="H9" t="s">
+        <v>346</v>
+      </c>
+      <c r="I9" t="s">
+        <v>346</v>
+      </c>
+      <c r="J9" t="s">
+        <v>381</v>
+      </c>
+      <c r="M9" t="s">
+        <v>382</v>
+      </c>
+      <c r="N9" t="s">
+        <v>273</v>
+      </c>
+      <c r="O9" t="s">
+        <v>383</v>
+      </c>
+      <c r="P9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16">
+      <c r="A10">
+        <v>71</v>
+      </c>
+      <c r="B10" t="s">
+        <v>299</v>
+      </c>
+      <c r="C10" t="s">
+        <v>299</v>
+      </c>
+      <c r="D10" t="s">
+        <v>380</v>
+      </c>
+      <c r="E10" t="s">
+        <v>288</v>
+      </c>
+      <c r="F10" t="s">
+        <v>287</v>
+      </c>
+      <c r="G10" t="s">
+        <v>347</v>
+      </c>
+      <c r="H10" t="s">
+        <v>346</v>
+      </c>
+      <c r="I10" t="s">
+        <v>346</v>
+      </c>
+      <c r="J10" t="s">
+        <v>381</v>
+      </c>
+      <c r="M10" t="s">
+        <v>382</v>
+      </c>
+      <c r="N10" t="s">
+        <v>273</v>
+      </c>
+      <c r="O10" t="s">
+        <v>383</v>
+      </c>
+      <c r="P10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16">
+      <c r="A11">
+        <v>72</v>
+      </c>
+      <c r="B11" t="s">
+        <v>299</v>
+      </c>
+      <c r="C11" t="s">
+        <v>299</v>
+      </c>
+      <c r="D11" t="s">
+        <v>380</v>
+      </c>
+      <c r="E11" t="s">
+        <v>288</v>
+      </c>
+      <c r="F11" t="s">
+        <v>287</v>
+      </c>
+      <c r="G11" t="s">
+        <v>347</v>
+      </c>
+      <c r="H11" t="s">
+        <v>346</v>
+      </c>
+      <c r="I11" t="s">
+        <v>346</v>
+      </c>
+      <c r="J11" t="s">
+        <v>381</v>
+      </c>
+      <c r="M11" t="s">
+        <v>382</v>
+      </c>
+      <c r="N11" t="s">
+        <v>273</v>
+      </c>
+      <c r="O11" t="s">
+        <v>383</v>
+      </c>
+      <c r="P11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16">
+      <c r="A12">
+        <v>73</v>
+      </c>
+      <c r="B12" t="s">
+        <v>299</v>
+      </c>
+      <c r="C12" t="s">
+        <v>299</v>
+      </c>
+      <c r="D12" t="s">
+        <v>380</v>
+      </c>
+      <c r="E12" t="s">
+        <v>288</v>
+      </c>
+      <c r="F12" t="s">
+        <v>287</v>
+      </c>
+      <c r="G12" t="s">
+        <v>347</v>
+      </c>
+      <c r="H12" t="s">
+        <v>346</v>
+      </c>
+      <c r="I12" t="s">
+        <v>346</v>
+      </c>
+      <c r="J12" t="s">
+        <v>381</v>
+      </c>
+      <c r="M12" t="s">
+        <v>382</v>
+      </c>
+      <c r="N12" t="s">
+        <v>273</v>
+      </c>
+      <c r="O12" t="s">
+        <v>383</v>
+      </c>
+      <c r="P12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16">
+      <c r="A13">
+        <v>74</v>
+      </c>
+      <c r="B13" t="s">
+        <v>299</v>
+      </c>
+      <c r="C13" t="s">
+        <v>299</v>
+      </c>
+      <c r="D13" t="s">
+        <v>380</v>
+      </c>
+      <c r="E13" t="s">
+        <v>288</v>
+      </c>
+      <c r="F13" t="s">
+        <v>287</v>
+      </c>
+      <c r="G13" t="s">
+        <v>347</v>
+      </c>
+      <c r="H13" t="s">
+        <v>346</v>
+      </c>
+      <c r="I13" t="s">
+        <v>346</v>
+      </c>
+      <c r="J13" t="s">
+        <v>381</v>
+      </c>
+      <c r="M13" t="s">
+        <v>382</v>
+      </c>
+      <c r="N13" t="s">
+        <v>273</v>
+      </c>
+      <c r="O13" t="s">
+        <v>383</v>
+      </c>
+      <c r="P13" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16">
+      <c r="A14">
+        <v>75</v>
+      </c>
+      <c r="B14" t="s">
+        <v>299</v>
+      </c>
+      <c r="C14" t="s">
+        <v>299</v>
+      </c>
+      <c r="D14" t="s">
+        <v>380</v>
+      </c>
+      <c r="E14" t="s">
+        <v>288</v>
+      </c>
+      <c r="F14" t="s">
+        <v>287</v>
+      </c>
+      <c r="G14" t="s">
+        <v>347</v>
+      </c>
+      <c r="H14" t="s">
+        <v>346</v>
+      </c>
+      <c r="I14" t="s">
+        <v>346</v>
+      </c>
+      <c r="J14" t="s">
+        <v>381</v>
+      </c>
+      <c r="M14" t="s">
+        <v>382</v>
+      </c>
+      <c r="N14" t="s">
+        <v>273</v>
+      </c>
+      <c r="O14" s="2"/>
+      <c r="P14" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16">
+      <c r="A15">
+        <v>76</v>
+      </c>
+      <c r="B15" t="s">
+        <v>299</v>
+      </c>
+      <c r="C15" t="s">
+        <v>299</v>
+      </c>
+      <c r="D15" t="s">
+        <v>380</v>
+      </c>
+      <c r="E15" t="s">
+        <v>288</v>
+      </c>
+      <c r="F15" t="s">
+        <v>287</v>
+      </c>
+      <c r="G15" t="s">
+        <v>347</v>
+      </c>
+      <c r="H15" t="s">
+        <v>346</v>
+      </c>
+      <c r="I15" t="s">
+        <v>346</v>
+      </c>
+      <c r="J15" t="s">
+        <v>381</v>
+      </c>
+      <c r="M15" t="s">
+        <v>382</v>
+      </c>
+      <c r="N15" t="s">
+        <v>273</v>
+      </c>
+      <c r="O15" s="2"/>
+      <c r="P15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16">
+      <c r="A16">
+        <v>77</v>
+      </c>
+      <c r="B16" t="s">
+        <v>299</v>
+      </c>
+      <c r="C16" t="s">
+        <v>299</v>
+      </c>
+      <c r="D16" t="s">
+        <v>380</v>
+      </c>
+      <c r="E16" t="s">
+        <v>288</v>
+      </c>
+      <c r="F16" t="s">
+        <v>287</v>
+      </c>
+      <c r="G16" t="s">
+        <v>347</v>
+      </c>
+      <c r="H16" t="s">
+        <v>346</v>
+      </c>
+      <c r="I16" t="s">
+        <v>346</v>
+      </c>
+      <c r="J16" t="s">
+        <v>381</v>
+      </c>
+      <c r="M16" t="s">
+        <v>382</v>
+      </c>
+      <c r="N16" t="s">
+        <v>273</v>
+      </c>
+      <c r="O16" s="2"/>
+      <c r="P16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16">
+      <c r="A17">
+        <v>78</v>
+      </c>
+      <c r="B17" t="s">
+        <v>299</v>
+      </c>
+      <c r="C17" t="s">
+        <v>299</v>
+      </c>
+      <c r="D17" t="s">
+        <v>380</v>
+      </c>
+      <c r="E17" t="s">
+        <v>288</v>
+      </c>
+      <c r="F17" t="s">
+        <v>287</v>
+      </c>
+      <c r="G17" t="s">
+        <v>347</v>
+      </c>
+      <c r="H17" t="s">
+        <v>346</v>
+      </c>
+      <c r="I17" t="s">
+        <v>346</v>
+      </c>
+      <c r="J17" t="s">
+        <v>381</v>
+      </c>
+      <c r="M17" t="s">
+        <v>382</v>
+      </c>
+      <c r="N17" t="s">
+        <v>273</v>
+      </c>
+      <c r="O17" t="s">
+        <v>383</v>
+      </c>
+      <c r="P17" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16">
+      <c r="A18">
+        <v>79</v>
+      </c>
+      <c r="B18" t="s">
+        <v>299</v>
+      </c>
+      <c r="C18" t="s">
+        <v>299</v>
+      </c>
+      <c r="D18" t="s">
+        <v>380</v>
+      </c>
+      <c r="E18" t="s">
+        <v>288</v>
+      </c>
+      <c r="F18" t="s">
+        <v>287</v>
+      </c>
+      <c r="G18" t="s">
+        <v>347</v>
+      </c>
+      <c r="H18" t="s">
+        <v>346</v>
+      </c>
+      <c r="I18" t="s">
+        <v>346</v>
+      </c>
+      <c r="J18" t="s">
+        <v>381</v>
+      </c>
+      <c r="M18" t="s">
+        <v>382</v>
+      </c>
+      <c r="N18" t="s">
+        <v>273</v>
+      </c>
+      <c r="O18" t="s">
+        <v>383</v>
+      </c>
+      <c r="P18" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16">
+      <c r="A19">
+        <v>80</v>
+      </c>
+      <c r="B19" t="s">
+        <v>299</v>
+      </c>
+      <c r="C19" t="s">
+        <v>299</v>
+      </c>
+      <c r="D19" t="s">
+        <v>380</v>
+      </c>
+      <c r="E19" t="s">
+        <v>288</v>
+      </c>
+      <c r="F19" t="s">
+        <v>287</v>
+      </c>
+      <c r="G19" t="s">
+        <v>347</v>
+      </c>
+      <c r="H19" t="s">
+        <v>346</v>
+      </c>
+      <c r="I19" t="s">
+        <v>346</v>
+      </c>
+      <c r="J19" t="s">
+        <v>381</v>
+      </c>
+      <c r="M19" t="s">
+        <v>382</v>
+      </c>
+      <c r="N19" t="s">
+        <v>273</v>
+      </c>
+      <c r="O19" t="s">
+        <v>383</v>
+      </c>
+      <c r="P19" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16">
+      <c r="A20">
+        <v>81</v>
+      </c>
+      <c r="B20" t="s">
+        <v>299</v>
+      </c>
+      <c r="C20" t="s">
+        <v>299</v>
+      </c>
+      <c r="D20" t="s">
+        <v>380</v>
+      </c>
+      <c r="E20" t="s">
+        <v>288</v>
+      </c>
+      <c r="F20" t="s">
+        <v>287</v>
+      </c>
+      <c r="G20" t="s">
+        <v>347</v>
+      </c>
+      <c r="H20" t="s">
+        <v>346</v>
+      </c>
+      <c r="I20" t="s">
+        <v>346</v>
+      </c>
+      <c r="J20" t="s">
+        <v>381</v>
+      </c>
+      <c r="M20" t="s">
+        <v>382</v>
+      </c>
+      <c r="N20" t="s">
+        <v>273</v>
+      </c>
+      <c r="O20" t="s">
+        <v>383</v>
+      </c>
+      <c r="P20" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16">
+      <c r="A21">
+        <v>82</v>
+      </c>
+      <c r="B21" t="s">
+        <v>299</v>
+      </c>
+      <c r="C21" t="s">
+        <v>299</v>
+      </c>
+      <c r="D21" t="s">
+        <v>380</v>
+      </c>
+      <c r="E21" t="s">
+        <v>288</v>
+      </c>
+      <c r="F21" t="s">
+        <v>287</v>
+      </c>
+      <c r="G21" t="s">
+        <v>347</v>
+      </c>
+      <c r="H21" t="s">
+        <v>346</v>
+      </c>
+      <c r="I21" t="s">
+        <v>346</v>
+      </c>
+      <c r="J21" t="s">
+        <v>381</v>
+      </c>
+      <c r="M21" t="s">
+        <v>382</v>
+      </c>
+      <c r="N21" t="s">
+        <v>273</v>
+      </c>
+      <c r="O21" t="s">
+        <v>383</v>
+      </c>
+      <c r="P21" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16">
+      <c r="A22">
+        <v>83</v>
+      </c>
+      <c r="B22" t="s">
+        <v>299</v>
+      </c>
+      <c r="C22" t="s">
+        <v>380</v>
+      </c>
+      <c r="D22" t="s">
+        <v>288</v>
+      </c>
+      <c r="E22" t="s">
+        <v>287</v>
+      </c>
+      <c r="F22" t="s">
+        <v>347</v>
+      </c>
+      <c r="G22" t="s">
+        <v>346</v>
+      </c>
+      <c r="H22" t="s">
+        <v>381</v>
+      </c>
+      <c r="I22" t="s">
+        <v>382</v>
+      </c>
+      <c r="J22" t="s">
+        <v>273</v>
+      </c>
+      <c r="K22" t="s">
+        <v>383</v>
+      </c>
+      <c r="L22" t="s">
+        <v>384</v>
+      </c>
+      <c r="M22" t="s">
+        <v>385</v>
+      </c>
+      <c r="N22" t="s">
+        <v>276</v>
+      </c>
+      <c r="O22" t="s">
+        <v>386</v>
+      </c>
+      <c r="P22" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16">
+      <c r="A23">
+        <v>84</v>
+      </c>
+      <c r="B23" t="s">
+        <v>299</v>
+      </c>
+      <c r="C23" t="s">
+        <v>380</v>
+      </c>
+      <c r="D23" t="s">
+        <v>288</v>
+      </c>
+      <c r="E23" t="s">
+        <v>287</v>
+      </c>
+      <c r="F23" t="s">
+        <v>347</v>
+      </c>
+      <c r="G23" t="s">
+        <v>346</v>
+      </c>
+      <c r="H23" t="s">
+        <v>381</v>
+      </c>
+      <c r="I23" t="s">
+        <v>382</v>
+      </c>
+      <c r="J23" t="s">
+        <v>273</v>
+      </c>
+      <c r="K23" t="s">
+        <v>383</v>
+      </c>
+      <c r="L23" t="s">
+        <v>384</v>
+      </c>
+      <c r="M23" t="s">
+        <v>385</v>
+      </c>
+      <c r="N23" t="s">
+        <v>276</v>
+      </c>
+      <c r="O23" t="s">
+        <v>386</v>
+      </c>
+      <c r="P23" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16">
+      <c r="A24">
+        <v>85</v>
+      </c>
+      <c r="B24" t="s">
+        <v>299</v>
+      </c>
+      <c r="C24" t="s">
+        <v>380</v>
+      </c>
+      <c r="D24" t="s">
+        <v>288</v>
+      </c>
+      <c r="E24" t="s">
+        <v>287</v>
+      </c>
+      <c r="F24" t="s">
+        <v>347</v>
+      </c>
+      <c r="G24" t="s">
+        <v>346</v>
+      </c>
+      <c r="H24" t="s">
+        <v>381</v>
+      </c>
+      <c r="I24" t="s">
+        <v>382</v>
+      </c>
+      <c r="J24" t="s">
+        <v>273</v>
+      </c>
+      <c r="K24" t="s">
+        <v>383</v>
+      </c>
+      <c r="L24" t="s">
+        <v>384</v>
+      </c>
+      <c r="M24" t="s">
+        <v>385</v>
+      </c>
+      <c r="N24" t="s">
+        <v>276</v>
+      </c>
+      <c r="O24" t="s">
+        <v>386</v>
+      </c>
+      <c r="P24" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16">
+      <c r="A25">
+        <v>86</v>
+      </c>
+      <c r="B25" t="s">
+        <v>299</v>
+      </c>
+      <c r="C25" t="s">
+        <v>380</v>
+      </c>
+      <c r="D25" t="s">
+        <v>288</v>
+      </c>
+      <c r="E25" t="s">
+        <v>287</v>
+      </c>
+      <c r="F25" t="s">
+        <v>347</v>
+      </c>
+      <c r="G25" t="s">
+        <v>346</v>
+      </c>
+      <c r="H25" t="s">
+        <v>381</v>
+      </c>
+      <c r="I25" t="s">
+        <v>382</v>
+      </c>
+      <c r="J25" t="s">
+        <v>273</v>
+      </c>
+      <c r="K25" t="s">
+        <v>383</v>
+      </c>
+      <c r="L25" t="s">
+        <v>384</v>
+      </c>
+      <c r="M25" t="s">
+        <v>385</v>
+      </c>
+      <c r="N25" t="s">
+        <v>276</v>
+      </c>
+      <c r="O25" t="s">
+        <v>386</v>
+      </c>
+      <c r="P25" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16">
+      <c r="A26">
+        <v>87</v>
+      </c>
+      <c r="B26" t="s">
+        <v>299</v>
+      </c>
+      <c r="C26" t="s">
+        <v>380</v>
+      </c>
+      <c r="D26" t="s">
+        <v>288</v>
+      </c>
+      <c r="E26" t="s">
+        <v>287</v>
+      </c>
+      <c r="F26" t="s">
+        <v>347</v>
+      </c>
+      <c r="G26" t="s">
+        <v>346</v>
+      </c>
+      <c r="H26" t="s">
+        <v>381</v>
+      </c>
+      <c r="I26" t="s">
+        <v>382</v>
+      </c>
+      <c r="J26" t="s">
+        <v>273</v>
+      </c>
+      <c r="K26" t="s">
+        <v>383</v>
+      </c>
+      <c r="L26" t="s">
+        <v>384</v>
+      </c>
+      <c r="M26" t="s">
+        <v>385</v>
+      </c>
+      <c r="N26" t="s">
+        <v>276</v>
+      </c>
+      <c r="O26" t="s">
+        <v>386</v>
+      </c>
+      <c r="P26" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16">
+      <c r="A27">
+        <v>88</v>
+      </c>
+      <c r="B27" t="s">
+        <v>299</v>
+      </c>
+      <c r="C27" t="s">
+        <v>380</v>
+      </c>
+      <c r="D27" t="s">
+        <v>288</v>
+      </c>
+      <c r="E27" t="s">
+        <v>287</v>
+      </c>
+      <c r="F27" t="s">
+        <v>347</v>
+      </c>
+      <c r="G27" t="s">
+        <v>346</v>
+      </c>
+      <c r="H27" t="s">
+        <v>381</v>
+      </c>
+      <c r="I27" t="s">
+        <v>382</v>
+      </c>
+      <c r="J27" t="s">
+        <v>273</v>
+      </c>
+      <c r="K27" t="s">
+        <v>383</v>
+      </c>
+      <c r="L27" t="s">
+        <v>384</v>
+      </c>
+      <c r="M27" t="s">
+        <v>385</v>
+      </c>
+      <c r="N27" t="s">
+        <v>276</v>
+      </c>
+      <c r="O27" t="s">
+        <v>386</v>
+      </c>
+      <c r="P27" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16">
+      <c r="A28">
+        <v>89</v>
+      </c>
+      <c r="B28" t="s">
+        <v>299</v>
+      </c>
+      <c r="C28" t="s">
+        <v>380</v>
+      </c>
+      <c r="D28" t="s">
+        <v>288</v>
+      </c>
+      <c r="E28" t="s">
+        <v>287</v>
+      </c>
+      <c r="F28" t="s">
+        <v>347</v>
+      </c>
+      <c r="G28" t="s">
+        <v>346</v>
+      </c>
+      <c r="H28" t="s">
+        <v>381</v>
+      </c>
+      <c r="I28" t="s">
+        <v>382</v>
+      </c>
+      <c r="J28" t="s">
+        <v>273</v>
+      </c>
+      <c r="K28" t="s">
+        <v>383</v>
+      </c>
+      <c r="L28" t="s">
+        <v>384</v>
+      </c>
+      <c r="M28" t="s">
+        <v>385</v>
+      </c>
+      <c r="N28" t="s">
+        <v>276</v>
+      </c>
+      <c r="O28" t="s">
+        <v>386</v>
+      </c>
+      <c r="P28" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16">
+      <c r="A29">
+        <v>90</v>
+      </c>
+      <c r="B29" t="s">
+        <v>299</v>
+      </c>
+      <c r="C29" t="s">
+        <v>380</v>
+      </c>
+      <c r="D29" t="s">
+        <v>288</v>
+      </c>
+      <c r="E29" t="s">
+        <v>287</v>
+      </c>
+      <c r="F29" t="s">
+        <v>347</v>
+      </c>
+      <c r="G29" t="s">
+        <v>346</v>
+      </c>
+      <c r="H29" t="s">
+        <v>381</v>
+      </c>
+      <c r="I29" t="s">
+        <v>382</v>
+      </c>
+      <c r="J29" t="s">
+        <v>273</v>
+      </c>
+      <c r="K29" t="s">
+        <v>383</v>
+      </c>
+      <c r="L29" t="s">
+        <v>384</v>
+      </c>
+      <c r="M29" t="s">
+        <v>385</v>
+      </c>
+      <c r="N29" t="s">
+        <v>276</v>
+      </c>
+      <c r="O29" t="s">
+        <v>386</v>
+      </c>
+      <c r="P29" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16">
+      <c r="A30">
+        <v>91</v>
+      </c>
+      <c r="B30" t="s">
+        <v>299</v>
+      </c>
+      <c r="C30" t="s">
+        <v>380</v>
+      </c>
+      <c r="D30" t="s">
+        <v>288</v>
+      </c>
+      <c r="E30" t="s">
+        <v>287</v>
+      </c>
+      <c r="F30" t="s">
+        <v>347</v>
+      </c>
+      <c r="G30" t="s">
+        <v>346</v>
+      </c>
+      <c r="H30" t="s">
+        <v>381</v>
+      </c>
+      <c r="I30" t="s">
+        <v>382</v>
+      </c>
+      <c r="J30" t="s">
+        <v>273</v>
+      </c>
+      <c r="K30" t="s">
+        <v>383</v>
+      </c>
+      <c r="L30" t="s">
+        <v>384</v>
+      </c>
+      <c r="M30" t="s">
+        <v>385</v>
+      </c>
+      <c r="N30" t="s">
+        <v>276</v>
+      </c>
+      <c r="O30" t="s">
+        <v>386</v>
+      </c>
+      <c r="P30" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16">
+      <c r="A31">
+        <v>92</v>
+      </c>
+      <c r="B31" t="s">
+        <v>299</v>
+      </c>
+      <c r="C31" t="s">
+        <v>380</v>
+      </c>
+      <c r="D31" t="s">
+        <v>288</v>
+      </c>
+      <c r="E31" t="s">
+        <v>287</v>
+      </c>
+      <c r="F31" t="s">
+        <v>347</v>
+      </c>
+      <c r="G31" t="s">
+        <v>346</v>
+      </c>
+      <c r="H31" t="s">
+        <v>381</v>
+      </c>
+      <c r="I31" t="s">
+        <v>382</v>
+      </c>
+      <c r="J31" t="s">
+        <v>273</v>
+      </c>
+      <c r="K31" t="s">
+        <v>383</v>
+      </c>
+      <c r="L31" t="s">
+        <v>384</v>
+      </c>
+      <c r="M31" t="s">
+        <v>385</v>
+      </c>
+      <c r="N31" t="s">
+        <v>276</v>
+      </c>
+      <c r="O31" t="s">
+        <v>386</v>
+      </c>
+      <c r="P31" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16">
+      <c r="A32">
+        <v>93</v>
+      </c>
+      <c r="B32" t="s">
+        <v>299</v>
+      </c>
+      <c r="C32" t="s">
+        <v>380</v>
+      </c>
+      <c r="D32" t="s">
+        <v>288</v>
+      </c>
+      <c r="E32" t="s">
+        <v>287</v>
+      </c>
+      <c r="F32" t="s">
+        <v>347</v>
+      </c>
+      <c r="G32" t="s">
+        <v>346</v>
+      </c>
+      <c r="H32" t="s">
+        <v>381</v>
+      </c>
+      <c r="I32" t="s">
+        <v>382</v>
+      </c>
+      <c r="J32" t="s">
+        <v>273</v>
+      </c>
+      <c r="K32" t="s">
+        <v>383</v>
+      </c>
+      <c r="L32" t="s">
+        <v>384</v>
+      </c>
+      <c r="M32" t="s">
+        <v>385</v>
+      </c>
+      <c r="N32" t="s">
+        <v>276</v>
+      </c>
+      <c r="O32" t="s">
+        <v>386</v>
+      </c>
+      <c r="P32" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16">
+      <c r="A33">
+        <v>94</v>
+      </c>
+      <c r="B33" t="s">
+        <v>299</v>
+      </c>
+      <c r="C33" t="s">
+        <v>380</v>
+      </c>
+      <c r="D33" t="s">
+        <v>288</v>
+      </c>
+      <c r="E33" t="s">
+        <v>287</v>
+      </c>
+      <c r="F33" t="s">
+        <v>347</v>
+      </c>
+      <c r="G33" t="s">
+        <v>346</v>
+      </c>
+      <c r="H33" t="s">
+        <v>381</v>
+      </c>
+      <c r="I33" t="s">
+        <v>382</v>
+      </c>
+      <c r="J33" t="s">
+        <v>273</v>
+      </c>
+      <c r="K33" t="s">
+        <v>383</v>
+      </c>
+      <c r="L33" t="s">
+        <v>384</v>
+      </c>
+      <c r="M33" t="s">
+        <v>385</v>
+      </c>
+      <c r="N33" t="s">
+        <v>276</v>
+      </c>
+      <c r="O33" t="s">
+        <v>386</v>
+      </c>
+      <c r="P33" t="s">
+        <v>66</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R33"/>
@@ -12694,6 +14306,2361 @@
       </c>
       <c r="N33" t="s">
         <v>75</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J33"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O20" sqref="O20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="14.140625" customWidth="1"/>
+    <col min="10" max="10" width="12.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>269</v>
+      </c>
+      <c r="C1" t="s">
+        <v>291</v>
+      </c>
+      <c r="D1" t="s">
+        <v>292</v>
+      </c>
+      <c r="E1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G1" t="s">
+        <v>300</v>
+      </c>
+      <c r="H1" t="s">
+        <v>352</v>
+      </c>
+      <c r="I1" t="s">
+        <v>353</v>
+      </c>
+      <c r="J1" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2">
+        <v>63</v>
+      </c>
+      <c r="B2" t="s">
+        <v>380</v>
+      </c>
+      <c r="E2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F2" t="s">
+        <v>274</v>
+      </c>
+      <c r="G2" t="s">
+        <v>304</v>
+      </c>
+      <c r="J2" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3">
+        <v>64</v>
+      </c>
+      <c r="B3" t="s">
+        <v>380</v>
+      </c>
+      <c r="E3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F3" t="s">
+        <v>274</v>
+      </c>
+      <c r="G3" t="s">
+        <v>304</v>
+      </c>
+      <c r="J3" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4">
+        <v>65</v>
+      </c>
+      <c r="B4" t="s">
+        <v>380</v>
+      </c>
+      <c r="E4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F4" t="s">
+        <v>274</v>
+      </c>
+      <c r="G4" t="s">
+        <v>304</v>
+      </c>
+      <c r="J4" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5">
+        <v>66</v>
+      </c>
+      <c r="B5" t="s">
+        <v>380</v>
+      </c>
+      <c r="E5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F5" t="s">
+        <v>274</v>
+      </c>
+      <c r="G5" t="s">
+        <v>304</v>
+      </c>
+      <c r="J5" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6">
+        <v>67</v>
+      </c>
+      <c r="B6" t="s">
+        <v>380</v>
+      </c>
+      <c r="E6" t="s">
+        <v>51</v>
+      </c>
+      <c r="F6" t="s">
+        <v>274</v>
+      </c>
+      <c r="G6" t="s">
+        <v>304</v>
+      </c>
+      <c r="J6" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7">
+        <v>68</v>
+      </c>
+      <c r="B7" t="s">
+        <v>380</v>
+      </c>
+      <c r="E7" t="s">
+        <v>51</v>
+      </c>
+      <c r="F7" t="s">
+        <v>274</v>
+      </c>
+      <c r="G7" t="s">
+        <v>304</v>
+      </c>
+      <c r="J7" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8">
+        <v>69</v>
+      </c>
+      <c r="B8" t="s">
+        <v>380</v>
+      </c>
+      <c r="E8" t="s">
+        <v>51</v>
+      </c>
+      <c r="F8" t="s">
+        <v>274</v>
+      </c>
+      <c r="G8" t="s">
+        <v>304</v>
+      </c>
+      <c r="H8" t="s">
+        <v>275</v>
+      </c>
+      <c r="I8" t="s">
+        <v>285</v>
+      </c>
+      <c r="J8" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9">
+        <v>70</v>
+      </c>
+      <c r="B9" t="s">
+        <v>380</v>
+      </c>
+      <c r="E9" t="s">
+        <v>51</v>
+      </c>
+      <c r="F9" t="s">
+        <v>274</v>
+      </c>
+      <c r="G9" t="s">
+        <v>304</v>
+      </c>
+      <c r="H9" t="s">
+        <v>275</v>
+      </c>
+      <c r="J9" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10">
+        <v>71</v>
+      </c>
+      <c r="B10" t="s">
+        <v>380</v>
+      </c>
+      <c r="E10" t="s">
+        <v>51</v>
+      </c>
+      <c r="F10" t="s">
+        <v>274</v>
+      </c>
+      <c r="G10" t="s">
+        <v>304</v>
+      </c>
+      <c r="H10" t="s">
+        <v>275</v>
+      </c>
+      <c r="J10" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11">
+        <v>72</v>
+      </c>
+      <c r="B11" t="s">
+        <v>380</v>
+      </c>
+      <c r="E11" t="s">
+        <v>51</v>
+      </c>
+      <c r="F11" t="s">
+        <v>274</v>
+      </c>
+      <c r="G11" t="s">
+        <v>304</v>
+      </c>
+      <c r="H11" t="s">
+        <v>275</v>
+      </c>
+      <c r="J11" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12">
+        <v>73</v>
+      </c>
+      <c r="B12" t="s">
+        <v>380</v>
+      </c>
+      <c r="E12" t="s">
+        <v>51</v>
+      </c>
+      <c r="F12" t="s">
+        <v>274</v>
+      </c>
+      <c r="G12" t="s">
+        <v>304</v>
+      </c>
+      <c r="H12" t="s">
+        <v>275</v>
+      </c>
+      <c r="J12" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13">
+        <v>74</v>
+      </c>
+      <c r="B13" t="s">
+        <v>380</v>
+      </c>
+      <c r="E13" t="s">
+        <v>51</v>
+      </c>
+      <c r="F13" t="s">
+        <v>274</v>
+      </c>
+      <c r="G13" t="s">
+        <v>304</v>
+      </c>
+      <c r="J13" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14">
+        <v>75</v>
+      </c>
+      <c r="B14" t="s">
+        <v>380</v>
+      </c>
+      <c r="E14" t="s">
+        <v>51</v>
+      </c>
+      <c r="F14" t="s">
+        <v>274</v>
+      </c>
+      <c r="G14" t="s">
+        <v>304</v>
+      </c>
+      <c r="J14" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15">
+        <v>76</v>
+      </c>
+      <c r="B15" t="s">
+        <v>380</v>
+      </c>
+      <c r="E15" t="s">
+        <v>51</v>
+      </c>
+      <c r="F15" t="s">
+        <v>274</v>
+      </c>
+      <c r="G15" t="s">
+        <v>304</v>
+      </c>
+      <c r="J15" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16">
+        <v>77</v>
+      </c>
+      <c r="B16" t="s">
+        <v>380</v>
+      </c>
+      <c r="E16" t="s">
+        <v>51</v>
+      </c>
+      <c r="F16" t="s">
+        <v>274</v>
+      </c>
+      <c r="G16" t="s">
+        <v>304</v>
+      </c>
+      <c r="J16" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17">
+        <v>78</v>
+      </c>
+      <c r="B17" t="s">
+        <v>380</v>
+      </c>
+      <c r="E17" t="s">
+        <v>51</v>
+      </c>
+      <c r="F17" t="s">
+        <v>274</v>
+      </c>
+      <c r="G17" t="s">
+        <v>304</v>
+      </c>
+      <c r="J17" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18">
+        <v>79</v>
+      </c>
+      <c r="B18" t="s">
+        <v>380</v>
+      </c>
+      <c r="E18" t="s">
+        <v>51</v>
+      </c>
+      <c r="F18" t="s">
+        <v>274</v>
+      </c>
+      <c r="G18" t="s">
+        <v>304</v>
+      </c>
+      <c r="J18" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19">
+        <v>80</v>
+      </c>
+      <c r="B19" t="s">
+        <v>380</v>
+      </c>
+      <c r="E19" t="s">
+        <v>51</v>
+      </c>
+      <c r="F19" t="s">
+        <v>274</v>
+      </c>
+      <c r="G19" t="s">
+        <v>304</v>
+      </c>
+      <c r="J19" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20">
+        <v>81</v>
+      </c>
+      <c r="B20" t="s">
+        <v>380</v>
+      </c>
+      <c r="E20" t="s">
+        <v>51</v>
+      </c>
+      <c r="F20" t="s">
+        <v>274</v>
+      </c>
+      <c r="G20" t="s">
+        <v>304</v>
+      </c>
+      <c r="J20" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21">
+        <v>82</v>
+      </c>
+      <c r="B21" t="s">
+        <v>380</v>
+      </c>
+      <c r="E21" t="s">
+        <v>51</v>
+      </c>
+      <c r="F21" t="s">
+        <v>274</v>
+      </c>
+      <c r="G21" t="s">
+        <v>304</v>
+      </c>
+      <c r="J21" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22">
+        <v>83</v>
+      </c>
+      <c r="B22" t="s">
+        <v>288</v>
+      </c>
+      <c r="E22" t="s">
+        <v>51</v>
+      </c>
+      <c r="F22" t="s">
+        <v>274</v>
+      </c>
+      <c r="G22" t="s">
+        <v>304</v>
+      </c>
+      <c r="J22" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23">
+        <v>84</v>
+      </c>
+      <c r="B23" t="s">
+        <v>288</v>
+      </c>
+      <c r="E23" t="s">
+        <v>66</v>
+      </c>
+      <c r="F23" t="s">
+        <v>67</v>
+      </c>
+      <c r="G23" t="s">
+        <v>277</v>
+      </c>
+      <c r="J23" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24">
+        <v>85</v>
+      </c>
+      <c r="B24" t="s">
+        <v>288</v>
+      </c>
+      <c r="E24" t="s">
+        <v>51</v>
+      </c>
+      <c r="F24" t="s">
+        <v>67</v>
+      </c>
+      <c r="G24" t="s">
+        <v>277</v>
+      </c>
+      <c r="J24" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25">
+        <v>86</v>
+      </c>
+      <c r="B25" t="s">
+        <v>288</v>
+      </c>
+      <c r="E25" t="s">
+        <v>66</v>
+      </c>
+      <c r="F25" t="s">
+        <v>67</v>
+      </c>
+      <c r="G25" t="s">
+        <v>277</v>
+      </c>
+      <c r="J25" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26">
+        <v>87</v>
+      </c>
+      <c r="B26" t="s">
+        <v>288</v>
+      </c>
+      <c r="E26" t="s">
+        <v>66</v>
+      </c>
+      <c r="F26" t="s">
+        <v>67</v>
+      </c>
+      <c r="G26" t="s">
+        <v>277</v>
+      </c>
+      <c r="J26" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27">
+        <v>88</v>
+      </c>
+      <c r="B27" t="s">
+        <v>288</v>
+      </c>
+      <c r="E27" t="s">
+        <v>66</v>
+      </c>
+      <c r="F27" t="s">
+        <v>67</v>
+      </c>
+      <c r="G27" t="s">
+        <v>277</v>
+      </c>
+      <c r="J27" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28">
+        <v>89</v>
+      </c>
+      <c r="B28" t="s">
+        <v>288</v>
+      </c>
+      <c r="E28" t="s">
+        <v>66</v>
+      </c>
+      <c r="F28" t="s">
+        <v>67</v>
+      </c>
+      <c r="G28" t="s">
+        <v>277</v>
+      </c>
+      <c r="J28" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29">
+        <v>90</v>
+      </c>
+      <c r="B29" t="s">
+        <v>288</v>
+      </c>
+      <c r="E29" t="s">
+        <v>66</v>
+      </c>
+      <c r="F29" t="s">
+        <v>67</v>
+      </c>
+      <c r="G29" t="s">
+        <v>277</v>
+      </c>
+      <c r="J29" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="A30">
+        <v>91</v>
+      </c>
+      <c r="B30" t="s">
+        <v>288</v>
+      </c>
+      <c r="E30" t="s">
+        <v>66</v>
+      </c>
+      <c r="F30" t="s">
+        <v>67</v>
+      </c>
+      <c r="G30" t="s">
+        <v>277</v>
+      </c>
+      <c r="J30" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="A31">
+        <v>92</v>
+      </c>
+      <c r="B31" t="s">
+        <v>288</v>
+      </c>
+      <c r="E31" t="s">
+        <v>66</v>
+      </c>
+      <c r="F31" t="s">
+        <v>67</v>
+      </c>
+      <c r="G31" t="s">
+        <v>277</v>
+      </c>
+      <c r="J31" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="A32">
+        <v>93</v>
+      </c>
+      <c r="B32" t="s">
+        <v>288</v>
+      </c>
+      <c r="E32" t="s">
+        <v>66</v>
+      </c>
+      <c r="F32" t="s">
+        <v>67</v>
+      </c>
+      <c r="G32" t="s">
+        <v>277</v>
+      </c>
+      <c r="J32" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
+      <c r="A33">
+        <v>94</v>
+      </c>
+      <c r="B33" t="s">
+        <v>288</v>
+      </c>
+      <c r="E33" t="s">
+        <v>66</v>
+      </c>
+      <c r="F33" t="s">
+        <v>67</v>
+      </c>
+      <c r="G33" t="s">
+        <v>277</v>
+      </c>
+      <c r="J33" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J33"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" customWidth="1"/>
+    <col min="10" max="10" width="12.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>269</v>
+      </c>
+      <c r="C1" t="s">
+        <v>291</v>
+      </c>
+      <c r="D1" t="s">
+        <v>292</v>
+      </c>
+      <c r="E1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G1" t="s">
+        <v>300</v>
+      </c>
+      <c r="H1" t="s">
+        <v>352</v>
+      </c>
+      <c r="I1" t="s">
+        <v>353</v>
+      </c>
+      <c r="J1" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2">
+        <v>63</v>
+      </c>
+      <c r="B2" t="s">
+        <v>288</v>
+      </c>
+      <c r="C2">
+        <v>32110</v>
+      </c>
+      <c r="D2">
+        <v>32244</v>
+      </c>
+      <c r="E2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F2" t="s">
+        <v>274</v>
+      </c>
+      <c r="G2" t="s">
+        <v>304</v>
+      </c>
+      <c r="J2" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3">
+        <v>64</v>
+      </c>
+      <c r="B3" t="s">
+        <v>288</v>
+      </c>
+      <c r="C3">
+        <v>32110</v>
+      </c>
+      <c r="D3">
+        <v>32244</v>
+      </c>
+      <c r="E3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F3" t="s">
+        <v>274</v>
+      </c>
+      <c r="G3" t="s">
+        <v>304</v>
+      </c>
+      <c r="J3" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4">
+        <v>65</v>
+      </c>
+      <c r="B4" t="s">
+        <v>288</v>
+      </c>
+      <c r="C4">
+        <v>32110</v>
+      </c>
+      <c r="D4">
+        <v>32244</v>
+      </c>
+      <c r="E4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F4" t="s">
+        <v>274</v>
+      </c>
+      <c r="G4" t="s">
+        <v>304</v>
+      </c>
+      <c r="J4" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5">
+        <v>66</v>
+      </c>
+      <c r="B5" t="s">
+        <v>288</v>
+      </c>
+      <c r="C5">
+        <v>32110</v>
+      </c>
+      <c r="D5">
+        <v>32244</v>
+      </c>
+      <c r="E5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F5" t="s">
+        <v>274</v>
+      </c>
+      <c r="G5" t="s">
+        <v>304</v>
+      </c>
+      <c r="J5" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6">
+        <v>67</v>
+      </c>
+      <c r="B6" t="s">
+        <v>288</v>
+      </c>
+      <c r="C6">
+        <v>32110</v>
+      </c>
+      <c r="D6">
+        <v>32244</v>
+      </c>
+      <c r="E6" t="s">
+        <v>51</v>
+      </c>
+      <c r="F6" t="s">
+        <v>274</v>
+      </c>
+      <c r="G6" t="s">
+        <v>304</v>
+      </c>
+      <c r="J6" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7">
+        <v>68</v>
+      </c>
+      <c r="B7" t="s">
+        <v>288</v>
+      </c>
+      <c r="C7">
+        <v>32110</v>
+      </c>
+      <c r="D7">
+        <v>32244</v>
+      </c>
+      <c r="E7" t="s">
+        <v>51</v>
+      </c>
+      <c r="F7" t="s">
+        <v>274</v>
+      </c>
+      <c r="G7" t="s">
+        <v>304</v>
+      </c>
+      <c r="J7" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8">
+        <v>69</v>
+      </c>
+      <c r="B8" t="s">
+        <v>288</v>
+      </c>
+      <c r="C8">
+        <v>32110</v>
+      </c>
+      <c r="D8">
+        <v>32244</v>
+      </c>
+      <c r="E8" t="s">
+        <v>51</v>
+      </c>
+      <c r="F8" t="s">
+        <v>274</v>
+      </c>
+      <c r="G8" t="s">
+        <v>304</v>
+      </c>
+      <c r="H8" t="s">
+        <v>275</v>
+      </c>
+      <c r="I8" t="s">
+        <v>285</v>
+      </c>
+      <c r="J8" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9">
+        <v>70</v>
+      </c>
+      <c r="B9" t="s">
+        <v>288</v>
+      </c>
+      <c r="C9">
+        <v>32110</v>
+      </c>
+      <c r="D9">
+        <v>32244</v>
+      </c>
+      <c r="E9" t="s">
+        <v>51</v>
+      </c>
+      <c r="F9" t="s">
+        <v>274</v>
+      </c>
+      <c r="G9" t="s">
+        <v>304</v>
+      </c>
+      <c r="H9" t="s">
+        <v>275</v>
+      </c>
+      <c r="J9" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10">
+        <v>71</v>
+      </c>
+      <c r="B10" t="s">
+        <v>288</v>
+      </c>
+      <c r="C10">
+        <v>32110</v>
+      </c>
+      <c r="D10">
+        <v>32244</v>
+      </c>
+      <c r="E10" t="s">
+        <v>51</v>
+      </c>
+      <c r="F10" t="s">
+        <v>274</v>
+      </c>
+      <c r="G10" t="s">
+        <v>304</v>
+      </c>
+      <c r="H10" t="s">
+        <v>275</v>
+      </c>
+      <c r="J10" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11">
+        <v>72</v>
+      </c>
+      <c r="B11" t="s">
+        <v>288</v>
+      </c>
+      <c r="C11">
+        <v>32110</v>
+      </c>
+      <c r="D11">
+        <v>32244</v>
+      </c>
+      <c r="E11" t="s">
+        <v>51</v>
+      </c>
+      <c r="F11" t="s">
+        <v>274</v>
+      </c>
+      <c r="G11" t="s">
+        <v>304</v>
+      </c>
+      <c r="H11" t="s">
+        <v>275</v>
+      </c>
+      <c r="J11" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12">
+        <v>73</v>
+      </c>
+      <c r="B12" t="s">
+        <v>288</v>
+      </c>
+      <c r="C12">
+        <v>32110</v>
+      </c>
+      <c r="D12">
+        <v>32244</v>
+      </c>
+      <c r="E12" t="s">
+        <v>51</v>
+      </c>
+      <c r="F12" t="s">
+        <v>274</v>
+      </c>
+      <c r="G12" t="s">
+        <v>304</v>
+      </c>
+      <c r="H12" t="s">
+        <v>275</v>
+      </c>
+      <c r="J12" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13">
+        <v>74</v>
+      </c>
+      <c r="B13" t="s">
+        <v>288</v>
+      </c>
+      <c r="C13">
+        <v>32110</v>
+      </c>
+      <c r="D13">
+        <v>32244</v>
+      </c>
+      <c r="E13" t="s">
+        <v>51</v>
+      </c>
+      <c r="F13" t="s">
+        <v>274</v>
+      </c>
+      <c r="G13" t="s">
+        <v>304</v>
+      </c>
+      <c r="J13" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14">
+        <v>75</v>
+      </c>
+      <c r="B14" t="s">
+        <v>288</v>
+      </c>
+      <c r="C14">
+        <v>32110</v>
+      </c>
+      <c r="D14">
+        <v>32244</v>
+      </c>
+      <c r="E14" t="s">
+        <v>51</v>
+      </c>
+      <c r="F14" t="s">
+        <v>274</v>
+      </c>
+      <c r="G14" t="s">
+        <v>304</v>
+      </c>
+      <c r="J14" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15">
+        <v>76</v>
+      </c>
+      <c r="B15" t="s">
+        <v>288</v>
+      </c>
+      <c r="C15">
+        <v>32110</v>
+      </c>
+      <c r="D15">
+        <v>32244</v>
+      </c>
+      <c r="E15" t="s">
+        <v>51</v>
+      </c>
+      <c r="F15" t="s">
+        <v>274</v>
+      </c>
+      <c r="G15" t="s">
+        <v>304</v>
+      </c>
+      <c r="J15" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16">
+        <v>77</v>
+      </c>
+      <c r="B16" t="s">
+        <v>288</v>
+      </c>
+      <c r="C16">
+        <v>32110</v>
+      </c>
+      <c r="D16">
+        <v>32244</v>
+      </c>
+      <c r="E16" t="s">
+        <v>51</v>
+      </c>
+      <c r="F16" t="s">
+        <v>274</v>
+      </c>
+      <c r="G16" t="s">
+        <v>304</v>
+      </c>
+      <c r="J16" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17">
+        <v>78</v>
+      </c>
+      <c r="B17" t="s">
+        <v>288</v>
+      </c>
+      <c r="C17">
+        <v>32110</v>
+      </c>
+      <c r="D17">
+        <v>32244</v>
+      </c>
+      <c r="E17" t="s">
+        <v>51</v>
+      </c>
+      <c r="F17" t="s">
+        <v>274</v>
+      </c>
+      <c r="G17" t="s">
+        <v>304</v>
+      </c>
+      <c r="J17" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18">
+        <v>79</v>
+      </c>
+      <c r="B18" t="s">
+        <v>288</v>
+      </c>
+      <c r="C18">
+        <v>32110</v>
+      </c>
+      <c r="D18">
+        <v>32244</v>
+      </c>
+      <c r="E18" t="s">
+        <v>51</v>
+      </c>
+      <c r="F18" t="s">
+        <v>274</v>
+      </c>
+      <c r="G18" t="s">
+        <v>304</v>
+      </c>
+      <c r="J18" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19">
+        <v>80</v>
+      </c>
+      <c r="B19" t="s">
+        <v>288</v>
+      </c>
+      <c r="C19">
+        <v>32110</v>
+      </c>
+      <c r="D19">
+        <v>32244</v>
+      </c>
+      <c r="E19" t="s">
+        <v>51</v>
+      </c>
+      <c r="F19" t="s">
+        <v>274</v>
+      </c>
+      <c r="G19" t="s">
+        <v>304</v>
+      </c>
+      <c r="J19" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20">
+        <v>81</v>
+      </c>
+      <c r="B20" t="s">
+        <v>288</v>
+      </c>
+      <c r="C20">
+        <v>32110</v>
+      </c>
+      <c r="D20">
+        <v>32244</v>
+      </c>
+      <c r="E20" t="s">
+        <v>51</v>
+      </c>
+      <c r="F20" t="s">
+        <v>274</v>
+      </c>
+      <c r="G20" t="s">
+        <v>304</v>
+      </c>
+      <c r="J20" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21">
+        <v>82</v>
+      </c>
+      <c r="B21" t="s">
+        <v>288</v>
+      </c>
+      <c r="C21">
+        <v>32110</v>
+      </c>
+      <c r="D21">
+        <v>32244</v>
+      </c>
+      <c r="E21" t="s">
+        <v>51</v>
+      </c>
+      <c r="F21" t="s">
+        <v>274</v>
+      </c>
+      <c r="G21" t="s">
+        <v>304</v>
+      </c>
+      <c r="J21" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22">
+        <v>83</v>
+      </c>
+      <c r="B22" t="s">
+        <v>287</v>
+      </c>
+      <c r="C22">
+        <v>44111</v>
+      </c>
+      <c r="D22">
+        <v>45414</v>
+      </c>
+      <c r="E22" t="s">
+        <v>51</v>
+      </c>
+      <c r="F22" t="s">
+        <v>274</v>
+      </c>
+      <c r="G22" t="s">
+        <v>304</v>
+      </c>
+      <c r="J22" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23">
+        <v>84</v>
+      </c>
+      <c r="B23" t="s">
+        <v>287</v>
+      </c>
+      <c r="C23">
+        <v>44111</v>
+      </c>
+      <c r="D23">
+        <v>45414</v>
+      </c>
+      <c r="E23" t="s">
+        <v>66</v>
+      </c>
+      <c r="F23" t="s">
+        <v>67</v>
+      </c>
+      <c r="G23" t="s">
+        <v>277</v>
+      </c>
+      <c r="H23" t="s">
+        <v>68</v>
+      </c>
+      <c r="J23" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24">
+        <v>85</v>
+      </c>
+      <c r="B24" t="s">
+        <v>287</v>
+      </c>
+      <c r="C24">
+        <v>44111</v>
+      </c>
+      <c r="D24">
+        <v>45414</v>
+      </c>
+      <c r="E24" t="s">
+        <v>51</v>
+      </c>
+      <c r="F24" t="s">
+        <v>67</v>
+      </c>
+      <c r="G24" t="s">
+        <v>277</v>
+      </c>
+      <c r="H24" t="s">
+        <v>68</v>
+      </c>
+      <c r="J24" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25">
+        <v>86</v>
+      </c>
+      <c r="B25" t="s">
+        <v>287</v>
+      </c>
+      <c r="C25">
+        <v>44111</v>
+      </c>
+      <c r="D25">
+        <v>45414</v>
+      </c>
+      <c r="E25" t="s">
+        <v>66</v>
+      </c>
+      <c r="F25" t="s">
+        <v>67</v>
+      </c>
+      <c r="G25" t="s">
+        <v>277</v>
+      </c>
+      <c r="H25" t="s">
+        <v>68</v>
+      </c>
+      <c r="J25" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26">
+        <v>87</v>
+      </c>
+      <c r="B26" t="s">
+        <v>287</v>
+      </c>
+      <c r="C26">
+        <v>44111</v>
+      </c>
+      <c r="D26">
+        <v>45414</v>
+      </c>
+      <c r="E26" t="s">
+        <v>66</v>
+      </c>
+      <c r="F26" t="s">
+        <v>67</v>
+      </c>
+      <c r="G26" t="s">
+        <v>277</v>
+      </c>
+      <c r="H26" t="s">
+        <v>68</v>
+      </c>
+      <c r="J26" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27">
+        <v>88</v>
+      </c>
+      <c r="B27" t="s">
+        <v>287</v>
+      </c>
+      <c r="C27">
+        <v>44111</v>
+      </c>
+      <c r="D27">
+        <v>45414</v>
+      </c>
+      <c r="E27" t="s">
+        <v>66</v>
+      </c>
+      <c r="F27" t="s">
+        <v>67</v>
+      </c>
+      <c r="G27" t="s">
+        <v>277</v>
+      </c>
+      <c r="H27" t="s">
+        <v>68</v>
+      </c>
+      <c r="J27" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28">
+        <v>89</v>
+      </c>
+      <c r="B28" t="s">
+        <v>287</v>
+      </c>
+      <c r="C28">
+        <v>44111</v>
+      </c>
+      <c r="D28">
+        <v>45414</v>
+      </c>
+      <c r="E28" t="s">
+        <v>284</v>
+      </c>
+      <c r="F28" t="s">
+        <v>278</v>
+      </c>
+      <c r="G28" t="s">
+        <v>280</v>
+      </c>
+      <c r="H28" t="s">
+        <v>282</v>
+      </c>
+      <c r="J28" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29">
+        <v>90</v>
+      </c>
+      <c r="B29" t="s">
+        <v>287</v>
+      </c>
+      <c r="C29">
+        <v>44111</v>
+      </c>
+      <c r="D29">
+        <v>45414</v>
+      </c>
+      <c r="E29" t="s">
+        <v>66</v>
+      </c>
+      <c r="F29" t="s">
+        <v>67</v>
+      </c>
+      <c r="G29" t="s">
+        <v>277</v>
+      </c>
+      <c r="H29" t="s">
+        <v>68</v>
+      </c>
+      <c r="J29" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="A30">
+        <v>91</v>
+      </c>
+      <c r="B30" t="s">
+        <v>287</v>
+      </c>
+      <c r="C30">
+        <v>44111</v>
+      </c>
+      <c r="D30">
+        <v>45414</v>
+      </c>
+      <c r="E30" t="s">
+        <v>66</v>
+      </c>
+      <c r="F30" t="s">
+        <v>67</v>
+      </c>
+      <c r="G30" t="s">
+        <v>277</v>
+      </c>
+      <c r="H30" t="s">
+        <v>68</v>
+      </c>
+      <c r="J30" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="A31">
+        <v>92</v>
+      </c>
+      <c r="B31" t="s">
+        <v>287</v>
+      </c>
+      <c r="C31">
+        <v>44111</v>
+      </c>
+      <c r="D31">
+        <v>45414</v>
+      </c>
+      <c r="E31" t="s">
+        <v>66</v>
+      </c>
+      <c r="F31" t="s">
+        <v>67</v>
+      </c>
+      <c r="G31" t="s">
+        <v>277</v>
+      </c>
+      <c r="H31" t="s">
+        <v>68</v>
+      </c>
+      <c r="J31" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="A32">
+        <v>93</v>
+      </c>
+      <c r="B32" t="s">
+        <v>287</v>
+      </c>
+      <c r="C32">
+        <v>44111</v>
+      </c>
+      <c r="D32">
+        <v>45414</v>
+      </c>
+      <c r="E32" t="s">
+        <v>66</v>
+      </c>
+      <c r="F32" t="s">
+        <v>67</v>
+      </c>
+      <c r="G32" t="s">
+        <v>277</v>
+      </c>
+      <c r="H32" t="s">
+        <v>68</v>
+      </c>
+      <c r="J32" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
+      <c r="A33">
+        <v>94</v>
+      </c>
+      <c r="B33" t="s">
+        <v>287</v>
+      </c>
+      <c r="C33">
+        <v>44111</v>
+      </c>
+      <c r="D33">
+        <v>45414</v>
+      </c>
+      <c r="E33" t="s">
+        <v>66</v>
+      </c>
+      <c r="F33" t="s">
+        <v>67</v>
+      </c>
+      <c r="G33" t="s">
+        <v>277</v>
+      </c>
+      <c r="H33" t="s">
+        <v>68</v>
+      </c>
+      <c r="J33" t="s">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J33"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>269</v>
+      </c>
+      <c r="C1" t="s">
+        <v>291</v>
+      </c>
+      <c r="D1" t="s">
+        <v>292</v>
+      </c>
+      <c r="E1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G1" t="s">
+        <v>300</v>
+      </c>
+      <c r="H1" t="s">
+        <v>352</v>
+      </c>
+      <c r="I1" t="s">
+        <v>353</v>
+      </c>
+      <c r="J1" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2">
+        <v>63</v>
+      </c>
+      <c r="B2" t="s">
+        <v>287</v>
+      </c>
+      <c r="E2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F2" t="s">
+        <v>274</v>
+      </c>
+      <c r="G2" t="s">
+        <v>304</v>
+      </c>
+      <c r="J2" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3">
+        <v>64</v>
+      </c>
+      <c r="B3" t="s">
+        <v>287</v>
+      </c>
+      <c r="E3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F3" t="s">
+        <v>274</v>
+      </c>
+      <c r="G3" t="s">
+        <v>304</v>
+      </c>
+      <c r="J3" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4">
+        <v>65</v>
+      </c>
+      <c r="B4" t="s">
+        <v>287</v>
+      </c>
+      <c r="E4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F4" t="s">
+        <v>274</v>
+      </c>
+      <c r="G4" t="s">
+        <v>304</v>
+      </c>
+      <c r="J4" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5">
+        <v>66</v>
+      </c>
+      <c r="B5" t="s">
+        <v>287</v>
+      </c>
+      <c r="E5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F5" t="s">
+        <v>274</v>
+      </c>
+      <c r="G5" t="s">
+        <v>304</v>
+      </c>
+      <c r="J5" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6">
+        <v>67</v>
+      </c>
+      <c r="B6" t="s">
+        <v>287</v>
+      </c>
+      <c r="E6" t="s">
+        <v>51</v>
+      </c>
+      <c r="F6" t="s">
+        <v>274</v>
+      </c>
+      <c r="G6" t="s">
+        <v>304</v>
+      </c>
+      <c r="J6" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7">
+        <v>68</v>
+      </c>
+      <c r="B7" t="s">
+        <v>287</v>
+      </c>
+      <c r="E7" t="s">
+        <v>51</v>
+      </c>
+      <c r="F7" t="s">
+        <v>274</v>
+      </c>
+      <c r="G7" t="s">
+        <v>304</v>
+      </c>
+      <c r="J7" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8">
+        <v>69</v>
+      </c>
+      <c r="B8" t="s">
+        <v>287</v>
+      </c>
+      <c r="E8" t="s">
+        <v>51</v>
+      </c>
+      <c r="F8" t="s">
+        <v>274</v>
+      </c>
+      <c r="G8" t="s">
+        <v>304</v>
+      </c>
+      <c r="H8" t="s">
+        <v>275</v>
+      </c>
+      <c r="I8" t="s">
+        <v>285</v>
+      </c>
+      <c r="J8" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9">
+        <v>70</v>
+      </c>
+      <c r="B9" t="s">
+        <v>287</v>
+      </c>
+      <c r="E9" t="s">
+        <v>51</v>
+      </c>
+      <c r="F9" t="s">
+        <v>274</v>
+      </c>
+      <c r="G9" t="s">
+        <v>304</v>
+      </c>
+      <c r="H9" t="s">
+        <v>275</v>
+      </c>
+      <c r="J9" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10">
+        <v>71</v>
+      </c>
+      <c r="B10" t="s">
+        <v>287</v>
+      </c>
+      <c r="E10" t="s">
+        <v>51</v>
+      </c>
+      <c r="F10" t="s">
+        <v>274</v>
+      </c>
+      <c r="G10" t="s">
+        <v>304</v>
+      </c>
+      <c r="H10" t="s">
+        <v>275</v>
+      </c>
+      <c r="J10" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11">
+        <v>72</v>
+      </c>
+      <c r="B11" t="s">
+        <v>287</v>
+      </c>
+      <c r="E11" t="s">
+        <v>51</v>
+      </c>
+      <c r="F11" t="s">
+        <v>274</v>
+      </c>
+      <c r="G11" t="s">
+        <v>304</v>
+      </c>
+      <c r="H11" t="s">
+        <v>275</v>
+      </c>
+      <c r="J11" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12">
+        <v>73</v>
+      </c>
+      <c r="B12" t="s">
+        <v>287</v>
+      </c>
+      <c r="E12" t="s">
+        <v>51</v>
+      </c>
+      <c r="F12" t="s">
+        <v>274</v>
+      </c>
+      <c r="G12" t="s">
+        <v>304</v>
+      </c>
+      <c r="H12" t="s">
+        <v>275</v>
+      </c>
+      <c r="J12" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13">
+        <v>74</v>
+      </c>
+      <c r="B13" t="s">
+        <v>287</v>
+      </c>
+      <c r="E13" t="s">
+        <v>51</v>
+      </c>
+      <c r="F13" t="s">
+        <v>274</v>
+      </c>
+      <c r="G13" t="s">
+        <v>304</v>
+      </c>
+      <c r="J13" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14">
+        <v>75</v>
+      </c>
+      <c r="B14" t="s">
+        <v>287</v>
+      </c>
+      <c r="E14" t="s">
+        <v>51</v>
+      </c>
+      <c r="F14" t="s">
+        <v>274</v>
+      </c>
+      <c r="G14" t="s">
+        <v>304</v>
+      </c>
+      <c r="J14" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15">
+        <v>76</v>
+      </c>
+      <c r="B15" t="s">
+        <v>287</v>
+      </c>
+      <c r="E15" t="s">
+        <v>51</v>
+      </c>
+      <c r="F15" t="s">
+        <v>274</v>
+      </c>
+      <c r="G15" t="s">
+        <v>304</v>
+      </c>
+      <c r="J15" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16">
+        <v>77</v>
+      </c>
+      <c r="B16" t="s">
+        <v>287</v>
+      </c>
+      <c r="E16" t="s">
+        <v>51</v>
+      </c>
+      <c r="F16" t="s">
+        <v>274</v>
+      </c>
+      <c r="G16" t="s">
+        <v>304</v>
+      </c>
+      <c r="J16" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17">
+        <v>78</v>
+      </c>
+      <c r="B17" t="s">
+        <v>287</v>
+      </c>
+      <c r="E17" t="s">
+        <v>51</v>
+      </c>
+      <c r="F17" t="s">
+        <v>274</v>
+      </c>
+      <c r="G17" t="s">
+        <v>304</v>
+      </c>
+      <c r="J17" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18">
+        <v>79</v>
+      </c>
+      <c r="B18" t="s">
+        <v>287</v>
+      </c>
+      <c r="E18" t="s">
+        <v>51</v>
+      </c>
+      <c r="F18" t="s">
+        <v>274</v>
+      </c>
+      <c r="G18" t="s">
+        <v>304</v>
+      </c>
+      <c r="J18" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19">
+        <v>80</v>
+      </c>
+      <c r="B19" t="s">
+        <v>287</v>
+      </c>
+      <c r="E19" t="s">
+        <v>51</v>
+      </c>
+      <c r="F19" t="s">
+        <v>274</v>
+      </c>
+      <c r="G19" t="s">
+        <v>304</v>
+      </c>
+      <c r="J19" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20">
+        <v>81</v>
+      </c>
+      <c r="B20" t="s">
+        <v>287</v>
+      </c>
+      <c r="E20" t="s">
+        <v>51</v>
+      </c>
+      <c r="F20" t="s">
+        <v>274</v>
+      </c>
+      <c r="G20" t="s">
+        <v>304</v>
+      </c>
+      <c r="J20" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21">
+        <v>82</v>
+      </c>
+      <c r="B21" t="s">
+        <v>287</v>
+      </c>
+      <c r="E21" t="s">
+        <v>51</v>
+      </c>
+      <c r="F21" t="s">
+        <v>274</v>
+      </c>
+      <c r="G21" t="s">
+        <v>304</v>
+      </c>
+      <c r="J21" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22">
+        <v>83</v>
+      </c>
+      <c r="B22" t="s">
+        <v>347</v>
+      </c>
+      <c r="E22" t="s">
+        <v>51</v>
+      </c>
+      <c r="F22" t="s">
+        <v>274</v>
+      </c>
+      <c r="G22" t="s">
+        <v>304</v>
+      </c>
+      <c r="J22" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23">
+        <v>84</v>
+      </c>
+      <c r="B23" t="s">
+        <v>347</v>
+      </c>
+      <c r="E23" t="s">
+        <v>66</v>
+      </c>
+      <c r="F23" t="s">
+        <v>67</v>
+      </c>
+      <c r="G23" t="s">
+        <v>277</v>
+      </c>
+      <c r="J23" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24">
+        <v>85</v>
+      </c>
+      <c r="B24" t="s">
+        <v>347</v>
+      </c>
+      <c r="E24" t="s">
+        <v>51</v>
+      </c>
+      <c r="F24" t="s">
+        <v>67</v>
+      </c>
+      <c r="G24" t="s">
+        <v>277</v>
+      </c>
+      <c r="J24" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25">
+        <v>86</v>
+      </c>
+      <c r="B25" t="s">
+        <v>347</v>
+      </c>
+      <c r="E25" t="s">
+        <v>66</v>
+      </c>
+      <c r="F25" t="s">
+        <v>67</v>
+      </c>
+      <c r="G25" t="s">
+        <v>277</v>
+      </c>
+      <c r="J25" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26">
+        <v>87</v>
+      </c>
+      <c r="B26" t="s">
+        <v>347</v>
+      </c>
+      <c r="E26" t="s">
+        <v>66</v>
+      </c>
+      <c r="F26" t="s">
+        <v>67</v>
+      </c>
+      <c r="G26" t="s">
+        <v>277</v>
+      </c>
+      <c r="J26" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27">
+        <v>88</v>
+      </c>
+      <c r="B27" t="s">
+        <v>347</v>
+      </c>
+      <c r="E27" t="s">
+        <v>66</v>
+      </c>
+      <c r="F27" t="s">
+        <v>67</v>
+      </c>
+      <c r="G27" t="s">
+        <v>277</v>
+      </c>
+      <c r="J27" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28">
+        <v>89</v>
+      </c>
+      <c r="B28" t="s">
+        <v>347</v>
+      </c>
+      <c r="E28" t="s">
+        <v>66</v>
+      </c>
+      <c r="F28" t="s">
+        <v>67</v>
+      </c>
+      <c r="G28" t="s">
+        <v>277</v>
+      </c>
+      <c r="J28" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29">
+        <v>90</v>
+      </c>
+      <c r="B29" t="s">
+        <v>347</v>
+      </c>
+      <c r="E29" t="s">
+        <v>66</v>
+      </c>
+      <c r="F29" t="s">
+        <v>67</v>
+      </c>
+      <c r="G29" t="s">
+        <v>277</v>
+      </c>
+      <c r="J29" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="A30">
+        <v>91</v>
+      </c>
+      <c r="B30" t="s">
+        <v>347</v>
+      </c>
+      <c r="E30" t="s">
+        <v>66</v>
+      </c>
+      <c r="F30" t="s">
+        <v>67</v>
+      </c>
+      <c r="G30" t="s">
+        <v>277</v>
+      </c>
+      <c r="J30" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="A31">
+        <v>92</v>
+      </c>
+      <c r="B31" t="s">
+        <v>347</v>
+      </c>
+      <c r="E31" t="s">
+        <v>66</v>
+      </c>
+      <c r="F31" t="s">
+        <v>67</v>
+      </c>
+      <c r="G31" t="s">
+        <v>277</v>
+      </c>
+      <c r="J31" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="A32">
+        <v>93</v>
+      </c>
+      <c r="B32" t="s">
+        <v>347</v>
+      </c>
+      <c r="E32" t="s">
+        <v>66</v>
+      </c>
+      <c r="F32" t="s">
+        <v>67</v>
+      </c>
+      <c r="G32" t="s">
+        <v>277</v>
+      </c>
+      <c r="J32" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
+      <c r="A33">
+        <v>94</v>
+      </c>
+      <c r="B33" t="s">
+        <v>347</v>
+      </c>
+      <c r="E33" t="s">
+        <v>66</v>
+      </c>
+      <c r="F33" t="s">
+        <v>67</v>
+      </c>
+      <c r="G33" t="s">
+        <v>277</v>
+      </c>
+      <c r="J33" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -14747,7 +18714,7 @@
   <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F8" sqref="A1:H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Updated Some Income Codes
</commit_message>
<xml_diff>
--- a/Data/MetaData.xlsx
+++ b/Data/MetaData.xlsx
@@ -9,8 +9,8 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17100" windowHeight="6600" firstSheet="8" activeTab="8"/>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17100" windowHeight="6600" firstSheet="8" activeTab="9"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="17100" windowHeight="6600" firstSheet="8" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17100" windowHeight="6600" tabRatio="544" firstSheet="8" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="CompressedFileNames" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
     <sheet name="PubWageTable" sheetId="12" r:id="rId8"/>
     <sheet name="PrvWageTable" sheetId="15" r:id="rId9"/>
     <sheet name="BussIncTable" sheetId="17" r:id="rId10"/>
-    <sheet name="AggrIncTable" sheetId="16" r:id="rId11"/>
+    <sheet name="AgriIncTable" sheetId="16" r:id="rId11"/>
     <sheet name="OthrIncTable" sheetId="18" r:id="rId12"/>
     <sheet name="SubsidyTable" sheetId="19" r:id="rId13"/>
     <sheet name="FoodTables" sheetId="10" r:id="rId14"/>
@@ -71,13 +71,12 @@
     <sheet name="Biscuit" sheetId="1026" r:id="rId56"/>
     <sheet name="Khoshkbar" sheetId="1027" r:id="rId57"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13186" uniqueCount="466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13188" uniqueCount="467">
   <si>
     <t>Year</t>
   </si>
@@ -1384,9 +1383,6 @@
     <t>WorkType</t>
   </si>
   <si>
-    <t>NonWageSector</t>
-  </si>
-  <si>
     <t>PubWageGrossIncomeM</t>
   </si>
   <si>
@@ -1435,9 +1431,6 @@
     <t>PrvWageNetIncomeY</t>
   </si>
   <si>
-    <t>AggrNetIncomeY</t>
-  </si>
-  <si>
     <t>Retirment</t>
   </si>
   <si>
@@ -1476,11 +1469,20 @@
   <si>
     <t>B</t>
   </si>
+  <si>
+    <t>BussNetIncomeY</t>
+  </si>
+  <si>
+    <t>JobType</t>
+  </si>
+  <si>
+    <t>AgriNetIncomeY</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2014,48 +2016,48 @@
     </xf>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="‏20% - تأکید1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="‏20% - تاکید2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="‏20% - تاکید3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="‏20% - تاکید4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="‏20% - تاکید5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="‏20% - تاکید6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - آکسان 1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="‏40% - تاکید2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="‏40% - تاکید3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="‏40% - تاکید4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="‏40% - تاکید5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="‏40% - تاکید6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="‏60% - تأکید1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="‏60% - تاکید2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="‏60% - تاکید3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="‏60% - تاکید4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="‏60% - تاکید5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="‏60% - تاکید6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="بد" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="بررسی سلول" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="تأکید1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="تاکید2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="تاکید3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="تاکید4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="تاکید5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="تاکید6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="خروجی" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="خنثی" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="خوب" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="سلول پیوندی" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="عنوان" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="عنوان 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="عنوان 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="عنوان 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="عنوان 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="متن توصیفی" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="متن هشدار" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="مجموع" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="محاسبه" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="معمولی" xfId="0" builtinId="0"/>
-    <cellStyle name="ورودی" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="یادداشت" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2622,19 +2624,22 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R34"/>
+  <dimension ref="A1:S34"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="1">
-      <selection activeCell="R1" sqref="R1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
+    </sheetView>
+    <sheetView workbookViewId="1">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="18" max="18" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="10.5703125" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2657,40 +2662,43 @@
         <v>433</v>
       </c>
       <c r="H1" t="s">
+        <v>432</v>
+      </c>
+      <c r="I1" t="s">
         <v>434</v>
       </c>
-      <c r="I1" t="s">
-        <v>435</v>
-      </c>
       <c r="J1" t="s">
+        <v>465</v>
+      </c>
+      <c r="K1" t="s">
         <v>428</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>429</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>343</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>344</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>345</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>346</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>347</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>348</v>
       </c>
-      <c r="R1" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S1" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>63</v>
       </c>
@@ -2706,32 +2714,32 @@
       <c r="F2" t="s">
         <v>330</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>53</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>54</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>55</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>58</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>56</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>57</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>59</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>64</v>
       </c>
@@ -2747,32 +2755,32 @@
       <c r="F3" t="s">
         <v>330</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>53</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>54</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>55</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>58</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>56</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>57</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="R3" t="s">
         <v>59</v>
       </c>
-      <c r="R3" t="s">
+      <c r="S3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>65</v>
       </c>
@@ -2788,32 +2796,32 @@
       <c r="F4" t="s">
         <v>330</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>53</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>54</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>55</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>58</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>56</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
         <v>57</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="R4" t="s">
         <v>59</v>
       </c>
-      <c r="R4" t="s">
+      <c r="S4" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>66</v>
       </c>
@@ -2829,32 +2837,32 @@
       <c r="F5" t="s">
         <v>330</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>53</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>54</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>55</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>58</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
         <v>56</v>
       </c>
-      <c r="P5" t="s">
+      <c r="Q5" t="s">
         <v>57</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="R5" t="s">
         <v>59</v>
       </c>
-      <c r="R5" t="s">
+      <c r="S5" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>67</v>
       </c>
@@ -2870,32 +2878,32 @@
       <c r="F6" t="s">
         <v>330</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>53</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>54</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>55</v>
       </c>
-      <c r="N6" t="s">
+      <c r="O6" t="s">
         <v>58</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>56</v>
       </c>
-      <c r="P6" t="s">
+      <c r="Q6" t="s">
         <v>57</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="R6" t="s">
         <v>59</v>
       </c>
-      <c r="R6" t="s">
+      <c r="S6" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>68</v>
       </c>
@@ -2911,32 +2919,32 @@
       <c r="F7" t="s">
         <v>330</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>53</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
         <v>54</v>
       </c>
-      <c r="M7" t="s">
+      <c r="N7" t="s">
         <v>55</v>
       </c>
-      <c r="N7" t="s">
+      <c r="O7" t="s">
         <v>58</v>
       </c>
-      <c r="O7" t="s">
+      <c r="P7" t="s">
         <v>56</v>
       </c>
-      <c r="P7" t="s">
+      <c r="Q7" t="s">
         <v>57</v>
       </c>
-      <c r="Q7" t="s">
+      <c r="R7" t="s">
         <v>59</v>
       </c>
-      <c r="R7" t="s">
+      <c r="S7" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>69</v>
       </c>
@@ -2955,35 +2963,35 @@
       <c r="G8" t="s">
         <v>53</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>54</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>55</v>
       </c>
-      <c r="L8" t="s">
+      <c r="M8" t="s">
         <v>58</v>
       </c>
-      <c r="M8" t="s">
+      <c r="N8" t="s">
         <v>56</v>
       </c>
-      <c r="N8" t="s">
+      <c r="O8" t="s">
         <v>57</v>
       </c>
-      <c r="O8" t="s">
+      <c r="P8" t="s">
         <v>59</v>
       </c>
-      <c r="P8" t="s">
+      <c r="Q8" t="s">
         <v>60</v>
       </c>
-      <c r="Q8" t="s">
+      <c r="R8" t="s">
         <v>61</v>
       </c>
-      <c r="R8" t="s">
+      <c r="S8" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>70</v>
       </c>
@@ -3002,35 +3010,35 @@
       <c r="G9" t="s">
         <v>53</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>54</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>55</v>
       </c>
-      <c r="L9" t="s">
+      <c r="M9" t="s">
         <v>58</v>
       </c>
-      <c r="M9" t="s">
+      <c r="N9" t="s">
         <v>56</v>
       </c>
-      <c r="N9" t="s">
+      <c r="O9" t="s">
         <v>57</v>
       </c>
-      <c r="O9" t="s">
+      <c r="P9" t="s">
         <v>59</v>
       </c>
-      <c r="P9" t="s">
+      <c r="Q9" t="s">
         <v>60</v>
       </c>
-      <c r="Q9" t="s">
+      <c r="R9" t="s">
         <v>61</v>
       </c>
-      <c r="R9" t="s">
+      <c r="S9" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>71</v>
       </c>
@@ -3049,35 +3057,35 @@
       <c r="G10" t="s">
         <v>53</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>54</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
         <v>55</v>
       </c>
-      <c r="L10" t="s">
+      <c r="M10" t="s">
         <v>58</v>
       </c>
-      <c r="M10" t="s">
+      <c r="N10" t="s">
         <v>56</v>
       </c>
-      <c r="N10" t="s">
+      <c r="O10" t="s">
         <v>57</v>
       </c>
-      <c r="O10" t="s">
+      <c r="P10" t="s">
         <v>59</v>
       </c>
-      <c r="P10" t="s">
+      <c r="Q10" t="s">
         <v>60</v>
       </c>
-      <c r="Q10" t="s">
+      <c r="R10" t="s">
         <v>61</v>
       </c>
-      <c r="R10" t="s">
+      <c r="S10" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>72</v>
       </c>
@@ -3096,35 +3104,35 @@
       <c r="G11" t="s">
         <v>53</v>
       </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
         <v>54</v>
       </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
         <v>55</v>
       </c>
-      <c r="L11" t="s">
+      <c r="M11" t="s">
         <v>58</v>
       </c>
-      <c r="M11" t="s">
+      <c r="N11" t="s">
         <v>56</v>
       </c>
-      <c r="N11" t="s">
+      <c r="O11" t="s">
         <v>57</v>
       </c>
-      <c r="O11" t="s">
+      <c r="P11" t="s">
         <v>59</v>
       </c>
-      <c r="P11" t="s">
+      <c r="Q11" t="s">
         <v>60</v>
       </c>
-      <c r="Q11" t="s">
+      <c r="R11" t="s">
         <v>61</v>
       </c>
-      <c r="R11" t="s">
+      <c r="S11" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>73</v>
       </c>
@@ -3143,35 +3151,35 @@
       <c r="G12" t="s">
         <v>53</v>
       </c>
-      <c r="H12" t="s">
+      <c r="I12" t="s">
         <v>54</v>
       </c>
-      <c r="I12" t="s">
+      <c r="J12" t="s">
         <v>55</v>
       </c>
-      <c r="L12" t="s">
+      <c r="M12" t="s">
         <v>58</v>
       </c>
-      <c r="M12" t="s">
+      <c r="N12" t="s">
         <v>56</v>
       </c>
-      <c r="N12" t="s">
+      <c r="O12" t="s">
         <v>57</v>
       </c>
-      <c r="O12" t="s">
+      <c r="P12" t="s">
         <v>59</v>
       </c>
-      <c r="P12" t="s">
+      <c r="Q12" t="s">
         <v>60</v>
       </c>
-      <c r="Q12" t="s">
+      <c r="R12" t="s">
         <v>61</v>
       </c>
-      <c r="R12" t="s">
+      <c r="S12" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>74</v>
       </c>
@@ -3193,35 +3201,35 @@
       <c r="G13" t="s">
         <v>54</v>
       </c>
-      <c r="H13" t="s">
+      <c r="I13" t="s">
         <v>55</v>
       </c>
-      <c r="I13" t="s">
+      <c r="J13" t="s">
         <v>58</v>
       </c>
-      <c r="L13" t="s">
+      <c r="M13" t="s">
         <v>56</v>
       </c>
-      <c r="M13" t="s">
+      <c r="N13" t="s">
         <v>57</v>
       </c>
-      <c r="N13" t="s">
+      <c r="O13" t="s">
         <v>59</v>
       </c>
-      <c r="O13" t="s">
+      <c r="P13" t="s">
         <v>60</v>
       </c>
-      <c r="P13" t="s">
+      <c r="Q13" t="s">
         <v>61</v>
       </c>
-      <c r="Q13" t="s">
+      <c r="R13" t="s">
         <v>62</v>
       </c>
-      <c r="R13" t="s">
+      <c r="S13" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>75</v>
       </c>
@@ -3243,35 +3251,35 @@
       <c r="G14" t="s">
         <v>54</v>
       </c>
-      <c r="H14" t="s">
+      <c r="I14" t="s">
         <v>55</v>
       </c>
-      <c r="I14" t="s">
+      <c r="J14" t="s">
         <v>58</v>
       </c>
-      <c r="L14" t="s">
+      <c r="M14" t="s">
         <v>56</v>
       </c>
-      <c r="M14" t="s">
+      <c r="N14" t="s">
         <v>57</v>
       </c>
-      <c r="N14" t="s">
+      <c r="O14" t="s">
         <v>59</v>
       </c>
-      <c r="O14" t="s">
+      <c r="P14" t="s">
         <v>60</v>
       </c>
-      <c r="P14" t="s">
+      <c r="Q14" t="s">
         <v>61</v>
       </c>
-      <c r="Q14" t="s">
+      <c r="R14" t="s">
         <v>62</v>
       </c>
-      <c r="R14" t="s">
+      <c r="S14" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>76</v>
       </c>
@@ -3293,35 +3301,35 @@
       <c r="G15" t="s">
         <v>54</v>
       </c>
-      <c r="H15" t="s">
+      <c r="I15" t="s">
         <v>55</v>
       </c>
-      <c r="I15" t="s">
+      <c r="J15" t="s">
         <v>58</v>
       </c>
-      <c r="L15" t="s">
+      <c r="M15" t="s">
         <v>56</v>
       </c>
-      <c r="M15" t="s">
+      <c r="N15" t="s">
         <v>57</v>
       </c>
-      <c r="N15" t="s">
+      <c r="O15" t="s">
         <v>59</v>
       </c>
-      <c r="O15" t="s">
+      <c r="P15" t="s">
         <v>60</v>
       </c>
-      <c r="P15" t="s">
+      <c r="Q15" t="s">
         <v>61</v>
       </c>
-      <c r="Q15" t="s">
+      <c r="R15" t="s">
         <v>62</v>
       </c>
-      <c r="R15" t="s">
+      <c r="S15" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>77</v>
       </c>
@@ -3343,35 +3351,35 @@
       <c r="G16" t="s">
         <v>54</v>
       </c>
-      <c r="H16" t="s">
+      <c r="I16" t="s">
         <v>55</v>
       </c>
-      <c r="I16" t="s">
+      <c r="J16" t="s">
         <v>58</v>
       </c>
-      <c r="L16" t="s">
+      <c r="M16" t="s">
         <v>56</v>
       </c>
-      <c r="M16" t="s">
+      <c r="N16" t="s">
         <v>57</v>
       </c>
-      <c r="N16" t="s">
+      <c r="O16" t="s">
         <v>59</v>
       </c>
-      <c r="O16" t="s">
+      <c r="P16" t="s">
         <v>60</v>
       </c>
-      <c r="P16" t="s">
+      <c r="Q16" t="s">
         <v>61</v>
       </c>
-      <c r="Q16" t="s">
+      <c r="R16" t="s">
         <v>62</v>
       </c>
-      <c r="R16" t="s">
+      <c r="S16" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>78</v>
       </c>
@@ -3393,35 +3401,35 @@
       <c r="G17" t="s">
         <v>54</v>
       </c>
-      <c r="H17" t="s">
+      <c r="I17" t="s">
         <v>55</v>
       </c>
-      <c r="I17" t="s">
+      <c r="J17" t="s">
         <v>58</v>
       </c>
-      <c r="L17" t="s">
+      <c r="M17" t="s">
         <v>56</v>
       </c>
-      <c r="M17" t="s">
+      <c r="N17" t="s">
         <v>57</v>
       </c>
-      <c r="N17" t="s">
+      <c r="O17" t="s">
         <v>59</v>
       </c>
-      <c r="O17" t="s">
+      <c r="P17" t="s">
         <v>60</v>
       </c>
-      <c r="P17" t="s">
+      <c r="Q17" t="s">
         <v>61</v>
       </c>
-      <c r="Q17" t="s">
+      <c r="R17" t="s">
         <v>62</v>
       </c>
-      <c r="R17" t="s">
+      <c r="S17" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>79</v>
       </c>
@@ -3443,35 +3451,35 @@
       <c r="G18" t="s">
         <v>54</v>
       </c>
-      <c r="H18" t="s">
+      <c r="I18" t="s">
         <v>55</v>
       </c>
-      <c r="I18" t="s">
+      <c r="J18" t="s">
         <v>58</v>
       </c>
-      <c r="L18" t="s">
+      <c r="M18" t="s">
         <v>56</v>
       </c>
-      <c r="M18" t="s">
+      <c r="N18" t="s">
         <v>57</v>
       </c>
-      <c r="N18" t="s">
+      <c r="O18" t="s">
         <v>59</v>
       </c>
-      <c r="O18" t="s">
+      <c r="P18" t="s">
         <v>60</v>
       </c>
-      <c r="P18" t="s">
+      <c r="Q18" t="s">
         <v>61</v>
       </c>
-      <c r="Q18" t="s">
+      <c r="R18" t="s">
         <v>62</v>
       </c>
-      <c r="R18" t="s">
+      <c r="S18" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>80</v>
       </c>
@@ -3493,35 +3501,35 @@
       <c r="G19" t="s">
         <v>54</v>
       </c>
-      <c r="H19" t="s">
+      <c r="I19" t="s">
         <v>55</v>
       </c>
-      <c r="I19" t="s">
+      <c r="J19" t="s">
         <v>58</v>
       </c>
-      <c r="L19" t="s">
+      <c r="M19" t="s">
         <v>56</v>
       </c>
-      <c r="M19" t="s">
+      <c r="N19" t="s">
         <v>57</v>
       </c>
-      <c r="N19" t="s">
+      <c r="O19" t="s">
         <v>59</v>
       </c>
-      <c r="O19" t="s">
+      <c r="P19" t="s">
         <v>60</v>
       </c>
-      <c r="P19" t="s">
+      <c r="Q19" t="s">
         <v>61</v>
       </c>
-      <c r="Q19" t="s">
+      <c r="R19" t="s">
         <v>62</v>
       </c>
-      <c r="R19" t="s">
+      <c r="S19" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>81</v>
       </c>
@@ -3543,35 +3551,35 @@
       <c r="G20" t="s">
         <v>54</v>
       </c>
-      <c r="H20" t="s">
+      <c r="I20" t="s">
         <v>55</v>
       </c>
-      <c r="I20" t="s">
+      <c r="J20" t="s">
         <v>58</v>
       </c>
-      <c r="L20" t="s">
+      <c r="M20" t="s">
         <v>56</v>
       </c>
-      <c r="M20" t="s">
+      <c r="N20" t="s">
         <v>57</v>
       </c>
-      <c r="N20" t="s">
+      <c r="O20" t="s">
         <v>59</v>
       </c>
-      <c r="O20" t="s">
+      <c r="P20" t="s">
         <v>60</v>
       </c>
-      <c r="P20" t="s">
+      <c r="Q20" t="s">
         <v>61</v>
       </c>
-      <c r="Q20" t="s">
+      <c r="R20" t="s">
         <v>62</v>
       </c>
-      <c r="R20" t="s">
+      <c r="S20" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>82</v>
       </c>
@@ -3593,35 +3601,35 @@
       <c r="G21" t="s">
         <v>54</v>
       </c>
-      <c r="H21" t="s">
+      <c r="I21" t="s">
         <v>55</v>
       </c>
-      <c r="I21" t="s">
+      <c r="J21" t="s">
         <v>58</v>
       </c>
-      <c r="L21" t="s">
+      <c r="M21" t="s">
         <v>56</v>
       </c>
-      <c r="M21" t="s">
+      <c r="N21" t="s">
         <v>57</v>
       </c>
-      <c r="N21" t="s">
+      <c r="O21" t="s">
         <v>59</v>
       </c>
-      <c r="O21" t="s">
+      <c r="P21" t="s">
         <v>60</v>
       </c>
-      <c r="P21" t="s">
+      <c r="Q21" t="s">
         <v>61</v>
       </c>
-      <c r="Q21" t="s">
+      <c r="R21" t="s">
         <v>62</v>
       </c>
-      <c r="R21" t="s">
+      <c r="S21" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>83</v>
       </c>
@@ -3643,35 +3651,35 @@
       <c r="G22" t="s">
         <v>54</v>
       </c>
-      <c r="H22" t="s">
+      <c r="I22" t="s">
         <v>55</v>
       </c>
-      <c r="I22" t="s">
+      <c r="J22" t="s">
         <v>58</v>
       </c>
-      <c r="L22" t="s">
+      <c r="M22" t="s">
         <v>56</v>
       </c>
-      <c r="M22" t="s">
+      <c r="N22" t="s">
         <v>57</v>
       </c>
-      <c r="N22" t="s">
+      <c r="O22" t="s">
         <v>59</v>
       </c>
-      <c r="O22" t="s">
+      <c r="P22" t="s">
         <v>60</v>
       </c>
-      <c r="P22" t="s">
+      <c r="Q22" t="s">
         <v>61</v>
       </c>
-      <c r="Q22" t="s">
+      <c r="R22" t="s">
         <v>62</v>
       </c>
-      <c r="R22" t="s">
+      <c r="S22" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>84</v>
       </c>
@@ -3693,41 +3701,41 @@
       <c r="G23" t="s">
         <v>69</v>
       </c>
-      <c r="H23" t="s">
+      <c r="I23" t="s">
         <v>70</v>
       </c>
-      <c r="I23" t="s">
+      <c r="J23" t="s">
         <v>72</v>
       </c>
-      <c r="J23" t="s">
+      <c r="K23" t="s">
         <v>73</v>
       </c>
-      <c r="K23" t="s">
+      <c r="L23" t="s">
         <v>74</v>
       </c>
-      <c r="L23" t="s">
+      <c r="M23" t="s">
         <v>75</v>
       </c>
-      <c r="M23" t="s">
+      <c r="N23" t="s">
         <v>71</v>
       </c>
-      <c r="N23" t="s">
+      <c r="O23" t="s">
         <v>325</v>
       </c>
-      <c r="O23" t="s">
+      <c r="P23" t="s">
         <v>326</v>
       </c>
-      <c r="P23" t="s">
+      <c r="Q23" t="s">
         <v>327</v>
       </c>
-      <c r="Q23" t="s">
+      <c r="R23" t="s">
         <v>328</v>
       </c>
-      <c r="R23" t="s">
+      <c r="S23" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>85</v>
       </c>
@@ -3749,41 +3757,41 @@
       <c r="G24" t="s">
         <v>69</v>
       </c>
-      <c r="H24" t="s">
+      <c r="I24" t="s">
         <v>70</v>
       </c>
-      <c r="I24" t="s">
+      <c r="J24" t="s">
         <v>72</v>
       </c>
-      <c r="J24" t="s">
+      <c r="K24" t="s">
         <v>73</v>
       </c>
-      <c r="K24" t="s">
+      <c r="L24" t="s">
         <v>74</v>
       </c>
-      <c r="L24" t="s">
+      <c r="M24" t="s">
         <v>75</v>
       </c>
-      <c r="M24" t="s">
+      <c r="N24" t="s">
         <v>71</v>
       </c>
-      <c r="N24" t="s">
+      <c r="O24" t="s">
         <v>325</v>
       </c>
-      <c r="O24" t="s">
+      <c r="P24" t="s">
         <v>326</v>
       </c>
-      <c r="P24" t="s">
+      <c r="Q24" t="s">
         <v>327</v>
       </c>
-      <c r="Q24" t="s">
+      <c r="R24" t="s">
         <v>328</v>
       </c>
-      <c r="R24" t="s">
+      <c r="S24" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>86</v>
       </c>
@@ -3805,41 +3813,41 @@
       <c r="G25" t="s">
         <v>69</v>
       </c>
-      <c r="H25" t="s">
+      <c r="I25" t="s">
         <v>70</v>
       </c>
-      <c r="I25" t="s">
+      <c r="J25" t="s">
         <v>72</v>
       </c>
-      <c r="J25" t="s">
+      <c r="K25" t="s">
         <v>73</v>
       </c>
-      <c r="K25" t="s">
+      <c r="L25" t="s">
         <v>74</v>
       </c>
-      <c r="L25" t="s">
+      <c r="M25" t="s">
         <v>75</v>
       </c>
-      <c r="M25" t="s">
+      <c r="N25" t="s">
         <v>71</v>
       </c>
-      <c r="N25" t="s">
+      <c r="O25" t="s">
         <v>325</v>
       </c>
-      <c r="O25" t="s">
+      <c r="P25" t="s">
         <v>326</v>
       </c>
-      <c r="P25" t="s">
+      <c r="Q25" t="s">
         <v>327</v>
       </c>
-      <c r="Q25" t="s">
+      <c r="R25" t="s">
         <v>328</v>
       </c>
-      <c r="R25" t="s">
+      <c r="S25" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>87</v>
       </c>
@@ -3861,41 +3869,41 @@
       <c r="G26" t="s">
         <v>69</v>
       </c>
-      <c r="H26" t="s">
+      <c r="I26" t="s">
         <v>70</v>
       </c>
-      <c r="I26" t="s">
+      <c r="J26" t="s">
         <v>72</v>
       </c>
-      <c r="J26" t="s">
+      <c r="K26" t="s">
         <v>73</v>
       </c>
-      <c r="K26" t="s">
+      <c r="L26" t="s">
         <v>74</v>
       </c>
-      <c r="L26" t="s">
+      <c r="M26" t="s">
         <v>75</v>
       </c>
-      <c r="M26" t="s">
+      <c r="N26" t="s">
         <v>71</v>
       </c>
-      <c r="N26" t="s">
+      <c r="O26" t="s">
         <v>325</v>
       </c>
-      <c r="O26" t="s">
+      <c r="P26" t="s">
         <v>326</v>
       </c>
-      <c r="P26" t="s">
+      <c r="Q26" t="s">
         <v>327</v>
       </c>
-      <c r="Q26" t="s">
+      <c r="R26" t="s">
         <v>328</v>
       </c>
-      <c r="R26" t="s">
+      <c r="S26" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>88</v>
       </c>
@@ -3917,41 +3925,41 @@
       <c r="G27" t="s">
         <v>69</v>
       </c>
-      <c r="H27" t="s">
+      <c r="I27" t="s">
         <v>70</v>
       </c>
-      <c r="I27" t="s">
+      <c r="J27" t="s">
         <v>72</v>
       </c>
-      <c r="J27" t="s">
+      <c r="K27" t="s">
         <v>73</v>
       </c>
-      <c r="K27" t="s">
+      <c r="L27" t="s">
         <v>74</v>
       </c>
-      <c r="L27" t="s">
+      <c r="M27" t="s">
         <v>75</v>
       </c>
-      <c r="M27" t="s">
+      <c r="N27" t="s">
         <v>71</v>
       </c>
-      <c r="N27" t="s">
+      <c r="O27" t="s">
         <v>325</v>
       </c>
-      <c r="O27" t="s">
+      <c r="P27" t="s">
         <v>326</v>
       </c>
-      <c r="P27" t="s">
+      <c r="Q27" t="s">
         <v>327</v>
       </c>
-      <c r="Q27" t="s">
+      <c r="R27" t="s">
         <v>328</v>
       </c>
-      <c r="R27" t="s">
+      <c r="S27" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>89</v>
       </c>
@@ -3973,41 +3981,41 @@
       <c r="G28" t="s">
         <v>69</v>
       </c>
-      <c r="H28" t="s">
+      <c r="I28" t="s">
         <v>70</v>
       </c>
-      <c r="I28" t="s">
+      <c r="J28" t="s">
         <v>72</v>
       </c>
-      <c r="J28" t="s">
+      <c r="K28" t="s">
         <v>73</v>
       </c>
-      <c r="K28" t="s">
+      <c r="L28" t="s">
         <v>74</v>
       </c>
-      <c r="L28" t="s">
+      <c r="M28" t="s">
         <v>75</v>
       </c>
-      <c r="M28" t="s">
+      <c r="N28" t="s">
         <v>71</v>
       </c>
-      <c r="N28" t="s">
+      <c r="O28" t="s">
         <v>325</v>
       </c>
-      <c r="O28" t="s">
+      <c r="P28" t="s">
         <v>326</v>
       </c>
-      <c r="P28" t="s">
+      <c r="Q28" t="s">
         <v>327</v>
       </c>
-      <c r="Q28" t="s">
+      <c r="R28" t="s">
         <v>328</v>
       </c>
-      <c r="R28" t="s">
+      <c r="S28" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>90</v>
       </c>
@@ -4029,41 +4037,41 @@
       <c r="G29" t="s">
         <v>69</v>
       </c>
-      <c r="H29" t="s">
+      <c r="I29" t="s">
         <v>70</v>
       </c>
-      <c r="I29" t="s">
+      <c r="J29" t="s">
         <v>72</v>
       </c>
-      <c r="J29" t="s">
+      <c r="K29" t="s">
         <v>73</v>
       </c>
-      <c r="K29" t="s">
+      <c r="L29" t="s">
         <v>74</v>
       </c>
-      <c r="L29" t="s">
+      <c r="M29" t="s">
         <v>75</v>
       </c>
-      <c r="M29" t="s">
+      <c r="N29" t="s">
         <v>71</v>
       </c>
-      <c r="N29" t="s">
+      <c r="O29" t="s">
         <v>325</v>
       </c>
-      <c r="O29" t="s">
+      <c r="P29" t="s">
         <v>326</v>
       </c>
-      <c r="P29" t="s">
+      <c r="Q29" t="s">
         <v>327</v>
       </c>
-      <c r="Q29" t="s">
+      <c r="R29" t="s">
         <v>328</v>
       </c>
-      <c r="R29" t="s">
+      <c r="S29" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>91</v>
       </c>
@@ -4085,41 +4093,41 @@
       <c r="G30" t="s">
         <v>69</v>
       </c>
-      <c r="H30" t="s">
+      <c r="I30" t="s">
         <v>70</v>
       </c>
-      <c r="I30" t="s">
+      <c r="J30" t="s">
         <v>72</v>
       </c>
-      <c r="J30" t="s">
+      <c r="K30" t="s">
         <v>73</v>
       </c>
-      <c r="K30" t="s">
+      <c r="L30" t="s">
         <v>74</v>
       </c>
-      <c r="L30" t="s">
+      <c r="M30" t="s">
         <v>75</v>
       </c>
-      <c r="M30" t="s">
+      <c r="N30" t="s">
         <v>71</v>
       </c>
-      <c r="N30" t="s">
+      <c r="O30" t="s">
         <v>325</v>
       </c>
-      <c r="O30" t="s">
+      <c r="P30" t="s">
         <v>326</v>
       </c>
-      <c r="P30" t="s">
+      <c r="Q30" t="s">
         <v>327</v>
       </c>
-      <c r="Q30" t="s">
+      <c r="R30" t="s">
         <v>328</v>
       </c>
-      <c r="R30" t="s">
+      <c r="S30" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>92</v>
       </c>
@@ -4141,41 +4149,41 @@
       <c r="G31" t="s">
         <v>69</v>
       </c>
-      <c r="H31" t="s">
+      <c r="I31" t="s">
         <v>70</v>
       </c>
-      <c r="I31" t="s">
+      <c r="J31" t="s">
         <v>72</v>
       </c>
-      <c r="J31" t="s">
+      <c r="K31" t="s">
         <v>73</v>
       </c>
-      <c r="K31" t="s">
+      <c r="L31" t="s">
         <v>74</v>
       </c>
-      <c r="L31" t="s">
+      <c r="M31" t="s">
         <v>75</v>
       </c>
-      <c r="M31" t="s">
+      <c r="N31" t="s">
         <v>71</v>
       </c>
-      <c r="N31" t="s">
+      <c r="O31" t="s">
         <v>325</v>
       </c>
-      <c r="O31" t="s">
+      <c r="P31" t="s">
         <v>326</v>
       </c>
-      <c r="P31" t="s">
+      <c r="Q31" t="s">
         <v>327</v>
       </c>
-      <c r="Q31" t="s">
+      <c r="R31" t="s">
         <v>328</v>
       </c>
-      <c r="R31" t="s">
+      <c r="S31" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>93</v>
       </c>
@@ -4197,41 +4205,41 @@
       <c r="G32" t="s">
         <v>69</v>
       </c>
-      <c r="H32" t="s">
+      <c r="I32" t="s">
         <v>70</v>
       </c>
-      <c r="I32" t="s">
+      <c r="J32" t="s">
         <v>72</v>
       </c>
-      <c r="J32" t="s">
+      <c r="K32" t="s">
         <v>73</v>
       </c>
-      <c r="K32" t="s">
+      <c r="L32" t="s">
         <v>74</v>
       </c>
-      <c r="L32" t="s">
+      <c r="M32" t="s">
         <v>75</v>
       </c>
-      <c r="M32" t="s">
+      <c r="N32" t="s">
         <v>71</v>
       </c>
-      <c r="N32" t="s">
+      <c r="O32" t="s">
         <v>325</v>
       </c>
-      <c r="O32" t="s">
+      <c r="P32" t="s">
         <v>326</v>
       </c>
-      <c r="P32" t="s">
+      <c r="Q32" t="s">
         <v>327</v>
       </c>
-      <c r="Q32" t="s">
+      <c r="R32" t="s">
         <v>328</v>
       </c>
-      <c r="R32" t="s">
+      <c r="S32" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>94</v>
       </c>
@@ -4253,41 +4261,41 @@
       <c r="G33" t="s">
         <v>69</v>
       </c>
-      <c r="H33" t="s">
+      <c r="I33" t="s">
         <v>70</v>
       </c>
-      <c r="I33" t="s">
+      <c r="J33" t="s">
         <v>72</v>
       </c>
-      <c r="J33" t="s">
+      <c r="K33" t="s">
         <v>73</v>
       </c>
-      <c r="K33" t="s">
+      <c r="L33" t="s">
         <v>74</v>
       </c>
-      <c r="L33" t="s">
+      <c r="M33" t="s">
         <v>75</v>
       </c>
-      <c r="M33" t="s">
+      <c r="N33" t="s">
         <v>71</v>
       </c>
-      <c r="N33" t="s">
+      <c r="O33" t="s">
         <v>325</v>
       </c>
-      <c r="O33" t="s">
+      <c r="P33" t="s">
         <v>326</v>
       </c>
-      <c r="P33" t="s">
+      <c r="Q33" t="s">
         <v>327</v>
       </c>
-      <c r="Q33" t="s">
+      <c r="R33" t="s">
         <v>328</v>
       </c>
-      <c r="R33" t="s">
+      <c r="S33" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>95</v>
       </c>
@@ -4309,37 +4317,37 @@
       <c r="G34" t="s">
         <v>69</v>
       </c>
-      <c r="H34" t="s">
+      <c r="I34" t="s">
         <v>70</v>
       </c>
-      <c r="I34" t="s">
+      <c r="J34" t="s">
         <v>72</v>
       </c>
-      <c r="J34" t="s">
+      <c r="K34" t="s">
         <v>73</v>
       </c>
-      <c r="K34" t="s">
+      <c r="L34" t="s">
         <v>74</v>
       </c>
-      <c r="L34" t="s">
+      <c r="M34" t="s">
         <v>75</v>
       </c>
-      <c r="M34" t="s">
+      <c r="N34" t="s">
         <v>71</v>
       </c>
-      <c r="N34" t="s">
+      <c r="O34" t="s">
         <v>325</v>
       </c>
-      <c r="O34" t="s">
+      <c r="P34" t="s">
         <v>326</v>
       </c>
-      <c r="P34" t="s">
+      <c r="Q34" t="s">
         <v>327</v>
       </c>
-      <c r="Q34" t="s">
+      <c r="R34" t="s">
         <v>328</v>
       </c>
-      <c r="R34" t="s">
+      <c r="S34" t="s">
         <v>329</v>
       </c>
     </row>
@@ -4350,18 +4358,20 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R34"/>
+  <dimension ref="A1:S34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="1">
+      <selection activeCell="J13" sqref="J13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4384,40 +4394,43 @@
         <v>433</v>
       </c>
       <c r="H1" t="s">
+        <v>432</v>
+      </c>
+      <c r="I1" t="s">
         <v>434</v>
       </c>
-      <c r="I1" t="s">
-        <v>435</v>
-      </c>
       <c r="J1" t="s">
+        <v>465</v>
+      </c>
+      <c r="K1" t="s">
         <v>428</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>429</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>343</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>344</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>345</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>346</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>347</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>348</v>
       </c>
-      <c r="R1" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S1" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>63</v>
       </c>
@@ -4433,29 +4446,29 @@
       <c r="F2" t="s">
         <v>330</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>53</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>54</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>55</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>58</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>56</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>57</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>64</v>
       </c>
@@ -4471,29 +4484,29 @@
       <c r="F3" t="s">
         <v>330</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>53</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>54</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>55</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>58</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>56</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="R3" t="s">
         <v>57</v>
       </c>
-      <c r="R3" t="s">
+      <c r="S3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>65</v>
       </c>
@@ -4509,29 +4522,29 @@
       <c r="F4" t="s">
         <v>330</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>53</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>54</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>55</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>58</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>56</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="R4" t="s">
         <v>57</v>
       </c>
-      <c r="R4" t="s">
+      <c r="S4" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>66</v>
       </c>
@@ -4547,29 +4560,29 @@
       <c r="F5" t="s">
         <v>330</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>53</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>54</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>55</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>58</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
         <v>56</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="R5" t="s">
         <v>57</v>
       </c>
-      <c r="R5" t="s">
+      <c r="S5" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>67</v>
       </c>
@@ -4585,29 +4598,29 @@
       <c r="F6" t="s">
         <v>330</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>53</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>54</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>55</v>
       </c>
-      <c r="N6" t="s">
+      <c r="O6" t="s">
         <v>58</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>56</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="R6" t="s">
         <v>57</v>
       </c>
-      <c r="R6" t="s">
+      <c r="S6" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>68</v>
       </c>
@@ -4623,29 +4636,29 @@
       <c r="F7" t="s">
         <v>330</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>53</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
         <v>54</v>
       </c>
-      <c r="M7" t="s">
+      <c r="N7" t="s">
         <v>55</v>
       </c>
-      <c r="N7" t="s">
+      <c r="O7" t="s">
         <v>58</v>
       </c>
-      <c r="O7" t="s">
+      <c r="P7" t="s">
         <v>56</v>
       </c>
-      <c r="Q7" t="s">
+      <c r="R7" t="s">
         <v>57</v>
       </c>
-      <c r="R7" t="s">
+      <c r="S7" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>69</v>
       </c>
@@ -4664,35 +4677,35 @@
       <c r="G8" t="s">
         <v>53</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>54</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>55</v>
       </c>
-      <c r="L8" t="s">
+      <c r="M8" t="s">
         <v>58</v>
       </c>
-      <c r="M8" t="s">
+      <c r="N8" t="s">
         <v>56</v>
       </c>
-      <c r="N8" t="s">
+      <c r="O8" t="s">
         <v>57</v>
       </c>
-      <c r="O8" t="s">
+      <c r="P8" t="s">
         <v>59</v>
       </c>
-      <c r="P8" t="s">
+      <c r="Q8" t="s">
         <v>60</v>
       </c>
-      <c r="Q8" t="s">
+      <c r="R8" t="s">
         <v>61</v>
       </c>
-      <c r="R8" t="s">
+      <c r="S8" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>70</v>
       </c>
@@ -4711,35 +4724,35 @@
       <c r="G9" t="s">
         <v>53</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>54</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>55</v>
       </c>
-      <c r="L9" t="s">
+      <c r="M9" t="s">
         <v>58</v>
       </c>
-      <c r="M9" t="s">
+      <c r="N9" t="s">
         <v>56</v>
       </c>
-      <c r="N9" t="s">
+      <c r="O9" t="s">
         <v>57</v>
       </c>
-      <c r="O9" t="s">
+      <c r="P9" t="s">
         <v>59</v>
       </c>
-      <c r="P9" t="s">
+      <c r="Q9" t="s">
         <v>60</v>
       </c>
-      <c r="Q9" t="s">
+      <c r="R9" t="s">
         <v>61</v>
       </c>
-      <c r="R9" t="s">
+      <c r="S9" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>71</v>
       </c>
@@ -4758,35 +4771,35 @@
       <c r="G10" t="s">
         <v>53</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>54</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
         <v>55</v>
       </c>
-      <c r="L10" t="s">
+      <c r="M10" t="s">
         <v>58</v>
       </c>
-      <c r="M10" t="s">
+      <c r="N10" t="s">
         <v>56</v>
       </c>
-      <c r="N10" t="s">
+      <c r="O10" t="s">
         <v>57</v>
       </c>
-      <c r="O10" t="s">
+      <c r="P10" t="s">
         <v>59</v>
       </c>
-      <c r="P10" t="s">
+      <c r="Q10" t="s">
         <v>60</v>
       </c>
-      <c r="Q10" t="s">
+      <c r="R10" t="s">
         <v>61</v>
       </c>
-      <c r="R10" t="s">
+      <c r="S10" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>72</v>
       </c>
@@ -4805,35 +4818,35 @@
       <c r="G11" t="s">
         <v>53</v>
       </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
         <v>54</v>
       </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
         <v>55</v>
       </c>
-      <c r="L11" t="s">
+      <c r="M11" t="s">
         <v>58</v>
       </c>
-      <c r="M11" t="s">
+      <c r="N11" t="s">
         <v>56</v>
       </c>
-      <c r="N11" t="s">
+      <c r="O11" t="s">
         <v>57</v>
       </c>
-      <c r="O11" t="s">
+      <c r="P11" t="s">
         <v>59</v>
       </c>
-      <c r="P11" t="s">
+      <c r="Q11" t="s">
         <v>60</v>
       </c>
-      <c r="Q11" t="s">
+      <c r="R11" t="s">
         <v>61</v>
       </c>
-      <c r="R11" t="s">
+      <c r="S11" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>73</v>
       </c>
@@ -4852,35 +4865,35 @@
       <c r="G12" t="s">
         <v>53</v>
       </c>
-      <c r="H12" t="s">
+      <c r="I12" t="s">
         <v>54</v>
       </c>
-      <c r="I12" t="s">
+      <c r="J12" t="s">
         <v>55</v>
       </c>
-      <c r="L12" t="s">
+      <c r="M12" t="s">
         <v>58</v>
       </c>
-      <c r="M12" t="s">
+      <c r="N12" t="s">
         <v>56</v>
       </c>
-      <c r="N12" t="s">
+      <c r="O12" t="s">
         <v>57</v>
       </c>
-      <c r="O12" t="s">
+      <c r="P12" t="s">
         <v>59</v>
       </c>
-      <c r="P12" t="s">
+      <c r="Q12" t="s">
         <v>60</v>
       </c>
-      <c r="Q12" t="s">
+      <c r="R12" t="s">
         <v>61</v>
       </c>
-      <c r="R12" t="s">
+      <c r="S12" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>74</v>
       </c>
@@ -4902,35 +4915,35 @@
       <c r="G13" t="s">
         <v>54</v>
       </c>
-      <c r="H13" t="s">
+      <c r="I13" t="s">
         <v>55</v>
       </c>
-      <c r="I13" t="s">
+      <c r="J13" t="s">
         <v>58</v>
       </c>
-      <c r="L13" t="s">
+      <c r="M13" t="s">
         <v>56</v>
       </c>
-      <c r="M13" t="s">
+      <c r="N13" t="s">
         <v>57</v>
       </c>
-      <c r="N13" t="s">
+      <c r="O13" t="s">
         <v>59</v>
       </c>
-      <c r="O13" t="s">
+      <c r="P13" t="s">
         <v>60</v>
       </c>
-      <c r="P13" t="s">
+      <c r="Q13" t="s">
         <v>61</v>
       </c>
-      <c r="Q13" t="s">
+      <c r="R13" t="s">
         <v>62</v>
       </c>
-      <c r="R13" t="s">
+      <c r="S13" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>75</v>
       </c>
@@ -4952,35 +4965,35 @@
       <c r="G14" t="s">
         <v>54</v>
       </c>
-      <c r="H14" t="s">
+      <c r="I14" t="s">
         <v>55</v>
       </c>
-      <c r="I14" t="s">
+      <c r="J14" t="s">
         <v>58</v>
       </c>
-      <c r="L14" t="s">
+      <c r="M14" t="s">
         <v>56</v>
       </c>
-      <c r="M14" t="s">
+      <c r="N14" t="s">
         <v>57</v>
       </c>
-      <c r="N14" t="s">
+      <c r="O14" t="s">
         <v>59</v>
       </c>
-      <c r="O14" t="s">
+      <c r="P14" t="s">
         <v>60</v>
       </c>
-      <c r="P14" t="s">
+      <c r="Q14" t="s">
         <v>61</v>
       </c>
-      <c r="Q14" t="s">
+      <c r="R14" t="s">
         <v>62</v>
       </c>
-      <c r="R14" t="s">
+      <c r="S14" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>76</v>
       </c>
@@ -5002,35 +5015,35 @@
       <c r="G15" t="s">
         <v>54</v>
       </c>
-      <c r="H15" t="s">
+      <c r="I15" t="s">
         <v>55</v>
       </c>
-      <c r="I15" t="s">
+      <c r="J15" t="s">
         <v>58</v>
       </c>
-      <c r="L15" t="s">
+      <c r="M15" t="s">
         <v>56</v>
       </c>
-      <c r="M15" t="s">
+      <c r="N15" t="s">
         <v>57</v>
       </c>
-      <c r="N15" t="s">
+      <c r="O15" t="s">
         <v>59</v>
       </c>
-      <c r="O15" t="s">
+      <c r="P15" t="s">
         <v>60</v>
       </c>
-      <c r="P15" t="s">
+      <c r="Q15" t="s">
         <v>61</v>
       </c>
-      <c r="Q15" t="s">
+      <c r="R15" t="s">
         <v>62</v>
       </c>
-      <c r="R15" t="s">
+      <c r="S15" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>77</v>
       </c>
@@ -5052,35 +5065,35 @@
       <c r="G16" t="s">
         <v>54</v>
       </c>
-      <c r="H16" t="s">
+      <c r="I16" t="s">
         <v>55</v>
       </c>
-      <c r="I16" t="s">
+      <c r="J16" t="s">
         <v>58</v>
       </c>
-      <c r="L16" t="s">
+      <c r="M16" t="s">
         <v>56</v>
       </c>
-      <c r="M16" t="s">
+      <c r="N16" t="s">
         <v>57</v>
       </c>
-      <c r="N16" t="s">
+      <c r="O16" t="s">
         <v>59</v>
       </c>
-      <c r="O16" t="s">
+      <c r="P16" t="s">
         <v>60</v>
       </c>
-      <c r="P16" t="s">
+      <c r="Q16" t="s">
         <v>61</v>
       </c>
-      <c r="Q16" t="s">
+      <c r="R16" t="s">
         <v>62</v>
       </c>
-      <c r="R16" t="s">
+      <c r="S16" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>78</v>
       </c>
@@ -5102,35 +5115,35 @@
       <c r="G17" t="s">
         <v>54</v>
       </c>
-      <c r="H17" t="s">
+      <c r="I17" t="s">
         <v>55</v>
       </c>
-      <c r="I17" t="s">
+      <c r="J17" t="s">
         <v>58</v>
       </c>
-      <c r="L17" t="s">
+      <c r="M17" t="s">
         <v>56</v>
       </c>
-      <c r="M17" t="s">
+      <c r="N17" t="s">
         <v>57</v>
       </c>
-      <c r="N17" t="s">
+      <c r="O17" t="s">
         <v>59</v>
       </c>
-      <c r="O17" t="s">
+      <c r="P17" t="s">
         <v>60</v>
       </c>
-      <c r="P17" t="s">
+      <c r="Q17" t="s">
         <v>61</v>
       </c>
-      <c r="Q17" t="s">
+      <c r="R17" t="s">
         <v>62</v>
       </c>
-      <c r="R17" t="s">
+      <c r="S17" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>79</v>
       </c>
@@ -5152,35 +5165,35 @@
       <c r="G18" t="s">
         <v>54</v>
       </c>
-      <c r="H18" t="s">
+      <c r="I18" t="s">
         <v>55</v>
       </c>
-      <c r="I18" t="s">
+      <c r="J18" t="s">
         <v>58</v>
       </c>
-      <c r="L18" t="s">
+      <c r="M18" t="s">
         <v>56</v>
       </c>
-      <c r="M18" t="s">
+      <c r="N18" t="s">
         <v>57</v>
       </c>
-      <c r="N18" t="s">
+      <c r="O18" t="s">
         <v>59</v>
       </c>
-      <c r="O18" t="s">
+      <c r="P18" t="s">
         <v>60</v>
       </c>
-      <c r="P18" t="s">
+      <c r="Q18" t="s">
         <v>61</v>
       </c>
-      <c r="Q18" t="s">
+      <c r="R18" t="s">
         <v>62</v>
       </c>
-      <c r="R18" t="s">
+      <c r="S18" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>80</v>
       </c>
@@ -5202,35 +5215,35 @@
       <c r="G19" t="s">
         <v>54</v>
       </c>
-      <c r="H19" t="s">
+      <c r="I19" t="s">
         <v>55</v>
       </c>
-      <c r="I19" t="s">
+      <c r="J19" t="s">
         <v>58</v>
       </c>
-      <c r="L19" t="s">
+      <c r="M19" t="s">
         <v>56</v>
       </c>
-      <c r="M19" t="s">
+      <c r="N19" t="s">
         <v>57</v>
       </c>
-      <c r="N19" t="s">
+      <c r="O19" t="s">
         <v>59</v>
       </c>
-      <c r="O19" t="s">
+      <c r="P19" t="s">
         <v>60</v>
       </c>
-      <c r="P19" t="s">
+      <c r="Q19" t="s">
         <v>61</v>
       </c>
-      <c r="Q19" t="s">
+      <c r="R19" t="s">
         <v>62</v>
       </c>
-      <c r="R19" t="s">
+      <c r="S19" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>81</v>
       </c>
@@ -5252,35 +5265,35 @@
       <c r="G20" t="s">
         <v>54</v>
       </c>
-      <c r="H20" t="s">
+      <c r="I20" t="s">
         <v>55</v>
       </c>
-      <c r="I20" t="s">
+      <c r="J20" t="s">
         <v>58</v>
       </c>
-      <c r="L20" t="s">
+      <c r="M20" t="s">
         <v>56</v>
       </c>
-      <c r="M20" t="s">
+      <c r="N20" t="s">
         <v>57</v>
       </c>
-      <c r="N20" t="s">
+      <c r="O20" t="s">
         <v>59</v>
       </c>
-      <c r="O20" t="s">
+      <c r="P20" t="s">
         <v>60</v>
       </c>
-      <c r="P20" t="s">
+      <c r="Q20" t="s">
         <v>61</v>
       </c>
-      <c r="Q20" t="s">
+      <c r="R20" t="s">
         <v>62</v>
       </c>
-      <c r="R20" t="s">
+      <c r="S20" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>82</v>
       </c>
@@ -5302,35 +5315,35 @@
       <c r="G21" t="s">
         <v>54</v>
       </c>
-      <c r="H21" t="s">
+      <c r="I21" t="s">
         <v>55</v>
       </c>
-      <c r="I21" t="s">
+      <c r="J21" t="s">
         <v>58</v>
       </c>
-      <c r="L21" t="s">
+      <c r="M21" t="s">
         <v>56</v>
       </c>
-      <c r="M21" t="s">
+      <c r="N21" t="s">
         <v>57</v>
       </c>
-      <c r="N21" t="s">
+      <c r="O21" t="s">
         <v>59</v>
       </c>
-      <c r="O21" t="s">
+      <c r="P21" t="s">
         <v>60</v>
       </c>
-      <c r="P21" t="s">
+      <c r="Q21" t="s">
         <v>61</v>
       </c>
-      <c r="Q21" t="s">
+      <c r="R21" t="s">
         <v>62</v>
       </c>
-      <c r="R21" t="s">
+      <c r="S21" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>83</v>
       </c>
@@ -5352,35 +5365,35 @@
       <c r="G22" t="s">
         <v>54</v>
       </c>
-      <c r="H22" t="s">
+      <c r="I22" t="s">
         <v>55</v>
       </c>
-      <c r="I22" t="s">
+      <c r="J22" t="s">
         <v>58</v>
       </c>
-      <c r="L22" t="s">
+      <c r="M22" t="s">
         <v>56</v>
       </c>
-      <c r="M22" t="s">
+      <c r="N22" t="s">
         <v>57</v>
       </c>
-      <c r="N22" t="s">
+      <c r="O22" t="s">
         <v>59</v>
       </c>
-      <c r="O22" t="s">
+      <c r="P22" t="s">
         <v>60</v>
       </c>
-      <c r="P22" t="s">
+      <c r="Q22" t="s">
         <v>61</v>
       </c>
-      <c r="Q22" t="s">
+      <c r="R22" t="s">
         <v>62</v>
       </c>
-      <c r="R22" t="s">
+      <c r="S22" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>84</v>
       </c>
@@ -5402,41 +5415,41 @@
       <c r="G23" t="s">
         <v>69</v>
       </c>
-      <c r="H23" t="s">
+      <c r="I23" t="s">
         <v>70</v>
       </c>
-      <c r="I23" t="s">
+      <c r="J23" t="s">
         <v>72</v>
       </c>
-      <c r="J23" t="s">
+      <c r="K23" t="s">
         <v>73</v>
       </c>
-      <c r="K23" t="s">
+      <c r="L23" t="s">
         <v>74</v>
       </c>
-      <c r="L23" t="s">
+      <c r="M23" t="s">
         <v>75</v>
       </c>
-      <c r="M23" t="s">
+      <c r="N23" t="s">
         <v>71</v>
       </c>
-      <c r="N23" t="s">
+      <c r="O23" t="s">
         <v>325</v>
       </c>
-      <c r="O23" t="s">
+      <c r="P23" t="s">
         <v>326</v>
       </c>
-      <c r="P23" t="s">
+      <c r="Q23" t="s">
         <v>327</v>
       </c>
-      <c r="Q23" t="s">
+      <c r="R23" t="s">
         <v>328</v>
       </c>
-      <c r="R23" t="s">
+      <c r="S23" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>85</v>
       </c>
@@ -5458,41 +5471,41 @@
       <c r="G24" t="s">
         <v>69</v>
       </c>
-      <c r="H24" t="s">
+      <c r="I24" t="s">
         <v>70</v>
       </c>
-      <c r="I24" t="s">
+      <c r="J24" t="s">
         <v>72</v>
       </c>
-      <c r="J24" t="s">
+      <c r="K24" t="s">
         <v>73</v>
       </c>
-      <c r="K24" t="s">
+      <c r="L24" t="s">
         <v>74</v>
       </c>
-      <c r="L24" t="s">
+      <c r="M24" t="s">
         <v>75</v>
       </c>
-      <c r="M24" t="s">
+      <c r="N24" t="s">
         <v>71</v>
       </c>
-      <c r="N24" t="s">
+      <c r="O24" t="s">
         <v>325</v>
       </c>
-      <c r="O24" t="s">
+      <c r="P24" t="s">
         <v>326</v>
       </c>
-      <c r="P24" t="s">
+      <c r="Q24" t="s">
         <v>327</v>
       </c>
-      <c r="Q24" t="s">
+      <c r="R24" t="s">
         <v>328</v>
       </c>
-      <c r="R24" t="s">
+      <c r="S24" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>86</v>
       </c>
@@ -5514,41 +5527,41 @@
       <c r="G25" t="s">
         <v>69</v>
       </c>
-      <c r="H25" t="s">
+      <c r="I25" t="s">
         <v>70</v>
       </c>
-      <c r="I25" t="s">
+      <c r="J25" t="s">
         <v>72</v>
       </c>
-      <c r="J25" t="s">
+      <c r="K25" t="s">
         <v>73</v>
       </c>
-      <c r="K25" t="s">
+      <c r="L25" t="s">
         <v>74</v>
       </c>
-      <c r="L25" t="s">
+      <c r="M25" t="s">
         <v>75</v>
       </c>
-      <c r="M25" t="s">
+      <c r="N25" t="s">
         <v>71</v>
       </c>
-      <c r="N25" t="s">
+      <c r="O25" t="s">
         <v>325</v>
       </c>
-      <c r="O25" t="s">
+      <c r="P25" t="s">
         <v>326</v>
       </c>
-      <c r="P25" t="s">
+      <c r="Q25" t="s">
         <v>327</v>
       </c>
-      <c r="Q25" t="s">
+      <c r="R25" t="s">
         <v>328</v>
       </c>
-      <c r="R25" t="s">
+      <c r="S25" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>87</v>
       </c>
@@ -5570,41 +5583,41 @@
       <c r="G26" t="s">
         <v>69</v>
       </c>
-      <c r="H26" t="s">
+      <c r="I26" t="s">
         <v>70</v>
       </c>
-      <c r="I26" t="s">
+      <c r="J26" t="s">
         <v>72</v>
       </c>
-      <c r="J26" t="s">
+      <c r="K26" t="s">
         <v>73</v>
       </c>
-      <c r="K26" t="s">
+      <c r="L26" t="s">
         <v>74</v>
       </c>
-      <c r="L26" t="s">
+      <c r="M26" t="s">
         <v>75</v>
       </c>
-      <c r="M26" t="s">
+      <c r="N26" t="s">
         <v>71</v>
       </c>
-      <c r="N26" t="s">
+      <c r="O26" t="s">
         <v>325</v>
       </c>
-      <c r="O26" t="s">
+      <c r="P26" t="s">
         <v>326</v>
       </c>
-      <c r="P26" t="s">
+      <c r="Q26" t="s">
         <v>327</v>
       </c>
-      <c r="Q26" t="s">
+      <c r="R26" t="s">
         <v>328</v>
       </c>
-      <c r="R26" t="s">
+      <c r="S26" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>88</v>
       </c>
@@ -5626,41 +5639,41 @@
       <c r="G27" t="s">
         <v>69</v>
       </c>
-      <c r="H27" t="s">
+      <c r="I27" t="s">
         <v>70</v>
       </c>
-      <c r="I27" t="s">
+      <c r="J27" t="s">
         <v>72</v>
       </c>
-      <c r="J27" t="s">
+      <c r="K27" t="s">
         <v>73</v>
       </c>
-      <c r="K27" t="s">
+      <c r="L27" t="s">
         <v>74</v>
       </c>
-      <c r="L27" t="s">
+      <c r="M27" t="s">
         <v>75</v>
       </c>
-      <c r="M27" t="s">
+      <c r="N27" t="s">
         <v>71</v>
       </c>
-      <c r="N27" t="s">
+      <c r="O27" t="s">
         <v>325</v>
       </c>
-      <c r="O27" t="s">
+      <c r="P27" t="s">
         <v>326</v>
       </c>
-      <c r="P27" t="s">
+      <c r="Q27" t="s">
         <v>327</v>
       </c>
-      <c r="Q27" t="s">
+      <c r="R27" t="s">
         <v>328</v>
       </c>
-      <c r="R27" t="s">
+      <c r="S27" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>89</v>
       </c>
@@ -5682,41 +5695,41 @@
       <c r="G28" t="s">
         <v>69</v>
       </c>
-      <c r="H28" t="s">
+      <c r="I28" t="s">
         <v>70</v>
       </c>
-      <c r="I28" t="s">
+      <c r="J28" t="s">
         <v>72</v>
       </c>
-      <c r="J28" t="s">
+      <c r="K28" t="s">
         <v>73</v>
       </c>
-      <c r="K28" t="s">
+      <c r="L28" t="s">
         <v>74</v>
       </c>
-      <c r="L28" t="s">
+      <c r="M28" t="s">
         <v>75</v>
       </c>
-      <c r="M28" t="s">
+      <c r="N28" t="s">
         <v>71</v>
       </c>
-      <c r="N28" t="s">
+      <c r="O28" t="s">
         <v>325</v>
       </c>
-      <c r="O28" t="s">
+      <c r="P28" t="s">
         <v>326</v>
       </c>
-      <c r="P28" t="s">
+      <c r="Q28" t="s">
         <v>327</v>
       </c>
-      <c r="Q28" t="s">
+      <c r="R28" t="s">
         <v>328</v>
       </c>
-      <c r="R28" t="s">
+      <c r="S28" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>90</v>
       </c>
@@ -5738,41 +5751,41 @@
       <c r="G29" t="s">
         <v>69</v>
       </c>
-      <c r="H29" t="s">
+      <c r="I29" t="s">
         <v>70</v>
       </c>
-      <c r="I29" t="s">
+      <c r="J29" t="s">
         <v>72</v>
       </c>
-      <c r="J29" t="s">
+      <c r="K29" t="s">
         <v>73</v>
       </c>
-      <c r="K29" t="s">
+      <c r="L29" t="s">
         <v>74</v>
       </c>
-      <c r="L29" t="s">
+      <c r="M29" t="s">
         <v>75</v>
       </c>
-      <c r="M29" t="s">
+      <c r="N29" t="s">
         <v>71</v>
       </c>
-      <c r="N29" t="s">
+      <c r="O29" t="s">
         <v>325</v>
       </c>
-      <c r="O29" t="s">
+      <c r="P29" t="s">
         <v>326</v>
       </c>
-      <c r="P29" t="s">
+      <c r="Q29" t="s">
         <v>327</v>
       </c>
-      <c r="Q29" t="s">
+      <c r="R29" t="s">
         <v>328</v>
       </c>
-      <c r="R29" t="s">
+      <c r="S29" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>91</v>
       </c>
@@ -5794,41 +5807,41 @@
       <c r="G30" t="s">
         <v>69</v>
       </c>
-      <c r="H30" t="s">
+      <c r="I30" t="s">
         <v>70</v>
       </c>
-      <c r="I30" t="s">
+      <c r="J30" t="s">
         <v>72</v>
       </c>
-      <c r="J30" t="s">
+      <c r="K30" t="s">
         <v>73</v>
       </c>
-      <c r="K30" t="s">
+      <c r="L30" t="s">
         <v>74</v>
       </c>
-      <c r="L30" t="s">
+      <c r="M30" t="s">
         <v>75</v>
       </c>
-      <c r="M30" t="s">
+      <c r="N30" t="s">
         <v>71</v>
       </c>
-      <c r="N30" t="s">
+      <c r="O30" t="s">
         <v>325</v>
       </c>
-      <c r="O30" t="s">
+      <c r="P30" t="s">
         <v>326</v>
       </c>
-      <c r="P30" t="s">
+      <c r="Q30" t="s">
         <v>327</v>
       </c>
-      <c r="Q30" t="s">
+      <c r="R30" t="s">
         <v>328</v>
       </c>
-      <c r="R30" t="s">
+      <c r="S30" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>92</v>
       </c>
@@ -5850,41 +5863,41 @@
       <c r="G31" t="s">
         <v>69</v>
       </c>
-      <c r="H31" t="s">
+      <c r="I31" t="s">
         <v>70</v>
       </c>
-      <c r="I31" t="s">
+      <c r="J31" t="s">
         <v>72</v>
       </c>
-      <c r="J31" t="s">
+      <c r="K31" t="s">
         <v>73</v>
       </c>
-      <c r="K31" t="s">
+      <c r="L31" t="s">
         <v>74</v>
       </c>
-      <c r="L31" t="s">
+      <c r="M31" t="s">
         <v>75</v>
       </c>
-      <c r="M31" t="s">
+      <c r="N31" t="s">
         <v>71</v>
       </c>
-      <c r="N31" t="s">
+      <c r="O31" t="s">
         <v>325</v>
       </c>
-      <c r="O31" t="s">
+      <c r="P31" t="s">
         <v>326</v>
       </c>
-      <c r="P31" t="s">
+      <c r="Q31" t="s">
         <v>327</v>
       </c>
-      <c r="Q31" t="s">
+      <c r="R31" t="s">
         <v>328</v>
       </c>
-      <c r="R31" t="s">
+      <c r="S31" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>93</v>
       </c>
@@ -5906,41 +5919,41 @@
       <c r="G32" t="s">
         <v>69</v>
       </c>
-      <c r="H32" t="s">
+      <c r="I32" t="s">
         <v>70</v>
       </c>
-      <c r="I32" t="s">
+      <c r="J32" t="s">
         <v>72</v>
       </c>
-      <c r="J32" t="s">
+      <c r="K32" t="s">
         <v>73</v>
       </c>
-      <c r="K32" t="s">
+      <c r="L32" t="s">
         <v>74</v>
       </c>
-      <c r="L32" t="s">
+      <c r="M32" t="s">
         <v>75</v>
       </c>
-      <c r="M32" t="s">
+      <c r="N32" t="s">
         <v>71</v>
       </c>
-      <c r="N32" t="s">
+      <c r="O32" t="s">
         <v>325</v>
       </c>
-      <c r="O32" t="s">
+      <c r="P32" t="s">
         <v>326</v>
       </c>
-      <c r="P32" t="s">
+      <c r="Q32" t="s">
         <v>327</v>
       </c>
-      <c r="Q32" t="s">
+      <c r="R32" t="s">
         <v>328</v>
       </c>
-      <c r="R32" t="s">
+      <c r="S32" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>94</v>
       </c>
@@ -5962,41 +5975,41 @@
       <c r="G33" t="s">
         <v>69</v>
       </c>
-      <c r="H33" t="s">
+      <c r="I33" t="s">
         <v>70</v>
       </c>
-      <c r="I33" t="s">
+      <c r="J33" t="s">
         <v>72</v>
       </c>
-      <c r="J33" t="s">
+      <c r="K33" t="s">
         <v>73</v>
       </c>
-      <c r="K33" t="s">
+      <c r="L33" t="s">
         <v>74</v>
       </c>
-      <c r="L33" t="s">
+      <c r="M33" t="s">
         <v>75</v>
       </c>
-      <c r="M33" t="s">
+      <c r="N33" t="s">
         <v>71</v>
       </c>
-      <c r="N33" t="s">
+      <c r="O33" t="s">
         <v>325</v>
       </c>
-      <c r="O33" t="s">
+      <c r="P33" t="s">
         <v>326</v>
       </c>
-      <c r="P33" t="s">
+      <c r="Q33" t="s">
         <v>327</v>
       </c>
-      <c r="Q33" t="s">
+      <c r="R33" t="s">
         <v>328</v>
       </c>
-      <c r="R33" t="s">
+      <c r="S33" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>95</v>
       </c>
@@ -6018,37 +6031,37 @@
       <c r="G34" t="s">
         <v>69</v>
       </c>
-      <c r="H34" t="s">
+      <c r="I34" t="s">
         <v>70</v>
       </c>
-      <c r="I34" t="s">
+      <c r="J34" t="s">
         <v>72</v>
       </c>
-      <c r="J34" t="s">
+      <c r="K34" t="s">
         <v>73</v>
       </c>
-      <c r="K34" t="s">
+      <c r="L34" t="s">
         <v>74</v>
       </c>
-      <c r="L34" t="s">
+      <c r="M34" t="s">
         <v>75</v>
       </c>
-      <c r="M34" t="s">
+      <c r="N34" t="s">
         <v>71</v>
       </c>
-      <c r="N34" t="s">
+      <c r="O34" t="s">
         <v>325</v>
       </c>
-      <c r="O34" t="s">
+      <c r="P34" t="s">
         <v>326</v>
       </c>
-      <c r="P34" t="s">
+      <c r="Q34" t="s">
         <v>327</v>
       </c>
-      <c r="Q34" t="s">
+      <c r="R34" t="s">
         <v>328</v>
       </c>
-      <c r="R34" t="s">
+      <c r="S34" t="s">
         <v>329</v>
       </c>
     </row>
@@ -6090,22 +6103,22 @@
         <v>35</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="G1" s="3" t="s">
+        <v>455</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>456</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>457</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>458</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>459</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>460</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>461</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -6126,13 +6139,13 @@
         <v>511</v>
       </c>
       <c r="G2" s="6" t="s">
+        <v>452</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>453</v>
+      </c>
+      <c r="I2" s="6" t="s">
         <v>454</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>455</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>456</v>
       </c>
       <c r="J2" s="6">
         <v>521</v>
@@ -7132,10 +7145,12 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
+    <sheetView tabSelected="1" workbookViewId="1">
+      <selection activeCell="A2" sqref="A2:XFD4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7157,10 +7172,10 @@
         <v>35</v>
       </c>
       <c r="E1" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="F1" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="G1" t="s">
         <v>350</v>
@@ -7168,139 +7183,274 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>90</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>324</v>
-      </c>
-      <c r="C2" t="s">
-        <v>66</v>
-      </c>
-      <c r="D2" t="s">
-        <v>351</v>
-      </c>
-      <c r="E2" t="s">
-        <v>352</v>
-      </c>
-      <c r="F2" t="s">
-        <v>353</v>
-      </c>
-      <c r="G2" t="s">
-        <v>360</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>91</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>324</v>
-      </c>
-      <c r="C3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D3" t="s">
-        <v>351</v>
-      </c>
-      <c r="E3" t="s">
-        <v>352</v>
-      </c>
-      <c r="F3" t="s">
-        <v>353</v>
-      </c>
-      <c r="G3" t="s">
-        <v>360</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>92</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>324</v>
-      </c>
-      <c r="C4" t="s">
-        <v>66</v>
-      </c>
-      <c r="D4" t="s">
-        <v>351</v>
-      </c>
-      <c r="E4" t="s">
-        <v>352</v>
-      </c>
-      <c r="F4" t="s">
-        <v>353</v>
-      </c>
-      <c r="G4" t="s">
-        <v>360</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>93</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>324</v>
-      </c>
-      <c r="C5" t="s">
-        <v>66</v>
-      </c>
-      <c r="D5" t="s">
-        <v>351</v>
-      </c>
-      <c r="E5" t="s">
-        <v>352</v>
-      </c>
-      <c r="F5" t="s">
-        <v>353</v>
-      </c>
-      <c r="G5" t="s">
-        <v>360</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>94</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>324</v>
-      </c>
-      <c r="C6" t="s">
-        <v>66</v>
-      </c>
-      <c r="D6" t="s">
-        <v>351</v>
-      </c>
-      <c r="E6" t="s">
-        <v>352</v>
-      </c>
-      <c r="F6" t="s">
-        <v>353</v>
-      </c>
-      <c r="G6" t="s">
-        <v>360</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>90</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="C29" t="s">
+        <v>66</v>
+      </c>
+      <c r="D29" t="s">
+        <v>351</v>
+      </c>
+      <c r="E29" t="s">
+        <v>352</v>
+      </c>
+      <c r="F29" t="s">
+        <v>353</v>
+      </c>
+      <c r="G29" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>91</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="C30" t="s">
+        <v>66</v>
+      </c>
+      <c r="D30" t="s">
+        <v>351</v>
+      </c>
+      <c r="E30" t="s">
+        <v>352</v>
+      </c>
+      <c r="F30" t="s">
+        <v>353</v>
+      </c>
+      <c r="G30" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>92</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="C31" t="s">
+        <v>66</v>
+      </c>
+      <c r="D31" t="s">
+        <v>351</v>
+      </c>
+      <c r="E31" t="s">
+        <v>352</v>
+      </c>
+      <c r="F31" t="s">
+        <v>353</v>
+      </c>
+      <c r="G31" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>93</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="C32" t="s">
+        <v>66</v>
+      </c>
+      <c r="D32" t="s">
+        <v>351</v>
+      </c>
+      <c r="E32" t="s">
+        <v>352</v>
+      </c>
+      <c r="F32" t="s">
+        <v>353</v>
+      </c>
+      <c r="G32" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>94</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="C33" t="s">
+        <v>66</v>
+      </c>
+      <c r="D33" t="s">
+        <v>351</v>
+      </c>
+      <c r="E33" t="s">
+        <v>352</v>
+      </c>
+      <c r="F33" t="s">
+        <v>353</v>
+      </c>
+      <c r="G33" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34">
         <v>95</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B34" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="C7" t="s">
-        <v>66</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="C34" t="s">
+        <v>66</v>
+      </c>
+      <c r="D34" t="s">
         <v>351</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E34" t="s">
         <v>352</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F34" t="s">
         <v>353</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G34" t="s">
         <v>360</v>
       </c>
     </row>
@@ -57043,28 +57193,28 @@
         <v>429</v>
       </c>
       <c r="M1" t="s">
+        <v>435</v>
+      </c>
+      <c r="N1" t="s">
         <v>436</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>437</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>438</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>439</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>440</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>441</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>442</v>
-      </c>
-      <c r="T1" t="s">
-        <v>443</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
@@ -57282,7 +57432,7 @@
         <v>63</v>
       </c>
       <c r="B8" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>315</v>
@@ -57314,7 +57464,7 @@
         <v>64</v>
       </c>
       <c r="B9" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>315</v>
@@ -57346,7 +57496,7 @@
         <v>65</v>
       </c>
       <c r="B10" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>315</v>
@@ -57378,7 +57528,7 @@
         <v>66</v>
       </c>
       <c r="B11" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>315</v>
@@ -57410,7 +57560,7 @@
         <v>67</v>
       </c>
       <c r="B12" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>315</v>
@@ -57442,7 +57592,7 @@
         <v>68</v>
       </c>
       <c r="B13" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>315</v>
@@ -57474,7 +57624,7 @@
         <v>69</v>
       </c>
       <c r="B14" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>315</v>
@@ -57512,7 +57662,7 @@
         <v>70</v>
       </c>
       <c r="B15" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>315</v>
@@ -57562,7 +57712,7 @@
         <v>71</v>
       </c>
       <c r="B16" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>315</v>
@@ -57612,7 +57762,7 @@
         <v>72</v>
       </c>
       <c r="B17" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>315</v>
@@ -57662,7 +57812,7 @@
         <v>73</v>
       </c>
       <c r="B18" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>315</v>
@@ -57712,7 +57862,7 @@
         <v>74</v>
       </c>
       <c r="B19" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>315</v>
@@ -57765,7 +57915,7 @@
         <v>75</v>
       </c>
       <c r="B20" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>315</v>
@@ -57818,7 +57968,7 @@
         <v>76</v>
       </c>
       <c r="B21" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>315</v>
@@ -57871,7 +58021,7 @@
         <v>77</v>
       </c>
       <c r="B22" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>315</v>
@@ -57924,7 +58074,7 @@
         <v>78</v>
       </c>
       <c r="B23" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>315</v>
@@ -57977,7 +58127,7 @@
         <v>79</v>
       </c>
       <c r="B24" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>315</v>
@@ -58030,7 +58180,7 @@
         <v>80</v>
       </c>
       <c r="B25" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>315</v>
@@ -58083,7 +58233,7 @@
         <v>81</v>
       </c>
       <c r="B26" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>315</v>
@@ -58136,7 +58286,7 @@
         <v>82</v>
       </c>
       <c r="B27" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>315</v>
@@ -58189,7 +58339,7 @@
         <v>83</v>
       </c>
       <c r="B28" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>315</v>
@@ -58242,7 +58392,7 @@
         <v>84</v>
       </c>
       <c r="B29" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>321</v>
@@ -58301,7 +58451,7 @@
         <v>85</v>
       </c>
       <c r="B30" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>321</v>
@@ -58360,7 +58510,7 @@
         <v>86</v>
       </c>
       <c r="B31" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>321</v>
@@ -58419,7 +58569,7 @@
         <v>87</v>
       </c>
       <c r="B32" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>321</v>
@@ -58478,7 +58628,7 @@
         <v>88</v>
       </c>
       <c r="B33" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>321</v>
@@ -58537,7 +58687,7 @@
         <v>89</v>
       </c>
       <c r="B34" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>321</v>
@@ -58596,7 +58746,7 @@
         <v>90</v>
       </c>
       <c r="B35" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>321</v>
@@ -58655,7 +58805,7 @@
         <v>91</v>
       </c>
       <c r="B36" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>321</v>
@@ -58714,7 +58864,7 @@
         <v>92</v>
       </c>
       <c r="B37" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>321</v>
@@ -58773,7 +58923,7 @@
         <v>93</v>
       </c>
       <c r="B38" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>321</v>
@@ -58832,7 +58982,7 @@
         <v>94</v>
       </c>
       <c r="B39" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>321</v>
@@ -58891,7 +59041,7 @@
         <v>95</v>
       </c>
       <c r="B40" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>321</v>
@@ -58954,8 +59104,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="T26" sqref="T26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J1" sqref="J1:J1048576"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
@@ -59011,28 +59161,28 @@
         <v>429</v>
       </c>
       <c r="M1" t="s">
+        <v>443</v>
+      </c>
+      <c r="N1" t="s">
         <v>444</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>445</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>446</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>447</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>448</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>449</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>450</v>
-      </c>
-      <c r="T1" t="s">
-        <v>451</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
@@ -59250,7 +59400,7 @@
         <v>63</v>
       </c>
       <c r="B8" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>316</v>
@@ -59282,7 +59432,7 @@
         <v>64</v>
       </c>
       <c r="B9" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>316</v>
@@ -59314,7 +59464,7 @@
         <v>65</v>
       </c>
       <c r="B10" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>316</v>
@@ -59346,7 +59496,7 @@
         <v>66</v>
       </c>
       <c r="B11" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>316</v>
@@ -59378,7 +59528,7 @@
         <v>67</v>
       </c>
       <c r="B12" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>316</v>
@@ -59410,7 +59560,7 @@
         <v>68</v>
       </c>
       <c r="B13" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>316</v>
@@ -59442,7 +59592,7 @@
         <v>69</v>
       </c>
       <c r="B14" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>315</v>
@@ -59492,7 +59642,7 @@
         <v>70</v>
       </c>
       <c r="B15" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>315</v>
@@ -59542,7 +59692,7 @@
         <v>71</v>
       </c>
       <c r="B16" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>315</v>
@@ -59592,7 +59742,7 @@
         <v>72</v>
       </c>
       <c r="B17" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>315</v>
@@ -59642,7 +59792,7 @@
         <v>73</v>
       </c>
       <c r="B18" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>315</v>
@@ -59692,7 +59842,7 @@
         <v>74</v>
       </c>
       <c r="B19" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>315</v>
@@ -59745,7 +59895,7 @@
         <v>75</v>
       </c>
       <c r="B20" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>315</v>
@@ -59798,7 +59948,7 @@
         <v>76</v>
       </c>
       <c r="B21" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>315</v>
@@ -59851,7 +60001,7 @@
         <v>77</v>
       </c>
       <c r="B22" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>315</v>
@@ -59904,7 +60054,7 @@
         <v>78</v>
       </c>
       <c r="B23" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>315</v>
@@ -59957,7 +60107,7 @@
         <v>79</v>
       </c>
       <c r="B24" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>315</v>
@@ -60010,7 +60160,7 @@
         <v>80</v>
       </c>
       <c r="B25" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>315</v>
@@ -60063,7 +60213,7 @@
         <v>81</v>
       </c>
       <c r="B26" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>315</v>
@@ -60116,7 +60266,7 @@
         <v>82</v>
       </c>
       <c r="B27" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>315</v>
@@ -60169,7 +60319,7 @@
         <v>83</v>
       </c>
       <c r="B28" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>315</v>
@@ -60222,7 +60372,7 @@
         <v>84</v>
       </c>
       <c r="B29" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>321</v>
@@ -60281,7 +60431,7 @@
         <v>85</v>
       </c>
       <c r="B30" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>321</v>
@@ -60340,7 +60490,7 @@
         <v>86</v>
       </c>
       <c r="B31" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>321</v>
@@ -60399,7 +60549,7 @@
         <v>87</v>
       </c>
       <c r="B32" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>321</v>
@@ -60458,7 +60608,7 @@
         <v>88</v>
       </c>
       <c r="B33" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>321</v>
@@ -60517,7 +60667,7 @@
         <v>89</v>
       </c>
       <c r="B34" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>321</v>
@@ -60576,7 +60726,7 @@
         <v>90</v>
       </c>
       <c r="B35" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>321</v>
@@ -60635,7 +60785,7 @@
         <v>91</v>
       </c>
       <c r="B36" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>321</v>
@@ -60694,7 +60844,7 @@
         <v>92</v>
       </c>
       <c r="B37" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>321</v>
@@ -60753,7 +60903,7 @@
         <v>93</v>
       </c>
       <c r="B38" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>321</v>
@@ -60812,7 +60962,7 @@
         <v>94</v>
       </c>
       <c r="B39" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>321</v>
@@ -60871,7 +61021,7 @@
         <v>95</v>
       </c>
       <c r="B40" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>321</v>

</xml_diff>

<commit_message>
Minor Mod on Income (INCOMPLETE)
</commit_message>
<xml_diff>
--- a/Data/MetaData.xlsx
+++ b/Data/MetaData.xlsx
@@ -9,8 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="17100" windowHeight="6600" firstSheet="8" activeTab="9"/>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17100" windowHeight="6600" tabRatio="544" firstSheet="8" activeTab="12"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17100" windowHeight="6600" tabRatio="544" firstSheet="8" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="CompressedFileNames" sheetId="1" r:id="rId1"/>
@@ -1473,17 +1472,17 @@
     <t>BussNetIncomeY</t>
   </si>
   <si>
-    <t>JobType</t>
+    <t>AgriNetIncomeY</t>
   </si>
   <si>
-    <t>AgriNetIncomeY</t>
+    <t>BSector</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1648,6 +1647,14 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="178"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1998,7 +2005,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2014,6 +2021,7 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2338,7 +2346,6 @@
   <dimension ref="A1:B34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2626,11 +2633,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
-    </sheetView>
-    <sheetView workbookViewId="1">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J23" sqref="J23:L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2668,7 +2672,7 @@
         <v>434</v>
       </c>
       <c r="J1" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="K1" t="s">
         <v>428</v>
@@ -3704,14 +3708,14 @@
       <c r="I23" t="s">
         <v>70</v>
       </c>
-      <c r="J23" t="s">
+      <c r="J23" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="K23" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="K23" t="s">
+      <c r="L23" s="7" t="s">
         <v>73</v>
-      </c>
-      <c r="L23" t="s">
-        <v>74</v>
       </c>
       <c r="M23" t="s">
         <v>75</v>
@@ -4360,9 +4364,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S34"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4400,7 +4403,7 @@
         <v>434</v>
       </c>
       <c r="J1" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="K1" t="s">
         <v>428</v>
@@ -4427,7 +4430,7 @@
         <v>348</v>
       </c>
       <c r="S1" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
@@ -5418,14 +5421,14 @@
       <c r="I23" t="s">
         <v>70</v>
       </c>
-      <c r="J23" t="s">
+      <c r="J23" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="K23" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="K23" t="s">
+      <c r="L23" s="7" t="s">
         <v>73</v>
-      </c>
-      <c r="L23" t="s">
-        <v>74</v>
       </c>
       <c r="M23" t="s">
         <v>75</v>
@@ -6075,7 +6078,6 @@
   <dimension ref="A1:K34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7147,8 +7149,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-    <sheetView tabSelected="1" workbookViewId="1">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD4"/>
     </sheetView>
   </sheetViews>
@@ -7464,7 +7465,6 @@
   <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -8612,7 +8612,6 @@
   <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -9397,7 +9396,6 @@
   <dimension ref="A1:K34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -10606,7 +10604,6 @@
   <dimension ref="A1:E123"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -12474,7 +12471,6 @@
   <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -13401,7 +13397,6 @@
   <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -14328,7 +14323,6 @@
   <dimension ref="A1:R34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -15625,7 +15619,6 @@
   <dimension ref="A1:K34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -16721,7 +16714,6 @@
   <dimension ref="A1:J34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -17450,7 +17442,6 @@
   <dimension ref="A1:J34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -18414,7 +18405,6 @@
   <dimension ref="A1:J34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -19142,7 +19132,6 @@
   <dimension ref="A1:J34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -19990,7 +19979,6 @@
   <dimension ref="A1:J34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -20838,7 +20826,6 @@
   <dimension ref="A1:J34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -21566,7 +21553,6 @@
   <dimension ref="A1:P34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -23211,7 +23197,6 @@
   <dimension ref="A1:J34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -24058,7 +24043,6 @@
   <dimension ref="A1:J34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -24905,7 +24889,6 @@
   <dimension ref="A1:C60"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -25582,7 +25565,6 @@
   <dimension ref="A1:K34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -26469,7 +26451,6 @@
   <dimension ref="A1:J34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -27260,7 +27241,6 @@
   <dimension ref="A1:K34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -28350,7 +28330,6 @@
   <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -29077,7 +29056,6 @@
   <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -29801,7 +29779,6 @@
   <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -30525,7 +30502,6 @@
   <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -31249,7 +31225,6 @@
   <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -31992,7 +31967,6 @@
   <dimension ref="A1:J34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -32696,7 +32670,6 @@
   <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -33837,7 +33810,6 @@
   <dimension ref="A1:D97"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -35071,7 +35043,6 @@
   <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -36209,7 +36180,6 @@
   <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -37347,7 +37317,6 @@
   <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -38485,7 +38454,6 @@
   <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -39623,7 +39591,6 @@
   <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -40761,7 +40728,6 @@
   <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -41899,7 +41865,6 @@
   <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -43037,7 +43002,6 @@
   <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -44175,7 +44139,6 @@
   <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -45313,7 +45276,6 @@
   <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -46451,7 +46413,6 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -46578,7 +46539,6 @@
   <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -47719,7 +47679,6 @@
   <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -48857,7 +48816,6 @@
   <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -49995,7 +49953,6 @@
   <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -51133,7 +51090,6 @@
   <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -52271,7 +52227,6 @@
   <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -53409,7 +53364,6 @@
   <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -54547,7 +54501,6 @@
   <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -55685,7 +55638,6 @@
   <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -56539,7 +56491,6 @@
   <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -57134,10 +57085,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T40"/>
   <sheetViews>
-    <sheetView topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="T1" sqref="T1"/>
-    </sheetView>
-    <sheetView workbookViewId="1">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD13"/>
     </sheetView>
   </sheetViews>
@@ -59104,10 +59052,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:J1048576"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Updated reading other sources of income
</commit_message>
<xml_diff>
--- a/Data/MetaData.xlsx
+++ b/Data/MetaData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17100" windowHeight="6600" tabRatio="544" firstSheet="8" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17100" windowHeight="6600" tabRatio="544" firstSheet="7" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="CompressedFileNames" sheetId="1" r:id="rId1"/>
@@ -70,12 +70,12 @@
     <sheet name="Biscuit" sheetId="1026" r:id="rId56"/>
     <sheet name="Khoshkbar" sheetId="1027" r:id="rId57"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13188" uniqueCount="467">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13185" uniqueCount="468">
   <si>
     <t>Year</t>
   </si>
@@ -1430,9 +1430,6 @@
     <t>PrvWageNetIncomeY</t>
   </si>
   <si>
-    <t>Retirment</t>
-  </si>
-  <si>
     <t>512:514</t>
   </si>
   <si>
@@ -1477,11 +1474,17 @@
   <si>
     <t>BSector</t>
   </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Retirement</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2024,48 +2027,48 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="‏20% - تأکید1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="‏20% - تاکید2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="‏20% - تاکید3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="‏20% - تاکید4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="‏20% - تاکید5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="‏20% - تاکید6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - آکسان 1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="‏40% - تاکید2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="‏40% - تاکید3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="‏40% - تاکید4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="‏40% - تاکید5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="‏40% - تاکید6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="‏60% - تأکید1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="‏60% - تاکید2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="‏60% - تاکید3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="‏60% - تاکید4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="‏60% - تاکید5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="‏60% - تاکید6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="بد" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="بررسی سلول" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="تأکید1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="تاکید2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="تاکید3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="تاکید4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="تاکید5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="تاکید6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="خروجی" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="خنثی" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="خوب" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="سلول پیوندی" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="عنوان" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="عنوان 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="عنوان 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="عنوان 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="عنوان 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="متن توصیفی" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="متن هشدار" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="مجموع" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="محاسبه" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="معمولی" xfId="0" builtinId="0"/>
+    <cellStyle name="ورودی" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="یادداشت" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2672,7 +2675,7 @@
         <v>434</v>
       </c>
       <c r="J1" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="K1" t="s">
         <v>428</v>
@@ -2699,7 +2702,7 @@
         <v>348</v>
       </c>
       <c r="S1" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
@@ -4364,7 +4367,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
@@ -4403,7 +4406,7 @@
         <v>434</v>
       </c>
       <c r="J1" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="K1" t="s">
         <v>428</v>
@@ -4430,7 +4433,7 @@
         <v>348</v>
       </c>
       <c r="S1" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
@@ -6075,20 +6078,24 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K34"/>
+  <dimension ref="A1:L34"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4:E7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="5" width="9.140625" style="3" collapsed="1"/>
-    <col min="6" max="6" width="10.7109375" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="9" width="9.140625" style="3" collapsed="1"/>
-    <col min="10" max="10" width="11.140625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="16384" width="9.140625" style="3" collapsed="1"/>
+    <col min="1" max="4" width="9.140625" style="3" collapsed="1"/>
+    <col min="5" max="5" width="9.140625" style="3"/>
+    <col min="6" max="6" width="9.140625" style="3" collapsed="1"/>
+    <col min="7" max="7" width="10.7109375" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="10" width="9.140625" style="3" collapsed="1"/>
+    <col min="11" max="11" width="11.140625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="16384" width="9.140625" style="3" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -6102,28 +6109,31 @@
         <v>76</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>466</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>451</v>
-      </c>
       <c r="G1" s="3" t="s">
+        <v>467</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>455</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>456</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>457</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>458</v>
       </c>
-      <c r="K1" s="3" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>63</v>
       </c>
@@ -6136,24 +6146,27 @@
       <c r="D2" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6">
+      <c r="E2" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6">
         <v>511</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="H2" s="6" t="s">
+        <v>451</v>
+      </c>
+      <c r="I2" s="6" t="s">
         <v>452</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="J2" s="6" t="s">
         <v>453</v>
       </c>
-      <c r="I2" s="6" t="s">
-        <v>454</v>
-      </c>
-      <c r="J2" s="6">
+      <c r="K2" s="6">
         <v>521</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>64</v>
       </c>
@@ -6166,24 +6179,27 @@
       <c r="D3" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6" t="s">
+      <c r="E3" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="G3" s="6" t="s">
-        <v>54</v>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6">
+        <v>511</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>54</v>
+        <v>451</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>54</v>
+        <v>452</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+        <v>453</v>
+      </c>
+      <c r="K3" s="6">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>65</v>
       </c>
@@ -6196,24 +6212,27 @@
       <c r="D4" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6" t="s">
+      <c r="E4" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="G4" s="6" t="s">
-        <v>54</v>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6">
+        <v>511</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>54</v>
+        <v>451</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>54</v>
+        <v>452</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+        <v>453</v>
+      </c>
+      <c r="K4" s="6">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>66</v>
       </c>
@@ -6226,24 +6245,27 @@
       <c r="D5" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6" t="s">
+      <c r="E5" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="G5" s="6" t="s">
-        <v>54</v>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6">
+        <v>511</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>54</v>
+        <v>451</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>54</v>
+        <v>452</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+        <v>453</v>
+      </c>
+      <c r="K5" s="6">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>67</v>
       </c>
@@ -6256,24 +6278,27 @@
       <c r="D6" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6" t="s">
+      <c r="E6" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="G6" s="6" t="s">
-        <v>54</v>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6">
+        <v>511</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>54</v>
+        <v>451</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>54</v>
+        <v>452</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+        <v>453</v>
+      </c>
+      <c r="K6" s="6">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>68</v>
       </c>
@@ -6286,24 +6311,27 @@
       <c r="D7" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6" t="s">
+      <c r="E7" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="G7" s="6" t="s">
-        <v>54</v>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6">
+        <v>511</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>54</v>
+        <v>451</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>54</v>
+        <v>452</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+        <v>453</v>
+      </c>
+      <c r="K7" s="6">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>69</v>
       </c>
@@ -6313,26 +6341,26 @@
       <c r="C8" t="s">
         <v>51</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="F8" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="G8" s="3" t="s">
         <v>330</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="H8" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="I8" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="I8" s="3" t="s">
+      <c r="J8" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="J8" s="3" t="s">
+      <c r="K8" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>70</v>
       </c>
@@ -6342,26 +6370,26 @@
       <c r="C9" t="s">
         <v>51</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="F9" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="G9" s="3" t="s">
         <v>330</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="H9" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="I9" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="I9" s="3" t="s">
+      <c r="J9" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="J9" s="3" t="s">
+      <c r="K9" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>71</v>
       </c>
@@ -6371,26 +6399,26 @@
       <c r="C10" t="s">
         <v>51</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="F10" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="G10" s="3" t="s">
         <v>330</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="H10" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="I10" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="I10" s="3" t="s">
+      <c r="J10" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="J10" s="3" t="s">
+      <c r="K10" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>72</v>
       </c>
@@ -6400,26 +6428,26 @@
       <c r="C11" t="s">
         <v>51</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="F11" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="G11" s="3" t="s">
         <v>330</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="H11" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="H11" s="3" t="s">
+      <c r="I11" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="I11" s="3" t="s">
+      <c r="J11" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="J11" s="3" t="s">
+      <c r="K11" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>73</v>
       </c>
@@ -6429,26 +6457,26 @@
       <c r="C12" t="s">
         <v>51</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="F12" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="G12" s="3" t="s">
         <v>330</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="H12" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="H12" s="3" t="s">
+      <c r="I12" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="I12" s="3" t="s">
+      <c r="J12" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="J12" s="3" t="s">
+      <c r="K12" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>74</v>
       </c>
@@ -6458,26 +6486,26 @@
       <c r="C13" t="s">
         <v>51</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="F13" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="G13" s="3" t="s">
         <v>330</v>
       </c>
-      <c r="G13" s="3" t="s">
+      <c r="H13" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="H13" s="3" t="s">
+      <c r="I13" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="I13" s="3" t="s">
+      <c r="J13" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="J13" s="3" t="s">
+      <c r="K13" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>75</v>
       </c>
@@ -6487,26 +6515,26 @@
       <c r="C14" t="s">
         <v>51</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="F14" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="G14" s="3" t="s">
         <v>330</v>
       </c>
-      <c r="G14" s="3" t="s">
+      <c r="H14" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="H14" s="3" t="s">
+      <c r="I14" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="I14" s="3" t="s">
+      <c r="J14" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="J14" s="3" t="s">
+      <c r="K14" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>76</v>
       </c>
@@ -6516,26 +6544,26 @@
       <c r="C15" t="s">
         <v>51</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="F15" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="G15" s="3" t="s">
         <v>330</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="H15" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="H15" s="3" t="s">
+      <c r="I15" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="I15" s="3" t="s">
+      <c r="J15" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="J15" s="3" t="s">
+      <c r="K15" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>77</v>
       </c>
@@ -6545,26 +6573,26 @@
       <c r="C16" t="s">
         <v>51</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="F16" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="G16" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="G16" s="3" t="s">
+      <c r="H16" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="H16" s="3" t="s">
+      <c r="I16" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="I16" s="3" t="s">
+      <c r="J16" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="J16" s="3" t="s">
+      <c r="K16" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>78</v>
       </c>
@@ -6574,29 +6602,29 @@
       <c r="C17" t="s">
         <v>51</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="F17" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="G17" s="3" t="s">
         <v>330</v>
       </c>
-      <c r="G17" s="3" t="s">
+      <c r="H17" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="H17" s="3" t="s">
+      <c r="I17" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="I17" s="3" t="s">
+      <c r="J17" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="J17" s="3" t="s">
+      <c r="K17" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="K17" s="3" t="s">
+      <c r="L17" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>79</v>
       </c>
@@ -6606,29 +6634,29 @@
       <c r="C18" t="s">
         <v>51</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="F18" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="F18" s="3" t="s">
+      <c r="G18" s="3" t="s">
         <v>330</v>
       </c>
-      <c r="G18" s="3" t="s">
+      <c r="H18" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="H18" s="3" t="s">
+      <c r="I18" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="I18" s="3" t="s">
+      <c r="J18" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="J18" s="3" t="s">
+      <c r="K18" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="K18" s="3" t="s">
+      <c r="L18" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>80</v>
       </c>
@@ -6638,29 +6666,29 @@
       <c r="C19" t="s">
         <v>51</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="F19" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="F19" s="3" t="s">
+      <c r="G19" s="3" t="s">
         <v>330</v>
       </c>
-      <c r="G19" s="3" t="s">
+      <c r="H19" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="H19" s="3" t="s">
+      <c r="I19" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="I19" s="3" t="s">
+      <c r="J19" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="J19" s="3" t="s">
+      <c r="K19" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="K19" s="3" t="s">
+      <c r="L19" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>81</v>
       </c>
@@ -6670,29 +6698,29 @@
       <c r="C20" t="s">
         <v>51</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="F20" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="G20" s="3" t="s">
         <v>330</v>
       </c>
-      <c r="G20" s="3" t="s">
+      <c r="H20" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="H20" s="3" t="s">
+      <c r="I20" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="I20" s="3" t="s">
+      <c r="J20" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="J20" s="3" t="s">
+      <c r="K20" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="K20" s="3" t="s">
+      <c r="L20" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>82</v>
       </c>
@@ -6702,29 +6730,29 @@
       <c r="C21" t="s">
         <v>51</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="F21" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="F21" s="3" t="s">
+      <c r="G21" s="3" t="s">
         <v>330</v>
       </c>
-      <c r="G21" s="3" t="s">
+      <c r="H21" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="H21" s="3" t="s">
+      <c r="I21" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="I21" s="3" t="s">
+      <c r="J21" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="J21" s="3" t="s">
+      <c r="K21" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="K21" s="3" t="s">
+      <c r="L21" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>83</v>
       </c>
@@ -6734,29 +6762,29 @@
       <c r="C22" t="s">
         <v>51</v>
       </c>
-      <c r="E22" s="3" t="s">
+      <c r="F22" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="F22" s="3" t="s">
+      <c r="G22" s="3" t="s">
         <v>330</v>
       </c>
-      <c r="G22" s="3" t="s">
+      <c r="H22" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="H22" s="3" t="s">
+      <c r="I22" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="I22" s="3" t="s">
+      <c r="J22" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="J22" s="3" t="s">
+      <c r="K22" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="K22" s="3" t="s">
+      <c r="L22" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>84</v>
       </c>
@@ -6766,29 +6794,29 @@
       <c r="C23" t="s">
         <v>66</v>
       </c>
-      <c r="E23" s="3" t="s">
-        <v>67</v>
-      </c>
       <c r="F23" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G23" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="G23" s="3" t="s">
+      <c r="H23" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="H23" s="3" t="s">
+      <c r="I23" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="I23" s="3" t="s">
+      <c r="J23" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="J23" s="3" t="s">
+      <c r="K23" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="K23" s="3" t="s">
+      <c r="L23" s="3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>85</v>
       </c>
@@ -6798,29 +6826,29 @@
       <c r="C24" t="s">
         <v>51</v>
       </c>
-      <c r="E24" s="3" t="s">
-        <v>67</v>
-      </c>
       <c r="F24" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G24" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="G24" s="3" t="s">
+      <c r="H24" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="H24" s="3" t="s">
+      <c r="I24" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="I24" s="3" t="s">
+      <c r="J24" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="J24" s="3" t="s">
+      <c r="K24" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="K24" s="3" t="s">
+      <c r="L24" s="3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>86</v>
       </c>
@@ -6830,29 +6858,29 @@
       <c r="C25" t="s">
         <v>66</v>
       </c>
-      <c r="E25" s="3" t="s">
-        <v>67</v>
-      </c>
       <c r="F25" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G25" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="G25" s="3" t="s">
+      <c r="H25" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="H25" s="3" t="s">
+      <c r="I25" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="I25" s="3" t="s">
+      <c r="J25" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="J25" s="3" t="s">
+      <c r="K25" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="K25" s="3" t="s">
+      <c r="L25" s="3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>87</v>
       </c>
@@ -6862,29 +6890,29 @@
       <c r="C26" t="s">
         <v>66</v>
       </c>
-      <c r="E26" s="3" t="s">
-        <v>67</v>
-      </c>
       <c r="F26" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G26" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="G26" s="3" t="s">
+      <c r="H26" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="H26" s="3" t="s">
+      <c r="I26" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="I26" s="3" t="s">
+      <c r="J26" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="J26" s="3" t="s">
+      <c r="K26" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="K26" s="3" t="s">
+      <c r="L26" s="3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>88</v>
       </c>
@@ -6894,29 +6922,29 @@
       <c r="C27" t="s">
         <v>66</v>
       </c>
-      <c r="E27" s="3" t="s">
-        <v>67</v>
-      </c>
       <c r="F27" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G27" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="G27" s="3" t="s">
+      <c r="H27" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="H27" s="3" t="s">
+      <c r="I27" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="I27" s="3" t="s">
+      <c r="J27" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="J27" s="3" t="s">
+      <c r="K27" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="K27" s="3" t="s">
+      <c r="L27" s="3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>89</v>
       </c>
@@ -6926,29 +6954,29 @@
       <c r="C28" t="s">
         <v>66</v>
       </c>
-      <c r="E28" s="3" t="s">
-        <v>67</v>
-      </c>
       <c r="F28" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G28" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="G28" s="3" t="s">
+      <c r="H28" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="H28" s="3" t="s">
+      <c r="I28" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="I28" s="3" t="s">
+      <c r="J28" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="J28" s="3" t="s">
+      <c r="K28" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="K28" s="3" t="s">
+      <c r="L28" s="3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>90</v>
       </c>
@@ -6958,29 +6986,29 @@
       <c r="C29" t="s">
         <v>66</v>
       </c>
-      <c r="E29" s="3" t="s">
-        <v>67</v>
-      </c>
       <c r="F29" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G29" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="G29" s="3" t="s">
+      <c r="H29" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="H29" s="3" t="s">
+      <c r="I29" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="I29" s="3" t="s">
+      <c r="J29" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="J29" s="3" t="s">
+      <c r="K29" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="K29" s="3" t="s">
+      <c r="L29" s="3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>91</v>
       </c>
@@ -6990,29 +7018,29 @@
       <c r="C30" t="s">
         <v>66</v>
       </c>
-      <c r="E30" s="3" t="s">
-        <v>67</v>
-      </c>
       <c r="F30" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G30" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="G30" s="3" t="s">
+      <c r="H30" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="H30" s="3" t="s">
+      <c r="I30" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="I30" s="3" t="s">
+      <c r="J30" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="J30" s="3" t="s">
+      <c r="K30" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="K30" s="3" t="s">
+      <c r="L30" s="3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>92</v>
       </c>
@@ -7022,29 +7050,29 @@
       <c r="C31" t="s">
         <v>66</v>
       </c>
-      <c r="E31" s="3" t="s">
-        <v>67</v>
-      </c>
       <c r="F31" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G31" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="G31" s="3" t="s">
+      <c r="H31" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="H31" s="3" t="s">
+      <c r="I31" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="I31" s="3" t="s">
+      <c r="J31" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="J31" s="3" t="s">
+      <c r="K31" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="K31" s="3" t="s">
+      <c r="L31" s="3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>93</v>
       </c>
@@ -7054,29 +7082,29 @@
       <c r="C32" t="s">
         <v>66</v>
       </c>
-      <c r="E32" s="3" t="s">
-        <v>67</v>
-      </c>
       <c r="F32" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G32" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="G32" s="3" t="s">
+      <c r="H32" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="H32" s="3" t="s">
+      <c r="I32" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="I32" s="3" t="s">
+      <c r="J32" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="J32" s="3" t="s">
+      <c r="K32" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="K32" s="3" t="s">
+      <c r="L32" s="3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>94</v>
       </c>
@@ -7086,29 +7114,29 @@
       <c r="C33" t="s">
         <v>66</v>
       </c>
-      <c r="E33" s="3" t="s">
-        <v>67</v>
-      </c>
       <c r="F33" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G33" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="G33" s="3" t="s">
+      <c r="H33" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="H33" s="3" t="s">
+      <c r="I33" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="I33" s="3" t="s">
+      <c r="J33" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="J33" s="3" t="s">
+      <c r="K33" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="K33" s="3" t="s">
+      <c r="L33" s="3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>95</v>
       </c>
@@ -7118,25 +7146,25 @@
       <c r="C34" t="s">
         <v>66</v>
       </c>
-      <c r="E34" s="3" t="s">
-        <v>67</v>
-      </c>
       <c r="F34" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G34" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="G34" s="3" t="s">
+      <c r="H34" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="H34" s="3" t="s">
+      <c r="I34" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="I34" s="3" t="s">
+      <c r="J34" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="J34" s="3" t="s">
+      <c r="K34" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="K34" s="3" t="s">
+      <c r="L34" s="3" t="s">
         <v>74</v>
       </c>
     </row>
@@ -7173,10 +7201,10 @@
         <v>35</v>
       </c>
       <c r="E1" t="s">
+        <v>459</v>
+      </c>
+      <c r="F1" t="s">
         <v>460</v>
-      </c>
-      <c r="F1" t="s">
-        <v>461</v>
       </c>
       <c r="G1" t="s">
         <v>350</v>
@@ -57086,7 +57114,7 @@
   <dimension ref="A1:T40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD13"/>
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -57380,7 +57408,7 @@
         <v>63</v>
       </c>
       <c r="B8" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>315</v>
@@ -57412,7 +57440,7 @@
         <v>64</v>
       </c>
       <c r="B9" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>315</v>
@@ -57444,7 +57472,7 @@
         <v>65</v>
       </c>
       <c r="B10" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>315</v>
@@ -57476,7 +57504,7 @@
         <v>66</v>
       </c>
       <c r="B11" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>315</v>
@@ -57508,7 +57536,7 @@
         <v>67</v>
       </c>
       <c r="B12" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>315</v>
@@ -57540,7 +57568,7 @@
         <v>68</v>
       </c>
       <c r="B13" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>315</v>
@@ -57572,7 +57600,7 @@
         <v>69</v>
       </c>
       <c r="B14" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>315</v>
@@ -57610,7 +57638,7 @@
         <v>70</v>
       </c>
       <c r="B15" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>315</v>
@@ -57660,7 +57688,7 @@
         <v>71</v>
       </c>
       <c r="B16" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>315</v>
@@ -57710,7 +57738,7 @@
         <v>72</v>
       </c>
       <c r="B17" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>315</v>
@@ -57760,7 +57788,7 @@
         <v>73</v>
       </c>
       <c r="B18" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>315</v>
@@ -57810,7 +57838,7 @@
         <v>74</v>
       </c>
       <c r="B19" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>315</v>
@@ -57863,7 +57891,7 @@
         <v>75</v>
       </c>
       <c r="B20" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>315</v>
@@ -57916,7 +57944,7 @@
         <v>76</v>
       </c>
       <c r="B21" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>315</v>
@@ -57969,7 +57997,7 @@
         <v>77</v>
       </c>
       <c r="B22" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>315</v>
@@ -58022,7 +58050,7 @@
         <v>78</v>
       </c>
       <c r="B23" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>315</v>
@@ -58075,7 +58103,7 @@
         <v>79</v>
       </c>
       <c r="B24" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>315</v>
@@ -58128,7 +58156,7 @@
         <v>80</v>
       </c>
       <c r="B25" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>315</v>
@@ -58181,7 +58209,7 @@
         <v>81</v>
       </c>
       <c r="B26" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>315</v>
@@ -58234,7 +58262,7 @@
         <v>82</v>
       </c>
       <c r="B27" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>315</v>
@@ -58287,7 +58315,7 @@
         <v>83</v>
       </c>
       <c r="B28" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>315</v>
@@ -58340,7 +58368,7 @@
         <v>84</v>
       </c>
       <c r="B29" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>321</v>
@@ -58399,7 +58427,7 @@
         <v>85</v>
       </c>
       <c r="B30" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>321</v>
@@ -58458,7 +58486,7 @@
         <v>86</v>
       </c>
       <c r="B31" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>321</v>
@@ -58517,7 +58545,7 @@
         <v>87</v>
       </c>
       <c r="B32" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>321</v>
@@ -58576,7 +58604,7 @@
         <v>88</v>
       </c>
       <c r="B33" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>321</v>
@@ -58635,7 +58663,7 @@
         <v>89</v>
       </c>
       <c r="B34" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>321</v>
@@ -58694,7 +58722,7 @@
         <v>90</v>
       </c>
       <c r="B35" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>321</v>
@@ -58753,7 +58781,7 @@
         <v>91</v>
       </c>
       <c r="B36" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>321</v>
@@ -58812,7 +58840,7 @@
         <v>92</v>
       </c>
       <c r="B37" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>321</v>
@@ -58871,7 +58899,7 @@
         <v>93</v>
       </c>
       <c r="B38" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>321</v>
@@ -58930,7 +58958,7 @@
         <v>94</v>
       </c>
       <c r="B39" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>321</v>
@@ -58989,7 +59017,7 @@
         <v>95</v>
       </c>
       <c r="B40" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>321</v>
@@ -59052,7 +59080,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T40"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -59345,7 +59375,7 @@
         <v>63</v>
       </c>
       <c r="B8" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>316</v>
@@ -59377,7 +59407,7 @@
         <v>64</v>
       </c>
       <c r="B9" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>316</v>
@@ -59409,7 +59439,7 @@
         <v>65</v>
       </c>
       <c r="B10" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>316</v>
@@ -59441,7 +59471,7 @@
         <v>66</v>
       </c>
       <c r="B11" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>316</v>
@@ -59473,7 +59503,7 @@
         <v>67</v>
       </c>
       <c r="B12" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>316</v>
@@ -59505,7 +59535,7 @@
         <v>68</v>
       </c>
       <c r="B13" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>316</v>
@@ -59537,7 +59567,7 @@
         <v>69</v>
       </c>
       <c r="B14" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>315</v>
@@ -59587,7 +59617,7 @@
         <v>70</v>
       </c>
       <c r="B15" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>315</v>
@@ -59637,7 +59667,7 @@
         <v>71</v>
       </c>
       <c r="B16" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>315</v>
@@ -59687,7 +59717,7 @@
         <v>72</v>
       </c>
       <c r="B17" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>315</v>
@@ -59737,7 +59767,7 @@
         <v>73</v>
       </c>
       <c r="B18" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>315</v>
@@ -59787,7 +59817,7 @@
         <v>74</v>
       </c>
       <c r="B19" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>315</v>
@@ -59840,7 +59870,7 @@
         <v>75</v>
       </c>
       <c r="B20" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>315</v>
@@ -59893,7 +59923,7 @@
         <v>76</v>
       </c>
       <c r="B21" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>315</v>
@@ -59946,7 +59976,7 @@
         <v>77</v>
       </c>
       <c r="B22" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>315</v>
@@ -59999,7 +60029,7 @@
         <v>78</v>
       </c>
       <c r="B23" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>315</v>
@@ -60052,7 +60082,7 @@
         <v>79</v>
       </c>
       <c r="B24" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>315</v>
@@ -60105,7 +60135,7 @@
         <v>80</v>
       </c>
       <c r="B25" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>315</v>
@@ -60158,7 +60188,7 @@
         <v>81</v>
       </c>
       <c r="B26" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>315</v>
@@ -60211,7 +60241,7 @@
         <v>82</v>
       </c>
       <c r="B27" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>315</v>
@@ -60264,7 +60294,7 @@
         <v>83</v>
       </c>
       <c r="B28" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>315</v>
@@ -60317,7 +60347,7 @@
         <v>84</v>
       </c>
       <c r="B29" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>321</v>
@@ -60376,7 +60406,7 @@
         <v>85</v>
       </c>
       <c r="B30" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>321</v>
@@ -60435,7 +60465,7 @@
         <v>86</v>
       </c>
       <c r="B31" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>321</v>
@@ -60494,7 +60524,7 @@
         <v>87</v>
       </c>
       <c r="B32" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>321</v>
@@ -60553,7 +60583,7 @@
         <v>88</v>
       </c>
       <c r="B33" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>321</v>
@@ -60612,7 +60642,7 @@
         <v>89</v>
       </c>
       <c r="B34" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>321</v>
@@ -60671,7 +60701,7 @@
         <v>90</v>
       </c>
       <c r="B35" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>321</v>
@@ -60730,7 +60760,7 @@
         <v>91</v>
       </c>
       <c r="B36" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>321</v>
@@ -60789,7 +60819,7 @@
         <v>92</v>
       </c>
       <c r="B37" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>321</v>
@@ -60848,7 +60878,7 @@
         <v>93</v>
       </c>
       <c r="B38" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>321</v>
@@ -60907,7 +60937,7 @@
         <v>94</v>
       </c>
       <c r="B39" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>321</v>
@@ -60966,7 +60996,7 @@
         <v>95</v>
       </c>
       <c r="B40" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>321</v>

</xml_diff>

<commit_message>
Improve Other Income data
</commit_message>
<xml_diff>
--- a/Data/MetaData.xlsx
+++ b/Data/MetaData.xlsx
@@ -6081,7 +6081,7 @@
   <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4:E7"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6345,19 +6345,19 @@
         <v>52</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>330</v>
+        <v>53</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -6374,19 +6374,19 @@
         <v>52</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>330</v>
+        <v>53</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -6403,19 +6403,19 @@
         <v>52</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>330</v>
+        <v>53</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -6432,19 +6432,19 @@
         <v>52</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>330</v>
+        <v>53</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -6461,19 +6461,19 @@
         <v>52</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>330</v>
+        <v>53</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -6490,19 +6490,19 @@
         <v>52</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>330</v>
+        <v>53</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -6519,19 +6519,19 @@
         <v>52</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>330</v>
+        <v>53</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -6548,19 +6548,19 @@
         <v>52</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>330</v>
+        <v>53</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -6606,22 +6606,22 @@
         <v>52</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>330</v>
+        <v>53</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="L17" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -6638,22 +6638,22 @@
         <v>52</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>330</v>
+        <v>53</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="L18" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -6670,22 +6670,22 @@
         <v>52</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>330</v>
+        <v>53</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="L19" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -6702,22 +6702,22 @@
         <v>52</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>330</v>
+        <v>53</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="K20" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="L20" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -6734,22 +6734,22 @@
         <v>52</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>330</v>
+        <v>53</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="K21" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="L21" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -6766,22 +6766,22 @@
         <v>52</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>330</v>
+        <v>53</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="L22" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Edit files (at cafe)
</commit_message>
<xml_diff>
--- a/Data/MetaData.xlsx
+++ b/Data/MetaData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17100" windowHeight="6600" tabRatio="544" firstSheet="35" activeTab="38"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17100" windowHeight="6600" tabRatio="544" firstSheet="48" activeTab="51"/>
   </bookViews>
   <sheets>
     <sheet name="CompressedFileNames" sheetId="1" r:id="rId1"/>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13226" uniqueCount="490">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13226" uniqueCount="472">
   <si>
     <t>Year</t>
   </si>
@@ -1258,64 +1258,7 @@
     <t>Cigar_Exp</t>
   </si>
   <si>
-    <t>GhandExpenditure</t>
-  </si>
-  <si>
-    <t>HoboobatExpenditure</t>
-  </si>
-  <si>
-    <t>RoghanExpenditure</t>
-  </si>
-  <si>
-    <t>BerenjExpenditure</t>
-  </si>
-  <si>
-    <t>NanExpenditure</t>
-  </si>
-  <si>
-    <t>GooshtExpenditure</t>
-  </si>
-  <si>
-    <t>MorghExpenditure</t>
-  </si>
-  <si>
-    <t>MahiExpenditure</t>
-  </si>
-  <si>
-    <t>ShirExpenditure</t>
-  </si>
-  <si>
-    <t>MastExpenditure</t>
-  </si>
-  <si>
-    <t>PanirExpenditure</t>
-  </si>
-  <si>
-    <t>TokhmemorghExpenditure</t>
-  </si>
-  <si>
-    <t>MiveExpenditure</t>
-  </si>
-  <si>
-    <t>SabziExpenditure</t>
-  </si>
-  <si>
     <t>95.rar</t>
-  </si>
-  <si>
-    <t>MakarooniExpenditure</t>
-  </si>
-  <si>
-    <t>SibzaminiExpenditure</t>
-  </si>
-  <si>
-    <t>ShiriniExpenditure</t>
-  </si>
-  <si>
-    <t>BiscuitExpenditure</t>
-  </si>
-  <si>
-    <t>KhoshkbarExpenditure</t>
   </si>
   <si>
     <t>Behdasht_Exp</t>
@@ -1541,6 +1484,9 @@
   </si>
   <si>
     <t>KCalories</t>
+  </si>
+  <si>
+    <t>Expenditure</t>
   </si>
 </sst>
 </file>
@@ -2687,7 +2633,7 @@
         <v>95</v>
       </c>
       <c r="B34" t="s">
-        <v>409</v>
+        <v>395</v>
       </c>
     </row>
   </sheetData>
@@ -2729,22 +2675,22 @@
         <v>47</v>
       </c>
       <c r="G1" t="s">
-        <v>433</v>
+        <v>414</v>
       </c>
       <c r="H1" t="s">
-        <v>432</v>
+        <v>413</v>
       </c>
       <c r="I1" t="s">
-        <v>434</v>
+        <v>415</v>
       </c>
       <c r="J1" t="s">
-        <v>465</v>
+        <v>446</v>
       </c>
       <c r="K1" t="s">
-        <v>428</v>
+        <v>409</v>
       </c>
       <c r="L1" t="s">
-        <v>429</v>
+        <v>410</v>
       </c>
       <c r="M1" t="s">
         <v>343</v>
@@ -2765,7 +2711,7 @@
         <v>348</v>
       </c>
       <c r="S1" t="s">
-        <v>463</v>
+        <v>444</v>
       </c>
     </row>
     <row r="2" spans="1:19">
@@ -4460,22 +4406,22 @@
         <v>47</v>
       </c>
       <c r="G1" t="s">
-        <v>433</v>
+        <v>414</v>
       </c>
       <c r="H1" t="s">
-        <v>432</v>
+        <v>413</v>
       </c>
       <c r="I1" t="s">
-        <v>434</v>
+        <v>415</v>
       </c>
       <c r="J1" t="s">
-        <v>465</v>
+        <v>446</v>
       </c>
       <c r="K1" t="s">
-        <v>428</v>
+        <v>409</v>
       </c>
       <c r="L1" t="s">
-        <v>429</v>
+        <v>410</v>
       </c>
       <c r="M1" t="s">
         <v>343</v>
@@ -4496,7 +4442,7 @@
         <v>348</v>
       </c>
       <c r="S1" t="s">
-        <v>464</v>
+        <v>445</v>
       </c>
     </row>
     <row r="2" spans="1:19">
@@ -6172,28 +6118,28 @@
         <v>76</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>466</v>
+        <v>447</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>35</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>467</v>
+        <v>448</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>454</v>
+        <v>435</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>455</v>
+        <v>436</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>456</v>
+        <v>437</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>457</v>
+        <v>438</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>458</v>
+        <v>439</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -6217,13 +6163,13 @@
         <v>511</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>451</v>
+        <v>432</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>452</v>
+        <v>433</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>453</v>
+        <v>434</v>
       </c>
       <c r="K2" s="6">
         <v>521</v>
@@ -6250,13 +6196,13 @@
         <v>511</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>451</v>
+        <v>432</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>452</v>
+        <v>433</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>453</v>
+        <v>434</v>
       </c>
       <c r="K3" s="6">
         <v>521</v>
@@ -6283,13 +6229,13 @@
         <v>511</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>451</v>
+        <v>432</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>452</v>
+        <v>433</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>453</v>
+        <v>434</v>
       </c>
       <c r="K4" s="6">
         <v>521</v>
@@ -6316,13 +6262,13 @@
         <v>511</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>451</v>
+        <v>432</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>452</v>
+        <v>433</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>453</v>
+        <v>434</v>
       </c>
       <c r="K5" s="6">
         <v>521</v>
@@ -6349,13 +6295,13 @@
         <v>511</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>451</v>
+        <v>432</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>452</v>
+        <v>433</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>453</v>
+        <v>434</v>
       </c>
       <c r="K6" s="6">
         <v>521</v>
@@ -6382,13 +6328,13 @@
         <v>511</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>451</v>
+        <v>432</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>452</v>
+        <v>433</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>453</v>
+        <v>434</v>
       </c>
       <c r="K7" s="6">
         <v>521</v>
@@ -7264,10 +7210,10 @@
         <v>35</v>
       </c>
       <c r="E1" t="s">
-        <v>459</v>
+        <v>440</v>
       </c>
       <c r="F1" t="s">
-        <v>460</v>
+        <v>441</v>
       </c>
       <c r="G1" t="s">
         <v>350</v>
@@ -9518,16 +9464,16 @@
         <v>286</v>
       </c>
       <c r="H1" t="s">
-        <v>416</v>
+        <v>397</v>
       </c>
       <c r="I1" t="s">
-        <v>425</v>
+        <v>406</v>
       </c>
       <c r="J1" t="s">
-        <v>417</v>
+        <v>398</v>
       </c>
       <c r="K1" t="s">
-        <v>421</v>
+        <v>402</v>
       </c>
     </row>
     <row r="2" spans="1:11">
@@ -9553,16 +9499,16 @@
         <v>275</v>
       </c>
       <c r="H2" t="s">
-        <v>418</v>
+        <v>399</v>
       </c>
       <c r="I2" t="s">
         <v>51</v>
       </c>
       <c r="J2" t="s">
-        <v>420</v>
+        <v>401</v>
       </c>
       <c r="K2" t="s">
-        <v>419</v>
+        <v>400</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -9588,16 +9534,16 @@
         <v>275</v>
       </c>
       <c r="H3" t="s">
-        <v>418</v>
+        <v>399</v>
       </c>
       <c r="I3" t="s">
         <v>51</v>
       </c>
       <c r="J3" t="s">
-        <v>423</v>
+        <v>404</v>
       </c>
       <c r="K3" t="s">
-        <v>422</v>
+        <v>403</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -9623,16 +9569,16 @@
         <v>275</v>
       </c>
       <c r="H4" t="s">
-        <v>418</v>
+        <v>399</v>
       </c>
       <c r="I4" t="s">
         <v>51</v>
       </c>
       <c r="J4" t="s">
-        <v>423</v>
+        <v>404</v>
       </c>
       <c r="K4" t="s">
-        <v>422</v>
+        <v>403</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -9658,16 +9604,16 @@
         <v>275</v>
       </c>
       <c r="H5" t="s">
-        <v>418</v>
+        <v>399</v>
       </c>
       <c r="I5" t="s">
         <v>51</v>
       </c>
       <c r="J5" t="s">
-        <v>420</v>
+        <v>401</v>
       </c>
       <c r="K5" t="s">
-        <v>419</v>
+        <v>400</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -9693,16 +9639,16 @@
         <v>275</v>
       </c>
       <c r="H6" t="s">
-        <v>418</v>
+        <v>399</v>
       </c>
       <c r="I6" t="s">
         <v>51</v>
       </c>
       <c r="J6" t="s">
-        <v>420</v>
+        <v>401</v>
       </c>
       <c r="K6" t="s">
-        <v>419</v>
+        <v>400</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -9728,16 +9674,16 @@
         <v>275</v>
       </c>
       <c r="H7" t="s">
-        <v>418</v>
+        <v>399</v>
       </c>
       <c r="I7" t="s">
         <v>51</v>
       </c>
       <c r="J7" t="s">
-        <v>420</v>
+        <v>401</v>
       </c>
       <c r="K7" t="s">
-        <v>419</v>
+        <v>400</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -9763,16 +9709,16 @@
         <v>289</v>
       </c>
       <c r="H8" t="s">
-        <v>418</v>
+        <v>399</v>
       </c>
       <c r="I8" t="s">
         <v>51</v>
       </c>
       <c r="J8" t="s">
-        <v>419</v>
+        <v>400</v>
       </c>
       <c r="K8" t="s">
-        <v>424</v>
+        <v>405</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -9798,16 +9744,16 @@
         <v>285</v>
       </c>
       <c r="H9" t="s">
-        <v>418</v>
+        <v>399</v>
       </c>
       <c r="I9" t="s">
         <v>51</v>
       </c>
       <c r="J9" t="s">
-        <v>419</v>
+        <v>400</v>
       </c>
       <c r="K9" t="s">
-        <v>424</v>
+        <v>405</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -9833,16 +9779,16 @@
         <v>285</v>
       </c>
       <c r="H10" t="s">
-        <v>418</v>
+        <v>399</v>
       </c>
       <c r="I10" t="s">
         <v>51</v>
       </c>
       <c r="J10" t="s">
-        <v>419</v>
+        <v>400</v>
       </c>
       <c r="K10" t="s">
-        <v>424</v>
+        <v>405</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -9868,16 +9814,16 @@
         <v>285</v>
       </c>
       <c r="H11" t="s">
-        <v>418</v>
+        <v>399</v>
       </c>
       <c r="I11" t="s">
         <v>51</v>
       </c>
       <c r="J11" t="s">
-        <v>419</v>
+        <v>400</v>
       </c>
       <c r="K11" t="s">
-        <v>424</v>
+        <v>405</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -9903,16 +9849,16 @@
         <v>285</v>
       </c>
       <c r="H12" t="s">
-        <v>418</v>
+        <v>399</v>
       </c>
       <c r="I12" t="s">
         <v>51</v>
       </c>
       <c r="J12" t="s">
-        <v>419</v>
+        <v>400</v>
       </c>
       <c r="K12" t="s">
-        <v>424</v>
+        <v>405</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -9938,16 +9884,16 @@
         <v>275</v>
       </c>
       <c r="H13" t="s">
-        <v>418</v>
+        <v>399</v>
       </c>
       <c r="I13" t="s">
         <v>51</v>
       </c>
       <c r="J13" t="s">
-        <v>419</v>
+        <v>400</v>
       </c>
       <c r="K13" t="s">
-        <v>424</v>
+        <v>405</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -9973,16 +9919,16 @@
         <v>275</v>
       </c>
       <c r="H14" t="s">
-        <v>418</v>
+        <v>399</v>
       </c>
       <c r="I14" t="s">
         <v>51</v>
       </c>
       <c r="J14" t="s">
-        <v>419</v>
+        <v>400</v>
       </c>
       <c r="K14" t="s">
-        <v>424</v>
+        <v>405</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -10008,16 +9954,16 @@
         <v>275</v>
       </c>
       <c r="H15" t="s">
-        <v>418</v>
+        <v>399</v>
       </c>
       <c r="I15" t="s">
         <v>51</v>
       </c>
       <c r="J15" t="s">
-        <v>419</v>
+        <v>400</v>
       </c>
       <c r="K15" t="s">
-        <v>424</v>
+        <v>405</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -10043,16 +9989,16 @@
         <v>275</v>
       </c>
       <c r="H16" t="s">
-        <v>418</v>
+        <v>399</v>
       </c>
       <c r="I16" t="s">
         <v>51</v>
       </c>
       <c r="J16" t="s">
-        <v>419</v>
+        <v>400</v>
       </c>
       <c r="K16" t="s">
-        <v>424</v>
+        <v>405</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -10078,16 +10024,16 @@
         <v>275</v>
       </c>
       <c r="H17" t="s">
-        <v>418</v>
+        <v>399</v>
       </c>
       <c r="I17" t="s">
         <v>51</v>
       </c>
       <c r="J17" t="s">
-        <v>419</v>
+        <v>400</v>
       </c>
       <c r="K17" t="s">
-        <v>424</v>
+        <v>405</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -10113,16 +10059,16 @@
         <v>275</v>
       </c>
       <c r="H18" t="s">
-        <v>418</v>
+        <v>399</v>
       </c>
       <c r="I18" t="s">
         <v>51</v>
       </c>
       <c r="J18" t="s">
-        <v>419</v>
+        <v>400</v>
       </c>
       <c r="K18" t="s">
-        <v>424</v>
+        <v>405</v>
       </c>
     </row>
     <row r="19" spans="1:11">
@@ -10148,16 +10094,16 @@
         <v>275</v>
       </c>
       <c r="H19" t="s">
-        <v>418</v>
+        <v>399</v>
       </c>
       <c r="I19" t="s">
         <v>51</v>
       </c>
       <c r="J19" t="s">
-        <v>419</v>
+        <v>400</v>
       </c>
       <c r="K19" t="s">
-        <v>424</v>
+        <v>405</v>
       </c>
     </row>
     <row r="20" spans="1:11">
@@ -10183,16 +10129,16 @@
         <v>275</v>
       </c>
       <c r="H20" t="s">
-        <v>418</v>
+        <v>399</v>
       </c>
       <c r="I20" t="s">
         <v>51</v>
       </c>
       <c r="J20" t="s">
-        <v>419</v>
+        <v>400</v>
       </c>
       <c r="K20" t="s">
-        <v>424</v>
+        <v>405</v>
       </c>
     </row>
     <row r="21" spans="1:11">
@@ -10218,16 +10164,16 @@
         <v>275</v>
       </c>
       <c r="H21" t="s">
-        <v>418</v>
+        <v>399</v>
       </c>
       <c r="I21" t="s">
         <v>51</v>
       </c>
       <c r="J21" t="s">
-        <v>419</v>
+        <v>400</v>
       </c>
       <c r="K21" t="s">
-        <v>424</v>
+        <v>405</v>
       </c>
     </row>
     <row r="22" spans="1:11">
@@ -10253,7 +10199,7 @@
         <v>275</v>
       </c>
       <c r="H22" t="s">
-        <v>418</v>
+        <v>399</v>
       </c>
       <c r="I22" t="s">
         <v>66</v>
@@ -10288,7 +10234,7 @@
         <v>69</v>
       </c>
       <c r="H23" t="s">
-        <v>418</v>
+        <v>399</v>
       </c>
       <c r="I23" t="s">
         <v>66</v>
@@ -10323,7 +10269,7 @@
         <v>69</v>
       </c>
       <c r="H24" t="s">
-        <v>418</v>
+        <v>399</v>
       </c>
       <c r="I24" t="s">
         <v>51</v>
@@ -10358,7 +10304,7 @@
         <v>69</v>
       </c>
       <c r="H25" t="s">
-        <v>418</v>
+        <v>399</v>
       </c>
       <c r="I25" t="s">
         <v>66</v>
@@ -10393,7 +10339,7 @@
         <v>69</v>
       </c>
       <c r="H26" t="s">
-        <v>418</v>
+        <v>399</v>
       </c>
       <c r="I26" t="s">
         <v>66</v>
@@ -10428,7 +10374,7 @@
         <v>69</v>
       </c>
       <c r="H27" t="s">
-        <v>418</v>
+        <v>399</v>
       </c>
       <c r="I27" t="s">
         <v>66</v>
@@ -10463,7 +10409,7 @@
         <v>290</v>
       </c>
       <c r="H28" t="s">
-        <v>418</v>
+        <v>399</v>
       </c>
       <c r="I28" t="s">
         <v>66</v>
@@ -10498,7 +10444,7 @@
         <v>69</v>
       </c>
       <c r="H29" t="s">
-        <v>418</v>
+        <v>399</v>
       </c>
       <c r="I29" t="s">
         <v>66</v>
@@ -10533,7 +10479,7 @@
         <v>69</v>
       </c>
       <c r="H30" t="s">
-        <v>418</v>
+        <v>399</v>
       </c>
       <c r="I30" t="s">
         <v>66</v>
@@ -10568,7 +10514,7 @@
         <v>69</v>
       </c>
       <c r="H31" t="s">
-        <v>418</v>
+        <v>399</v>
       </c>
       <c r="I31" t="s">
         <v>66</v>
@@ -10603,7 +10549,7 @@
         <v>69</v>
       </c>
       <c r="H32" t="s">
-        <v>418</v>
+        <v>399</v>
       </c>
       <c r="I32" t="s">
         <v>66</v>
@@ -10638,7 +10584,7 @@
         <v>69</v>
       </c>
       <c r="H33" t="s">
-        <v>418</v>
+        <v>399</v>
       </c>
       <c r="I33" t="s">
         <v>66</v>
@@ -10673,7 +10619,7 @@
         <v>69</v>
       </c>
       <c r="H34" t="s">
-        <v>418</v>
+        <v>399</v>
       </c>
       <c r="I34" t="s">
         <v>66</v>
@@ -13519,7 +13465,7 @@
         <v>300</v>
       </c>
       <c r="H1" t="s">
-        <v>415</v>
+        <v>396</v>
       </c>
       <c r="I1" t="s">
         <v>335</v>
@@ -32760,8 +32706,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -32773,21 +32719,21 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>468</v>
+        <v>449</v>
       </c>
       <c r="B1" t="s">
-        <v>469</v>
+        <v>450</v>
       </c>
       <c r="C1" t="s">
-        <v>489</v>
+        <v>470</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>473</v>
+        <v>454</v>
       </c>
       <c r="B2" t="s">
-        <v>473</v>
+        <v>454</v>
       </c>
       <c r="C2">
         <v>1.2</v>
@@ -32795,10 +32741,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>487</v>
+        <v>468</v>
       </c>
       <c r="B3" t="s">
-        <v>487</v>
+        <v>468</v>
       </c>
       <c r="C3">
         <v>3</v>
@@ -32806,10 +32752,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>470</v>
+        <v>451</v>
       </c>
       <c r="B4" t="s">
-        <v>470</v>
+        <v>451</v>
       </c>
       <c r="C4">
         <v>4</v>
@@ -32817,10 +32763,10 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>475</v>
+        <v>456</v>
       </c>
       <c r="B5" t="s">
-        <v>475</v>
+        <v>456</v>
       </c>
       <c r="C5">
         <v>2.5</v>
@@ -32828,10 +32774,10 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>471</v>
+        <v>452</v>
       </c>
       <c r="B6" t="s">
-        <v>471</v>
+        <v>452</v>
       </c>
       <c r="C6">
         <v>3</v>
@@ -32839,10 +32785,10 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>488</v>
+        <v>469</v>
       </c>
       <c r="B7" t="s">
-        <v>488</v>
+        <v>469</v>
       </c>
       <c r="C7">
         <v>5</v>
@@ -32850,10 +32796,10 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>477</v>
+        <v>458</v>
       </c>
       <c r="B8" t="s">
-        <v>477</v>
+        <v>458</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -32861,10 +32807,10 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>484</v>
+        <v>465</v>
       </c>
       <c r="B9" t="s">
-        <v>484</v>
+        <v>465</v>
       </c>
       <c r="C9">
         <v>3.6</v>
@@ -32872,10 +32818,10 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>479</v>
+        <v>460</v>
       </c>
       <c r="B10" t="s">
-        <v>479</v>
+        <v>460</v>
       </c>
       <c r="C10">
         <v>1.5</v>
@@ -32883,10 +32829,10 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>482</v>
+        <v>463</v>
       </c>
       <c r="B11" t="s">
-        <v>482</v>
+        <v>463</v>
       </c>
       <c r="C11">
         <v>0.5</v>
@@ -32894,10 +32840,10 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>476</v>
+        <v>457</v>
       </c>
       <c r="B12" t="s">
-        <v>476</v>
+        <v>457</v>
       </c>
       <c r="C12">
         <v>2</v>
@@ -32905,10 +32851,10 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>474</v>
+        <v>455</v>
       </c>
       <c r="B13" t="s">
-        <v>474</v>
+        <v>455</v>
       </c>
       <c r="C13">
         <v>2.5</v>
@@ -32916,10 +32862,10 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>480</v>
+        <v>461</v>
       </c>
       <c r="B14" t="s">
-        <v>480</v>
+        <v>461</v>
       </c>
       <c r="C14">
         <v>2.5</v>
@@ -32927,10 +32873,10 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>472</v>
+        <v>453</v>
       </c>
       <c r="B15" t="s">
-        <v>472</v>
+        <v>453</v>
       </c>
       <c r="C15">
         <v>8</v>
@@ -32938,10 +32884,10 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>483</v>
+        <v>464</v>
       </c>
       <c r="B16" t="s">
-        <v>483</v>
+        <v>464</v>
       </c>
       <c r="C16">
         <v>0.5</v>
@@ -32949,10 +32895,10 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>478</v>
+        <v>459</v>
       </c>
       <c r="B17" t="s">
-        <v>478</v>
+        <v>459</v>
       </c>
       <c r="C17">
         <v>2.5</v>
@@ -32960,10 +32906,10 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>486</v>
+        <v>467</v>
       </c>
       <c r="B18" t="s">
-        <v>486</v>
+        <v>467</v>
       </c>
       <c r="C18">
         <v>3.5</v>
@@ -32971,10 +32917,10 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>485</v>
+        <v>466</v>
       </c>
       <c r="B19" t="s">
-        <v>485</v>
+        <v>466</v>
       </c>
       <c r="C19">
         <v>0.9</v>
@@ -32982,10 +32928,10 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>481</v>
+        <v>462</v>
       </c>
       <c r="B20" t="s">
-        <v>481</v>
+        <v>462</v>
       </c>
       <c r="C20">
         <v>1.4</v>
@@ -34236,7 +34182,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L34"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -34278,7 +34226,7 @@
         <v>303</v>
       </c>
       <c r="L1" t="s">
-        <v>395</v>
+        <v>471</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -35376,7 +35324,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L34"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
@@ -35415,7 +35365,7 @@
         <v>303</v>
       </c>
       <c r="L1" t="s">
-        <v>396</v>
+        <v>471</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -36513,7 +36463,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L34"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
@@ -36552,7 +36504,7 @@
         <v>303</v>
       </c>
       <c r="L1" t="s">
-        <v>397</v>
+        <v>471</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -37650,7 +37602,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L34"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
@@ -37689,7 +37643,7 @@
         <v>303</v>
       </c>
       <c r="L1" t="s">
-        <v>398</v>
+        <v>471</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -38787,7 +38741,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L34"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
@@ -38826,7 +38782,7 @@
         <v>303</v>
       </c>
       <c r="L1" t="s">
-        <v>399</v>
+        <v>471</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -39924,7 +39880,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L34"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
@@ -39963,7 +39921,7 @@
         <v>303</v>
       </c>
       <c r="L1" t="s">
-        <v>400</v>
+        <v>471</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -41061,7 +41019,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L34"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
@@ -41100,7 +41060,7 @@
         <v>303</v>
       </c>
       <c r="L1" t="s">
-        <v>401</v>
+        <v>471</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -42198,7 +42158,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L34"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
@@ -42237,7 +42199,7 @@
         <v>303</v>
       </c>
       <c r="L1" t="s">
-        <v>402</v>
+        <v>471</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -43335,7 +43297,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L34"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
@@ -43374,7 +43338,7 @@
         <v>303</v>
       </c>
       <c r="L1" t="s">
-        <v>403</v>
+        <v>471</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -44472,7 +44436,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L34"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
@@ -44511,7 +44477,7 @@
         <v>303</v>
       </c>
       <c r="L1" t="s">
-        <v>404</v>
+        <v>471</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -45735,7 +45701,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L34"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
@@ -45774,7 +45742,7 @@
         <v>303</v>
       </c>
       <c r="L1" t="s">
-        <v>405</v>
+        <v>471</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -46872,7 +46840,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L34"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -46914,7 +46884,7 @@
         <v>303</v>
       </c>
       <c r="L1" t="s">
-        <v>406</v>
+        <v>471</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -48012,8 +47982,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L34"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G39" sqref="G39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -48053,7 +48023,7 @@
         <v>303</v>
       </c>
       <c r="L1" t="s">
-        <v>407</v>
+        <v>471</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -49151,7 +49121,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L34"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
@@ -49190,7 +49162,7 @@
         <v>303</v>
       </c>
       <c r="L1" t="s">
-        <v>408</v>
+        <v>471</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -50288,7 +50260,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L34"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
@@ -50327,7 +50301,7 @@
         <v>303</v>
       </c>
       <c r="L1" t="s">
-        <v>410</v>
+        <v>471</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -51425,7 +51399,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L34"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
@@ -51464,7 +51440,7 @@
         <v>303</v>
       </c>
       <c r="L1" t="s">
-        <v>411</v>
+        <v>471</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -52562,7 +52538,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L34"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
@@ -52601,7 +52579,7 @@
         <v>303</v>
       </c>
       <c r="L1" t="s">
-        <v>412</v>
+        <v>471</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -53699,7 +53677,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L34"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
@@ -53738,7 +53718,7 @@
         <v>303</v>
       </c>
       <c r="L1" t="s">
-        <v>413</v>
+        <v>471</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -54836,7 +54816,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L34"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
@@ -54875,7 +54857,7 @@
         <v>303</v>
       </c>
       <c r="L1" t="s">
-        <v>414</v>
+        <v>471</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -56852,7 +56834,7 @@
         <v>63</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>430</v>
+        <v>411</v>
       </c>
       <c r="C2" t="s">
         <v>51</v>
@@ -56869,7 +56851,7 @@
         <v>64</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>430</v>
+        <v>411</v>
       </c>
       <c r="C3" t="s">
         <v>51</v>
@@ -56886,7 +56868,7 @@
         <v>65</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>430</v>
+        <v>411</v>
       </c>
       <c r="C4" t="s">
         <v>51</v>
@@ -56903,7 +56885,7 @@
         <v>66</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>430</v>
+        <v>411</v>
       </c>
       <c r="C5" t="s">
         <v>51</v>
@@ -56920,7 +56902,7 @@
         <v>67</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>430</v>
+        <v>411</v>
       </c>
       <c r="C6" t="s">
         <v>51</v>
@@ -56937,7 +56919,7 @@
         <v>68</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>430</v>
+        <v>411</v>
       </c>
       <c r="C7" t="s">
         <v>51</v>
@@ -56954,7 +56936,7 @@
         <v>69</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>430</v>
+        <v>411</v>
       </c>
       <c r="C8" t="s">
         <v>51</v>
@@ -56971,7 +56953,7 @@
         <v>70</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>430</v>
+        <v>411</v>
       </c>
       <c r="C9" t="s">
         <v>51</v>
@@ -56988,7 +56970,7 @@
         <v>71</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>430</v>
+        <v>411</v>
       </c>
       <c r="C10" t="s">
         <v>51</v>
@@ -57005,7 +56987,7 @@
         <v>72</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>430</v>
+        <v>411</v>
       </c>
       <c r="C11" t="s">
         <v>51</v>
@@ -57022,7 +57004,7 @@
         <v>73</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>430</v>
+        <v>411</v>
       </c>
       <c r="C12" t="s">
         <v>51</v>
@@ -57034,7 +57016,7 @@
         <v>59</v>
       </c>
       <c r="G12" t="s">
-        <v>431</v>
+        <v>412</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -57462,43 +57444,43 @@
         <v>47</v>
       </c>
       <c r="H1" t="s">
-        <v>427</v>
+        <v>408</v>
       </c>
       <c r="I1" t="s">
-        <v>426</v>
+        <v>407</v>
       </c>
       <c r="J1" t="s">
-        <v>432</v>
+        <v>413</v>
       </c>
       <c r="K1" t="s">
-        <v>428</v>
+        <v>409</v>
       </c>
       <c r="L1" t="s">
-        <v>429</v>
+        <v>410</v>
       </c>
       <c r="M1" t="s">
-        <v>435</v>
+        <v>416</v>
       </c>
       <c r="N1" t="s">
-        <v>436</v>
+        <v>417</v>
       </c>
       <c r="O1" t="s">
-        <v>437</v>
+        <v>418</v>
       </c>
       <c r="P1" t="s">
-        <v>438</v>
+        <v>419</v>
       </c>
       <c r="Q1" t="s">
-        <v>439</v>
+        <v>420</v>
       </c>
       <c r="R1" t="s">
-        <v>440</v>
+        <v>421</v>
       </c>
       <c r="S1" t="s">
-        <v>441</v>
+        <v>422</v>
       </c>
       <c r="T1" t="s">
-        <v>442</v>
+        <v>423</v>
       </c>
     </row>
     <row r="2" spans="1:20">
@@ -57716,7 +57698,7 @@
         <v>63</v>
       </c>
       <c r="B8" t="s">
-        <v>461</v>
+        <v>442</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>315</v>
@@ -57748,7 +57730,7 @@
         <v>64</v>
       </c>
       <c r="B9" t="s">
-        <v>461</v>
+        <v>442</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>315</v>
@@ -57780,7 +57762,7 @@
         <v>65</v>
       </c>
       <c r="B10" t="s">
-        <v>461</v>
+        <v>442</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>315</v>
@@ -57812,7 +57794,7 @@
         <v>66</v>
       </c>
       <c r="B11" t="s">
-        <v>461</v>
+        <v>442</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>315</v>
@@ -57844,7 +57826,7 @@
         <v>67</v>
       </c>
       <c r="B12" t="s">
-        <v>461</v>
+        <v>442</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>315</v>
@@ -57876,7 +57858,7 @@
         <v>68</v>
       </c>
       <c r="B13" t="s">
-        <v>461</v>
+        <v>442</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>315</v>
@@ -57908,7 +57890,7 @@
         <v>69</v>
       </c>
       <c r="B14" t="s">
-        <v>462</v>
+        <v>443</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>315</v>
@@ -57946,7 +57928,7 @@
         <v>70</v>
       </c>
       <c r="B15" t="s">
-        <v>462</v>
+        <v>443</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>315</v>
@@ -57996,7 +57978,7 @@
         <v>71</v>
       </c>
       <c r="B16" t="s">
-        <v>462</v>
+        <v>443</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>315</v>
@@ -58046,7 +58028,7 @@
         <v>72</v>
       </c>
       <c r="B17" t="s">
-        <v>462</v>
+        <v>443</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>315</v>
@@ -58096,7 +58078,7 @@
         <v>73</v>
       </c>
       <c r="B18" t="s">
-        <v>462</v>
+        <v>443</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>315</v>
@@ -58146,7 +58128,7 @@
         <v>74</v>
       </c>
       <c r="B19" t="s">
-        <v>462</v>
+        <v>443</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>315</v>
@@ -58199,7 +58181,7 @@
         <v>75</v>
       </c>
       <c r="B20" t="s">
-        <v>462</v>
+        <v>443</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>315</v>
@@ -58252,7 +58234,7 @@
         <v>76</v>
       </c>
       <c r="B21" t="s">
-        <v>462</v>
+        <v>443</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>315</v>
@@ -58305,7 +58287,7 @@
         <v>77</v>
       </c>
       <c r="B22" t="s">
-        <v>462</v>
+        <v>443</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>315</v>
@@ -58358,7 +58340,7 @@
         <v>78</v>
       </c>
       <c r="B23" t="s">
-        <v>462</v>
+        <v>443</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>315</v>
@@ -58411,7 +58393,7 @@
         <v>79</v>
       </c>
       <c r="B24" t="s">
-        <v>462</v>
+        <v>443</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>315</v>
@@ -58464,7 +58446,7 @@
         <v>80</v>
       </c>
       <c r="B25" t="s">
-        <v>462</v>
+        <v>443</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>315</v>
@@ -58517,7 +58499,7 @@
         <v>81</v>
       </c>
       <c r="B26" t="s">
-        <v>462</v>
+        <v>443</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>315</v>
@@ -58570,7 +58552,7 @@
         <v>82</v>
       </c>
       <c r="B27" t="s">
-        <v>462</v>
+        <v>443</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>315</v>
@@ -58623,7 +58605,7 @@
         <v>83</v>
       </c>
       <c r="B28" t="s">
-        <v>462</v>
+        <v>443</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>315</v>
@@ -58676,7 +58658,7 @@
         <v>84</v>
       </c>
       <c r="B29" t="s">
-        <v>462</v>
+        <v>443</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>321</v>
@@ -58735,7 +58717,7 @@
         <v>85</v>
       </c>
       <c r="B30" t="s">
-        <v>462</v>
+        <v>443</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>321</v>
@@ -58794,7 +58776,7 @@
         <v>86</v>
       </c>
       <c r="B31" t="s">
-        <v>462</v>
+        <v>443</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>321</v>
@@ -58853,7 +58835,7 @@
         <v>87</v>
       </c>
       <c r="B32" t="s">
-        <v>462</v>
+        <v>443</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>321</v>
@@ -58912,7 +58894,7 @@
         <v>88</v>
       </c>
       <c r="B33" t="s">
-        <v>462</v>
+        <v>443</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>321</v>
@@ -58971,7 +58953,7 @@
         <v>89</v>
       </c>
       <c r="B34" t="s">
-        <v>462</v>
+        <v>443</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>321</v>
@@ -59030,7 +59012,7 @@
         <v>90</v>
       </c>
       <c r="B35" t="s">
-        <v>462</v>
+        <v>443</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>321</v>
@@ -59089,7 +59071,7 @@
         <v>91</v>
       </c>
       <c r="B36" t="s">
-        <v>462</v>
+        <v>443</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>321</v>
@@ -59148,7 +59130,7 @@
         <v>92</v>
       </c>
       <c r="B37" t="s">
-        <v>462</v>
+        <v>443</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>321</v>
@@ -59207,7 +59189,7 @@
         <v>93</v>
       </c>
       <c r="B38" t="s">
-        <v>462</v>
+        <v>443</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>321</v>
@@ -59266,7 +59248,7 @@
         <v>94</v>
       </c>
       <c r="B39" t="s">
-        <v>462</v>
+        <v>443</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>321</v>
@@ -59325,7 +59307,7 @@
         <v>95</v>
       </c>
       <c r="B40" t="s">
-        <v>462</v>
+        <v>443</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>321</v>
@@ -59429,43 +59411,43 @@
         <v>47</v>
       </c>
       <c r="H1" t="s">
+        <v>408</v>
+      </c>
+      <c r="I1" t="s">
+        <v>407</v>
+      </c>
+      <c r="J1" t="s">
+        <v>413</v>
+      </c>
+      <c r="K1" t="s">
+        <v>409</v>
+      </c>
+      <c r="L1" t="s">
+        <v>410</v>
+      </c>
+      <c r="M1" t="s">
+        <v>424</v>
+      </c>
+      <c r="N1" t="s">
+        <v>425</v>
+      </c>
+      <c r="O1" t="s">
+        <v>426</v>
+      </c>
+      <c r="P1" t="s">
         <v>427</v>
       </c>
-      <c r="I1" t="s">
-        <v>426</v>
-      </c>
-      <c r="J1" t="s">
-        <v>432</v>
-      </c>
-      <c r="K1" t="s">
+      <c r="Q1" t="s">
         <v>428</v>
       </c>
-      <c r="L1" t="s">
+      <c r="R1" t="s">
         <v>429</v>
       </c>
-      <c r="M1" t="s">
-        <v>443</v>
-      </c>
-      <c r="N1" t="s">
-        <v>444</v>
-      </c>
-      <c r="O1" t="s">
-        <v>445</v>
-      </c>
-      <c r="P1" t="s">
-        <v>446</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>447</v>
-      </c>
-      <c r="R1" t="s">
-        <v>448</v>
-      </c>
       <c r="S1" t="s">
-        <v>449</v>
+        <v>430</v>
       </c>
       <c r="T1" t="s">
-        <v>450</v>
+        <v>431</v>
       </c>
     </row>
     <row r="2" spans="1:20">
@@ -59683,7 +59665,7 @@
         <v>63</v>
       </c>
       <c r="B8" t="s">
-        <v>461</v>
+        <v>442</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>316</v>
@@ -59715,7 +59697,7 @@
         <v>64</v>
       </c>
       <c r="B9" t="s">
-        <v>461</v>
+        <v>442</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>316</v>
@@ -59747,7 +59729,7 @@
         <v>65</v>
       </c>
       <c r="B10" t="s">
-        <v>461</v>
+        <v>442</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>316</v>
@@ -59779,7 +59761,7 @@
         <v>66</v>
       </c>
       <c r="B11" t="s">
-        <v>461</v>
+        <v>442</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>316</v>
@@ -59811,7 +59793,7 @@
         <v>67</v>
       </c>
       <c r="B12" t="s">
-        <v>461</v>
+        <v>442</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>316</v>
@@ -59843,7 +59825,7 @@
         <v>68</v>
       </c>
       <c r="B13" t="s">
-        <v>461</v>
+        <v>442</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>316</v>
@@ -59875,7 +59857,7 @@
         <v>69</v>
       </c>
       <c r="B14" t="s">
-        <v>462</v>
+        <v>443</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>315</v>
@@ -59925,7 +59907,7 @@
         <v>70</v>
       </c>
       <c r="B15" t="s">
-        <v>462</v>
+        <v>443</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>315</v>
@@ -59975,7 +59957,7 @@
         <v>71</v>
       </c>
       <c r="B16" t="s">
-        <v>462</v>
+        <v>443</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>315</v>
@@ -60025,7 +60007,7 @@
         <v>72</v>
       </c>
       <c r="B17" t="s">
-        <v>462</v>
+        <v>443</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>315</v>
@@ -60075,7 +60057,7 @@
         <v>73</v>
       </c>
       <c r="B18" t="s">
-        <v>462</v>
+        <v>443</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>315</v>
@@ -60125,7 +60107,7 @@
         <v>74</v>
       </c>
       <c r="B19" t="s">
-        <v>462</v>
+        <v>443</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>315</v>
@@ -60178,7 +60160,7 @@
         <v>75</v>
       </c>
       <c r="B20" t="s">
-        <v>462</v>
+        <v>443</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>315</v>
@@ -60231,7 +60213,7 @@
         <v>76</v>
       </c>
       <c r="B21" t="s">
-        <v>462</v>
+        <v>443</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>315</v>
@@ -60284,7 +60266,7 @@
         <v>77</v>
       </c>
       <c r="B22" t="s">
-        <v>462</v>
+        <v>443</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>315</v>
@@ -60337,7 +60319,7 @@
         <v>78</v>
       </c>
       <c r="B23" t="s">
-        <v>462</v>
+        <v>443</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>315</v>
@@ -60390,7 +60372,7 @@
         <v>79</v>
       </c>
       <c r="B24" t="s">
-        <v>462</v>
+        <v>443</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>315</v>
@@ -60443,7 +60425,7 @@
         <v>80</v>
       </c>
       <c r="B25" t="s">
-        <v>462</v>
+        <v>443</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>315</v>
@@ -60496,7 +60478,7 @@
         <v>81</v>
       </c>
       <c r="B26" t="s">
-        <v>462</v>
+        <v>443</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>315</v>
@@ -60549,7 +60531,7 @@
         <v>82</v>
       </c>
       <c r="B27" t="s">
-        <v>462</v>
+        <v>443</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>315</v>
@@ -60602,7 +60584,7 @@
         <v>83</v>
       </c>
       <c r="B28" t="s">
-        <v>462</v>
+        <v>443</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>315</v>
@@ -60655,7 +60637,7 @@
         <v>84</v>
       </c>
       <c r="B29" t="s">
-        <v>462</v>
+        <v>443</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>321</v>
@@ -60714,7 +60696,7 @@
         <v>85</v>
       </c>
       <c r="B30" t="s">
-        <v>462</v>
+        <v>443</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>321</v>
@@ -60773,7 +60755,7 @@
         <v>86</v>
       </c>
       <c r="B31" t="s">
-        <v>462</v>
+        <v>443</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>321</v>
@@ -60832,7 +60814,7 @@
         <v>87</v>
       </c>
       <c r="B32" t="s">
-        <v>462</v>
+        <v>443</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>321</v>
@@ -60891,7 +60873,7 @@
         <v>88</v>
       </c>
       <c r="B33" t="s">
-        <v>462</v>
+        <v>443</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>321</v>
@@ -60950,7 +60932,7 @@
         <v>89</v>
       </c>
       <c r="B34" t="s">
-        <v>462</v>
+        <v>443</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>321</v>
@@ -61009,7 +60991,7 @@
         <v>90</v>
       </c>
       <c r="B35" t="s">
-        <v>462</v>
+        <v>443</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>321</v>
@@ -61068,7 +61050,7 @@
         <v>91</v>
       </c>
       <c r="B36" t="s">
-        <v>462</v>
+        <v>443</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>321</v>
@@ -61127,7 +61109,7 @@
         <v>92</v>
       </c>
       <c r="B37" t="s">
-        <v>462</v>
+        <v>443</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>321</v>
@@ -61186,7 +61168,7 @@
         <v>93</v>
       </c>
       <c r="B38" t="s">
-        <v>462</v>
+        <v>443</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>321</v>
@@ -61245,7 +61227,7 @@
         <v>94</v>
       </c>
       <c r="B39" t="s">
-        <v>462</v>
+        <v>443</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>321</v>
@@ -61304,7 +61286,7 @@
         <v>95</v>
       </c>
       <c r="B40" t="s">
-        <v>462</v>
+        <v>443</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>321</v>

</xml_diff>

<commit_message>
Add codes to build TS 82-95
</commit_message>
<xml_diff>
--- a/Data/MetaData.xlsx
+++ b/Data/MetaData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17100" windowHeight="6600" tabRatio="544" firstSheet="37" activeTab="38"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17100" windowHeight="6600" tabRatio="544" firstSheet="26" activeTab="31"/>
   </bookViews>
   <sheets>
     <sheet name="CompressedFileNames" sheetId="1" r:id="rId1"/>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13220" uniqueCount="469">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13336" uniqueCount="471">
   <si>
     <t>Year</t>
   </si>
@@ -1479,6 +1479,12 @@
   <si>
     <t>Expenditure</t>
   </si>
+  <si>
+    <t>96.rar</t>
+  </si>
+  <si>
+    <t>P3</t>
+  </si>
 </sst>
 </file>
 
@@ -2338,7 +2344,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2346,9 +2352,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B34"/>
+  <dimension ref="A1:B35"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -2625,6 +2633,14 @@
       </c>
       <c r="B34" t="s">
         <v>395</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35">
+        <v>96</v>
+      </c>
+      <c r="B35" t="s">
+        <v>469</v>
       </c>
     </row>
   </sheetData>
@@ -7178,7 +7194,7 @@
   <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD4"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7490,9 +7506,11 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L34"/>
+  <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="L40" sqref="L40"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -8630,6 +8648,38 @@
         <v>72</v>
       </c>
     </row>
+    <row r="35" spans="1:12">
+      <c r="A35">
+        <v>96</v>
+      </c>
+      <c r="C35">
+        <v>11111</v>
+      </c>
+      <c r="D35">
+        <v>12218</v>
+      </c>
+      <c r="E35" t="s">
+        <v>66</v>
+      </c>
+      <c r="F35" t="s">
+        <v>67</v>
+      </c>
+      <c r="G35" t="s">
+        <v>277</v>
+      </c>
+      <c r="I35" t="s">
+        <v>68</v>
+      </c>
+      <c r="J35" t="s">
+        <v>69</v>
+      </c>
+      <c r="K35" t="s">
+        <v>70</v>
+      </c>
+      <c r="L35" t="s">
+        <v>72</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8639,7 +8689,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -9421,9 +9473,11 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K34"/>
+  <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -10622,6 +10676,41 @@
         <v>68</v>
       </c>
     </row>
+    <row r="35" spans="1:11">
+      <c r="A35">
+        <v>96</v>
+      </c>
+      <c r="B35" t="s">
+        <v>333</v>
+      </c>
+      <c r="C35">
+        <v>41111</v>
+      </c>
+      <c r="D35">
+        <v>42215</v>
+      </c>
+      <c r="E35" t="s">
+        <v>66</v>
+      </c>
+      <c r="F35" t="s">
+        <v>67</v>
+      </c>
+      <c r="G35" t="s">
+        <v>69</v>
+      </c>
+      <c r="H35" t="s">
+        <v>470</v>
+      </c>
+      <c r="I35" t="s">
+        <v>66</v>
+      </c>
+      <c r="J35" t="s">
+        <v>69</v>
+      </c>
+      <c r="K35" t="s">
+        <v>68</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10629,9 +10718,11 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E123"/>
+  <dimension ref="A1:E125"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A112" workbookViewId="0">
+      <selection activeCell="B128" sqref="B128"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -11560,932 +11651,949 @@
     </row>
     <row r="63" spans="1:5">
       <c r="A63">
-        <v>35</v>
+        <v>96</v>
       </c>
       <c r="B63" t="s">
-        <v>295</v>
-      </c>
-      <c r="C63">
-        <v>13078950</v>
+        <v>294</v>
       </c>
       <c r="E63" s="1"/>
     </row>
     <row r="64" spans="1:5">
       <c r="A64">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B64" t="s">
         <v>295</v>
       </c>
       <c r="C64">
-        <v>13351284</v>
+        <v>13078950</v>
       </c>
       <c r="E64" s="1"/>
     </row>
     <row r="65" spans="1:5">
       <c r="A65">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B65" t="s">
         <v>295</v>
       </c>
       <c r="C65">
-        <v>13628160</v>
+        <v>13351284</v>
       </c>
       <c r="E65" s="1"/>
     </row>
     <row r="66" spans="1:5">
       <c r="A66">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B66" t="s">
         <v>295</v>
       </c>
       <c r="C66">
-        <v>13909179</v>
+        <v>13628160</v>
       </c>
       <c r="E66" s="1"/>
     </row>
     <row r="67" spans="1:5">
       <c r="A67">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B67" t="s">
         <v>295</v>
       </c>
       <c r="C67">
-        <v>14194603.999999996</v>
+        <v>13909179</v>
       </c>
       <c r="E67" s="1"/>
     </row>
     <row r="68" spans="1:5">
       <c r="A68">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B68" t="s">
         <v>295</v>
       </c>
       <c r="C68">
-        <v>14484014.999999998</v>
+        <v>14194603.999999996</v>
       </c>
       <c r="E68" s="1"/>
     </row>
     <row r="69" spans="1:5">
       <c r="A69">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B69" t="s">
         <v>295</v>
       </c>
       <c r="C69">
-        <v>14777639.999999996</v>
+        <v>14484014.999999998</v>
       </c>
       <c r="E69" s="1"/>
     </row>
     <row r="70" spans="1:5">
       <c r="A70">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B70" t="s">
         <v>295</v>
       </c>
       <c r="C70">
-        <v>15075678.999999994</v>
+        <v>14777639.999999996</v>
       </c>
       <c r="E70" s="1"/>
     </row>
     <row r="71" spans="1:5">
       <c r="A71">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B71" t="s">
         <v>295</v>
       </c>
       <c r="C71">
-        <v>15377669.999999996</v>
+        <v>15075678.999999994</v>
       </c>
       <c r="E71" s="1"/>
     </row>
     <row r="72" spans="1:5">
       <c r="A72">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B72" t="s">
         <v>295</v>
       </c>
       <c r="C72">
-        <v>15683777.999999993</v>
+        <v>15377669.999999996</v>
       </c>
       <c r="E72" s="1"/>
     </row>
     <row r="73" spans="1:5">
       <c r="A73">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B73" t="s">
         <v>295</v>
       </c>
       <c r="C73">
-        <v>15989180</v>
+        <v>15683777.999999993</v>
       </c>
       <c r="E73" s="1"/>
     </row>
     <row r="74" spans="1:5">
       <c r="A74">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B74" t="s">
         <v>295</v>
       </c>
       <c r="C74">
-        <v>16184168</v>
+        <v>15989180</v>
       </c>
       <c r="E74" s="1"/>
     </row>
     <row r="75" spans="1:5">
       <c r="A75">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B75" t="s">
         <v>295</v>
       </c>
       <c r="C75">
-        <v>16377410</v>
+        <v>16184168</v>
       </c>
       <c r="E75" s="1"/>
     </row>
     <row r="76" spans="1:5">
       <c r="A76">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B76" t="s">
         <v>295</v>
       </c>
       <c r="C76">
-        <v>16570199.000000002</v>
+        <v>16377410</v>
       </c>
       <c r="E76" s="1"/>
     </row>
     <row r="77" spans="1:5">
       <c r="A77">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B77" t="s">
         <v>295</v>
       </c>
       <c r="C77">
-        <v>16760800.000000002</v>
+        <v>16570199.000000002</v>
       </c>
       <c r="E77" s="1"/>
     </row>
     <row r="78" spans="1:5">
       <c r="A78">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B78" t="s">
         <v>295</v>
       </c>
       <c r="C78">
-        <v>16949850.000000004</v>
+        <v>16760800.000000002</v>
       </c>
       <c r="E78" s="1"/>
     </row>
     <row r="79" spans="1:5">
       <c r="A79">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B79" t="s">
         <v>295</v>
       </c>
       <c r="C79">
-        <v>17136782</v>
+        <v>16949850.000000004</v>
       </c>
       <c r="E79" s="1"/>
     </row>
     <row r="80" spans="1:5">
       <c r="A80">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B80" t="s">
         <v>295</v>
       </c>
       <c r="C80">
-        <v>17321029.000000004</v>
+        <v>17136782</v>
       </c>
       <c r="E80" s="1"/>
     </row>
     <row r="81" spans="1:5">
       <c r="A81">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B81" t="s">
         <v>295</v>
       </c>
       <c r="C81">
-        <v>17503120.000000004</v>
+        <v>17321029.000000004</v>
       </c>
       <c r="E81" s="1"/>
     </row>
     <row r="82" spans="1:5">
       <c r="A82">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B82" t="s">
         <v>295</v>
       </c>
       <c r="C82">
-        <v>17681895.000000004</v>
+        <v>17503120.000000004</v>
       </c>
       <c r="E82" s="1"/>
     </row>
     <row r="83" spans="1:5">
       <c r="A83">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B83" t="s">
         <v>295</v>
       </c>
       <c r="C83">
-        <v>17865770</v>
+        <v>17681895.000000004</v>
       </c>
       <c r="E83" s="1"/>
     </row>
     <row r="84" spans="1:5">
       <c r="A84">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B84" t="s">
         <v>295</v>
       </c>
       <c r="C84">
-        <v>18319121</v>
+        <v>17865770</v>
       </c>
       <c r="E84" s="1"/>
     </row>
     <row r="85" spans="1:5">
       <c r="A85">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B85" t="s">
         <v>295</v>
       </c>
       <c r="C85">
-        <v>18780336</v>
+        <v>18319121</v>
       </c>
       <c r="E85" s="1"/>
     </row>
     <row r="86" spans="1:5">
       <c r="A86">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B86" t="s">
         <v>295</v>
       </c>
       <c r="C86">
-        <v>19249870.999999996</v>
+        <v>18780336</v>
       </c>
       <c r="E86" s="1"/>
     </row>
     <row r="87" spans="1:5">
       <c r="A87">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B87" t="s">
         <v>295</v>
       </c>
       <c r="C87">
-        <v>19727595.999999996</v>
+        <v>19249870.999999996</v>
       </c>
       <c r="E87" s="1"/>
     </row>
     <row r="88" spans="1:5">
       <c r="A88">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B88" t="s">
         <v>295</v>
       </c>
       <c r="C88">
-        <v>20213324.999999996</v>
+        <v>19727595.999999996</v>
       </c>
       <c r="E88" s="1"/>
     </row>
     <row r="89" spans="1:5">
       <c r="A89">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B89" t="s">
         <v>295</v>
       </c>
       <c r="C89">
-        <v>20706327.999999993</v>
+        <v>20213324.999999996</v>
       </c>
       <c r="E89" s="1"/>
     </row>
     <row r="90" spans="1:5">
       <c r="A90">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B90" t="s">
         <v>295</v>
       </c>
       <c r="C90">
-        <v>21207289.999999993</v>
+        <v>20706327.999999993</v>
       </c>
       <c r="E90" s="1"/>
     </row>
     <row r="91" spans="1:5">
       <c r="A91">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B91" t="s">
         <v>295</v>
       </c>
       <c r="C91">
-        <v>21715835.999999993</v>
-      </c>
-      <c r="D91">
-        <v>70169</v>
-      </c>
-      <c r="E91">
-        <f t="shared" ref="E91:E96" si="1">C91/D91</f>
-        <v>309.47905770354419</v>
-      </c>
+        <v>21207289.999999993</v>
+      </c>
+      <c r="E91" s="1"/>
     </row>
     <row r="92" spans="1:5">
       <c r="A92">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B92" t="s">
         <v>295</v>
       </c>
       <c r="C92">
+        <v>21715835.999999993</v>
+      </c>
+      <c r="D92">
+        <v>70169</v>
+      </c>
+      <c r="E92">
+        <f t="shared" ref="E92:E97" si="1">C92/D92</f>
+        <v>309.47905770354419</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5">
+      <c r="A93">
+        <v>64</v>
+      </c>
+      <c r="B93" t="s">
+        <v>295</v>
+      </c>
+      <c r="C93">
         <v>22232001.999999989</v>
       </c>
-      <c r="D92">
+      <c r="D93">
         <v>74852</v>
       </c>
-      <c r="E92">
+      <c r="E93">
         <f t="shared" si="1"/>
         <v>297.01279858921589</v>
       </c>
     </row>
-    <row r="93" spans="1:5">
-      <c r="A93">
+    <row r="94" spans="1:5">
+      <c r="A94">
         <v>65</v>
       </c>
-      <c r="B93" t="s">
+      <c r="B94" t="s">
         <v>295</v>
       </c>
-      <c r="C93">
+      <c r="C94">
         <v>22744700</v>
       </c>
-      <c r="D93">
+      <c r="D94">
         <v>16758</v>
       </c>
-      <c r="E93">
+      <c r="E94">
         <f t="shared" si="1"/>
         <v>1357.2443012292636</v>
       </c>
     </row>
-    <row r="94" spans="1:5">
-      <c r="A94">
-        <v>66</v>
-      </c>
-      <c r="B94" t="s">
+    <row r="95" spans="1:5">
+      <c r="A95">
+        <v>66</v>
+      </c>
+      <c r="B95" t="s">
         <v>295</v>
       </c>
-      <c r="C94">
+      <c r="C95">
         <v>22949433</v>
       </c>
-      <c r="D94">
+      <c r="D95">
         <v>17347</v>
       </c>
-      <c r="E94">
+      <c r="E95">
         <f t="shared" si="1"/>
         <v>1322.9626448377242</v>
       </c>
     </row>
-    <row r="95" spans="1:5">
-      <c r="A95">
-        <v>67</v>
-      </c>
-      <c r="B95" t="s">
+    <row r="96" spans="1:5">
+      <c r="A96">
+        <v>67</v>
+      </c>
+      <c r="B96" t="s">
         <v>295</v>
       </c>
-      <c r="C95">
+      <c r="C96">
         <v>23150968</v>
       </c>
-      <c r="D95">
+      <c r="D96">
         <v>25138</v>
       </c>
-      <c r="E95">
+      <c r="E96">
         <f t="shared" si="1"/>
         <v>920.95504813429864</v>
       </c>
     </row>
-    <row r="96" spans="1:5">
-      <c r="A96">
+    <row r="97" spans="1:5">
+      <c r="A97">
         <v>68</v>
       </c>
-      <c r="B96" t="s">
+      <c r="B97" t="s">
         <v>295</v>
       </c>
-      <c r="C96">
+      <c r="C97">
         <v>23348214.999999996</v>
       </c>
-      <c r="D96">
+      <c r="D97">
         <v>35647</v>
       </c>
-      <c r="E96">
+      <c r="E97">
         <f t="shared" si="1"/>
         <v>654.98400987460366</v>
       </c>
     </row>
-    <row r="97" spans="1:5">
-      <c r="A97">
-        <v>69</v>
-      </c>
-      <c r="B97" t="s">
-        <v>295</v>
-      </c>
-      <c r="C97">
-        <v>23540975.999999993</v>
-      </c>
-      <c r="D97">
-        <v>54789</v>
-      </c>
-      <c r="E97">
-        <f>C97/D97</f>
-        <v>429.66610085966147</v>
-      </c>
-    </row>
     <row r="98" spans="1:5">
       <c r="A98">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B98" t="s">
         <v>295</v>
       </c>
       <c r="C98">
-        <v>23730724.999999993</v>
+        <v>23540975.999999993</v>
       </c>
       <c r="D98">
-        <v>55650</v>
+        <v>54789</v>
       </c>
       <c r="E98">
-        <f t="shared" ref="E98:E123" si="2">C98/D98</f>
-        <v>426.42812219227301</v>
+        <f>C98/D98</f>
+        <v>429.66610085966147</v>
       </c>
     </row>
     <row r="99" spans="1:5">
       <c r="A99">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B99" t="s">
         <v>295</v>
       </c>
       <c r="C99">
+        <v>23730724.999999993</v>
+      </c>
+      <c r="D99">
+        <v>55650</v>
+      </c>
+      <c r="E99">
+        <f t="shared" ref="E99:E124" si="2">C99/D99</f>
+        <v>426.42812219227301</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5">
+      <c r="A100">
+        <v>71</v>
+      </c>
+      <c r="B100" t="s">
+        <v>295</v>
+      </c>
+      <c r="C100">
         <v>23683043.999999989</v>
       </c>
-      <c r="D99">
+      <c r="D100">
         <v>53936</v>
       </c>
-      <c r="E99">
+      <c r="E100">
         <f t="shared" si="2"/>
         <v>439.09529813111817</v>
       </c>
     </row>
-    <row r="100" spans="1:5">
-      <c r="A100">
+    <row r="101" spans="1:5">
+      <c r="A101">
         <v>72</v>
       </c>
-      <c r="B100" t="s">
+      <c r="B101" t="s">
         <v>295</v>
       </c>
-      <c r="C100">
+      <c r="C101">
         <v>23628800.999999985</v>
       </c>
-      <c r="D100">
+      <c r="D101">
         <v>33117</v>
       </c>
-      <c r="E100">
+      <c r="E101">
         <f t="shared" si="2"/>
         <v>713.49461001902296</v>
       </c>
     </row>
-    <row r="101" spans="1:5">
-      <c r="A101">
+    <row r="102" spans="1:5">
+      <c r="A102">
         <v>73</v>
       </c>
-      <c r="B101" t="s">
+      <c r="B102" t="s">
         <v>295</v>
       </c>
-      <c r="C101">
+      <c r="C102">
         <v>23567743.999999985</v>
       </c>
-      <c r="D101">
+      <c r="D102">
         <v>44146</v>
       </c>
-      <c r="E101">
+      <c r="E102">
         <f t="shared" si="2"/>
         <v>533.85910388257116</v>
       </c>
     </row>
-    <row r="102" spans="1:5">
-      <c r="A102">
+    <row r="103" spans="1:5">
+      <c r="A103">
         <v>74</v>
       </c>
-      <c r="B102" t="s">
+      <c r="B103" t="s">
         <v>295</v>
       </c>
-      <c r="C102">
+      <c r="C103">
         <v>23499620.999999985</v>
       </c>
-      <c r="D102">
+      <c r="D103">
         <v>92800</v>
       </c>
-      <c r="E102">
+      <c r="E103">
         <f t="shared" si="2"/>
         <v>253.22867456896535</v>
       </c>
     </row>
-    <row r="103" spans="1:5">
-      <c r="A103">
+    <row r="104" spans="1:5">
+      <c r="A104">
         <v>75</v>
       </c>
-      <c r="B103" t="s">
+      <c r="B104" t="s">
         <v>295</v>
       </c>
-      <c r="C103">
+      <c r="C104">
         <v>23421450</v>
       </c>
-      <c r="D103">
+      <c r="D104">
         <v>61055</v>
       </c>
-      <c r="E103">
+      <c r="E104">
         <f t="shared" si="2"/>
         <v>383.6123167635738</v>
       </c>
     </row>
-    <row r="104" spans="1:5">
-      <c r="A104">
+    <row r="105" spans="1:5">
+      <c r="A105">
         <v>76</v>
       </c>
-      <c r="B104" t="s">
+      <c r="B105" t="s">
         <v>295</v>
       </c>
-      <c r="C104">
+      <c r="C105">
         <v>23389810</v>
       </c>
-      <c r="D104">
+      <c r="D105">
         <v>59639</v>
       </c>
-      <c r="E104">
+      <c r="E105">
         <f t="shared" si="2"/>
         <v>392.18984221734098</v>
       </c>
     </row>
-    <row r="105" spans="1:5">
-      <c r="A105">
+    <row r="106" spans="1:5">
+      <c r="A106">
         <v>77</v>
       </c>
-      <c r="B105" t="s">
+      <c r="B106" t="s">
         <v>295</v>
       </c>
-      <c r="C105">
+      <c r="C106">
         <v>23350728</v>
       </c>
-      <c r="D105">
+      <c r="D106">
         <v>49905</v>
       </c>
-      <c r="E105">
+      <c r="E106">
         <f t="shared" si="2"/>
         <v>467.90357679591222</v>
       </c>
     </row>
-    <row r="106" spans="1:5">
-      <c r="A106">
+    <row r="107" spans="1:5">
+      <c r="A107">
         <v>78</v>
       </c>
-      <c r="B106" t="s">
+      <c r="B107" t="s">
         <v>295</v>
       </c>
-      <c r="C106">
+      <c r="C107">
         <v>23303087.999999993</v>
       </c>
-      <c r="D106">
+      <c r="D107">
         <v>79183</v>
       </c>
-      <c r="E106">
+      <c r="E107">
         <f t="shared" si="2"/>
         <v>294.294078274377</v>
       </c>
     </row>
-    <row r="107" spans="1:5">
-      <c r="A107">
+    <row r="108" spans="1:5">
+      <c r="A108">
         <v>79</v>
       </c>
-      <c r="B107" t="s">
+      <c r="B108" t="s">
         <v>295</v>
       </c>
-      <c r="C107">
+      <c r="C108">
         <v>23247277.999999993</v>
       </c>
-      <c r="D107">
+      <c r="D108">
         <v>77033</v>
       </c>
-      <c r="E107">
+      <c r="E108">
         <f t="shared" si="2"/>
         <v>301.78336557059953</v>
       </c>
     </row>
-    <row r="108" spans="1:5">
-      <c r="A108">
+    <row r="109" spans="1:5">
+      <c r="A109">
         <v>80</v>
       </c>
-      <c r="B108" t="s">
+      <c r="B109" t="s">
         <v>295</v>
       </c>
-      <c r="C108">
+      <c r="C109">
         <v>23181854.999999993</v>
       </c>
-      <c r="D108">
+      <c r="D109">
         <v>75787</v>
       </c>
-      <c r="E108">
+      <c r="E109">
         <f t="shared" si="2"/>
         <v>305.88168155488398</v>
       </c>
     </row>
-    <row r="109" spans="1:5">
-      <c r="A109">
+    <row r="110" spans="1:5">
+      <c r="A110">
         <v>81</v>
       </c>
-      <c r="B109" t="s">
+      <c r="B110" t="s">
         <v>295</v>
       </c>
-      <c r="C109">
+      <c r="C110">
         <v>23072399.999999993</v>
       </c>
-      <c r="D109">
+      <c r="D110">
         <v>86406</v>
       </c>
-      <c r="E109">
+      <c r="E110">
         <f t="shared" si="2"/>
         <v>267.02312339420865</v>
       </c>
     </row>
-    <row r="110" spans="1:5">
-      <c r="A110">
+    <row r="111" spans="1:5">
+      <c r="A111">
         <v>82</v>
       </c>
-      <c r="B110" t="s">
+      <c r="B111" t="s">
         <v>295</v>
       </c>
-      <c r="C110">
+      <c r="C111">
         <v>22954414.999999985</v>
       </c>
-      <c r="D110">
+      <c r="D111">
         <v>59940</v>
       </c>
-      <c r="E110">
+      <c r="E111">
         <f t="shared" si="2"/>
         <v>382.95653987320628</v>
       </c>
     </row>
-    <row r="111" spans="1:5">
-      <c r="A111">
+    <row r="112" spans="1:5">
+      <c r="A112">
         <v>83</v>
       </c>
-      <c r="B111" t="s">
+      <c r="B112" t="s">
         <v>295</v>
       </c>
-      <c r="C111">
+      <c r="C112">
         <v>22827229.999999985</v>
       </c>
-      <c r="D111">
+      <c r="D112">
         <v>62874</v>
       </c>
-      <c r="E111">
+      <c r="E112">
         <f t="shared" si="2"/>
         <v>363.06311034767924</v>
       </c>
     </row>
-    <row r="112" spans="1:5">
-      <c r="A112">
+    <row r="113" spans="1:5">
+      <c r="A113">
         <v>84</v>
       </c>
-      <c r="B112" t="s">
+      <c r="B113" t="s">
         <v>295</v>
       </c>
-      <c r="C112">
+      <c r="C113">
         <v>22690529.999999981</v>
       </c>
-      <c r="D112">
+      <c r="D113">
         <v>66361</v>
       </c>
-      <c r="E112">
+      <c r="E113">
         <f t="shared" si="2"/>
         <v>341.92567923931199</v>
       </c>
     </row>
-    <row r="113" spans="1:5">
-      <c r="A113">
+    <row r="114" spans="1:5">
+      <c r="A114">
         <v>85</v>
       </c>
-      <c r="B113" t="s">
+      <c r="B114" t="s">
         <v>295</v>
       </c>
-      <c r="C113">
+      <c r="C114">
         <v>22236000</v>
       </c>
-      <c r="D113">
+      <c r="D114">
         <v>77284</v>
       </c>
-      <c r="E113">
+      <c r="E114">
         <f t="shared" si="2"/>
         <v>287.71802701723516</v>
       </c>
     </row>
-    <row r="114" spans="1:5">
-      <c r="A114">
+    <row r="115" spans="1:5">
+      <c r="A115">
         <v>86</v>
       </c>
-      <c r="B114" t="s">
+      <c r="B115" t="s">
         <v>295</v>
       </c>
-      <c r="C114">
+      <c r="C115">
         <v>22078000</v>
       </c>
-      <c r="D114">
+      <c r="D115">
         <v>72814</v>
       </c>
-      <c r="E114">
+      <c r="E115">
         <f t="shared" si="2"/>
         <v>303.21092097673522</v>
       </c>
     </row>
-    <row r="115" spans="1:5">
-      <c r="A115">
+    <row r="116" spans="1:5">
+      <c r="A116">
         <v>87</v>
       </c>
-      <c r="B115" t="s">
+      <c r="B116" t="s">
         <v>295</v>
       </c>
-      <c r="C115">
+      <c r="C116">
         <v>21926000</v>
       </c>
-      <c r="D115">
+      <c r="D116">
         <v>83979</v>
       </c>
-      <c r="E115">
+      <c r="E116">
         <f t="shared" si="2"/>
         <v>261.08908179425811</v>
       </c>
     </row>
-    <row r="116" spans="1:5">
-      <c r="A116">
+    <row r="117" spans="1:5">
+      <c r="A117">
         <v>88</v>
       </c>
-      <c r="B116" t="s">
+      <c r="B117" t="s">
         <v>295</v>
       </c>
-      <c r="C116">
+      <c r="C117">
         <v>21780000</v>
       </c>
-      <c r="D116">
+      <c r="D117">
         <v>76072</v>
       </c>
-      <c r="E116">
+      <c r="E117">
         <f t="shared" si="2"/>
         <v>286.30770848669681</v>
       </c>
     </row>
-    <row r="117" spans="1:5">
-      <c r="A117">
+    <row r="118" spans="1:5">
+      <c r="A118">
         <v>89</v>
       </c>
-      <c r="B117" t="s">
+      <c r="B118" t="s">
         <v>295</v>
       </c>
-      <c r="C117">
+      <c r="C118">
         <v>21639000</v>
       </c>
-      <c r="D117">
+      <c r="D118">
         <v>79850</v>
       </c>
-      <c r="E117">
+      <c r="E118">
         <f t="shared" si="2"/>
         <v>270.99561678146523</v>
       </c>
     </row>
-    <row r="118" spans="1:5">
-      <c r="A118">
+    <row r="119" spans="1:5">
+      <c r="A119">
         <v>90</v>
       </c>
-      <c r="B118" t="s">
+      <c r="B119" t="s">
         <v>295</v>
       </c>
-      <c r="C118">
+      <c r="C119">
         <v>21503000</v>
       </c>
-      <c r="D118">
+      <c r="D119">
         <v>79079</v>
       </c>
-      <c r="E118">
+      <c r="E119">
         <f t="shared" si="2"/>
         <v>271.91795546225927</v>
       </c>
     </row>
-    <row r="119" spans="1:5">
-      <c r="A119">
+    <row r="120" spans="1:5">
+      <c r="A120">
         <v>91</v>
       </c>
-      <c r="B119" t="s">
+      <c r="B120" t="s">
         <v>295</v>
       </c>
-      <c r="C119">
+      <c r="C120">
         <v>21430000</v>
       </c>
-      <c r="D119">
+      <c r="D120">
         <v>76496</v>
       </c>
-      <c r="E119">
+      <c r="E120">
         <f t="shared" si="2"/>
         <v>280.14536707801716</v>
       </c>
     </row>
-    <row r="120" spans="1:5">
-      <c r="A120">
+    <row r="121" spans="1:5">
+      <c r="A121">
         <v>92</v>
       </c>
-      <c r="B120" t="s">
+      <c r="B121" t="s">
         <v>295</v>
       </c>
-      <c r="C120">
+      <c r="C121">
         <v>21441000</v>
       </c>
-      <c r="D120">
+      <c r="D121">
         <v>72301</v>
       </c>
-      <c r="E120">
+      <c r="E121">
         <f t="shared" si="2"/>
         <v>296.55191491127368</v>
       </c>
     </row>
-    <row r="121" spans="1:5">
-      <c r="A121">
+    <row r="122" spans="1:5">
+      <c r="A122">
         <v>93</v>
       </c>
-      <c r="B121" t="s">
+      <c r="B122" t="s">
         <v>295</v>
       </c>
-      <c r="C121">
+      <c r="C122">
         <v>21448000</v>
       </c>
-      <c r="D121">
+      <c r="D122">
         <v>71551</v>
       </c>
-      <c r="E121">
+      <c r="E122">
         <f t="shared" si="2"/>
         <v>299.75821442048328</v>
       </c>
     </row>
-    <row r="122" spans="1:5">
-      <c r="A122">
+    <row r="123" spans="1:5">
+      <c r="A123">
         <v>94</v>
       </c>
-      <c r="B122" t="s">
+      <c r="B123" t="s">
         <v>295</v>
       </c>
-      <c r="C122">
+      <c r="C123">
         <v>21446000</v>
       </c>
-      <c r="D122">
+      <c r="D123">
         <v>70439</v>
       </c>
-      <c r="E122">
+      <c r="E123">
         <f t="shared" si="2"/>
         <v>304.46201678047674</v>
       </c>
     </row>
-    <row r="123" spans="1:5">
-      <c r="A123">
+    <row r="124" spans="1:5">
+      <c r="A124">
         <v>95</v>
       </c>
-      <c r="B123" t="s">
+      <c r="B124" t="s">
         <v>295</v>
       </c>
-      <c r="C123">
+      <c r="C124">
         <v>21438000</v>
       </c>
-      <c r="D123">
+      <c r="D124">
         <v>69514</v>
       </c>
-      <c r="E123">
+      <c r="E124">
         <f t="shared" si="2"/>
         <v>308.39830825445233</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5">
+      <c r="A125">
+        <v>96</v>
+      </c>
+      <c r="B125" t="s">
+        <v>295</v>
       </c>
     </row>
   </sheetData>
@@ -12496,9 +12604,11 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L34"/>
+  <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -13415,6 +13525,32 @@
         <v>68</v>
       </c>
     </row>
+    <row r="35" spans="1:8">
+      <c r="A35">
+        <v>96</v>
+      </c>
+      <c r="B35" t="s">
+        <v>332</v>
+      </c>
+      <c r="C35">
+        <v>61116</v>
+      </c>
+      <c r="D35">
+        <v>61338</v>
+      </c>
+      <c r="E35" t="s">
+        <v>66</v>
+      </c>
+      <c r="F35" t="s">
+        <v>67</v>
+      </c>
+      <c r="G35" t="s">
+        <v>277</v>
+      </c>
+      <c r="H35" t="s">
+        <v>68</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -13422,9 +13558,11 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L34"/>
+  <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -14341,6 +14479,32 @@
         <v>68</v>
       </c>
     </row>
+    <row r="35" spans="1:8">
+      <c r="A35">
+        <v>96</v>
+      </c>
+      <c r="B35" t="s">
+        <v>332</v>
+      </c>
+      <c r="C35">
+        <v>62117</v>
+      </c>
+      <c r="D35">
+        <v>64114</v>
+      </c>
+      <c r="E35" t="s">
+        <v>66</v>
+      </c>
+      <c r="F35" t="s">
+        <v>67</v>
+      </c>
+      <c r="G35" t="s">
+        <v>277</v>
+      </c>
+      <c r="H35" t="s">
+        <v>68</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -14348,9 +14512,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R34"/>
+  <dimension ref="A1:R35"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="I39" sqref="I39"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
@@ -15634,6 +15800,41 @@
         <v>74</v>
       </c>
       <c r="N34" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14">
+      <c r="A35">
+        <v>96</v>
+      </c>
+      <c r="B35" t="s">
+        <v>66</v>
+      </c>
+      <c r="C35" t="s">
+        <v>67</v>
+      </c>
+      <c r="D35" t="s">
+        <v>68</v>
+      </c>
+      <c r="E35" t="s">
+        <v>69</v>
+      </c>
+      <c r="F35" t="s">
+        <v>70</v>
+      </c>
+      <c r="G35" t="s">
+        <v>71</v>
+      </c>
+      <c r="K35" t="s">
+        <v>72</v>
+      </c>
+      <c r="L35" t="s">
+        <v>73</v>
+      </c>
+      <c r="M35" t="s">
+        <v>74</v>
+      </c>
+      <c r="N35" t="s">
         <v>75</v>
       </c>
     </row>
@@ -16739,9 +16940,11 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J34"/>
+  <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="N38" sqref="N38"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -17460,6 +17663,26 @@
         <v>68</v>
       </c>
     </row>
+    <row r="35" spans="1:10">
+      <c r="A35">
+        <v>96</v>
+      </c>
+      <c r="B35" t="s">
+        <v>288</v>
+      </c>
+      <c r="E35" t="s">
+        <v>66</v>
+      </c>
+      <c r="F35" t="s">
+        <v>67</v>
+      </c>
+      <c r="G35" t="s">
+        <v>277</v>
+      </c>
+      <c r="J35" t="s">
+        <v>68</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -17467,9 +17690,11 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J34"/>
+  <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -18423,6 +18648,35 @@
         <v>69</v>
       </c>
     </row>
+    <row r="35" spans="1:10">
+      <c r="A35">
+        <v>96</v>
+      </c>
+      <c r="B35" t="s">
+        <v>333</v>
+      </c>
+      <c r="C35">
+        <v>44111</v>
+      </c>
+      <c r="D35">
+        <v>45414</v>
+      </c>
+      <c r="E35" t="s">
+        <v>66</v>
+      </c>
+      <c r="F35" t="s">
+        <v>67</v>
+      </c>
+      <c r="G35" t="s">
+        <v>277</v>
+      </c>
+      <c r="H35" t="s">
+        <v>68</v>
+      </c>
+      <c r="J35" t="s">
+        <v>69</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -18430,9 +18684,11 @@
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J34"/>
+  <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="L31" sqref="L31"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -19150,6 +19406,26 @@
         <v>68</v>
       </c>
     </row>
+    <row r="35" spans="1:10">
+      <c r="A35">
+        <v>96</v>
+      </c>
+      <c r="B35" t="s">
+        <v>332</v>
+      </c>
+      <c r="E35" t="s">
+        <v>66</v>
+      </c>
+      <c r="F35" t="s">
+        <v>67</v>
+      </c>
+      <c r="G35" t="s">
+        <v>277</v>
+      </c>
+      <c r="J35" t="s">
+        <v>68</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -19157,9 +19433,11 @@
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J34"/>
+  <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="M29" sqref="M29"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -19997,6 +20275,26 @@
         <v>68</v>
       </c>
     </row>
+    <row r="35" spans="1:10">
+      <c r="A35">
+        <v>96</v>
+      </c>
+      <c r="B35" t="s">
+        <v>362</v>
+      </c>
+      <c r="E35" t="s">
+        <v>66</v>
+      </c>
+      <c r="F35" t="s">
+        <v>67</v>
+      </c>
+      <c r="G35" t="s">
+        <v>277</v>
+      </c>
+      <c r="J35" t="s">
+        <v>68</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -20004,9 +20302,11 @@
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J34"/>
+  <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H36" sqref="H36"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -20844,6 +21144,26 @@
         <v>68</v>
       </c>
     </row>
+    <row r="35" spans="1:10">
+      <c r="A35">
+        <v>96</v>
+      </c>
+      <c r="B35" t="s">
+        <v>363</v>
+      </c>
+      <c r="E35" t="s">
+        <v>66</v>
+      </c>
+      <c r="F35" t="s">
+        <v>67</v>
+      </c>
+      <c r="G35" t="s">
+        <v>277</v>
+      </c>
+      <c r="J35" t="s">
+        <v>68</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -20851,9 +21171,11 @@
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J34"/>
+  <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="I38" sqref="I38"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -21571,6 +21893,26 @@
         <v>68</v>
       </c>
     </row>
+    <row r="35" spans="1:10">
+      <c r="A35">
+        <v>96</v>
+      </c>
+      <c r="B35" t="s">
+        <v>364</v>
+      </c>
+      <c r="E35" t="s">
+        <v>66</v>
+      </c>
+      <c r="F35" t="s">
+        <v>67</v>
+      </c>
+      <c r="G35" t="s">
+        <v>277</v>
+      </c>
+      <c r="J35" t="s">
+        <v>68</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -21578,9 +21920,11 @@
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P34"/>
+  <dimension ref="A1:P35"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="Q31" sqref="Q31"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -23215,6 +23559,56 @@
         <v>66</v>
       </c>
     </row>
+    <row r="35" spans="1:16">
+      <c r="A35">
+        <v>96</v>
+      </c>
+      <c r="B35" t="s">
+        <v>299</v>
+      </c>
+      <c r="C35" t="s">
+        <v>361</v>
+      </c>
+      <c r="D35" t="s">
+        <v>288</v>
+      </c>
+      <c r="E35" t="s">
+        <v>287</v>
+      </c>
+      <c r="F35" t="s">
+        <v>333</v>
+      </c>
+      <c r="G35" t="s">
+        <v>332</v>
+      </c>
+      <c r="H35" t="s">
+        <v>362</v>
+      </c>
+      <c r="I35" t="s">
+        <v>363</v>
+      </c>
+      <c r="J35" t="s">
+        <v>273</v>
+      </c>
+      <c r="K35" t="s">
+        <v>364</v>
+      </c>
+      <c r="L35" t="s">
+        <v>365</v>
+      </c>
+      <c r="M35" t="s">
+        <v>366</v>
+      </c>
+      <c r="N35" t="s">
+        <v>276</v>
+      </c>
+      <c r="O35" t="s">
+        <v>367</v>
+      </c>
+      <c r="P35" t="s">
+        <v>66</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -23222,9 +23616,11 @@
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J34"/>
+  <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="J38" sqref="J38"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -24061,6 +24457,26 @@
         <v>68</v>
       </c>
     </row>
+    <row r="35" spans="1:10">
+      <c r="A35">
+        <v>96</v>
+      </c>
+      <c r="B35" t="s">
+        <v>365</v>
+      </c>
+      <c r="E35" t="s">
+        <v>66</v>
+      </c>
+      <c r="F35" t="s">
+        <v>67</v>
+      </c>
+      <c r="G35" t="s">
+        <v>277</v>
+      </c>
+      <c r="J35" t="s">
+        <v>68</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -24068,9 +24484,11 @@
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J34"/>
+  <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B34" sqref="B33:J35"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -24907,6 +25325,26 @@
         <v>68</v>
       </c>
     </row>
+    <row r="35" spans="1:10">
+      <c r="A35">
+        <v>96</v>
+      </c>
+      <c r="B35" t="s">
+        <v>366</v>
+      </c>
+      <c r="E35" t="s">
+        <v>66</v>
+      </c>
+      <c r="F35" t="s">
+        <v>67</v>
+      </c>
+      <c r="G35" t="s">
+        <v>277</v>
+      </c>
+      <c r="J35" t="s">
+        <v>68</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -24916,7 +25354,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C60"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A37" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -25590,9 +26028,11 @@
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K34"/>
+  <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="J42" sqref="J42"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -26469,6 +26909,35 @@
         <v>72</v>
       </c>
     </row>
+    <row r="35" spans="1:11">
+      <c r="A35">
+        <v>96</v>
+      </c>
+      <c r="B35" t="s">
+        <v>276</v>
+      </c>
+      <c r="E35" t="s">
+        <v>66</v>
+      </c>
+      <c r="F35" t="s">
+        <v>67</v>
+      </c>
+      <c r="G35" t="s">
+        <v>277</v>
+      </c>
+      <c r="H35" t="s">
+        <v>68</v>
+      </c>
+      <c r="I35" t="s">
+        <v>69</v>
+      </c>
+      <c r="J35" t="s">
+        <v>70</v>
+      </c>
+      <c r="K35" t="s">
+        <v>72</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -26476,9 +26945,11 @@
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J34"/>
+  <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="I41" sqref="I41"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -27259,6 +27730,29 @@
         <v>69</v>
       </c>
     </row>
+    <row r="35" spans="1:10">
+      <c r="A35">
+        <v>96</v>
+      </c>
+      <c r="B35" t="s">
+        <v>367</v>
+      </c>
+      <c r="E35" t="s">
+        <v>66</v>
+      </c>
+      <c r="F35" t="s">
+        <v>67</v>
+      </c>
+      <c r="G35" t="s">
+        <v>277</v>
+      </c>
+      <c r="I35" t="s">
+        <v>68</v>
+      </c>
+      <c r="J35" t="s">
+        <v>69</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -27266,9 +27760,11 @@
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K34"/>
+  <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="I46" sqref="I46"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -28345,6 +28841,35 @@
         <v>70</v>
       </c>
       <c r="K34" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11">
+      <c r="A35" s="3">
+        <v>96</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="H35" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="I35" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="J35" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="K35" s="3" t="s">
         <v>72</v>
       </c>
     </row>
@@ -32697,8 +33222,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -32907,7 +33432,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D97"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
@@ -55911,9 +56436,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H34"/>
+  <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -56756,6 +57283,11 @@
         <v>66</v>
       </c>
     </row>
+    <row r="35" spans="1:8">
+      <c r="A35">
+        <v>96</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -56766,7 +57298,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>

</xml_diff>

<commit_message>
Add 1396 data and information to codes
</commit_message>
<xml_diff>
--- a/Data/MetaData.xlsx
+++ b/Data/MetaData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17100" windowHeight="6600" tabRatio="544" firstSheet="26" activeTab="31"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17100" windowHeight="6600" tabRatio="544" firstSheet="50" activeTab="57"/>
   </bookViews>
   <sheets>
     <sheet name="CompressedFileNames" sheetId="1" r:id="rId1"/>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13336" uniqueCount="471">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13496" uniqueCount="471">
   <si>
     <t>Year</t>
   </si>
@@ -2344,7 +2344,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -15845,9 +15845,11 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K34"/>
+  <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -16930,6 +16932,41 @@
         <v>70</v>
       </c>
       <c r="K34" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11">
+      <c r="A35">
+        <v>96</v>
+      </c>
+      <c r="B35" t="s">
+        <v>276</v>
+      </c>
+      <c r="C35">
+        <v>101111</v>
+      </c>
+      <c r="D35">
+        <v>105115</v>
+      </c>
+      <c r="E35" t="s">
+        <v>66</v>
+      </c>
+      <c r="F35" t="s">
+        <v>67</v>
+      </c>
+      <c r="G35" t="s">
+        <v>277</v>
+      </c>
+      <c r="H35" t="s">
+        <v>68</v>
+      </c>
+      <c r="I35" t="s">
+        <v>69</v>
+      </c>
+      <c r="J35" t="s">
+        <v>70</v>
+      </c>
+      <c r="K35" t="s">
         <v>72</v>
       </c>
     </row>
@@ -21173,8 +21210,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="I38" sqref="I38"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -21898,7 +21935,7 @@
         <v>96</v>
       </c>
       <c r="B35" t="s">
-        <v>364</v>
+        <v>273</v>
       </c>
       <c r="E35" t="s">
         <v>66</v>
@@ -26030,8 +26067,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="J42" sqref="J42"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="P38" sqref="P38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -27762,7 +27799,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="I46" sqref="I46"/>
     </sheetView>
   </sheetViews>
@@ -34663,10 +34700,10 @@
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L34"/>
+  <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -35798,6 +35835,41 @@
         <v>72</v>
       </c>
     </row>
+    <row r="35" spans="1:12">
+      <c r="A35">
+        <v>96</v>
+      </c>
+      <c r="B35" t="s">
+        <v>299</v>
+      </c>
+      <c r="C35">
+        <v>11811</v>
+      </c>
+      <c r="D35">
+        <v>11845</v>
+      </c>
+      <c r="E35" t="s">
+        <v>66</v>
+      </c>
+      <c r="F35" t="s">
+        <v>67</v>
+      </c>
+      <c r="G35" t="s">
+        <v>277</v>
+      </c>
+      <c r="I35" t="s">
+        <v>68</v>
+      </c>
+      <c r="J35" t="s">
+        <v>69</v>
+      </c>
+      <c r="K35" t="s">
+        <v>70</v>
+      </c>
+      <c r="L35" t="s">
+        <v>72</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -35805,10 +35877,10 @@
 
 <file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L34"/>
+  <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -36937,6 +37009,41 @@
         <v>72</v>
       </c>
     </row>
+    <row r="35" spans="1:12">
+      <c r="A35">
+        <v>96</v>
+      </c>
+      <c r="B35" t="s">
+        <v>299</v>
+      </c>
+      <c r="C35">
+        <v>11761</v>
+      </c>
+      <c r="D35">
+        <v>11769</v>
+      </c>
+      <c r="E35" t="s">
+        <v>66</v>
+      </c>
+      <c r="F35" t="s">
+        <v>67</v>
+      </c>
+      <c r="G35" t="s">
+        <v>277</v>
+      </c>
+      <c r="I35" t="s">
+        <v>68</v>
+      </c>
+      <c r="J35" t="s">
+        <v>69</v>
+      </c>
+      <c r="K35" t="s">
+        <v>70</v>
+      </c>
+      <c r="L35" t="s">
+        <v>72</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -36944,10 +37051,10 @@
 
 <file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L34"/>
+  <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -38076,6 +38183,41 @@
         <v>72</v>
       </c>
     </row>
+    <row r="35" spans="1:12">
+      <c r="A35">
+        <v>96</v>
+      </c>
+      <c r="B35" t="s">
+        <v>299</v>
+      </c>
+      <c r="C35">
+        <v>11511</v>
+      </c>
+      <c r="D35">
+        <v>11533</v>
+      </c>
+      <c r="E35" t="s">
+        <v>66</v>
+      </c>
+      <c r="F35" t="s">
+        <v>67</v>
+      </c>
+      <c r="G35" t="s">
+        <v>277</v>
+      </c>
+      <c r="I35" t="s">
+        <v>68</v>
+      </c>
+      <c r="J35" t="s">
+        <v>69</v>
+      </c>
+      <c r="K35" t="s">
+        <v>70</v>
+      </c>
+      <c r="L35" t="s">
+        <v>72</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -38083,10 +38225,10 @@
 
 <file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L34"/>
+  <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -39215,6 +39357,41 @@
         <v>72</v>
       </c>
     </row>
+    <row r="35" spans="1:12">
+      <c r="A35">
+        <v>96</v>
+      </c>
+      <c r="B35" t="s">
+        <v>299</v>
+      </c>
+      <c r="C35">
+        <v>11111</v>
+      </c>
+      <c r="D35">
+        <v>11118</v>
+      </c>
+      <c r="E35" t="s">
+        <v>66</v>
+      </c>
+      <c r="F35" t="s">
+        <v>67</v>
+      </c>
+      <c r="G35" t="s">
+        <v>277</v>
+      </c>
+      <c r="I35" t="s">
+        <v>68</v>
+      </c>
+      <c r="J35" t="s">
+        <v>69</v>
+      </c>
+      <c r="K35" t="s">
+        <v>70</v>
+      </c>
+      <c r="L35" t="s">
+        <v>72</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -39222,10 +39399,10 @@
 
 <file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L34"/>
+  <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -40354,6 +40531,41 @@
         <v>72</v>
       </c>
     </row>
+    <row r="35" spans="1:12">
+      <c r="A35">
+        <v>96</v>
+      </c>
+      <c r="B35" t="s">
+        <v>299</v>
+      </c>
+      <c r="C35">
+        <v>11141</v>
+      </c>
+      <c r="D35">
+        <v>11153</v>
+      </c>
+      <c r="E35" t="s">
+        <v>66</v>
+      </c>
+      <c r="F35" t="s">
+        <v>67</v>
+      </c>
+      <c r="G35" t="s">
+        <v>277</v>
+      </c>
+      <c r="I35" t="s">
+        <v>68</v>
+      </c>
+      <c r="J35" t="s">
+        <v>69</v>
+      </c>
+      <c r="K35" t="s">
+        <v>70</v>
+      </c>
+      <c r="L35" t="s">
+        <v>72</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -40361,10 +40573,10 @@
 
 <file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L34"/>
+  <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -41493,6 +41705,41 @@
         <v>72</v>
       </c>
     </row>
+    <row r="35" spans="1:12">
+      <c r="A35">
+        <v>96</v>
+      </c>
+      <c r="B35" t="s">
+        <v>299</v>
+      </c>
+      <c r="C35">
+        <v>11211</v>
+      </c>
+      <c r="D35">
+        <v>11221</v>
+      </c>
+      <c r="E35" t="s">
+        <v>66</v>
+      </c>
+      <c r="F35" t="s">
+        <v>67</v>
+      </c>
+      <c r="G35" t="s">
+        <v>277</v>
+      </c>
+      <c r="I35" t="s">
+        <v>68</v>
+      </c>
+      <c r="J35" t="s">
+        <v>69</v>
+      </c>
+      <c r="K35" t="s">
+        <v>70</v>
+      </c>
+      <c r="L35" t="s">
+        <v>72</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -41500,10 +41747,10 @@
 
 <file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L34"/>
+  <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -42632,6 +42879,41 @@
         <v>72</v>
       </c>
     </row>
+    <row r="35" spans="1:12">
+      <c r="A35">
+        <v>96</v>
+      </c>
+      <c r="B35" t="s">
+        <v>299</v>
+      </c>
+      <c r="C35">
+        <v>11231</v>
+      </c>
+      <c r="D35">
+        <v>11239</v>
+      </c>
+      <c r="E35" t="s">
+        <v>66</v>
+      </c>
+      <c r="F35" t="s">
+        <v>67</v>
+      </c>
+      <c r="G35" t="s">
+        <v>277</v>
+      </c>
+      <c r="I35" t="s">
+        <v>68</v>
+      </c>
+      <c r="J35" t="s">
+        <v>69</v>
+      </c>
+      <c r="K35" t="s">
+        <v>70</v>
+      </c>
+      <c r="L35" t="s">
+        <v>72</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -42639,10 +42921,10 @@
 
 <file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L34"/>
+  <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -43771,6 +44053,41 @@
         <v>72</v>
       </c>
     </row>
+    <row r="35" spans="1:12">
+      <c r="A35">
+        <v>96</v>
+      </c>
+      <c r="B35" t="s">
+        <v>299</v>
+      </c>
+      <c r="C35">
+        <v>11311</v>
+      </c>
+      <c r="D35">
+        <v>11321</v>
+      </c>
+      <c r="E35" t="s">
+        <v>66</v>
+      </c>
+      <c r="F35" t="s">
+        <v>67</v>
+      </c>
+      <c r="G35" t="s">
+        <v>277</v>
+      </c>
+      <c r="I35" t="s">
+        <v>68</v>
+      </c>
+      <c r="J35" t="s">
+        <v>69</v>
+      </c>
+      <c r="K35" t="s">
+        <v>70</v>
+      </c>
+      <c r="L35" t="s">
+        <v>72</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -43778,10 +44095,10 @@
 
 <file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L34"/>
+  <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -44910,6 +45227,41 @@
         <v>72</v>
       </c>
     </row>
+    <row r="35" spans="1:12">
+      <c r="A35">
+        <v>96</v>
+      </c>
+      <c r="B35" t="s">
+        <v>299</v>
+      </c>
+      <c r="C35">
+        <v>11411</v>
+      </c>
+      <c r="D35">
+        <v>11414</v>
+      </c>
+      <c r="E35" t="s">
+        <v>66</v>
+      </c>
+      <c r="F35" t="s">
+        <v>67</v>
+      </c>
+      <c r="G35" t="s">
+        <v>277</v>
+      </c>
+      <c r="I35" t="s">
+        <v>68</v>
+      </c>
+      <c r="J35" t="s">
+        <v>69</v>
+      </c>
+      <c r="K35" t="s">
+        <v>70</v>
+      </c>
+      <c r="L35" t="s">
+        <v>72</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -44917,10 +45269,10 @@
 
 <file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L34"/>
+  <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -46046,6 +46398,41 @@
         <v>70</v>
       </c>
       <c r="L34" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12">
+      <c r="A35">
+        <v>96</v>
+      </c>
+      <c r="B35" t="s">
+        <v>299</v>
+      </c>
+      <c r="C35">
+        <v>11424</v>
+      </c>
+      <c r="D35">
+        <v>11426</v>
+      </c>
+      <c r="E35" t="s">
+        <v>66</v>
+      </c>
+      <c r="F35" t="s">
+        <v>67</v>
+      </c>
+      <c r="G35" t="s">
+        <v>277</v>
+      </c>
+      <c r="I35" t="s">
+        <v>68</v>
+      </c>
+      <c r="J35" t="s">
+        <v>69</v>
+      </c>
+      <c r="K35" t="s">
+        <v>70</v>
+      </c>
+      <c r="L35" t="s">
         <v>72</v>
       </c>
     </row>
@@ -46182,10 +46569,10 @@
 
 <file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L34"/>
+  <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -47314,6 +47701,41 @@
         <v>72</v>
       </c>
     </row>
+    <row r="35" spans="1:12">
+      <c r="A35">
+        <v>96</v>
+      </c>
+      <c r="B35" t="s">
+        <v>299</v>
+      </c>
+      <c r="C35">
+        <v>11428</v>
+      </c>
+      <c r="D35">
+        <v>11432</v>
+      </c>
+      <c r="E35" t="s">
+        <v>66</v>
+      </c>
+      <c r="F35" t="s">
+        <v>67</v>
+      </c>
+      <c r="G35" t="s">
+        <v>277</v>
+      </c>
+      <c r="I35" t="s">
+        <v>68</v>
+      </c>
+      <c r="J35" t="s">
+        <v>69</v>
+      </c>
+      <c r="K35" t="s">
+        <v>70</v>
+      </c>
+      <c r="L35" t="s">
+        <v>72</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -47321,10 +47743,10 @@
 
 <file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L34"/>
+  <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -48456,6 +48878,41 @@
         <v>72</v>
       </c>
     </row>
+    <row r="35" spans="1:12">
+      <c r="A35">
+        <v>96</v>
+      </c>
+      <c r="B35" t="s">
+        <v>299</v>
+      </c>
+      <c r="C35">
+        <v>11441</v>
+      </c>
+      <c r="D35">
+        <v>11443</v>
+      </c>
+      <c r="E35" t="s">
+        <v>66</v>
+      </c>
+      <c r="F35" t="s">
+        <v>67</v>
+      </c>
+      <c r="G35" t="s">
+        <v>277</v>
+      </c>
+      <c r="I35" t="s">
+        <v>68</v>
+      </c>
+      <c r="J35" t="s">
+        <v>69</v>
+      </c>
+      <c r="K35" t="s">
+        <v>70</v>
+      </c>
+      <c r="L35" t="s">
+        <v>72</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -48463,10 +48920,10 @@
 
 <file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L34"/>
+  <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -49595,6 +50052,41 @@
         <v>72</v>
       </c>
     </row>
+    <row r="35" spans="1:12">
+      <c r="A35">
+        <v>96</v>
+      </c>
+      <c r="B35" t="s">
+        <v>299</v>
+      </c>
+      <c r="C35">
+        <v>11611</v>
+      </c>
+      <c r="D35">
+        <v>11643</v>
+      </c>
+      <c r="E35" t="s">
+        <v>66</v>
+      </c>
+      <c r="F35" t="s">
+        <v>67</v>
+      </c>
+      <c r="G35" t="s">
+        <v>277</v>
+      </c>
+      <c r="I35" t="s">
+        <v>68</v>
+      </c>
+      <c r="J35" t="s">
+        <v>69</v>
+      </c>
+      <c r="K35" t="s">
+        <v>70</v>
+      </c>
+      <c r="L35" t="s">
+        <v>72</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -49602,10 +50094,10 @@
 
 <file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L34"/>
+  <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -50734,6 +51226,41 @@
         <v>72</v>
       </c>
     </row>
+    <row r="35" spans="1:12">
+      <c r="A35">
+        <v>96</v>
+      </c>
+      <c r="B35" t="s">
+        <v>299</v>
+      </c>
+      <c r="C35">
+        <v>11711</v>
+      </c>
+      <c r="D35">
+        <v>11754</v>
+      </c>
+      <c r="E35" t="s">
+        <v>66</v>
+      </c>
+      <c r="F35" t="s">
+        <v>67</v>
+      </c>
+      <c r="G35" t="s">
+        <v>277</v>
+      </c>
+      <c r="I35" t="s">
+        <v>68</v>
+      </c>
+      <c r="J35" t="s">
+        <v>69</v>
+      </c>
+      <c r="K35" t="s">
+        <v>70</v>
+      </c>
+      <c r="L35" t="s">
+        <v>72</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -50741,10 +51268,10 @@
 
 <file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L34"/>
+  <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -51873,6 +52400,41 @@
         <v>72</v>
       </c>
     </row>
+    <row r="35" spans="1:12">
+      <c r="A35">
+        <v>96</v>
+      </c>
+      <c r="B35" t="s">
+        <v>299</v>
+      </c>
+      <c r="C35">
+        <v>11161</v>
+      </c>
+      <c r="D35">
+        <v>11166</v>
+      </c>
+      <c r="E35" t="s">
+        <v>66</v>
+      </c>
+      <c r="F35" t="s">
+        <v>67</v>
+      </c>
+      <c r="G35" t="s">
+        <v>277</v>
+      </c>
+      <c r="I35" t="s">
+        <v>68</v>
+      </c>
+      <c r="J35" t="s">
+        <v>69</v>
+      </c>
+      <c r="K35" t="s">
+        <v>70</v>
+      </c>
+      <c r="L35" t="s">
+        <v>72</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -51880,10 +52442,10 @@
 
 <file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L34"/>
+  <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -53012,6 +53574,41 @@
         <v>72</v>
       </c>
     </row>
+    <row r="35" spans="1:12">
+      <c r="A35">
+        <v>96</v>
+      </c>
+      <c r="B35" t="s">
+        <v>299</v>
+      </c>
+      <c r="C35">
+        <v>11731</v>
+      </c>
+      <c r="D35">
+        <v>11731</v>
+      </c>
+      <c r="E35" t="s">
+        <v>66</v>
+      </c>
+      <c r="F35" t="s">
+        <v>67</v>
+      </c>
+      <c r="G35" t="s">
+        <v>277</v>
+      </c>
+      <c r="I35" t="s">
+        <v>68</v>
+      </c>
+      <c r="J35" t="s">
+        <v>69</v>
+      </c>
+      <c r="K35" t="s">
+        <v>70</v>
+      </c>
+      <c r="L35" t="s">
+        <v>72</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -53019,10 +53616,10 @@
 
 <file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L34"/>
+  <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -54151,6 +54748,41 @@
         <v>72</v>
       </c>
     </row>
+    <row r="35" spans="1:12">
+      <c r="A35">
+        <v>96</v>
+      </c>
+      <c r="B35" t="s">
+        <v>299</v>
+      </c>
+      <c r="C35">
+        <v>11821</v>
+      </c>
+      <c r="D35">
+        <v>11845</v>
+      </c>
+      <c r="E35" t="s">
+        <v>66</v>
+      </c>
+      <c r="F35" t="s">
+        <v>67</v>
+      </c>
+      <c r="G35" t="s">
+        <v>277</v>
+      </c>
+      <c r="I35" t="s">
+        <v>68</v>
+      </c>
+      <c r="J35" t="s">
+        <v>69</v>
+      </c>
+      <c r="K35" t="s">
+        <v>70</v>
+      </c>
+      <c r="L35" t="s">
+        <v>72</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -54158,10 +54790,10 @@
 
 <file path=xl/worksheets/sheet57.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L34"/>
+  <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -55290,6 +55922,41 @@
         <v>72</v>
       </c>
     </row>
+    <row r="35" spans="1:12">
+      <c r="A35">
+        <v>96</v>
+      </c>
+      <c r="B35" t="s">
+        <v>299</v>
+      </c>
+      <c r="C35">
+        <v>11171</v>
+      </c>
+      <c r="D35">
+        <v>11175</v>
+      </c>
+      <c r="E35" t="s">
+        <v>66</v>
+      </c>
+      <c r="F35" t="s">
+        <v>67</v>
+      </c>
+      <c r="G35" t="s">
+        <v>277</v>
+      </c>
+      <c r="I35" t="s">
+        <v>68</v>
+      </c>
+      <c r="J35" t="s">
+        <v>69</v>
+      </c>
+      <c r="K35" t="s">
+        <v>70</v>
+      </c>
+      <c r="L35" t="s">
+        <v>72</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -55297,10 +55964,10 @@
 
 <file path=xl/worksheets/sheet58.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L34"/>
+  <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="I40" sqref="I40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -56426,6 +57093,41 @@
         <v>70</v>
       </c>
       <c r="L34" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12">
+      <c r="A35">
+        <v>96</v>
+      </c>
+      <c r="B35" t="s">
+        <v>299</v>
+      </c>
+      <c r="C35">
+        <v>11651</v>
+      </c>
+      <c r="D35">
+        <v>11662</v>
+      </c>
+      <c r="E35" t="s">
+        <v>66</v>
+      </c>
+      <c r="F35" t="s">
+        <v>67</v>
+      </c>
+      <c r="G35" t="s">
+        <v>277</v>
+      </c>
+      <c r="I35" t="s">
+        <v>68</v>
+      </c>
+      <c r="J35" t="s">
+        <v>69</v>
+      </c>
+      <c r="K35" t="s">
+        <v>70</v>
+      </c>
+      <c r="L35" t="s">
         <v>72</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Edit HEIS Part2 codes
</commit_message>
<xml_diff>
--- a/Data/MetaData.xlsx
+++ b/Data/MetaData.xlsx
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14188" uniqueCount="592">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14187" uniqueCount="592">
   <si>
     <t>Year</t>
   </si>
@@ -2711,7 +2711,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -16164,8 +16164,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BL35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AZ1" workbookViewId="0">
-      <selection activeCell="BF42" sqref="BF42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I43" sqref="I43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -19445,9 +19445,7 @@
       <c r="C35" s="9" t="s">
         <v>470</v>
       </c>
-      <c r="D35" s="9" t="s">
-        <v>591</v>
-      </c>
+      <c r="D35" s="9"/>
       <c r="E35" s="9" t="s">
         <v>471</v>
       </c>

</xml_diff>

<commit_message>
Mrs. Azizkhani work + update for MRC session
</commit_message>
<xml_diff>
--- a/Data/MetaData.xlsx
+++ b/Data/MetaData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17100" windowHeight="6600" tabRatio="858" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17100" windowHeight="6600" tabRatio="858" firstSheet="3" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="CompressedFileNames" sheetId="1" r:id="rId1"/>
@@ -2711,7 +2711,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -16165,7 +16165,7 @@
   <dimension ref="A1:BL35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I43" sqref="I43"/>
+      <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
update some expenditures codes
</commit_message>
<xml_diff>
--- a/Data/MetaData.xlsx
+++ b/Data/MetaData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17100" windowHeight="6600" tabRatio="858" firstSheet="3" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17100" windowHeight="6600" tabRatio="858" firstSheet="22" activeTab="27"/>
   </bookViews>
   <sheets>
     <sheet name="CompressedFileNames" sheetId="1" r:id="rId1"/>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14187" uniqueCount="592">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14189" uniqueCount="592">
   <si>
     <t>Year</t>
   </si>
@@ -2711,7 +2711,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -15211,13 +15211,13 @@
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="C21" sqref="C21:D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="12" max="12" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
@@ -15744,13 +15744,13 @@
         <v>81</v>
       </c>
       <c r="B20" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="C20">
-        <v>61116</v>
+        <v>51318</v>
       </c>
       <c r="D20">
-        <v>61338</v>
+        <v>51624</v>
       </c>
       <c r="E20" t="s">
         <v>51</v>
@@ -15770,13 +15770,13 @@
         <v>82</v>
       </c>
       <c r="B21" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="C21">
-        <v>61116</v>
+        <v>51318</v>
       </c>
       <c r="D21">
-        <v>61338</v>
+        <v>51624</v>
       </c>
       <c r="E21" t="s">
         <v>51</v>
@@ -16164,7 +16164,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BL35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
@@ -19602,7 +19602,7 @@
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -20135,13 +20135,13 @@
         <v>81</v>
       </c>
       <c r="B20" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="C20">
-        <v>62117</v>
+        <v>51114</v>
       </c>
       <c r="D20">
-        <v>64114</v>
+        <v>51191</v>
       </c>
       <c r="E20" t="s">
         <v>51</v>
@@ -20161,13 +20161,13 @@
         <v>82</v>
       </c>
       <c r="B21" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="C21">
-        <v>62117</v>
+        <v>51114</v>
       </c>
       <c r="D21">
-        <v>64114</v>
+        <v>51191</v>
       </c>
       <c r="E21" t="s">
         <v>51</v>
@@ -20555,8 +20555,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -21248,14 +21248,11 @@
       <c r="H23" t="s">
         <v>68</v>
       </c>
-      <c r="I23" t="s">
+      <c r="J23" t="s">
         <v>69</v>
       </c>
-      <c r="J23" t="s">
+      <c r="K23" t="s">
         <v>70</v>
-      </c>
-      <c r="K23" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="24" spans="1:11">
@@ -21283,14 +21280,11 @@
       <c r="H24" t="s">
         <v>68</v>
       </c>
-      <c r="I24" t="s">
+      <c r="J24" t="s">
         <v>69</v>
       </c>
-      <c r="J24" t="s">
+      <c r="K24" t="s">
         <v>70</v>
-      </c>
-      <c r="K24" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="25" spans="1:11">
@@ -21318,14 +21312,11 @@
       <c r="H25" t="s">
         <v>68</v>
       </c>
-      <c r="I25" t="s">
+      <c r="J25" t="s">
         <v>69</v>
       </c>
-      <c r="J25" t="s">
+      <c r="K25" t="s">
         <v>70</v>
-      </c>
-      <c r="K25" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="26" spans="1:11">
@@ -21353,14 +21344,11 @@
       <c r="H26" t="s">
         <v>68</v>
       </c>
-      <c r="I26" t="s">
+      <c r="J26" t="s">
         <v>69</v>
       </c>
-      <c r="J26" t="s">
+      <c r="K26" t="s">
         <v>70</v>
-      </c>
-      <c r="K26" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="27" spans="1:11">
@@ -21688,7 +21676,7 @@
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="N38" sqref="N38"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -22437,8 +22425,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView topLeftCell="A12" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
+      <selection activeCell="B21" sqref="B20:B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -23431,7 +23419,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
@@ -25050,7 +25038,7 @@
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -25918,7 +25906,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
@@ -26667,8 +26655,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P35"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="Q31" sqref="Q31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -27405,6 +27393,9 @@
       <c r="J16" t="s">
         <v>362</v>
       </c>
+      <c r="K16" t="s">
+        <v>273</v>
+      </c>
       <c r="L16" t="s">
         <v>363</v>
       </c>
@@ -27450,6 +27441,9 @@
       <c r="J17" t="s">
         <v>362</v>
       </c>
+      <c r="K17" t="s">
+        <v>273</v>
+      </c>
       <c r="L17" t="s">
         <v>363</v>
       </c>
@@ -27497,6 +27491,9 @@
       <c r="J18" t="s">
         <v>362</v>
       </c>
+      <c r="K18" t="s">
+        <v>273</v>
+      </c>
       <c r="L18" t="s">
         <v>363</v>
       </c>
@@ -27544,6 +27541,9 @@
       <c r="J19" t="s">
         <v>362</v>
       </c>
+      <c r="K19" t="s">
+        <v>273</v>
+      </c>
       <c r="L19" t="s">
         <v>363</v>
       </c>
@@ -27591,6 +27591,9 @@
       <c r="J20" t="s">
         <v>362</v>
       </c>
+      <c r="K20" t="s">
+        <v>273</v>
+      </c>
       <c r="L20" t="s">
         <v>363</v>
       </c>
@@ -27637,6 +27640,9 @@
       </c>
       <c r="J21" t="s">
         <v>362</v>
+      </c>
+      <c r="K21" t="s">
+        <v>273</v>
       </c>
       <c r="L21" t="s">
         <v>363</v>
@@ -28363,8 +28369,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B21" sqref="B20:B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -30564,7 +30570,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="B34" sqref="B33:J35"/>
     </sheetView>
   </sheetViews>
@@ -31432,8 +31438,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="P38" sqref="P38"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -32349,7 +32355,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="I41" sqref="I41"/>
     </sheetView>
   </sheetViews>
@@ -33164,7 +33170,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="I46" sqref="I46"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
some updates + code for clustering (93-96)
</commit_message>
<xml_diff>
--- a/Data/MetaData.xlsx
+++ b/Data/MetaData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17100" windowHeight="6600" tabRatio="858" firstSheet="22" activeTab="27"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17100" windowHeight="6600" tabRatio="858" firstSheet="32" activeTab="39"/>
   </bookViews>
   <sheets>
     <sheet name="CompressedFileNames" sheetId="1" r:id="rId1"/>
@@ -2711,7 +2711,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -16165,7 +16165,7 @@
   <dimension ref="A1:BL35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G39" sqref="G39"/>
+      <selection activeCell="H42" sqref="H42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -26655,7 +26655,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
@@ -39438,14 +39438,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.140625" style="8"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Update codes in clustering and Calorie parts
</commit_message>
<xml_diff>
--- a/Data/MetaData.xlsx
+++ b/Data/MetaData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17100" windowHeight="6600" tabRatio="858" firstSheet="35" activeTab="40"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17100" windowHeight="6600" tabRatio="858" firstSheet="38" activeTab="39"/>
   </bookViews>
   <sheets>
     <sheet name="CompressedFileNames" sheetId="1" r:id="rId1"/>
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14381" uniqueCount="596">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14383" uniqueCount="596">
   <si>
     <t>Year</t>
   </si>
@@ -39455,10 +39455,10 @@
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G14:G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -39652,6 +39652,17 @@
       </c>
       <c r="C17">
         <v>1.4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>593</v>
+      </c>
+      <c r="B18" t="s">
+        <v>593</v>
+      </c>
+      <c r="C18">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -39666,7 +39677,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
@@ -40616,7 +40627,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Updated codes in session
</commit_message>
<xml_diff>
--- a/Data/MetaData.xlsx
+++ b/Data/MetaData.xlsx
@@ -39627,7 +39627,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -39658,7 +39658,7 @@
         <v>454</v>
       </c>
       <c r="C2">
-        <v>1.2</v>
+        <v>3.6</v>
       </c>
       <c r="D2">
         <v>0.09</v>
@@ -40402,7 +40402,7 @@
   <dimension ref="A1:B235"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="B9" sqref="A2:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Update Codes for new report
</commit_message>
<xml_diff>
--- a/Data/MetaData.xlsx
+++ b/Data/MetaData.xlsx
@@ -39627,7 +39627,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -39658,7 +39658,7 @@
         <v>454</v>
       </c>
       <c r="C2">
-        <v>1.2</v>
+        <v>2.4</v>
       </c>
       <c r="D2">
         <v>0.09</v>

</xml_diff>

<commit_message>
Update for report's results
</commit_message>
<xml_diff>
--- a/Data/MetaData.xlsx
+++ b/Data/MetaData.xlsx
@@ -78,13 +78,14 @@
     <sheet name="Shirini" sheetId="1025" r:id="rId64"/>
     <sheet name="Biscuit" sheetId="1026" r:id="rId65"/>
     <sheet name="Khoshkbar" sheetId="1027" r:id="rId66"/>
+    <sheet name="Nooshabe" sheetId="1041" r:id="rId67"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15007" uniqueCount="623">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15268" uniqueCount="623">
   <si>
     <t>Year</t>
   </si>
@@ -39627,7 +39628,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -40401,8 +40402,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B235"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B9" sqref="A2:B9"/>
+    <sheetView topLeftCell="A219" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B229" sqref="B229"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -46213,10 +46214,13 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C2"/>
+      <selection activeCell="C3" sqref="A1:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
@@ -66414,7 +66418,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
@@ -68762,8 +68766,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="J42" sqref="J42"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G14" sqref="A1:L35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -69904,6 +69908,1184 @@
       </c>
       <c r="D35">
         <v>11662</v>
+      </c>
+      <c r="E35" t="s">
+        <v>66</v>
+      </c>
+      <c r="F35" t="s">
+        <v>67</v>
+      </c>
+      <c r="G35" t="s">
+        <v>277</v>
+      </c>
+      <c r="I35" t="s">
+        <v>68</v>
+      </c>
+      <c r="J35" t="s">
+        <v>69</v>
+      </c>
+      <c r="K35" t="s">
+        <v>70</v>
+      </c>
+      <c r="L35" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet67.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L35"/>
+  <sheetViews>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>269</v>
+      </c>
+      <c r="C1" t="s">
+        <v>291</v>
+      </c>
+      <c r="D1" t="s">
+        <v>292</v>
+      </c>
+      <c r="E1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G1" t="s">
+        <v>300</v>
+      </c>
+      <c r="H1" t="s">
+        <v>309</v>
+      </c>
+      <c r="I1" t="s">
+        <v>301</v>
+      </c>
+      <c r="J1" t="s">
+        <v>302</v>
+      </c>
+      <c r="K1" t="s">
+        <v>303</v>
+      </c>
+      <c r="L1" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2">
+        <v>63</v>
+      </c>
+      <c r="B2" t="s">
+        <v>299</v>
+      </c>
+      <c r="C2">
+        <v>12211</v>
+      </c>
+      <c r="D2">
+        <v>12216</v>
+      </c>
+      <c r="E2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F2" t="s">
+        <v>274</v>
+      </c>
+      <c r="G2" t="s">
+        <v>304</v>
+      </c>
+      <c r="J2" t="s">
+        <v>306</v>
+      </c>
+      <c r="L2" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3">
+        <v>64</v>
+      </c>
+      <c r="B3" t="s">
+        <v>299</v>
+      </c>
+      <c r="C3">
+        <v>12211</v>
+      </c>
+      <c r="D3">
+        <v>12216</v>
+      </c>
+      <c r="E3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F3" t="s">
+        <v>274</v>
+      </c>
+      <c r="G3" t="s">
+        <v>304</v>
+      </c>
+      <c r="J3" t="s">
+        <v>306</v>
+      </c>
+      <c r="L3" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4">
+        <v>65</v>
+      </c>
+      <c r="B4" t="s">
+        <v>299</v>
+      </c>
+      <c r="C4">
+        <v>12211</v>
+      </c>
+      <c r="D4">
+        <v>12216</v>
+      </c>
+      <c r="E4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F4" t="s">
+        <v>274</v>
+      </c>
+      <c r="G4" t="s">
+        <v>304</v>
+      </c>
+      <c r="J4" t="s">
+        <v>306</v>
+      </c>
+      <c r="L4" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5">
+        <v>66</v>
+      </c>
+      <c r="B5" t="s">
+        <v>299</v>
+      </c>
+      <c r="C5">
+        <v>12211</v>
+      </c>
+      <c r="D5">
+        <v>12216</v>
+      </c>
+      <c r="E5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F5" t="s">
+        <v>274</v>
+      </c>
+      <c r="G5" t="s">
+        <v>304</v>
+      </c>
+      <c r="J5" t="s">
+        <v>306</v>
+      </c>
+      <c r="L5" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6">
+        <v>67</v>
+      </c>
+      <c r="B6" t="s">
+        <v>299</v>
+      </c>
+      <c r="C6">
+        <v>12211</v>
+      </c>
+      <c r="D6">
+        <v>12216</v>
+      </c>
+      <c r="E6" t="s">
+        <v>51</v>
+      </c>
+      <c r="F6" t="s">
+        <v>274</v>
+      </c>
+      <c r="G6" t="s">
+        <v>304</v>
+      </c>
+      <c r="J6" t="s">
+        <v>306</v>
+      </c>
+      <c r="L6" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7">
+        <v>68</v>
+      </c>
+      <c r="B7" t="s">
+        <v>299</v>
+      </c>
+      <c r="C7">
+        <v>12211</v>
+      </c>
+      <c r="D7">
+        <v>12216</v>
+      </c>
+      <c r="E7" t="s">
+        <v>51</v>
+      </c>
+      <c r="F7" t="s">
+        <v>274</v>
+      </c>
+      <c r="G7" t="s">
+        <v>304</v>
+      </c>
+      <c r="J7" t="s">
+        <v>306</v>
+      </c>
+      <c r="L7" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8">
+        <v>69</v>
+      </c>
+      <c r="B8" t="s">
+        <v>299</v>
+      </c>
+      <c r="C8">
+        <v>12211</v>
+      </c>
+      <c r="D8">
+        <v>12216</v>
+      </c>
+      <c r="E8" t="s">
+        <v>51</v>
+      </c>
+      <c r="F8" t="s">
+        <v>274</v>
+      </c>
+      <c r="G8" t="s">
+        <v>304</v>
+      </c>
+      <c r="H8" t="s">
+        <v>275</v>
+      </c>
+      <c r="J8" t="s">
+        <v>308</v>
+      </c>
+      <c r="K8" t="s">
+        <v>305</v>
+      </c>
+      <c r="L8" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9">
+        <v>70</v>
+      </c>
+      <c r="B9" t="s">
+        <v>299</v>
+      </c>
+      <c r="C9">
+        <v>12211</v>
+      </c>
+      <c r="D9">
+        <v>12216</v>
+      </c>
+      <c r="E9" t="s">
+        <v>51</v>
+      </c>
+      <c r="F9" t="s">
+        <v>274</v>
+      </c>
+      <c r="G9" t="s">
+        <v>304</v>
+      </c>
+      <c r="H9" t="s">
+        <v>275</v>
+      </c>
+      <c r="J9" t="s">
+        <v>308</v>
+      </c>
+      <c r="L9" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10">
+        <v>71</v>
+      </c>
+      <c r="B10" t="s">
+        <v>299</v>
+      </c>
+      <c r="C10">
+        <v>12211</v>
+      </c>
+      <c r="D10">
+        <v>12216</v>
+      </c>
+      <c r="E10" t="s">
+        <v>51</v>
+      </c>
+      <c r="F10" t="s">
+        <v>274</v>
+      </c>
+      <c r="G10" t="s">
+        <v>304</v>
+      </c>
+      <c r="H10" t="s">
+        <v>275</v>
+      </c>
+      <c r="J10" t="s">
+        <v>308</v>
+      </c>
+      <c r="L10" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11">
+        <v>72</v>
+      </c>
+      <c r="B11" t="s">
+        <v>299</v>
+      </c>
+      <c r="C11">
+        <v>12211</v>
+      </c>
+      <c r="D11">
+        <v>12216</v>
+      </c>
+      <c r="E11" t="s">
+        <v>51</v>
+      </c>
+      <c r="F11" t="s">
+        <v>274</v>
+      </c>
+      <c r="G11" t="s">
+        <v>304</v>
+      </c>
+      <c r="H11" t="s">
+        <v>275</v>
+      </c>
+      <c r="J11" t="s">
+        <v>308</v>
+      </c>
+      <c r="K11" t="s">
+        <v>305</v>
+      </c>
+      <c r="L11" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12">
+        <v>73</v>
+      </c>
+      <c r="B12" t="s">
+        <v>299</v>
+      </c>
+      <c r="C12">
+        <v>12211</v>
+      </c>
+      <c r="D12">
+        <v>12216</v>
+      </c>
+      <c r="E12" t="s">
+        <v>51</v>
+      </c>
+      <c r="F12" t="s">
+        <v>274</v>
+      </c>
+      <c r="G12" t="s">
+        <v>304</v>
+      </c>
+      <c r="H12" t="s">
+        <v>275</v>
+      </c>
+      <c r="J12" t="s">
+        <v>308</v>
+      </c>
+      <c r="K12" t="s">
+        <v>305</v>
+      </c>
+      <c r="L12" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13">
+        <v>74</v>
+      </c>
+      <c r="B13" t="s">
+        <v>299</v>
+      </c>
+      <c r="C13">
+        <v>12211</v>
+      </c>
+      <c r="D13">
+        <v>12216</v>
+      </c>
+      <c r="E13" t="s">
+        <v>51</v>
+      </c>
+      <c r="F13" t="s">
+        <v>274</v>
+      </c>
+      <c r="G13" t="s">
+        <v>304</v>
+      </c>
+      <c r="J13" t="s">
+        <v>306</v>
+      </c>
+      <c r="K13" t="s">
+        <v>289</v>
+      </c>
+      <c r="L13" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14">
+        <v>75</v>
+      </c>
+      <c r="B14" t="s">
+        <v>299</v>
+      </c>
+      <c r="C14">
+        <v>12211</v>
+      </c>
+      <c r="D14">
+        <v>12216</v>
+      </c>
+      <c r="E14" t="s">
+        <v>51</v>
+      </c>
+      <c r="F14" t="s">
+        <v>274</v>
+      </c>
+      <c r="G14" t="s">
+        <v>304</v>
+      </c>
+      <c r="J14" t="s">
+        <v>306</v>
+      </c>
+      <c r="K14" t="s">
+        <v>289</v>
+      </c>
+      <c r="L14" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15">
+        <v>76</v>
+      </c>
+      <c r="B15" t="s">
+        <v>299</v>
+      </c>
+      <c r="C15">
+        <v>12211</v>
+      </c>
+      <c r="D15">
+        <v>12216</v>
+      </c>
+      <c r="E15" t="s">
+        <v>51</v>
+      </c>
+      <c r="F15" t="s">
+        <v>274</v>
+      </c>
+      <c r="G15" t="s">
+        <v>304</v>
+      </c>
+      <c r="J15" t="s">
+        <v>306</v>
+      </c>
+      <c r="K15" t="s">
+        <v>289</v>
+      </c>
+      <c r="L15" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16">
+        <v>77</v>
+      </c>
+      <c r="B16" t="s">
+        <v>299</v>
+      </c>
+      <c r="C16">
+        <v>12211</v>
+      </c>
+      <c r="D16">
+        <v>12216</v>
+      </c>
+      <c r="E16" t="s">
+        <v>51</v>
+      </c>
+      <c r="F16" t="s">
+        <v>274</v>
+      </c>
+      <c r="G16" t="s">
+        <v>304</v>
+      </c>
+      <c r="J16" t="s">
+        <v>306</v>
+      </c>
+      <c r="K16" t="s">
+        <v>289</v>
+      </c>
+      <c r="L16" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17">
+        <v>78</v>
+      </c>
+      <c r="B17" t="s">
+        <v>299</v>
+      </c>
+      <c r="C17">
+        <v>12211</v>
+      </c>
+      <c r="D17">
+        <v>12216</v>
+      </c>
+      <c r="E17" t="s">
+        <v>51</v>
+      </c>
+      <c r="F17" t="s">
+        <v>274</v>
+      </c>
+      <c r="G17" t="s">
+        <v>304</v>
+      </c>
+      <c r="J17" t="s">
+        <v>306</v>
+      </c>
+      <c r="K17" t="s">
+        <v>289</v>
+      </c>
+      <c r="L17" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18">
+        <v>79</v>
+      </c>
+      <c r="B18" t="s">
+        <v>299</v>
+      </c>
+      <c r="C18">
+        <v>12211</v>
+      </c>
+      <c r="D18">
+        <v>12216</v>
+      </c>
+      <c r="E18" t="s">
+        <v>51</v>
+      </c>
+      <c r="F18" t="s">
+        <v>274</v>
+      </c>
+      <c r="G18" t="s">
+        <v>304</v>
+      </c>
+      <c r="J18" t="s">
+        <v>306</v>
+      </c>
+      <c r="K18" t="s">
+        <v>289</v>
+      </c>
+      <c r="L18" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19">
+        <v>80</v>
+      </c>
+      <c r="B19" t="s">
+        <v>299</v>
+      </c>
+      <c r="C19">
+        <v>12211</v>
+      </c>
+      <c r="D19">
+        <v>12216</v>
+      </c>
+      <c r="E19" t="s">
+        <v>51</v>
+      </c>
+      <c r="F19" t="s">
+        <v>274</v>
+      </c>
+      <c r="G19" t="s">
+        <v>304</v>
+      </c>
+      <c r="J19" t="s">
+        <v>306</v>
+      </c>
+      <c r="K19" t="s">
+        <v>289</v>
+      </c>
+      <c r="L19" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20">
+        <v>81</v>
+      </c>
+      <c r="B20" t="s">
+        <v>299</v>
+      </c>
+      <c r="C20">
+        <v>12211</v>
+      </c>
+      <c r="D20">
+        <v>12216</v>
+      </c>
+      <c r="E20" t="s">
+        <v>51</v>
+      </c>
+      <c r="F20" t="s">
+        <v>274</v>
+      </c>
+      <c r="G20" t="s">
+        <v>304</v>
+      </c>
+      <c r="J20" t="s">
+        <v>306</v>
+      </c>
+      <c r="K20" t="s">
+        <v>289</v>
+      </c>
+      <c r="L20" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21">
+        <v>82</v>
+      </c>
+      <c r="B21" t="s">
+        <v>299</v>
+      </c>
+      <c r="C21">
+        <v>12211</v>
+      </c>
+      <c r="D21">
+        <v>12216</v>
+      </c>
+      <c r="E21" t="s">
+        <v>51</v>
+      </c>
+      <c r="F21" t="s">
+        <v>274</v>
+      </c>
+      <c r="G21" t="s">
+        <v>304</v>
+      </c>
+      <c r="J21" t="s">
+        <v>306</v>
+      </c>
+      <c r="K21" t="s">
+        <v>289</v>
+      </c>
+      <c r="L21" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22">
+        <v>83</v>
+      </c>
+      <c r="B22" t="s">
+        <v>299</v>
+      </c>
+      <c r="C22">
+        <v>12211</v>
+      </c>
+      <c r="D22">
+        <v>12216</v>
+      </c>
+      <c r="E22" t="s">
+        <v>51</v>
+      </c>
+      <c r="F22" t="s">
+        <v>274</v>
+      </c>
+      <c r="G22" t="s">
+        <v>304</v>
+      </c>
+      <c r="I22" t="s">
+        <v>275</v>
+      </c>
+      <c r="J22" t="s">
+        <v>285</v>
+      </c>
+      <c r="K22" t="s">
+        <v>289</v>
+      </c>
+      <c r="L22" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="A23">
+        <v>84</v>
+      </c>
+      <c r="B23" t="s">
+        <v>299</v>
+      </c>
+      <c r="C23">
+        <v>12211</v>
+      </c>
+      <c r="D23">
+        <v>12216</v>
+      </c>
+      <c r="E23" t="s">
+        <v>66</v>
+      </c>
+      <c r="F23" t="s">
+        <v>67</v>
+      </c>
+      <c r="G23" t="s">
+        <v>277</v>
+      </c>
+      <c r="I23" t="s">
+        <v>68</v>
+      </c>
+      <c r="J23" t="s">
+        <v>69</v>
+      </c>
+      <c r="K23" t="s">
+        <v>70</v>
+      </c>
+      <c r="L23" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="A24">
+        <v>85</v>
+      </c>
+      <c r="B24" t="s">
+        <v>299</v>
+      </c>
+      <c r="C24">
+        <v>12211</v>
+      </c>
+      <c r="D24">
+        <v>12216</v>
+      </c>
+      <c r="E24" t="s">
+        <v>51</v>
+      </c>
+      <c r="F24" t="s">
+        <v>67</v>
+      </c>
+      <c r="G24" t="s">
+        <v>277</v>
+      </c>
+      <c r="I24" t="s">
+        <v>68</v>
+      </c>
+      <c r="J24" t="s">
+        <v>69</v>
+      </c>
+      <c r="K24" t="s">
+        <v>70</v>
+      </c>
+      <c r="L24" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="A25">
+        <v>86</v>
+      </c>
+      <c r="B25" t="s">
+        <v>299</v>
+      </c>
+      <c r="C25">
+        <v>12211</v>
+      </c>
+      <c r="D25">
+        <v>12216</v>
+      </c>
+      <c r="E25" t="s">
+        <v>66</v>
+      </c>
+      <c r="F25" t="s">
+        <v>67</v>
+      </c>
+      <c r="G25" t="s">
+        <v>277</v>
+      </c>
+      <c r="I25" t="s">
+        <v>68</v>
+      </c>
+      <c r="J25" t="s">
+        <v>69</v>
+      </c>
+      <c r="K25" t="s">
+        <v>70</v>
+      </c>
+      <c r="L25" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="A26">
+        <v>87</v>
+      </c>
+      <c r="B26" t="s">
+        <v>299</v>
+      </c>
+      <c r="C26">
+        <v>12211</v>
+      </c>
+      <c r="D26">
+        <v>12216</v>
+      </c>
+      <c r="E26" t="s">
+        <v>66</v>
+      </c>
+      <c r="F26" t="s">
+        <v>67</v>
+      </c>
+      <c r="G26" t="s">
+        <v>277</v>
+      </c>
+      <c r="I26" t="s">
+        <v>68</v>
+      </c>
+      <c r="J26" t="s">
+        <v>69</v>
+      </c>
+      <c r="K26" t="s">
+        <v>70</v>
+      </c>
+      <c r="L26" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="A27">
+        <v>88</v>
+      </c>
+      <c r="B27" t="s">
+        <v>299</v>
+      </c>
+      <c r="C27">
+        <v>12211</v>
+      </c>
+      <c r="D27">
+        <v>12216</v>
+      </c>
+      <c r="E27" t="s">
+        <v>66</v>
+      </c>
+      <c r="F27" t="s">
+        <v>67</v>
+      </c>
+      <c r="G27" t="s">
+        <v>277</v>
+      </c>
+      <c r="I27" t="s">
+        <v>68</v>
+      </c>
+      <c r="J27" t="s">
+        <v>69</v>
+      </c>
+      <c r="K27" t="s">
+        <v>70</v>
+      </c>
+      <c r="L27" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
+      <c r="A28">
+        <v>89</v>
+      </c>
+      <c r="B28" t="s">
+        <v>299</v>
+      </c>
+      <c r="C28">
+        <v>12211</v>
+      </c>
+      <c r="D28">
+        <v>12216</v>
+      </c>
+      <c r="E28" t="s">
+        <v>66</v>
+      </c>
+      <c r="F28" t="s">
+        <v>67</v>
+      </c>
+      <c r="G28" t="s">
+        <v>277</v>
+      </c>
+      <c r="I28" t="s">
+        <v>68</v>
+      </c>
+      <c r="J28" t="s">
+        <v>69</v>
+      </c>
+      <c r="K28" t="s">
+        <v>70</v>
+      </c>
+      <c r="L28" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
+      <c r="A29">
+        <v>90</v>
+      </c>
+      <c r="B29" t="s">
+        <v>299</v>
+      </c>
+      <c r="C29">
+        <v>12211</v>
+      </c>
+      <c r="D29">
+        <v>12216</v>
+      </c>
+      <c r="E29" t="s">
+        <v>66</v>
+      </c>
+      <c r="F29" t="s">
+        <v>67</v>
+      </c>
+      <c r="G29" t="s">
+        <v>277</v>
+      </c>
+      <c r="I29" t="s">
+        <v>68</v>
+      </c>
+      <c r="J29" t="s">
+        <v>69</v>
+      </c>
+      <c r="K29" t="s">
+        <v>70</v>
+      </c>
+      <c r="L29" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12">
+      <c r="A30">
+        <v>91</v>
+      </c>
+      <c r="B30" t="s">
+        <v>299</v>
+      </c>
+      <c r="C30">
+        <v>12211</v>
+      </c>
+      <c r="D30">
+        <v>12216</v>
+      </c>
+      <c r="E30" t="s">
+        <v>66</v>
+      </c>
+      <c r="F30" t="s">
+        <v>67</v>
+      </c>
+      <c r="G30" t="s">
+        <v>277</v>
+      </c>
+      <c r="I30" t="s">
+        <v>68</v>
+      </c>
+      <c r="J30" t="s">
+        <v>69</v>
+      </c>
+      <c r="K30" t="s">
+        <v>70</v>
+      </c>
+      <c r="L30" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12">
+      <c r="A31">
+        <v>92</v>
+      </c>
+      <c r="B31" t="s">
+        <v>299</v>
+      </c>
+      <c r="C31">
+        <v>12211</v>
+      </c>
+      <c r="D31">
+        <v>12216</v>
+      </c>
+      <c r="E31" t="s">
+        <v>66</v>
+      </c>
+      <c r="F31" t="s">
+        <v>67</v>
+      </c>
+      <c r="G31" t="s">
+        <v>277</v>
+      </c>
+      <c r="I31" t="s">
+        <v>68</v>
+      </c>
+      <c r="J31" t="s">
+        <v>69</v>
+      </c>
+      <c r="K31" t="s">
+        <v>70</v>
+      </c>
+      <c r="L31" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12">
+      <c r="A32">
+        <v>93</v>
+      </c>
+      <c r="B32" t="s">
+        <v>299</v>
+      </c>
+      <c r="C32">
+        <v>12211</v>
+      </c>
+      <c r="D32">
+        <v>12216</v>
+      </c>
+      <c r="E32" t="s">
+        <v>66</v>
+      </c>
+      <c r="F32" t="s">
+        <v>67</v>
+      </c>
+      <c r="G32" t="s">
+        <v>277</v>
+      </c>
+      <c r="I32" t="s">
+        <v>68</v>
+      </c>
+      <c r="J32" t="s">
+        <v>69</v>
+      </c>
+      <c r="K32" t="s">
+        <v>70</v>
+      </c>
+      <c r="L32" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12">
+      <c r="A33">
+        <v>94</v>
+      </c>
+      <c r="B33" t="s">
+        <v>299</v>
+      </c>
+      <c r="C33">
+        <v>12211</v>
+      </c>
+      <c r="D33">
+        <v>12216</v>
+      </c>
+      <c r="E33" t="s">
+        <v>66</v>
+      </c>
+      <c r="F33" t="s">
+        <v>67</v>
+      </c>
+      <c r="G33" t="s">
+        <v>277</v>
+      </c>
+      <c r="I33" t="s">
+        <v>68</v>
+      </c>
+      <c r="J33" t="s">
+        <v>69</v>
+      </c>
+      <c r="K33" t="s">
+        <v>70</v>
+      </c>
+      <c r="L33" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12">
+      <c r="A34">
+        <v>95</v>
+      </c>
+      <c r="B34" t="s">
+        <v>299</v>
+      </c>
+      <c r="C34">
+        <v>12211</v>
+      </c>
+      <c r="D34">
+        <v>12216</v>
+      </c>
+      <c r="E34" t="s">
+        <v>66</v>
+      </c>
+      <c r="F34" t="s">
+        <v>67</v>
+      </c>
+      <c r="G34" t="s">
+        <v>277</v>
+      </c>
+      <c r="I34" t="s">
+        <v>68</v>
+      </c>
+      <c r="J34" t="s">
+        <v>69</v>
+      </c>
+      <c r="K34" t="s">
+        <v>70</v>
+      </c>
+      <c r="L34" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12">
+      <c r="A35">
+        <v>96</v>
+      </c>
+      <c r="B35" t="s">
+        <v>299</v>
+      </c>
+      <c r="C35">
+        <v>12211</v>
+      </c>
+      <c r="D35">
+        <v>12216</v>
       </c>
       <c r="E35" t="s">
         <v>66</v>

</xml_diff>

<commit_message>
Revert "Initial 97 add"
This reverts commit c39b9f72e1e37250e683b1b510f8e4be7d057471.
</commit_message>
<xml_diff>
--- a/Data/MetaData.xlsx
+++ b/Data/MetaData.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Majid\Documents\GitHub\IRHEIS\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\IRHEIS\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18BE6EF2-E2D1-4855-B15C-0D09E84BEC10}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5511" yWindow="3026" windowWidth="18540" windowHeight="12565" tabRatio="858" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="6600" tabRatio="858" firstSheet="37" activeTab="39"/>
   </bookViews>
   <sheets>
     <sheet name="CompressedFileNames" sheetId="1" r:id="rId1"/>
@@ -80,19 +79,12 @@
     <sheet name="Biscuit" sheetId="1026" r:id="rId65"/>
     <sheet name="Khoshkbar" sheetId="1027" r:id="rId66"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15074" uniqueCount="624">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15007" uniqueCount="623">
   <si>
     <t>Year</t>
   </si>
@@ -1962,19 +1954,16 @@
   <si>
     <t>daily protein</t>
   </si>
-  <si>
-    <t>97.rar</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -1982,7 +1971,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -1990,7 +1979,7 @@
     <font>
       <sz val="18"/>
       <color theme="3"/>
-      <name val="Times New Roman"/>
+      <name val="Calibri Light"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="major"/>
@@ -1999,7 +1988,7 @@
       <b/>
       <sz val="15"/>
       <color theme="3"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -2008,7 +1997,7 @@
       <b/>
       <sz val="13"/>
       <color theme="3"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -2017,7 +2006,7 @@
       <b/>
       <sz val="11"/>
       <color theme="3"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -2025,7 +2014,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -2033,7 +2022,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -2041,7 +2030,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -2049,7 +2038,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -2058,7 +2047,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -2067,7 +2056,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -2075,7 +2064,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -2084,7 +2073,7 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -2092,7 +2081,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -2101,7 +2090,7 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -2110,7 +2099,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -2118,7 +2107,7 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -2126,13 +2115,13 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -2141,7 +2130,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -2597,48 +2586,48 @@
     </xf>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="‏20% - تأکید1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="‏20% - تاکید2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="‏20% - تاکید3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="‏20% - تاکید4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="‏20% - تاکید5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="‏20% - تاکید6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - آکسان 1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="‏40% - تاکید2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="‏40% - تاکید3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="‏40% - تاکید4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="‏40% - تاکید5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="‏40% - تاکید6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="‏60% - تأکید1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="‏60% - تاکید2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="‏60% - تاکید3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="‏60% - تاکید4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="‏60% - تاکید5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="‏60% - تاکید6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="بد" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="بررسی سلول" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="تأکید1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="تاکید2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="تاکید3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="تاکید4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="تاکید5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="تاکید6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="خروجی" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="خنثی" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="خوب" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="سلول پیوندی" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="عنوان" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="عنوان 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="عنوان 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="عنوان 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="عنوان 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="متن توصیفی" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="متن هشدار" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="مجموع" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="محاسبه" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="معمولی" xfId="0" builtinId="0"/>
-    <cellStyle name="ورودی" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="یادداشت" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2915,14 +2904,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B35"/>
   <sheetViews>
     <sheetView topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
@@ -3207,28 +3196,20 @@
         <v>469</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
-      <c r="A36">
-        <v>97</v>
-      </c>
-      <c r="B36" t="s">
-        <v>623</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T41"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="9" max="9" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="15" bestFit="1" customWidth="1" collapsed="1"/>
@@ -5259,14 +5240,14 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S35"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="8" max="8" width="10.5703125" customWidth="1" collapsed="1"/>
     <col min="19" max="19" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
@@ -7046,14 +7027,14 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S35"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="19" max="19" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
@@ -8815,14 +8796,14 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="4" width="9.140625" style="3" collapsed="1"/>
     <col min="5" max="5" width="9.140625" style="3"/>
@@ -9944,14 +9925,14 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="15" bestFit="1" customWidth="1" collapsed="1"/>
@@ -10282,14 +10263,14 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
@@ -11466,14 +11447,14 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
@@ -12281,14 +12262,14 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
@@ -13526,14 +13507,14 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E125"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E125" sqref="E125"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="2" width="11.42578125" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
@@ -15412,14 +15393,14 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
@@ -16366,14 +16347,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:BL36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:BL35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+      <selection activeCell="BI29" sqref="BI28:BI29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.85546875" bestFit="1" customWidth="1"/>
@@ -19797,177 +19778,20 @@
       <c r="BJ35" s="9"/>
       <c r="BK35" s="9"/>
     </row>
-    <row r="36" spans="1:63">
-      <c r="A36" s="9">
-        <v>97</v>
-      </c>
-      <c r="B36" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="C36" s="9" t="s">
-        <v>470</v>
-      </c>
-      <c r="D36" s="9"/>
-      <c r="E36" s="9" t="s">
-        <v>471</v>
-      </c>
-      <c r="F36" s="9" t="s">
-        <v>472</v>
-      </c>
-      <c r="G36" s="9" t="s">
-        <v>473</v>
-      </c>
-      <c r="H36" s="9" t="s">
-        <v>474</v>
-      </c>
-      <c r="I36" s="9" t="s">
-        <v>475</v>
-      </c>
-      <c r="J36" s="9" t="s">
-        <v>476</v>
-      </c>
-      <c r="K36" s="9" t="s">
-        <v>477</v>
-      </c>
-      <c r="L36" s="9" t="s">
-        <v>478</v>
-      </c>
-      <c r="M36" s="9" t="s">
-        <v>479</v>
-      </c>
-      <c r="N36" s="9" t="s">
-        <v>480</v>
-      </c>
-      <c r="O36" s="9" t="s">
-        <v>481</v>
-      </c>
-      <c r="P36" s="9" t="s">
-        <v>482</v>
-      </c>
-      <c r="Q36" s="9" t="s">
-        <v>483</v>
-      </c>
-      <c r="R36" s="9" t="s">
-        <v>484</v>
-      </c>
-      <c r="S36" s="9" t="s">
-        <v>485</v>
-      </c>
-      <c r="T36" s="9" t="s">
-        <v>486</v>
-      </c>
-      <c r="U36" s="9" t="s">
-        <v>487</v>
-      </c>
-      <c r="V36" s="9" t="s">
-        <v>488</v>
-      </c>
-      <c r="W36" s="9" t="s">
-        <v>489</v>
-      </c>
-      <c r="X36" s="9" t="s">
-        <v>490</v>
-      </c>
-      <c r="Y36" s="9" t="s">
-        <v>491</v>
-      </c>
-      <c r="Z36" s="9" t="s">
-        <v>492</v>
-      </c>
-      <c r="AA36" s="9" t="s">
-        <v>493</v>
-      </c>
-      <c r="AB36" s="9" t="s">
-        <v>494</v>
-      </c>
-      <c r="AC36" s="9" t="s">
-        <v>495</v>
-      </c>
-      <c r="AD36" s="9" t="s">
-        <v>496</v>
-      </c>
-      <c r="AE36" s="9" t="s">
-        <v>497</v>
-      </c>
-      <c r="AF36" s="9" t="s">
-        <v>498</v>
-      </c>
-      <c r="AG36" s="9" t="s">
-        <v>499</v>
-      </c>
-      <c r="AH36" s="9" t="s">
-        <v>500</v>
-      </c>
-      <c r="AI36" s="9" t="s">
-        <v>501</v>
-      </c>
-      <c r="AJ36" s="9" t="s">
-        <v>502</v>
-      </c>
-      <c r="AK36" s="9" t="s">
-        <v>503</v>
-      </c>
-      <c r="AL36" s="9" t="s">
-        <v>504</v>
-      </c>
-      <c r="AM36" s="9" t="s">
-        <v>505</v>
-      </c>
-      <c r="AN36" s="9" t="s">
-        <v>506</v>
-      </c>
-      <c r="AO36" s="9" t="s">
-        <v>507</v>
-      </c>
-      <c r="AP36" s="9" t="s">
-        <v>508</v>
-      </c>
-      <c r="AQ36" s="9" t="s">
-        <v>509</v>
-      </c>
-      <c r="AR36" s="9" t="s">
-        <v>510</v>
-      </c>
-      <c r="AS36" s="9" t="s">
-        <v>511</v>
-      </c>
-      <c r="AT36" s="9" t="s">
-        <v>512</v>
-      </c>
-      <c r="AU36" s="9" t="s">
-        <v>513</v>
-      </c>
-      <c r="AV36" s="9"/>
-      <c r="AW36" s="9"/>
-      <c r="AX36" s="9"/>
-      <c r="AY36" s="9"/>
-      <c r="AZ36" s="9"/>
-      <c r="BA36" s="9"/>
-      <c r="BB36" s="9"/>
-      <c r="BC36" s="9"/>
-      <c r="BD36" s="9"/>
-      <c r="BE36" s="9"/>
-      <c r="BF36" s="9"/>
-      <c r="BG36" s="9"/>
-      <c r="BH36" s="9"/>
-      <c r="BI36" s="9"/>
-      <c r="BJ36" s="9"/>
-      <c r="BK36" s="9"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="I13" sqref="I1:J13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
@@ -20914,14 +20738,14 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="10" max="10" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
@@ -22034,14 +21858,14 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="8" max="9" width="14.140625" customWidth="1" collapsed="1"/>
@@ -22784,14 +22608,14 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView topLeftCell="A11" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
       <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
@@ -23778,14 +23602,14 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
@@ -24527,14 +24351,14 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="M29" sqref="M29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
@@ -25396,14 +25220,14 @@
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
@@ -26265,14 +26089,14 @@
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="B32" sqref="A1:J35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
@@ -27014,14 +26838,14 @@
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="8" max="8" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="16.5703125" customWidth="1" collapsed="1"/>
@@ -28728,14 +28552,14 @@
 </file>
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="B21" sqref="B20:B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
@@ -29596,14 +29420,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:R36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R35"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:18">
       <c r="A1" t="s">
@@ -30920,41 +30744,6 @@
         <v>74</v>
       </c>
       <c r="N35" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14">
-      <c r="A36">
-        <v>97</v>
-      </c>
-      <c r="B36" t="s">
-        <v>66</v>
-      </c>
-      <c r="C36" t="s">
-        <v>67</v>
-      </c>
-      <c r="D36" t="s">
-        <v>68</v>
-      </c>
-      <c r="E36" t="s">
-        <v>69</v>
-      </c>
-      <c r="F36" t="s">
-        <v>70</v>
-      </c>
-      <c r="G36" t="s">
-        <v>71</v>
-      </c>
-      <c r="K36" t="s">
-        <v>72</v>
-      </c>
-      <c r="L36" t="s">
-        <v>73</v>
-      </c>
-      <c r="M36" t="s">
-        <v>74</v>
-      </c>
-      <c r="N36" t="s">
         <v>75</v>
       </c>
     </row>
@@ -30964,14 +30753,14 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="B34" sqref="B33:J35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
@@ -31832,14 +31621,14 @@
 </file>
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
@@ -32749,14 +32538,14 @@
 </file>
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="I41" sqref="I41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
@@ -33564,14 +33353,14 @@
 </file>
 
 <file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K35"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="I46" sqref="I46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="2" width="9.140625" style="3" collapsed="1"/>
     <col min="3" max="3" width="9.7109375" style="3" bestFit="1" customWidth="1" collapsed="1"/>
@@ -34684,14 +34473,14 @@
 </file>
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
@@ -35432,14 +35221,14 @@
 </file>
 
 <file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="3" t="s">
@@ -36177,14 +35966,14 @@
 </file>
 
 <file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="3" t="s">
@@ -36922,14 +36711,14 @@
 </file>
 
 <file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="3" t="s">
@@ -37667,14 +37456,14 @@
 </file>
 
 <file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
@@ -38431,14 +38220,14 @@
 </file>
 
 <file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="4" t="s">
@@ -39156,14 +38945,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="96.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
@@ -39834,14 +39623,14 @@
 </file>
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="2" width="14" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.140625" style="8"/>
@@ -40109,14 +39898,14 @@
 </file>
 
 <file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
@@ -40124,7 +39913,7 @@
     <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="14.6" thickBot="1">
+    <row r="1" spans="1:10" ht="15.75" thickBot="1">
       <c r="A1" s="15"/>
       <c r="B1" s="3" t="s">
         <v>620</v>
@@ -40142,7 +39931,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="14.6" thickBot="1">
+    <row r="2" spans="1:10" ht="15.75" thickBot="1">
       <c r="A2" s="10" t="s">
         <v>601</v>
       </c>
@@ -40171,7 +39960,7 @@
         <v>0.10124999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="14.6" thickBot="1">
+    <row r="3" spans="1:10" ht="15.75" thickBot="1">
       <c r="A3" s="11" t="s">
         <v>602</v>
       </c>
@@ -40200,7 +39989,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="14.6" thickBot="1">
+    <row r="4" spans="1:10" ht="15.75" thickBot="1">
       <c r="A4" s="11" t="s">
         <v>603</v>
       </c>
@@ -40229,7 +40018,7 @@
         <v>6.4285714285714293E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="14.6" thickBot="1">
+    <row r="5" spans="1:10" ht="15.75" thickBot="1">
       <c r="A5" s="11" t="s">
         <v>615</v>
       </c>
@@ -40258,7 +40047,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="14.6" thickBot="1">
+    <row r="6" spans="1:10" ht="15.75" thickBot="1">
       <c r="A6" s="11" t="s">
         <v>604</v>
       </c>
@@ -40287,7 +40076,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="14.6" thickBot="1">
+    <row r="7" spans="1:10" ht="15.75" thickBot="1">
       <c r="A7" s="11" t="s">
         <v>605</v>
       </c>
@@ -40316,7 +40105,7 @@
         <v>3.214285714285714E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="14.6" thickBot="1">
+    <row r="8" spans="1:10" ht="15.75" thickBot="1">
       <c r="A8" s="11" t="s">
         <v>606</v>
       </c>
@@ -40345,7 +40134,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="14.6" thickBot="1">
+    <row r="9" spans="1:10" ht="29.25" thickBot="1">
       <c r="A9" s="11" t="s">
         <v>608</v>
       </c>
@@ -40374,7 +40163,7 @@
         <v>0.22500000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="14.6" thickBot="1">
+    <row r="10" spans="1:10" ht="15.75" thickBot="1">
       <c r="A10" s="11" t="s">
         <v>616</v>
       </c>
@@ -40403,7 +40192,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="14.6" thickBot="1">
+    <row r="11" spans="1:10" ht="15.75" thickBot="1">
       <c r="A11" s="11" t="s">
         <v>609</v>
       </c>
@@ -40432,7 +40221,7 @@
         <v>8.8235294117647051E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="14.6" thickBot="1">
+    <row r="12" spans="1:10" ht="15.75" thickBot="1">
       <c r="A12" s="11" t="s">
         <v>607</v>
       </c>
@@ -40461,7 +40250,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="14.6" thickBot="1">
+    <row r="13" spans="1:10" ht="15.75" thickBot="1">
       <c r="A13" s="11" t="s">
         <v>617</v>
       </c>
@@ -40487,7 +40276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="28.75" thickBot="1">
+    <row r="14" spans="1:10" ht="29.25" thickBot="1">
       <c r="A14" s="11" t="s">
         <v>611</v>
       </c>
@@ -40516,7 +40305,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="28.75" thickBot="1">
+    <row r="15" spans="1:10" ht="29.25" thickBot="1">
       <c r="A15" s="11" t="s">
         <v>612</v>
       </c>
@@ -40545,7 +40334,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="14.6" thickBot="1">
+    <row r="16" spans="1:10" ht="15.75" thickBot="1">
       <c r="A16" s="11" t="s">
         <v>613</v>
       </c>
@@ -40571,7 +40360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="14.6" thickBot="1">
+    <row r="17" spans="1:10" ht="15.75" thickBot="1">
       <c r="A17" s="11" t="s">
         <v>614</v>
       </c>
@@ -40597,7 +40386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="14.6" thickBot="1">
+    <row r="18" spans="1:10" ht="15.75" thickBot="1">
       <c r="A18" s="11"/>
       <c r="B18" s="12"/>
       <c r="C18" s="12"/>
@@ -40609,14 +40398,14 @@
 </file>
 
 <file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B235"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B9" sqref="A2:B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -42507,14 +42296,14 @@
 </file>
 
 <file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="C35" sqref="C35:D35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
@@ -43456,14 +43245,14 @@
 </file>
 
 <file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
@@ -44444,14 +44233,14 @@
 </file>
 
 <file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
@@ -45432,14 +45221,14 @@
 </file>
 
 <file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
@@ -46420,14 +46209,14 @@
 </file>
 
 <file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
@@ -46468,14 +46257,14 @@
 </file>
 
 <file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="E35" sqref="E35:L35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="12" max="12" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
@@ -47645,14 +47434,14 @@
 </file>
 
 <file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -48819,12 +48608,12 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D97"/>
   <sheetViews>
     <sheetView topLeftCell="A85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
@@ -50052,14 +49841,14 @@
 </file>
 
 <file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -51226,14 +51015,14 @@
 </file>
 
 <file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -52400,14 +52189,14 @@
 </file>
 
 <file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="12" max="12" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -53577,14 +53366,14 @@
 </file>
 
 <file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -54751,14 +54540,14 @@
 </file>
 
 <file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -55925,14 +55714,14 @@
 </file>
 
 <file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -57099,14 +56888,14 @@
 </file>
 
 <file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -58273,14 +58062,14 @@
 </file>
 
 <file path=xl/worksheets/sheet57.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -59447,14 +59236,14 @@
 </file>
 
 <file path=xl/worksheets/sheet58.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -60621,14 +60410,14 @@
 </file>
 
 <file path=xl/worksheets/sheet59.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="12" max="12" width="25.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
@@ -61798,14 +61587,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
@@ -61926,14 +61715,14 @@
 </file>
 
 <file path=xl/worksheets/sheet60.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -63100,14 +62889,14 @@
 </file>
 
 <file path=xl/worksheets/sheet61.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -64274,14 +64063,14 @@
 </file>
 
 <file path=xl/worksheets/sheet62.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="P30" sqref="P30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -65448,14 +65237,14 @@
 </file>
 
 <file path=xl/worksheets/sheet63.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -66622,14 +66411,14 @@
 </file>
 
 <file path=xl/worksheets/sheet64.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -67796,14 +67585,14 @@
 </file>
 
 <file path=xl/worksheets/sheet65.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -68970,14 +68759,14 @@
 </file>
 
 <file path=xl/worksheets/sheet66.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="J42" sqref="J42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -70144,14 +69933,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:H36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
@@ -71018,32 +70807,6 @@
         <v>66</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
-      <c r="A36">
-        <v>97</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>321</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>321</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>322</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>322</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>323</v>
-      </c>
-      <c r="G36" s="2" t="s">
-        <v>324</v>
-      </c>
-      <c r="H36" t="s">
-        <v>66</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -71051,14 +70814,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:G36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
@@ -71655,23 +71418,6 @@
         <v>67</v>
       </c>
       <c r="E35" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
-      <c r="A36">
-        <v>97</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>321</v>
-      </c>
-      <c r="C36" t="s">
-        <v>66</v>
-      </c>
-      <c r="D36" t="s">
-        <v>67</v>
-      </c>
-      <c r="E36" t="s">
         <v>277</v>
       </c>
     </row>
@@ -71682,14 +71428,14 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T41"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="12" bestFit="1" customWidth="1" collapsed="1"/>

</xml_diff>

<commit_message>
Revert "Revert "Initial 97 add""
This reverts commit b49765ad0cfa24eafcc5b3ceabdfe27e4f45dda6.
</commit_message>
<xml_diff>
--- a/Data/MetaData.xlsx
+++ b/Data/MetaData.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\IRHEIS\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Majid\Documents\GitHub\IRHEIS\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18BE6EF2-E2D1-4855-B15C-0D09E84BEC10}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="6600" tabRatio="858" firstSheet="37" activeTab="39"/>
+    <workbookView xWindow="5511" yWindow="3026" windowWidth="18540" windowHeight="12565" tabRatio="858" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CompressedFileNames" sheetId="1" r:id="rId1"/>
@@ -79,12 +80,19 @@
     <sheet name="Biscuit" sheetId="1026" r:id="rId65"/>
     <sheet name="Khoshkbar" sheetId="1027" r:id="rId66"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15007" uniqueCount="623">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15074" uniqueCount="624">
   <si>
     <t>Year</t>
   </si>
@@ -1954,16 +1962,19 @@
   <si>
     <t>daily protein</t>
   </si>
+  <si>
+    <t>97.rar</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -1971,7 +1982,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -1979,7 +1990,7 @@
     <font>
       <sz val="18"/>
       <color theme="3"/>
-      <name val="Calibri Light"/>
+      <name val="Times New Roman"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="major"/>
@@ -1988,7 +1999,7 @@
       <b/>
       <sz val="15"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -1997,7 +2008,7 @@
       <b/>
       <sz val="13"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -2006,7 +2017,7 @@
       <b/>
       <sz val="11"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -2014,7 +2025,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -2022,7 +2033,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -2030,7 +2041,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -2038,7 +2049,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -2047,7 +2058,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -2056,7 +2067,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -2064,7 +2075,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -2073,7 +2084,7 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -2081,7 +2092,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -2090,7 +2101,7 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -2099,7 +2110,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -2107,7 +2118,7 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -2115,13 +2126,13 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -2130,7 +2141,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -2586,48 +2597,48 @@
     </xf>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="‏20% - تأکید1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="‏20% - تاکید2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="‏20% - تاکید3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="‏20% - تاکید4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="‏20% - تاکید5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="‏20% - تاکید6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - آکسان 1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="‏40% - تاکید2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="‏40% - تاکید3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="‏40% - تاکید4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="‏40% - تاکید5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="‏40% - تاکید6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="‏60% - تأکید1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="‏60% - تاکید2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="‏60% - تاکید3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="‏60% - تاکید4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="‏60% - تاکید5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="‏60% - تاکید6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="بد" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="بررسی سلول" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="تأکید1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="تاکید2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="تاکید3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="تاکید4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="تاکید5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="تاکید6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="خروجی" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="خنثی" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="خوب" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="سلول پیوندی" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="عنوان" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="عنوان 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="عنوان 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="عنوان 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="عنوان 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="متن توصیفی" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="متن هشدار" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="مجموع" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="محاسبه" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="معمولی" xfId="0" builtinId="0"/>
+    <cellStyle name="ورودی" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="یادداشت" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2904,14 +2915,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B35"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
     <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
@@ -3196,20 +3207,28 @@
         <v>469</v>
       </c>
     </row>
+    <row r="36" spans="1:2">
+      <c r="A36">
+        <v>97</v>
+      </c>
+      <c r="B36" t="s">
+        <v>623</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:T41"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
     <col min="9" max="9" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="15" bestFit="1" customWidth="1" collapsed="1"/>
@@ -5240,14 +5259,14 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:S35"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
     <col min="8" max="8" width="10.5703125" customWidth="1" collapsed="1"/>
     <col min="19" max="19" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
@@ -7027,14 +7046,14 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:S35"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="19" max="19" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
@@ -8796,14 +8815,14 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
     <col min="1" max="4" width="9.140625" style="3" collapsed="1"/>
     <col min="5" max="5" width="9.140625" style="3"/>
@@ -9925,14 +9944,14 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
     <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="15" bestFit="1" customWidth="1" collapsed="1"/>
@@ -10263,14 +10282,14 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
     <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
@@ -11447,14 +11466,14 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
     <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
@@ -12262,14 +12281,14 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:K35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
@@ -13507,14 +13526,14 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:E125"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E125" sqref="E125"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
     <col min="1" max="2" width="11.42578125" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
@@ -15393,14 +15412,14 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
     <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
@@ -16347,14 +16366,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BL35"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:BL36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="BI29" sqref="BI28:BI29"/>
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
     <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.85546875" bestFit="1" customWidth="1"/>
@@ -19778,20 +19797,177 @@
       <c r="BJ35" s="9"/>
       <c r="BK35" s="9"/>
     </row>
+    <row r="36" spans="1:63">
+      <c r="A36" s="9">
+        <v>97</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>470</v>
+      </c>
+      <c r="D36" s="9"/>
+      <c r="E36" s="9" t="s">
+        <v>471</v>
+      </c>
+      <c r="F36" s="9" t="s">
+        <v>472</v>
+      </c>
+      <c r="G36" s="9" t="s">
+        <v>473</v>
+      </c>
+      <c r="H36" s="9" t="s">
+        <v>474</v>
+      </c>
+      <c r="I36" s="9" t="s">
+        <v>475</v>
+      </c>
+      <c r="J36" s="9" t="s">
+        <v>476</v>
+      </c>
+      <c r="K36" s="9" t="s">
+        <v>477</v>
+      </c>
+      <c r="L36" s="9" t="s">
+        <v>478</v>
+      </c>
+      <c r="M36" s="9" t="s">
+        <v>479</v>
+      </c>
+      <c r="N36" s="9" t="s">
+        <v>480</v>
+      </c>
+      <c r="O36" s="9" t="s">
+        <v>481</v>
+      </c>
+      <c r="P36" s="9" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q36" s="9" t="s">
+        <v>483</v>
+      </c>
+      <c r="R36" s="9" t="s">
+        <v>484</v>
+      </c>
+      <c r="S36" s="9" t="s">
+        <v>485</v>
+      </c>
+      <c r="T36" s="9" t="s">
+        <v>486</v>
+      </c>
+      <c r="U36" s="9" t="s">
+        <v>487</v>
+      </c>
+      <c r="V36" s="9" t="s">
+        <v>488</v>
+      </c>
+      <c r="W36" s="9" t="s">
+        <v>489</v>
+      </c>
+      <c r="X36" s="9" t="s">
+        <v>490</v>
+      </c>
+      <c r="Y36" s="9" t="s">
+        <v>491</v>
+      </c>
+      <c r="Z36" s="9" t="s">
+        <v>492</v>
+      </c>
+      <c r="AA36" s="9" t="s">
+        <v>493</v>
+      </c>
+      <c r="AB36" s="9" t="s">
+        <v>494</v>
+      </c>
+      <c r="AC36" s="9" t="s">
+        <v>495</v>
+      </c>
+      <c r="AD36" s="9" t="s">
+        <v>496</v>
+      </c>
+      <c r="AE36" s="9" t="s">
+        <v>497</v>
+      </c>
+      <c r="AF36" s="9" t="s">
+        <v>498</v>
+      </c>
+      <c r="AG36" s="9" t="s">
+        <v>499</v>
+      </c>
+      <c r="AH36" s="9" t="s">
+        <v>500</v>
+      </c>
+      <c r="AI36" s="9" t="s">
+        <v>501</v>
+      </c>
+      <c r="AJ36" s="9" t="s">
+        <v>502</v>
+      </c>
+      <c r="AK36" s="9" t="s">
+        <v>503</v>
+      </c>
+      <c r="AL36" s="9" t="s">
+        <v>504</v>
+      </c>
+      <c r="AM36" s="9" t="s">
+        <v>505</v>
+      </c>
+      <c r="AN36" s="9" t="s">
+        <v>506</v>
+      </c>
+      <c r="AO36" s="9" t="s">
+        <v>507</v>
+      </c>
+      <c r="AP36" s="9" t="s">
+        <v>508</v>
+      </c>
+      <c r="AQ36" s="9" t="s">
+        <v>509</v>
+      </c>
+      <c r="AR36" s="9" t="s">
+        <v>510</v>
+      </c>
+      <c r="AS36" s="9" t="s">
+        <v>511</v>
+      </c>
+      <c r="AT36" s="9" t="s">
+        <v>512</v>
+      </c>
+      <c r="AU36" s="9" t="s">
+        <v>513</v>
+      </c>
+      <c r="AV36" s="9"/>
+      <c r="AW36" s="9"/>
+      <c r="AX36" s="9"/>
+      <c r="AY36" s="9"/>
+      <c r="AZ36" s="9"/>
+      <c r="BA36" s="9"/>
+      <c r="BB36" s="9"/>
+      <c r="BC36" s="9"/>
+      <c r="BD36" s="9"/>
+      <c r="BE36" s="9"/>
+      <c r="BF36" s="9"/>
+      <c r="BG36" s="9"/>
+      <c r="BH36" s="9"/>
+      <c r="BI36" s="9"/>
+      <c r="BJ36" s="9"/>
+      <c r="BK36" s="9"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="I13" sqref="I1:J13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
     <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
@@ -20738,14 +20914,14 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:K35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
     <col min="10" max="10" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
@@ -21858,14 +22034,14 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
     <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="8" max="9" width="14.140625" customWidth="1" collapsed="1"/>
@@ -22608,14 +22784,14 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView topLeftCell="A11" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
       <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
     <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
@@ -23602,14 +23778,14 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
     <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
@@ -24351,14 +24527,14 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="M29" sqref="M29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
     <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
@@ -25220,14 +25396,14 @@
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
     <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
@@ -26089,14 +26265,14 @@
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="B32" sqref="A1:J35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
     <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
@@ -26838,14 +27014,14 @@
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
   <dimension ref="A1:P35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
     <col min="8" max="8" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="16.5703125" customWidth="1" collapsed="1"/>
@@ -28552,14 +28728,14 @@
 </file>
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="B21" sqref="B20:B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
     <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
@@ -29420,14 +29596,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R35"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:R36"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <sheetData>
     <row r="1" spans="1:18">
       <c r="A1" t="s">
@@ -30744,6 +30920,41 @@
         <v>74</v>
       </c>
       <c r="N35" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14">
+      <c r="A36">
+        <v>97</v>
+      </c>
+      <c r="B36" t="s">
+        <v>66</v>
+      </c>
+      <c r="C36" t="s">
+        <v>67</v>
+      </c>
+      <c r="D36" t="s">
+        <v>68</v>
+      </c>
+      <c r="E36" t="s">
+        <v>69</v>
+      </c>
+      <c r="F36" t="s">
+        <v>70</v>
+      </c>
+      <c r="G36" t="s">
+        <v>71</v>
+      </c>
+      <c r="K36" t="s">
+        <v>72</v>
+      </c>
+      <c r="L36" t="s">
+        <v>73</v>
+      </c>
+      <c r="M36" t="s">
+        <v>74</v>
+      </c>
+      <c r="N36" t="s">
         <v>75</v>
       </c>
     </row>
@@ -30753,14 +30964,14 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1D00-000000000000}">
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="B34" sqref="B33:J35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
     <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
@@ -31621,14 +31832,14 @@
 </file>
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1E00-000000000000}">
   <dimension ref="A1:K35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
     <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
@@ -32538,14 +32749,14 @@
 </file>
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1F00-000000000000}">
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="I41" sqref="I41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
     <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
@@ -33353,14 +33564,14 @@
 </file>
 
 <file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2000-000000000000}">
   <dimension ref="A1:K35"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="I46" sqref="I46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
     <col min="1" max="2" width="9.140625" style="3" collapsed="1"/>
     <col min="3" max="3" width="9.7109375" style="3" bestFit="1" customWidth="1" collapsed="1"/>
@@ -34473,14 +34684,14 @@
 </file>
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2100-000000000000}">
   <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
     <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
@@ -35221,14 +35432,14 @@
 </file>
 
 <file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2200-000000000000}">
   <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="3" t="s">
@@ -35966,14 +36177,14 @@
 </file>
 
 <file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2300-000000000000}">
   <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="3" t="s">
@@ -36711,14 +36922,14 @@
 </file>
 
 <file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2400-000000000000}">
   <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="3" t="s">
@@ -37456,14 +37667,14 @@
 </file>
 
 <file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2500-000000000000}">
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
     <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
@@ -38220,14 +38431,14 @@
 </file>
 
 <file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2600-000000000000}">
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="4" t="s">
@@ -38945,14 +39156,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C60"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
     <col min="2" max="2" width="96.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
@@ -39623,14 +39834,14 @@
 </file>
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2700-000000000000}">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
     <col min="1" max="2" width="14" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.140625" style="8"/>
@@ -39898,14 +40109,14 @@
 </file>
 
 <file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2800-000000000000}">
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
     <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
@@ -39913,7 +40124,7 @@
     <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" thickBot="1">
+    <row r="1" spans="1:10" ht="14.6" thickBot="1">
       <c r="A1" s="15"/>
       <c r="B1" s="3" t="s">
         <v>620</v>
@@ -39931,7 +40142,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.75" thickBot="1">
+    <row r="2" spans="1:10" ht="14.6" thickBot="1">
       <c r="A2" s="10" t="s">
         <v>601</v>
       </c>
@@ -39960,7 +40171,7 @@
         <v>0.10124999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.75" thickBot="1">
+    <row r="3" spans="1:10" ht="14.6" thickBot="1">
       <c r="A3" s="11" t="s">
         <v>602</v>
       </c>
@@ -39989,7 +40200,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15.75" thickBot="1">
+    <row r="4" spans="1:10" ht="14.6" thickBot="1">
       <c r="A4" s="11" t="s">
         <v>603</v>
       </c>
@@ -40018,7 +40229,7 @@
         <v>6.4285714285714293E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15.75" thickBot="1">
+    <row r="5" spans="1:10" ht="14.6" thickBot="1">
       <c r="A5" s="11" t="s">
         <v>615</v>
       </c>
@@ -40047,7 +40258,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15.75" thickBot="1">
+    <row r="6" spans="1:10" ht="14.6" thickBot="1">
       <c r="A6" s="11" t="s">
         <v>604</v>
       </c>
@@ -40076,7 +40287,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15.75" thickBot="1">
+    <row r="7" spans="1:10" ht="14.6" thickBot="1">
       <c r="A7" s="11" t="s">
         <v>605</v>
       </c>
@@ -40105,7 +40316,7 @@
         <v>3.214285714285714E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15.75" thickBot="1">
+    <row r="8" spans="1:10" ht="14.6" thickBot="1">
       <c r="A8" s="11" t="s">
         <v>606</v>
       </c>
@@ -40134,7 +40345,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="29.25" thickBot="1">
+    <row r="9" spans="1:10" ht="14.6" thickBot="1">
       <c r="A9" s="11" t="s">
         <v>608</v>
       </c>
@@ -40163,7 +40374,7 @@
         <v>0.22500000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15.75" thickBot="1">
+    <row r="10" spans="1:10" ht="14.6" thickBot="1">
       <c r="A10" s="11" t="s">
         <v>616</v>
       </c>
@@ -40192,7 +40403,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="15.75" thickBot="1">
+    <row r="11" spans="1:10" ht="14.6" thickBot="1">
       <c r="A11" s="11" t="s">
         <v>609</v>
       </c>
@@ -40221,7 +40432,7 @@
         <v>8.8235294117647051E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="15.75" thickBot="1">
+    <row r="12" spans="1:10" ht="14.6" thickBot="1">
       <c r="A12" s="11" t="s">
         <v>607</v>
       </c>
@@ -40250,7 +40461,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="15.75" thickBot="1">
+    <row r="13" spans="1:10" ht="14.6" thickBot="1">
       <c r="A13" s="11" t="s">
         <v>617</v>
       </c>
@@ -40276,7 +40487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="29.25" thickBot="1">
+    <row r="14" spans="1:10" ht="28.75" thickBot="1">
       <c r="A14" s="11" t="s">
         <v>611</v>
       </c>
@@ -40305,7 +40516,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="29.25" thickBot="1">
+    <row r="15" spans="1:10" ht="28.75" thickBot="1">
       <c r="A15" s="11" t="s">
         <v>612</v>
       </c>
@@ -40334,7 +40545,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15.75" thickBot="1">
+    <row r="16" spans="1:10" ht="14.6" thickBot="1">
       <c r="A16" s="11" t="s">
         <v>613</v>
       </c>
@@ -40360,7 +40571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="15.75" thickBot="1">
+    <row r="17" spans="1:10" ht="14.6" thickBot="1">
       <c r="A17" s="11" t="s">
         <v>614</v>
       </c>
@@ -40386,7 +40597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="15.75" thickBot="1">
+    <row r="18" spans="1:10" ht="14.6" thickBot="1">
       <c r="A18" s="11"/>
       <c r="B18" s="12"/>
       <c r="C18" s="12"/>
@@ -40398,14 +40609,14 @@
 </file>
 
 <file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2900-000000000000}">
   <dimension ref="A1:B235"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B9" sqref="A2:B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
     <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -42296,14 +42507,14 @@
 </file>
 
 <file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2A00-000000000000}">
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="C35" sqref="C35:D35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
@@ -43245,14 +43456,14 @@
 </file>
 
 <file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2B00-000000000000}">
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
@@ -44233,14 +44444,14 @@
 </file>
 
 <file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2C00-000000000000}">
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
@@ -45221,14 +45432,14 @@
 </file>
 
 <file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2D00-000000000000}">
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
@@ -46209,14 +46420,14 @@
 </file>
 
 <file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2E00-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
@@ -46257,14 +46468,14 @@
 </file>
 
 <file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2F00-000000000000}">
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="E35" sqref="E35:L35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
     <col min="12" max="12" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
@@ -47434,14 +47645,14 @@
 </file>
 
 <file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3000-000000000000}">
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -48608,12 +48819,12 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D97"/>
   <sheetViews>
     <sheetView topLeftCell="A85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
@@ -49841,14 +50052,14 @@
 </file>
 
 <file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3100-000000000000}">
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -51015,14 +51226,14 @@
 </file>
 
 <file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3200-000000000000}">
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -52189,14 +52400,14 @@
 </file>
 
 <file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3300-000000000000}">
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
     <col min="12" max="12" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -53366,14 +53577,14 @@
 </file>
 
 <file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3400-000000000000}">
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -54540,14 +54751,14 @@
 </file>
 
 <file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3500-000000000000}">
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -55714,14 +55925,14 @@
 </file>
 
 <file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3600-000000000000}">
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -56888,14 +57099,14 @@
 </file>
 
 <file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3700-000000000000}">
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -58062,14 +58273,14 @@
 </file>
 
 <file path=xl/worksheets/sheet57.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3800-000000000000}">
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -59236,14 +59447,14 @@
 </file>
 
 <file path=xl/worksheets/sheet58.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3900-000000000000}">
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -60410,14 +60621,14 @@
 </file>
 
 <file path=xl/worksheets/sheet59.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3A00-000000000000}">
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
     <col min="12" max="12" width="25.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
@@ -61587,14 +61798,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
@@ -61715,14 +61926,14 @@
 </file>
 
 <file path=xl/worksheets/sheet60.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3B00-000000000000}">
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -62889,14 +63100,14 @@
 </file>
 
 <file path=xl/worksheets/sheet61.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3C00-000000000000}">
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -64063,14 +64274,14 @@
 </file>
 
 <file path=xl/worksheets/sheet62.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3D00-000000000000}">
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="P30" sqref="P30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -65237,14 +65448,14 @@
 </file>
 
 <file path=xl/worksheets/sheet63.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3E00-000000000000}">
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -66411,14 +66622,14 @@
 </file>
 
 <file path=xl/worksheets/sheet64.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3F00-000000000000}">
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -67585,14 +67796,14 @@
 </file>
 
 <file path=xl/worksheets/sheet65.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4000-000000000000}">
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -68759,14 +68970,14 @@
 </file>
 
 <file path=xl/worksheets/sheet66.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4100-000000000000}">
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="J42" sqref="J42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -69933,14 +70144,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H35"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K30" sqref="K30"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
     <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
@@ -70807,6 +71018,32 @@
         <v>66</v>
       </c>
     </row>
+    <row r="36" spans="1:8">
+      <c r="A36">
+        <v>97</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="H36" t="s">
+        <v>66</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -70814,14 +71051,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G35"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
@@ -71418,6 +71655,23 @@
         <v>67</v>
       </c>
       <c r="E35" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36">
+        <v>97</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="C36" t="s">
+        <v>66</v>
+      </c>
+      <c r="D36" t="s">
+        <v>67</v>
+      </c>
+      <c r="E36" t="s">
         <v>277</v>
       </c>
     </row>
@@ -71428,14 +71682,14 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:T41"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="12" bestFit="1" customWidth="1" collapsed="1"/>

</xml_diff>

<commit_message>
Revert "Revert "Revert "Initial 97 add"""
This reverts commit cf69693c47b47bfd5c71f21f32e3bf382e3d5de1.
</commit_message>
<xml_diff>
--- a/Data/MetaData.xlsx
+++ b/Data/MetaData.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Majid\Documents\GitHub\IRHEIS\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\IRHEIS\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18BE6EF2-E2D1-4855-B15C-0D09E84BEC10}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5511" yWindow="3026" windowWidth="18540" windowHeight="12565" tabRatio="858" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="6600" tabRatio="858" firstSheet="37" activeTab="39"/>
   </bookViews>
   <sheets>
     <sheet name="CompressedFileNames" sheetId="1" r:id="rId1"/>
@@ -80,19 +79,12 @@
     <sheet name="Biscuit" sheetId="1026" r:id="rId65"/>
     <sheet name="Khoshkbar" sheetId="1027" r:id="rId66"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15074" uniqueCount="624">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15007" uniqueCount="623">
   <si>
     <t>Year</t>
   </si>
@@ -1962,19 +1954,16 @@
   <si>
     <t>daily protein</t>
   </si>
-  <si>
-    <t>97.rar</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -1982,7 +1971,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -1990,7 +1979,7 @@
     <font>
       <sz val="18"/>
       <color theme="3"/>
-      <name val="Times New Roman"/>
+      <name val="Calibri Light"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="major"/>
@@ -1999,7 +1988,7 @@
       <b/>
       <sz val="15"/>
       <color theme="3"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -2008,7 +1997,7 @@
       <b/>
       <sz val="13"/>
       <color theme="3"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -2017,7 +2006,7 @@
       <b/>
       <sz val="11"/>
       <color theme="3"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -2025,7 +2014,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -2033,7 +2022,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -2041,7 +2030,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -2049,7 +2038,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -2058,7 +2047,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -2067,7 +2056,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -2075,7 +2064,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -2084,7 +2073,7 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -2092,7 +2081,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -2101,7 +2090,7 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -2110,7 +2099,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -2118,7 +2107,7 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -2126,13 +2115,13 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -2141,7 +2130,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -2597,48 +2586,48 @@
     </xf>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="‏20% - تأکید1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="‏20% - تاکید2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="‏20% - تاکید3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="‏20% - تاکید4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="‏20% - تاکید5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="‏20% - تاکید6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - آکسان 1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="‏40% - تاکید2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="‏40% - تاکید3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="‏40% - تاکید4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="‏40% - تاکید5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="‏40% - تاکید6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="‏60% - تأکید1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="‏60% - تاکید2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="‏60% - تاکید3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="‏60% - تاکید4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="‏60% - تاکید5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="‏60% - تاکید6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="بد" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="بررسی سلول" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="تأکید1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="تاکید2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="تاکید3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="تاکید4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="تاکید5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="تاکید6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="خروجی" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="خنثی" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="خوب" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="سلول پیوندی" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="عنوان" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="عنوان 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="عنوان 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="عنوان 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="عنوان 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="متن توصیفی" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="متن هشدار" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="مجموع" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="محاسبه" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="معمولی" xfId="0" builtinId="0"/>
-    <cellStyle name="ورودی" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="یادداشت" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2915,14 +2904,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B35"/>
   <sheetViews>
     <sheetView topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
@@ -3207,28 +3196,20 @@
         <v>469</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
-      <c r="A36">
-        <v>97</v>
-      </c>
-      <c r="B36" t="s">
-        <v>623</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T41"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="9" max="9" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="15" bestFit="1" customWidth="1" collapsed="1"/>
@@ -5259,14 +5240,14 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S35"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="8" max="8" width="10.5703125" customWidth="1" collapsed="1"/>
     <col min="19" max="19" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
@@ -7046,14 +7027,14 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S35"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="19" max="19" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
@@ -8815,14 +8796,14 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="4" width="9.140625" style="3" collapsed="1"/>
     <col min="5" max="5" width="9.140625" style="3"/>
@@ -9944,14 +9925,14 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="15" bestFit="1" customWidth="1" collapsed="1"/>
@@ -10282,14 +10263,14 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
@@ -11466,14 +11447,14 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
@@ -12281,14 +12262,14 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
@@ -13526,14 +13507,14 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E125"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E125" sqref="E125"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="2" width="11.42578125" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
@@ -15412,14 +15393,14 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
@@ -16366,14 +16347,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:BL36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:BL35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+      <selection activeCell="BI29" sqref="BI28:BI29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.85546875" bestFit="1" customWidth="1"/>
@@ -19797,177 +19778,20 @@
       <c r="BJ35" s="9"/>
       <c r="BK35" s="9"/>
     </row>
-    <row r="36" spans="1:63">
-      <c r="A36" s="9">
-        <v>97</v>
-      </c>
-      <c r="B36" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="C36" s="9" t="s">
-        <v>470</v>
-      </c>
-      <c r="D36" s="9"/>
-      <c r="E36" s="9" t="s">
-        <v>471</v>
-      </c>
-      <c r="F36" s="9" t="s">
-        <v>472</v>
-      </c>
-      <c r="G36" s="9" t="s">
-        <v>473</v>
-      </c>
-      <c r="H36" s="9" t="s">
-        <v>474</v>
-      </c>
-      <c r="I36" s="9" t="s">
-        <v>475</v>
-      </c>
-      <c r="J36" s="9" t="s">
-        <v>476</v>
-      </c>
-      <c r="K36" s="9" t="s">
-        <v>477</v>
-      </c>
-      <c r="L36" s="9" t="s">
-        <v>478</v>
-      </c>
-      <c r="M36" s="9" t="s">
-        <v>479</v>
-      </c>
-      <c r="N36" s="9" t="s">
-        <v>480</v>
-      </c>
-      <c r="O36" s="9" t="s">
-        <v>481</v>
-      </c>
-      <c r="P36" s="9" t="s">
-        <v>482</v>
-      </c>
-      <c r="Q36" s="9" t="s">
-        <v>483</v>
-      </c>
-      <c r="R36" s="9" t="s">
-        <v>484</v>
-      </c>
-      <c r="S36" s="9" t="s">
-        <v>485</v>
-      </c>
-      <c r="T36" s="9" t="s">
-        <v>486</v>
-      </c>
-      <c r="U36" s="9" t="s">
-        <v>487</v>
-      </c>
-      <c r="V36" s="9" t="s">
-        <v>488</v>
-      </c>
-      <c r="W36" s="9" t="s">
-        <v>489</v>
-      </c>
-      <c r="X36" s="9" t="s">
-        <v>490</v>
-      </c>
-      <c r="Y36" s="9" t="s">
-        <v>491</v>
-      </c>
-      <c r="Z36" s="9" t="s">
-        <v>492</v>
-      </c>
-      <c r="AA36" s="9" t="s">
-        <v>493</v>
-      </c>
-      <c r="AB36" s="9" t="s">
-        <v>494</v>
-      </c>
-      <c r="AC36" s="9" t="s">
-        <v>495</v>
-      </c>
-      <c r="AD36" s="9" t="s">
-        <v>496</v>
-      </c>
-      <c r="AE36" s="9" t="s">
-        <v>497</v>
-      </c>
-      <c r="AF36" s="9" t="s">
-        <v>498</v>
-      </c>
-      <c r="AG36" s="9" t="s">
-        <v>499</v>
-      </c>
-      <c r="AH36" s="9" t="s">
-        <v>500</v>
-      </c>
-      <c r="AI36" s="9" t="s">
-        <v>501</v>
-      </c>
-      <c r="AJ36" s="9" t="s">
-        <v>502</v>
-      </c>
-      <c r="AK36" s="9" t="s">
-        <v>503</v>
-      </c>
-      <c r="AL36" s="9" t="s">
-        <v>504</v>
-      </c>
-      <c r="AM36" s="9" t="s">
-        <v>505</v>
-      </c>
-      <c r="AN36" s="9" t="s">
-        <v>506</v>
-      </c>
-      <c r="AO36" s="9" t="s">
-        <v>507</v>
-      </c>
-      <c r="AP36" s="9" t="s">
-        <v>508</v>
-      </c>
-      <c r="AQ36" s="9" t="s">
-        <v>509</v>
-      </c>
-      <c r="AR36" s="9" t="s">
-        <v>510</v>
-      </c>
-      <c r="AS36" s="9" t="s">
-        <v>511</v>
-      </c>
-      <c r="AT36" s="9" t="s">
-        <v>512</v>
-      </c>
-      <c r="AU36" s="9" t="s">
-        <v>513</v>
-      </c>
-      <c r="AV36" s="9"/>
-      <c r="AW36" s="9"/>
-      <c r="AX36" s="9"/>
-      <c r="AY36" s="9"/>
-      <c r="AZ36" s="9"/>
-      <c r="BA36" s="9"/>
-      <c r="BB36" s="9"/>
-      <c r="BC36" s="9"/>
-      <c r="BD36" s="9"/>
-      <c r="BE36" s="9"/>
-      <c r="BF36" s="9"/>
-      <c r="BG36" s="9"/>
-      <c r="BH36" s="9"/>
-      <c r="BI36" s="9"/>
-      <c r="BJ36" s="9"/>
-      <c r="BK36" s="9"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="I13" sqref="I1:J13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
@@ -20914,14 +20738,14 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="10" max="10" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
@@ -22034,14 +21858,14 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="8" max="9" width="14.140625" customWidth="1" collapsed="1"/>
@@ -22784,14 +22608,14 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView topLeftCell="A11" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
       <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
@@ -23778,14 +23602,14 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
@@ -24527,14 +24351,14 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="M29" sqref="M29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
@@ -25396,14 +25220,14 @@
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
@@ -26265,14 +26089,14 @@
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="B32" sqref="A1:J35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
@@ -27014,14 +26838,14 @@
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="8" max="8" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="16.5703125" customWidth="1" collapsed="1"/>
@@ -28728,14 +28552,14 @@
 </file>
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="B21" sqref="B20:B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
@@ -29596,14 +29420,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:R36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R35"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:18">
       <c r="A1" t="s">
@@ -30920,41 +30744,6 @@
         <v>74</v>
       </c>
       <c r="N35" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14">
-      <c r="A36">
-        <v>97</v>
-      </c>
-      <c r="B36" t="s">
-        <v>66</v>
-      </c>
-      <c r="C36" t="s">
-        <v>67</v>
-      </c>
-      <c r="D36" t="s">
-        <v>68</v>
-      </c>
-      <c r="E36" t="s">
-        <v>69</v>
-      </c>
-      <c r="F36" t="s">
-        <v>70</v>
-      </c>
-      <c r="G36" t="s">
-        <v>71</v>
-      </c>
-      <c r="K36" t="s">
-        <v>72</v>
-      </c>
-      <c r="L36" t="s">
-        <v>73</v>
-      </c>
-      <c r="M36" t="s">
-        <v>74</v>
-      </c>
-      <c r="N36" t="s">
         <v>75</v>
       </c>
     </row>
@@ -30964,14 +30753,14 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="B34" sqref="B33:J35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
@@ -31832,14 +31621,14 @@
 </file>
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
@@ -32749,14 +32538,14 @@
 </file>
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="I41" sqref="I41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
@@ -33564,14 +33353,14 @@
 </file>
 
 <file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K35"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="I46" sqref="I46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="2" width="9.140625" style="3" collapsed="1"/>
     <col min="3" max="3" width="9.7109375" style="3" bestFit="1" customWidth="1" collapsed="1"/>
@@ -34684,14 +34473,14 @@
 </file>
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
@@ -35432,14 +35221,14 @@
 </file>
 
 <file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="3" t="s">
@@ -36177,14 +35966,14 @@
 </file>
 
 <file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="3" t="s">
@@ -36922,14 +36711,14 @@
 </file>
 
 <file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="3" t="s">
@@ -37667,14 +37456,14 @@
 </file>
 
 <file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
@@ -38431,14 +38220,14 @@
 </file>
 
 <file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="4" t="s">
@@ -39156,14 +38945,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="96.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
@@ -39834,14 +39623,14 @@
 </file>
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="2" width="14" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.140625" style="8"/>
@@ -40109,14 +39898,14 @@
 </file>
 
 <file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
@@ -40124,7 +39913,7 @@
     <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="14.6" thickBot="1">
+    <row r="1" spans="1:10" ht="15.75" thickBot="1">
       <c r="A1" s="15"/>
       <c r="B1" s="3" t="s">
         <v>620</v>
@@ -40142,7 +39931,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="14.6" thickBot="1">
+    <row r="2" spans="1:10" ht="15.75" thickBot="1">
       <c r="A2" s="10" t="s">
         <v>601</v>
       </c>
@@ -40171,7 +39960,7 @@
         <v>0.10124999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="14.6" thickBot="1">
+    <row r="3" spans="1:10" ht="15.75" thickBot="1">
       <c r="A3" s="11" t="s">
         <v>602</v>
       </c>
@@ -40200,7 +39989,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="14.6" thickBot="1">
+    <row r="4" spans="1:10" ht="15.75" thickBot="1">
       <c r="A4" s="11" t="s">
         <v>603</v>
       </c>
@@ -40229,7 +40018,7 @@
         <v>6.4285714285714293E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="14.6" thickBot="1">
+    <row r="5" spans="1:10" ht="15.75" thickBot="1">
       <c r="A5" s="11" t="s">
         <v>615</v>
       </c>
@@ -40258,7 +40047,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="14.6" thickBot="1">
+    <row r="6" spans="1:10" ht="15.75" thickBot="1">
       <c r="A6" s="11" t="s">
         <v>604</v>
       </c>
@@ -40287,7 +40076,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="14.6" thickBot="1">
+    <row r="7" spans="1:10" ht="15.75" thickBot="1">
       <c r="A7" s="11" t="s">
         <v>605</v>
       </c>
@@ -40316,7 +40105,7 @@
         <v>3.214285714285714E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="14.6" thickBot="1">
+    <row r="8" spans="1:10" ht="15.75" thickBot="1">
       <c r="A8" s="11" t="s">
         <v>606</v>
       </c>
@@ -40345,7 +40134,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="14.6" thickBot="1">
+    <row r="9" spans="1:10" ht="29.25" thickBot="1">
       <c r="A9" s="11" t="s">
         <v>608</v>
       </c>
@@ -40374,7 +40163,7 @@
         <v>0.22500000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="14.6" thickBot="1">
+    <row r="10" spans="1:10" ht="15.75" thickBot="1">
       <c r="A10" s="11" t="s">
         <v>616</v>
       </c>
@@ -40403,7 +40192,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="14.6" thickBot="1">
+    <row r="11" spans="1:10" ht="15.75" thickBot="1">
       <c r="A11" s="11" t="s">
         <v>609</v>
       </c>
@@ -40432,7 +40221,7 @@
         <v>8.8235294117647051E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="14.6" thickBot="1">
+    <row r="12" spans="1:10" ht="15.75" thickBot="1">
       <c r="A12" s="11" t="s">
         <v>607</v>
       </c>
@@ -40461,7 +40250,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="14.6" thickBot="1">
+    <row r="13" spans="1:10" ht="15.75" thickBot="1">
       <c r="A13" s="11" t="s">
         <v>617</v>
       </c>
@@ -40487,7 +40276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="28.75" thickBot="1">
+    <row r="14" spans="1:10" ht="29.25" thickBot="1">
       <c r="A14" s="11" t="s">
         <v>611</v>
       </c>
@@ -40516,7 +40305,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="28.75" thickBot="1">
+    <row r="15" spans="1:10" ht="29.25" thickBot="1">
       <c r="A15" s="11" t="s">
         <v>612</v>
       </c>
@@ -40545,7 +40334,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="14.6" thickBot="1">
+    <row r="16" spans="1:10" ht="15.75" thickBot="1">
       <c r="A16" s="11" t="s">
         <v>613</v>
       </c>
@@ -40571,7 +40360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="14.6" thickBot="1">
+    <row r="17" spans="1:10" ht="15.75" thickBot="1">
       <c r="A17" s="11" t="s">
         <v>614</v>
       </c>
@@ -40597,7 +40386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="14.6" thickBot="1">
+    <row r="18" spans="1:10" ht="15.75" thickBot="1">
       <c r="A18" s="11"/>
       <c r="B18" s="12"/>
       <c r="C18" s="12"/>
@@ -40609,14 +40398,14 @@
 </file>
 
 <file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B235"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B9" sqref="A2:B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -42507,14 +42296,14 @@
 </file>
 
 <file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="C35" sqref="C35:D35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
@@ -43456,14 +43245,14 @@
 </file>
 
 <file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
@@ -44444,14 +44233,14 @@
 </file>
 
 <file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
@@ -45432,14 +45221,14 @@
 </file>
 
 <file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
@@ -46420,14 +46209,14 @@
 </file>
 
 <file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
@@ -46468,14 +46257,14 @@
 </file>
 
 <file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="E35" sqref="E35:L35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="12" max="12" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
@@ -47645,14 +47434,14 @@
 </file>
 
 <file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -48819,12 +48608,12 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D97"/>
   <sheetViews>
     <sheetView topLeftCell="A85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
@@ -50052,14 +49841,14 @@
 </file>
 
 <file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -51226,14 +51015,14 @@
 </file>
 
 <file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -52400,14 +52189,14 @@
 </file>
 
 <file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="12" max="12" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -53577,14 +53366,14 @@
 </file>
 
 <file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -54751,14 +54540,14 @@
 </file>
 
 <file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -55925,14 +55714,14 @@
 </file>
 
 <file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -57099,14 +56888,14 @@
 </file>
 
 <file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -58273,14 +58062,14 @@
 </file>
 
 <file path=xl/worksheets/sheet57.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -59447,14 +59236,14 @@
 </file>
 
 <file path=xl/worksheets/sheet58.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -60621,14 +60410,14 @@
 </file>
 
 <file path=xl/worksheets/sheet59.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="12" max="12" width="25.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
@@ -61798,14 +61587,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
@@ -61926,14 +61715,14 @@
 </file>
 
 <file path=xl/worksheets/sheet60.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -63100,14 +62889,14 @@
 </file>
 
 <file path=xl/worksheets/sheet61.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -64274,14 +64063,14 @@
 </file>
 
 <file path=xl/worksheets/sheet62.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="P30" sqref="P30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -65448,14 +65237,14 @@
 </file>
 
 <file path=xl/worksheets/sheet63.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -66622,14 +66411,14 @@
 </file>
 
 <file path=xl/worksheets/sheet64.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -67796,14 +67585,14 @@
 </file>
 
 <file path=xl/worksheets/sheet65.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -68970,14 +68759,14 @@
 </file>
 
 <file path=xl/worksheets/sheet66.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="J42" sqref="J42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -70144,14 +69933,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:H36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
@@ -71018,32 +70807,6 @@
         <v>66</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
-      <c r="A36">
-        <v>97</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>321</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>321</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>322</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>322</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>323</v>
-      </c>
-      <c r="G36" s="2" t="s">
-        <v>324</v>
-      </c>
-      <c r="H36" t="s">
-        <v>66</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -71051,14 +70814,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:G36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
@@ -71655,23 +71418,6 @@
         <v>67</v>
       </c>
       <c r="E35" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
-      <c r="A36">
-        <v>97</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>321</v>
-      </c>
-      <c r="C36" t="s">
-        <v>66</v>
-      </c>
-      <c r="D36" t="s">
-        <v>67</v>
-      </c>
-      <c r="E36" t="s">
         <v>277</v>
       </c>
     </row>
@@ -71682,14 +71428,14 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T41"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="12" bestFit="1" customWidth="1" collapsed="1"/>

</xml_diff>

<commit_message>
Update codes + CV codes
</commit_message>
<xml_diff>
--- a/Data/MetaData.xlsx
+++ b/Data/MetaData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="6600" tabRatio="858" firstSheet="14" activeTab="17"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="6600" tabRatio="858" firstSheet="35" activeTab="40"/>
   </bookViews>
   <sheets>
     <sheet name="CompressedFileNames" sheetId="1" r:id="rId1"/>
@@ -14432,7 +14432,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
@@ -42391,8 +42391,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -42423,7 +42423,7 @@
         <v>454</v>
       </c>
       <c r="C2">
-        <v>2.4</v>
+        <v>3.56</v>
       </c>
       <c r="D2">
         <v>0.09</v>

</xml_diff>

<commit_message>
Update Calories Need Method
</commit_message>
<xml_diff>
--- a/Data/MetaData.xlsx
+++ b/Data/MetaData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="6600" tabRatio="858" firstSheet="35" activeTab="40"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="6600" tabRatio="858" firstSheet="40" activeTab="40"/>
   </bookViews>
   <sheets>
     <sheet name="CompressedFileNames" sheetId="1" r:id="rId1"/>
@@ -2643,7 +2643,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2682,6 +2682,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -42389,10 +42391,10 @@
 
 <file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -42401,7 +42403,7 @@
     <col min="6" max="6" width="9.140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>449</v>
       </c>
@@ -42415,7 +42417,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>454</v>
       </c>
@@ -42428,8 +42430,18 @@
       <c r="D2">
         <v>0.09</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="E2">
+        <v>356</v>
+      </c>
+      <c r="F2" s="8">
+        <v>100</v>
+      </c>
+      <c r="G2" s="17">
+        <f>E2/F2</f>
+        <v>3.56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>451</v>
       </c>
@@ -42442,8 +42454,18 @@
       <c r="D3">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="E3">
+        <v>256</v>
+      </c>
+      <c r="F3" s="8">
+        <v>66</v>
+      </c>
+      <c r="G3" s="17">
+        <f t="shared" ref="G3:G18" si="0">E3/F3</f>
+        <v>3.8787878787878789</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>456</v>
       </c>
@@ -42456,8 +42478,18 @@
       <c r="D4">
         <v>0.22500000000000001</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="E4">
+        <v>95</v>
+      </c>
+      <c r="F4" s="8">
+        <v>34</v>
+      </c>
+      <c r="G4" s="17">
+        <f t="shared" si="0"/>
+        <v>2.7941176470588234</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>452</v>
       </c>
@@ -42470,8 +42502,18 @@
       <c r="D5">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="E5">
+        <v>63</v>
+      </c>
+      <c r="F5" s="16">
+        <v>18</v>
+      </c>
+      <c r="G5" s="17">
+        <f t="shared" si="0"/>
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>458</v>
       </c>
@@ -42484,8 +42526,18 @@
       <c r="D6">
         <v>0.22</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="E6">
+        <v>79</v>
+      </c>
+      <c r="F6" s="16">
+        <v>62</v>
+      </c>
+      <c r="G6" s="17">
+        <f t="shared" si="0"/>
+        <v>1.2741935483870968</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>465</v>
       </c>
@@ -42498,8 +42550,18 @@
       <c r="D7">
         <v>6.4285714285714293E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="E7">
+        <v>58</v>
+      </c>
+      <c r="F7" s="8">
+        <v>16</v>
+      </c>
+      <c r="G7" s="17">
+        <f t="shared" si="0"/>
+        <v>3.625</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>460</v>
       </c>
@@ -42507,13 +42569,23 @@
         <v>460</v>
       </c>
       <c r="C8">
-        <v>1.5</v>
+        <v>1.2</v>
       </c>
       <c r="D8">
         <v>0.04</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="E8">
+        <v>158</v>
+      </c>
+      <c r="F8" s="16">
+        <v>190</v>
+      </c>
+      <c r="G8" s="17">
+        <f t="shared" si="0"/>
+        <v>0.83157894736842108</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>463</v>
       </c>
@@ -42526,8 +42598,18 @@
       <c r="D9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="E9">
+        <v>107</v>
+      </c>
+      <c r="F9" s="16">
+        <v>212</v>
+      </c>
+      <c r="G9" s="17">
+        <f t="shared" si="0"/>
+        <v>0.50471698113207553</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>457</v>
       </c>
@@ -42540,8 +42622,19 @@
       <c r="D10">
         <v>0.22</v>
       </c>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="E10">
+        <v>79</v>
+      </c>
+      <c r="F10" s="16">
+        <v>62</v>
+      </c>
+      <c r="G10" s="17">
+        <f t="shared" si="0"/>
+        <v>1.2741935483870968</v>
+      </c>
+      <c r="H10" s="8"/>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
         <v>455</v>
       </c>
@@ -42554,8 +42647,19 @@
       <c r="D11">
         <v>0.10124999999999999</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="E11">
+        <v>907</v>
+      </c>
+      <c r="F11" s="8">
+        <v>320</v>
+      </c>
+      <c r="G11" s="17">
+        <f t="shared" si="0"/>
+        <v>2.8343750000000001</v>
+      </c>
+      <c r="H11" s="8"/>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12" t="s">
         <v>461</v>
       </c>
@@ -42568,8 +42672,19 @@
       <c r="D12">
         <v>0.33333333333333331</v>
       </c>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="E12">
+        <v>158</v>
+      </c>
+      <c r="F12" s="16">
+        <v>190</v>
+      </c>
+      <c r="G12" s="17">
+        <f t="shared" si="0"/>
+        <v>0.83157894736842108</v>
+      </c>
+      <c r="H12" s="8"/>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" t="s">
         <v>453</v>
       </c>
@@ -42582,8 +42697,18 @@
       <c r="D13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="E13">
+        <v>414</v>
+      </c>
+      <c r="F13" s="16">
+        <v>46</v>
+      </c>
+      <c r="G13" s="17">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14" t="s">
         <v>464</v>
       </c>
@@ -42596,8 +42721,18 @@
       <c r="D14">
         <v>0.04</v>
       </c>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="E14">
+        <v>64</v>
+      </c>
+      <c r="F14" s="16">
+        <v>228</v>
+      </c>
+      <c r="G14" s="17">
+        <f t="shared" si="0"/>
+        <v>0.2807017543859649</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15" t="s">
         <v>459</v>
       </c>
@@ -42605,13 +42740,23 @@
         <v>459</v>
       </c>
       <c r="C15">
-        <v>2.5</v>
+        <v>0.6</v>
       </c>
       <c r="D15">
         <v>3.214285714285714E-2</v>
       </c>
-    </row>
-    <row r="16" spans="1:4">
+      <c r="E15">
+        <v>158</v>
+      </c>
+      <c r="F15" s="16">
+        <v>190</v>
+      </c>
+      <c r="G15" s="17">
+        <f t="shared" si="0"/>
+        <v>0.83157894736842108</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
       <c r="A16" t="s">
         <v>466</v>
       </c>
@@ -42624,8 +42769,18 @@
       <c r="D16">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="E16">
+        <v>55</v>
+      </c>
+      <c r="F16" s="16">
+        <v>68</v>
+      </c>
+      <c r="G16" s="17">
+        <f t="shared" si="0"/>
+        <v>0.80882352941176472</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" t="s">
         <v>462</v>
       </c>
@@ -42638,8 +42793,18 @@
       <c r="D17">
         <v>8.8235294117647051E-2</v>
       </c>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="E17">
+        <v>32</v>
+      </c>
+      <c r="F17" s="8">
+        <v>25</v>
+      </c>
+      <c r="G17" s="17">
+        <f t="shared" si="0"/>
+        <v>1.28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18" t="s">
         <v>593</v>
       </c>

</xml_diff>

<commit_message>
Edir Age groups + drop figures
</commit_message>
<xml_diff>
--- a/Data/MetaData.xlsx
+++ b/Data/MetaData.xlsx
@@ -87,7 +87,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15670" uniqueCount="655">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15673" uniqueCount="658">
   <si>
     <t>Year</t>
   </si>
@@ -2053,6 +2053,15 @@
   <si>
     <t>سایر و غیررسمی</t>
   </si>
+  <si>
+    <t>Cal</t>
+  </si>
+  <si>
+    <t>Con</t>
+  </si>
+  <si>
+    <t>OtherCal</t>
+  </si>
 </sst>
 </file>
 
@@ -42392,19 +42401,18 @@
 
 <file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E18" sqref="E1:G18"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>449</v>
       </c>
@@ -42418,7 +42426,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:4" ht="15" customHeight="1">
       <c r="A2" t="s">
         <v>454</v>
       </c>
@@ -42431,9 +42439,8 @@
       <c r="D2">
         <v>0.09</v>
       </c>
-      <c r="G2" s="17"/>
-    </row>
-    <row r="3" spans="1:8">
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>451</v>
       </c>
@@ -42441,14 +42448,13 @@
         <v>451</v>
       </c>
       <c r="C3">
-        <v>4</v>
+        <v>3.8787878787878789</v>
       </c>
       <c r="D3">
         <v>0.03</v>
       </c>
-      <c r="G3" s="17"/>
-    </row>
-    <row r="4" spans="1:8">
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>456</v>
       </c>
@@ -42456,14 +42462,13 @@
         <v>456</v>
       </c>
       <c r="C4">
-        <v>2.5</v>
+        <v>2.7941176470588234</v>
       </c>
       <c r="D4">
         <v>0.22500000000000001</v>
       </c>
-      <c r="G4" s="17"/>
-    </row>
-    <row r="5" spans="1:8">
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>452</v>
       </c>
@@ -42471,15 +42476,13 @@
         <v>452</v>
       </c>
       <c r="C5">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="D5">
         <v>0.1</v>
       </c>
-      <c r="F5" s="16"/>
-      <c r="G5" s="17"/>
-    </row>
-    <row r="6" spans="1:8">
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>458</v>
       </c>
@@ -42492,10 +42495,8 @@
       <c r="D6">
         <v>0.22</v>
       </c>
-      <c r="F6" s="16"/>
-      <c r="G6" s="17"/>
-    </row>
-    <row r="7" spans="1:8">
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>465</v>
       </c>
@@ -42503,14 +42504,13 @@
         <v>465</v>
       </c>
       <c r="C7">
-        <v>3.6</v>
+        <v>3.625</v>
       </c>
       <c r="D7">
         <v>6.4285714285714293E-2</v>
       </c>
-      <c r="G7" s="17"/>
-    </row>
-    <row r="8" spans="1:8">
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>460</v>
       </c>
@@ -42523,10 +42523,8 @@
       <c r="D8">
         <v>0.04</v>
       </c>
-      <c r="F8" s="16"/>
-      <c r="G8" s="17"/>
-    </row>
-    <row r="9" spans="1:8">
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>463</v>
       </c>
@@ -42534,15 +42532,13 @@
         <v>463</v>
       </c>
       <c r="C9">
-        <v>0.5</v>
+        <v>0.50471698113207553</v>
       </c>
       <c r="D9">
         <v>0</v>
       </c>
-      <c r="F9" s="16"/>
-      <c r="G9" s="17"/>
-    </row>
-    <row r="10" spans="1:8">
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>457</v>
       </c>
@@ -42555,11 +42551,8 @@
       <c r="D10">
         <v>0.22</v>
       </c>
-      <c r="F10" s="16"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="8"/>
-    </row>
-    <row r="11" spans="1:8">
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>455</v>
       </c>
@@ -42567,15 +42560,13 @@
         <v>455</v>
       </c>
       <c r="C11">
-        <v>2.5</v>
+        <v>2.8343750000000001</v>
       </c>
       <c r="D11">
         <v>0.10124999999999999</v>
       </c>
-      <c r="G11" s="17"/>
-      <c r="H11" s="8"/>
-    </row>
-    <row r="12" spans="1:8">
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>461</v>
       </c>
@@ -42588,11 +42579,8 @@
       <c r="D12">
         <v>0.33333333333333331</v>
       </c>
-      <c r="F12" s="16"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="8"/>
-    </row>
-    <row r="13" spans="1:8">
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>453</v>
       </c>
@@ -42600,15 +42588,13 @@
         <v>453</v>
       </c>
       <c r="C13">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D13">
         <v>0</v>
       </c>
-      <c r="F13" s="16"/>
-      <c r="G13" s="17"/>
-    </row>
-    <row r="14" spans="1:8">
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
         <v>464</v>
       </c>
@@ -42616,15 +42602,13 @@
         <v>464</v>
       </c>
       <c r="C14">
-        <v>0.5</v>
+        <v>0.2807017543859649</v>
       </c>
       <c r="D14">
         <v>0.04</v>
       </c>
-      <c r="F14" s="16"/>
-      <c r="G14" s="17"/>
-    </row>
-    <row r="15" spans="1:8">
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15" t="s">
         <v>459</v>
       </c>
@@ -42637,10 +42621,8 @@
       <c r="D15">
         <v>3.214285714285714E-2</v>
       </c>
-      <c r="F15" s="16"/>
-      <c r="G15" s="17"/>
-    </row>
-    <row r="16" spans="1:8">
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16" t="s">
         <v>466</v>
       </c>
@@ -42648,15 +42630,13 @@
         <v>466</v>
       </c>
       <c r="C16">
-        <v>0.9</v>
+        <v>0.80882352941176472</v>
       </c>
       <c r="D16">
         <v>0.03</v>
       </c>
-      <c r="F16" s="16"/>
-      <c r="G16" s="17"/>
-    </row>
-    <row r="17" spans="1:7">
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
         <v>462</v>
       </c>
@@ -42664,14 +42644,13 @@
         <v>462</v>
       </c>
       <c r="C17">
-        <v>1.4</v>
+        <v>1.28</v>
       </c>
       <c r="D17">
         <v>8.8235294117647051E-2</v>
       </c>
-      <c r="G17" s="17"/>
-    </row>
-    <row r="18" spans="1:7">
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
         <v>593</v>
       </c>
@@ -42699,7 +42678,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -42721,7 +42700,15 @@
       <c r="D1" t="s">
         <v>600</v>
       </c>
-      <c r="F1" s="8"/>
+      <c r="E1" t="s">
+        <v>655</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>656</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>657</v>
+      </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
@@ -42881,14 +42868,14 @@
         <v>0.04</v>
       </c>
       <c r="E8">
-        <v>158</v>
+        <v>140</v>
       </c>
       <c r="F8" s="16">
-        <v>190</v>
+        <v>245</v>
       </c>
       <c r="G8" s="17">
         <f t="shared" si="0"/>
-        <v>0.83157894736842108</v>
+        <v>0.5714285714285714</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -43121,6 +43108,9 @@
         <v>0.2</v>
       </c>
       <c r="F18" s="8"/>
+      <c r="G18">
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Edit Metadata (Calorie + protein)
</commit_message>
<xml_diff>
--- a/Data/MetaData.xlsx
+++ b/Data/MetaData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="6600" tabRatio="858" firstSheet="40" activeTab="40"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="6600" tabRatio="858" firstSheet="36" activeTab="40"/>
   </bookViews>
   <sheets>
     <sheet name="CompressedFileNames" sheetId="1" r:id="rId1"/>
@@ -87,7 +87,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15673" uniqueCount="658">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15674" uniqueCount="659">
   <si>
     <t>Year</t>
   </si>
@@ -2062,6 +2062,9 @@
   <si>
     <t>OtherCal</t>
   </si>
+  <si>
+    <t>ProteinMRC</t>
+  </si>
 </sst>
 </file>
 
@@ -42404,7 +42407,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -42437,7 +42440,7 @@
         <v>3.56</v>
       </c>
       <c r="D2">
-        <v>0.09</v>
+        <v>6.9000000000000006E-2</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -42451,7 +42454,7 @@
         <v>3.8787878787878789</v>
       </c>
       <c r="D3">
-        <v>0.03</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -42465,7 +42468,7 @@
         <v>2.7941176470588234</v>
       </c>
       <c r="D4">
-        <v>0.22500000000000001</v>
+        <v>0.14117647058823529</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -42479,7 +42482,7 @@
         <v>3.5</v>
       </c>
       <c r="D5">
-        <v>0.1</v>
+        <v>0.22777777777777775</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -42493,7 +42496,7 @@
         <v>1</v>
       </c>
       <c r="D6">
-        <v>0.22</v>
+        <v>0.17903225806451611</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -42507,7 +42510,7 @@
         <v>3.625</v>
       </c>
       <c r="D7">
-        <v>6.4285714285714293E-2</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -42521,7 +42524,7 @@
         <v>1.2</v>
       </c>
       <c r="D8">
-        <v>0.04</v>
+        <v>5.2105263157894738E-2</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -42535,7 +42538,7 @@
         <v>0.50471698113207553</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>5.1886792452830195E-3</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -42549,7 +42552,7 @@
         <v>2</v>
       </c>
       <c r="D10">
-        <v>0.22</v>
+        <v>0.17903225806451611</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -42563,7 +42566,7 @@
         <v>2.8343750000000001</v>
       </c>
       <c r="D11">
-        <v>0.10124999999999999</v>
+        <v>8.9062500000000003E-2</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -42577,7 +42580,7 @@
         <v>2.5</v>
       </c>
       <c r="D12">
-        <v>0.33333333333333331</v>
+        <v>5.2105263157894738E-2</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -42605,7 +42608,7 @@
         <v>0.2807017543859649</v>
       </c>
       <c r="D14">
-        <v>0.04</v>
+        <v>1.4035087719298246E-2</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -42619,7 +42622,7 @@
         <v>0.6</v>
       </c>
       <c r="D15">
-        <v>3.214285714285714E-2</v>
+        <v>5.2105263157894738E-2</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -42633,7 +42636,7 @@
         <v>0.80882352941176472</v>
       </c>
       <c r="D16">
-        <v>0.03</v>
+        <v>2.3529411764705882E-2</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -42647,7 +42650,7 @@
         <v>1.28</v>
       </c>
       <c r="D17">
-        <v>8.8235294117647051E-2</v>
+        <v>0.10400000000000001</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -42675,10 +42678,10 @@
 
 <file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -42687,7 +42690,7 @@
     <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>449</v>
       </c>
@@ -42709,8 +42712,11 @@
       <c r="G1" s="16" t="s">
         <v>657</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="H1" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>454</v>
       </c>
@@ -42733,8 +42739,11 @@
         <f>E2/F2</f>
         <v>3.56</v>
       </c>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="H2">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>451</v>
       </c>
@@ -42757,8 +42766,21 @@
         <f t="shared" ref="G3:G17" si="0">E3/F3</f>
         <v>3.8787878787878789</v>
       </c>
-    </row>
-    <row r="4" spans="1:7">
+      <c r="H3">
+        <v>0.03</v>
+      </c>
+      <c r="I3">
+        <v>6.9</v>
+      </c>
+      <c r="J3">
+        <v>100</v>
+      </c>
+      <c r="K3">
+        <f>I3/J3</f>
+        <v>6.9000000000000006E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
         <v>456</v>
       </c>
@@ -42781,8 +42803,21 @@
         <f t="shared" si="0"/>
         <v>2.7941176470588234</v>
       </c>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="H4">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>66</v>
+      </c>
+      <c r="K4">
+        <f t="shared" ref="K4:K18" si="1">I4/J4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5" t="s">
         <v>452</v>
       </c>
@@ -42805,8 +42840,21 @@
         <f t="shared" si="0"/>
         <v>3.5</v>
       </c>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="H5">
+        <v>0.1</v>
+      </c>
+      <c r="I5">
+        <v>4.8</v>
+      </c>
+      <c r="J5">
+        <v>34</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="1"/>
+        <v>0.14117647058823529</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6" t="s">
         <v>458</v>
       </c>
@@ -42829,8 +42877,21 @@
         <f t="shared" si="0"/>
         <v>1.2741935483870968</v>
       </c>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="H6">
+        <v>0.22</v>
+      </c>
+      <c r="I6">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="J6">
+        <v>18</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="1"/>
+        <v>0.22777777777777775</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7" t="s">
         <v>465</v>
       </c>
@@ -42853,8 +42914,21 @@
         <f t="shared" si="0"/>
         <v>3.625</v>
       </c>
-    </row>
-    <row r="8" spans="1:7">
+      <c r="H7">
+        <v>6.4285714285714293E-2</v>
+      </c>
+      <c r="I7">
+        <v>11.1</v>
+      </c>
+      <c r="J7">
+        <v>62</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="1"/>
+        <v>0.17903225806451611</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8" t="s">
         <v>460</v>
       </c>
@@ -42877,8 +42951,21 @@
         <f t="shared" si="0"/>
         <v>0.5714285714285714</v>
       </c>
-    </row>
-    <row r="9" spans="1:7">
+      <c r="H8">
+        <v>0.04</v>
+      </c>
+      <c r="I8">
+        <v>2</v>
+      </c>
+      <c r="J8">
+        <v>16</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="1"/>
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9" t="s">
         <v>463</v>
       </c>
@@ -42901,8 +42988,21 @@
         <f t="shared" si="0"/>
         <v>0.50471698113207553</v>
       </c>
-    </row>
-    <row r="10" spans="1:7">
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>9.9</v>
+      </c>
+      <c r="J9">
+        <v>190</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="1"/>
+        <v>5.2105263157894738E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
       <c r="A10" t="s">
         <v>457</v>
       </c>
@@ -42925,8 +43025,21 @@
         <f t="shared" si="0"/>
         <v>1.2741935483870968</v>
       </c>
-    </row>
-    <row r="11" spans="1:7">
+      <c r="H10">
+        <v>0.22</v>
+      </c>
+      <c r="I10">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="J10">
+        <v>212</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="1"/>
+        <v>5.1886792452830195E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
       <c r="A11" t="s">
         <v>455</v>
       </c>
@@ -42949,8 +43062,21 @@
         <f t="shared" si="0"/>
         <v>2.8343750000000001</v>
       </c>
-    </row>
-    <row r="12" spans="1:7">
+      <c r="H11">
+        <v>0.10124999999999999</v>
+      </c>
+      <c r="I11">
+        <v>11.1</v>
+      </c>
+      <c r="J11">
+        <v>62</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="1"/>
+        <v>0.17903225806451611</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
       <c r="A12" t="s">
         <v>461</v>
       </c>
@@ -42973,8 +43099,21 @@
         <f t="shared" si="0"/>
         <v>0.83157894736842108</v>
       </c>
-    </row>
-    <row r="13" spans="1:7">
+      <c r="H12">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I12">
+        <v>28.5</v>
+      </c>
+      <c r="J12">
+        <v>320</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="1"/>
+        <v>8.9062500000000003E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
       <c r="A13" t="s">
         <v>453</v>
       </c>
@@ -42997,8 +43136,21 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="14" spans="1:7">
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>9.9</v>
+      </c>
+      <c r="J13">
+        <v>190</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="1"/>
+        <v>5.2105263157894738E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
       <c r="A14" t="s">
         <v>464</v>
       </c>
@@ -43021,8 +43173,21 @@
         <f t="shared" si="0"/>
         <v>0.2807017543859649</v>
       </c>
-    </row>
-    <row r="15" spans="1:7">
+      <c r="H14">
+        <v>0.04</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>46</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
       <c r="A15" t="s">
         <v>459</v>
       </c>
@@ -43045,8 +43210,21 @@
         <f t="shared" si="0"/>
         <v>0.83157894736842108</v>
       </c>
-    </row>
-    <row r="16" spans="1:7">
+      <c r="H15">
+        <v>3.214285714285714E-2</v>
+      </c>
+      <c r="I15">
+        <v>3.2</v>
+      </c>
+      <c r="J15">
+        <v>228</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="1"/>
+        <v>1.4035087719298246E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
       <c r="A16" t="s">
         <v>466</v>
       </c>
@@ -43069,8 +43247,21 @@
         <f t="shared" si="0"/>
         <v>0.80882352941176472</v>
       </c>
-    </row>
-    <row r="17" spans="1:7">
+      <c r="H16">
+        <v>0.03</v>
+      </c>
+      <c r="I16">
+        <v>9.9</v>
+      </c>
+      <c r="J16">
+        <v>190</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="1"/>
+        <v>5.2105263157894738E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
       <c r="A17" t="s">
         <v>462</v>
       </c>
@@ -43093,8 +43284,21 @@
         <f t="shared" si="0"/>
         <v>1.28</v>
       </c>
-    </row>
-    <row r="18" spans="1:7">
+      <c r="H17">
+        <v>8.8235294117647051E-2</v>
+      </c>
+      <c r="I17">
+        <v>1.6</v>
+      </c>
+      <c r="J17">
+        <v>68</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="1"/>
+        <v>2.3529411764705882E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
       <c r="A18" t="s">
         <v>593</v>
       </c>
@@ -43110,6 +43314,19 @@
       <c r="F18" s="8"/>
       <c r="G18">
         <v>6</v>
+      </c>
+      <c r="H18">
+        <v>0.2</v>
+      </c>
+      <c r="I18">
+        <v>2.6</v>
+      </c>
+      <c r="J18">
+        <v>25</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="1"/>
+        <v>0.10400000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add 97 to several sheets
</commit_message>
<xml_diff>
--- a/Data/MetaData.xlsx
+++ b/Data/MetaData.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\IRHEIS\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Majid\Documents\GitHub\IRHEIS\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{885044A2-3AD1-42D6-A6EC-A80320C2500D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="6600" tabRatio="858" firstSheet="36" activeTab="40"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="24257" windowHeight="17349" tabRatio="858" firstSheet="7" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CompressedFileNames" sheetId="1" r:id="rId1"/>
@@ -82,12 +83,19 @@
     <sheet name="Khoshkbar" sheetId="1027" r:id="rId68"/>
     <sheet name="Nooshabe" sheetId="1041" r:id="rId69"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15674" uniqueCount="659">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15789" uniqueCount="655">
   <si>
     <t>Year</t>
   </si>
@@ -2053,28 +2061,16 @@
   <si>
     <t>سایر و غیررسمی</t>
   </si>
-  <si>
-    <t>Cal</t>
-  </si>
-  <si>
-    <t>Con</t>
-  </si>
-  <si>
-    <t>OtherCal</t>
-  </si>
-  <si>
-    <t>ProteinMRC</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -2082,7 +2078,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -2090,7 +2086,7 @@
     <font>
       <sz val="18"/>
       <color theme="3"/>
-      <name val="Calibri Light"/>
+      <name val="Times New Roman"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="major"/>
@@ -2099,7 +2095,7 @@
       <b/>
       <sz val="15"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -2108,7 +2104,7 @@
       <b/>
       <sz val="13"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -2117,7 +2113,7 @@
       <b/>
       <sz val="11"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -2125,7 +2121,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -2133,7 +2129,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -2141,7 +2137,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -2149,7 +2145,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -2158,7 +2154,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -2167,7 +2163,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -2175,7 +2171,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -2184,7 +2180,7 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -2192,7 +2188,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -2201,7 +2197,7 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -2210,7 +2206,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -2218,7 +2214,7 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -2226,13 +2222,13 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -2241,7 +2237,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -2699,48 +2695,48 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="‏20% - تأکید1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="‏20% - تاکید2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="‏20% - تاکید3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="‏20% - تاکید4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="‏20% - تاکید5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="‏20% - تاکید6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - آکسان 1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="‏40% - تاکید2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="‏40% - تاکید3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="‏40% - تاکید4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="‏40% - تاکید5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="‏40% - تاکید6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="‏60% - تأکید1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="‏60% - تاکید2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="‏60% - تاکید3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="‏60% - تاکید4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="‏60% - تاکید5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="‏60% - تاکید6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="بد" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="بررسی سلول" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="تأکید1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="تاکید2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="تاکید3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="تاکید4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="تاکید5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="تاکید6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="خروجی" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="خنثی" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="خوب" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="سلول پیوندی" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="عنوان" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="عنوان 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="عنوان 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="عنوان 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="عنوان 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="متن توصیفی" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="متن هشدار" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="مجموع" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="محاسبه" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="معمولی" xfId="0" builtinId="0"/>
+    <cellStyle name="ورودی" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="یادداشت" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3017,14 +3013,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
     <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
@@ -3323,14 +3319,14 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T41"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+  <dimension ref="A1:T42"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView topLeftCell="A11" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="12" bestFit="1" customWidth="1" collapsed="1"/>
@@ -5343,20 +5339,79 @@
         <v>329</v>
       </c>
     </row>
+    <row r="42" spans="1:20">
+      <c r="A42">
+        <v>97</v>
+      </c>
+      <c r="B42" t="s">
+        <v>443</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="D42" t="s">
+        <v>66</v>
+      </c>
+      <c r="E42" t="s">
+        <v>67</v>
+      </c>
+      <c r="F42" t="s">
+        <v>277</v>
+      </c>
+      <c r="G42" t="s">
+        <v>68</v>
+      </c>
+      <c r="H42" t="s">
+        <v>69</v>
+      </c>
+      <c r="I42" t="s">
+        <v>70</v>
+      </c>
+      <c r="K42" t="s">
+        <v>72</v>
+      </c>
+      <c r="L42" t="s">
+        <v>73</v>
+      </c>
+      <c r="M42" t="s">
+        <v>74</v>
+      </c>
+      <c r="N42" t="s">
+        <v>75</v>
+      </c>
+      <c r="O42" t="s">
+        <v>71</v>
+      </c>
+      <c r="P42" t="s">
+        <v>325</v>
+      </c>
+      <c r="Q42" t="s">
+        <v>326</v>
+      </c>
+      <c r="R42" t="s">
+        <v>327</v>
+      </c>
+      <c r="S42" t="s">
+        <v>328</v>
+      </c>
+      <c r="T42" t="s">
+        <v>329</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T41"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+  <dimension ref="A1:T42"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
     <col min="9" max="9" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="15" bestFit="1" customWidth="1" collapsed="1"/>
@@ -7381,20 +7436,79 @@
         <v>329</v>
       </c>
     </row>
+    <row r="42" spans="1:20">
+      <c r="A42">
+        <v>97</v>
+      </c>
+      <c r="B42" t="s">
+        <v>443</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="D42" t="s">
+        <v>66</v>
+      </c>
+      <c r="E42" t="s">
+        <v>67</v>
+      </c>
+      <c r="F42" t="s">
+        <v>277</v>
+      </c>
+      <c r="G42" t="s">
+        <v>68</v>
+      </c>
+      <c r="H42" t="s">
+        <v>69</v>
+      </c>
+      <c r="I42" t="s">
+        <v>70</v>
+      </c>
+      <c r="K42" t="s">
+        <v>72</v>
+      </c>
+      <c r="L42" t="s">
+        <v>73</v>
+      </c>
+      <c r="M42" t="s">
+        <v>74</v>
+      </c>
+      <c r="N42" t="s">
+        <v>75</v>
+      </c>
+      <c r="O42" t="s">
+        <v>71</v>
+      </c>
+      <c r="P42" t="s">
+        <v>325</v>
+      </c>
+      <c r="Q42" t="s">
+        <v>326</v>
+      </c>
+      <c r="R42" t="s">
+        <v>327</v>
+      </c>
+      <c r="S42" t="s">
+        <v>328</v>
+      </c>
+      <c r="T42" t="s">
+        <v>329</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S35"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+  <dimension ref="A1:S36"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
     <col min="8" max="8" width="10.5703125" customWidth="1" collapsed="1"/>
     <col min="19" max="19" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
@@ -9168,20 +9282,76 @@
         <v>329</v>
       </c>
     </row>
+    <row r="36" spans="1:19">
+      <c r="A36">
+        <v>97</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="C36" t="s">
+        <v>66</v>
+      </c>
+      <c r="D36" t="s">
+        <v>67</v>
+      </c>
+      <c r="E36" t="s">
+        <v>277</v>
+      </c>
+      <c r="F36" t="s">
+        <v>68</v>
+      </c>
+      <c r="G36" t="s">
+        <v>69</v>
+      </c>
+      <c r="I36" t="s">
+        <v>70</v>
+      </c>
+      <c r="J36" t="s">
+        <v>72</v>
+      </c>
+      <c r="K36" t="s">
+        <v>73</v>
+      </c>
+      <c r="L36" t="s">
+        <v>74</v>
+      </c>
+      <c r="M36" t="s">
+        <v>75</v>
+      </c>
+      <c r="N36" t="s">
+        <v>71</v>
+      </c>
+      <c r="O36" t="s">
+        <v>325</v>
+      </c>
+      <c r="P36" t="s">
+        <v>326</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>327</v>
+      </c>
+      <c r="R36" t="s">
+        <v>328</v>
+      </c>
+      <c r="S36" t="s">
+        <v>329</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S35"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+  <dimension ref="A1:S36"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="19" max="19" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
@@ -10937,20 +11107,76 @@
         <v>329</v>
       </c>
     </row>
+    <row r="36" spans="1:19">
+      <c r="A36">
+        <v>97</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="C36" t="s">
+        <v>66</v>
+      </c>
+      <c r="D36" t="s">
+        <v>67</v>
+      </c>
+      <c r="E36" t="s">
+        <v>277</v>
+      </c>
+      <c r="F36" t="s">
+        <v>68</v>
+      </c>
+      <c r="G36" t="s">
+        <v>69</v>
+      </c>
+      <c r="I36" t="s">
+        <v>70</v>
+      </c>
+      <c r="J36" t="s">
+        <v>72</v>
+      </c>
+      <c r="K36" t="s">
+        <v>73</v>
+      </c>
+      <c r="L36" t="s">
+        <v>74</v>
+      </c>
+      <c r="M36" t="s">
+        <v>75</v>
+      </c>
+      <c r="N36" t="s">
+        <v>71</v>
+      </c>
+      <c r="O36" t="s">
+        <v>325</v>
+      </c>
+      <c r="P36" t="s">
+        <v>326</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>327</v>
+      </c>
+      <c r="R36" t="s">
+        <v>328</v>
+      </c>
+      <c r="S36" t="s">
+        <v>329</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L35"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+  <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
     <col min="1" max="4" width="9.140625" style="3" collapsed="1"/>
     <col min="5" max="5" width="9.140625" style="3"/>
@@ -12066,20 +12292,52 @@
         <v>74</v>
       </c>
     </row>
+    <row r="36" spans="1:12">
+      <c r="A36" s="3">
+        <v>97</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>323</v>
+      </c>
+      <c r="C36" t="s">
+        <v>66</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="H36" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="I36" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="J36" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="K36" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="L36" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G35"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+  <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
     <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="15" bestFit="1" customWidth="1" collapsed="1"/>
@@ -12404,20 +12662,43 @@
         <v>360</v>
       </c>
     </row>
+    <row r="36" spans="1:7">
+      <c r="A36">
+        <v>97</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="C36" t="s">
+        <v>66</v>
+      </c>
+      <c r="D36" t="s">
+        <v>351</v>
+      </c>
+      <c r="E36" t="s">
+        <v>352</v>
+      </c>
+      <c r="F36" t="s">
+        <v>353</v>
+      </c>
+      <c r="G36" t="s">
+        <v>360</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView topLeftCell="A28" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
     <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
@@ -13629,14 +13910,14 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I35"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+  <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
     <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
@@ -14438,20 +14719,49 @@
         <v>68</v>
       </c>
     </row>
+    <row r="36" spans="1:9">
+      <c r="A36">
+        <v>97</v>
+      </c>
+      <c r="B36" t="s">
+        <v>276</v>
+      </c>
+      <c r="C36">
+        <v>126112</v>
+      </c>
+      <c r="D36">
+        <v>126111</v>
+      </c>
+      <c r="E36" t="s">
+        <v>66</v>
+      </c>
+      <c r="F36" t="s">
+        <v>67</v>
+      </c>
+      <c r="G36" t="s">
+        <v>70</v>
+      </c>
+      <c r="H36" t="s">
+        <v>277</v>
+      </c>
+      <c r="I36" t="s">
+        <v>68</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:K36"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
@@ -15724,14 +16034,14 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:E125"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E125" sqref="E125"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
     <col min="1" max="2" width="11.42578125" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
@@ -17610,14 +17920,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:R36"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <sheetData>
     <row r="1" spans="1:18">
       <c r="A1" t="s">
@@ -18978,14 +19288,14 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
     <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
@@ -19958,14 +20268,14 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
     <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
@@ -20938,14 +21248,14 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:K36"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
     <col min="10" max="10" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
@@ -22093,14 +22403,14 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
     <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="8" max="9" width="14.140625" customWidth="1" collapsed="1"/>
@@ -22863,14 +23173,14 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView topLeftCell="A14" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
     <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
@@ -23886,14 +24196,14 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
     <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
@@ -24655,14 +24965,14 @@
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
     <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
@@ -25544,14 +25854,14 @@
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
     <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
@@ -26433,14 +26743,14 @@
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
     <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
@@ -27202,14 +27512,14 @@
 </file>
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
   <dimension ref="A1:P36"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
     <col min="8" max="8" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="16.5703125" customWidth="1" collapsed="1"/>
@@ -28966,14 +29276,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:BL36"/>
   <sheetViews>
     <sheetView topLeftCell="AN1" workbookViewId="0">
       <selection activeCell="AR42" sqref="AR42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
     <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.85546875" bestFit="1" customWidth="1"/>
@@ -32544,14 +32854,14 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1D00-000000000000}">
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
     <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
@@ -33432,14 +33742,14 @@
 </file>
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1E00-000000000000}">
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="O29" sqref="O29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
     <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
@@ -34320,14 +34630,14 @@
 </file>
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1F00-000000000000}">
   <dimension ref="A1:K36"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
     <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
@@ -35266,14 +35576,14 @@
 </file>
 
 <file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2000-000000000000}">
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
     <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
@@ -36104,14 +36414,14 @@
 </file>
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2100-000000000000}">
   <dimension ref="A1:K36"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
     <col min="1" max="2" width="9.140625" style="3" collapsed="1"/>
     <col min="3" max="3" width="9.7109375" style="3" bestFit="1" customWidth="1" collapsed="1"/>
@@ -37253,14 +37563,14 @@
 </file>
 
 <file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H35"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2200-000000000000}">
+  <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
     <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
@@ -37995,20 +38305,40 @@
         <v>68</v>
       </c>
     </row>
+    <row r="36" spans="1:8">
+      <c r="A36" s="3">
+        <v>97</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>323</v>
+      </c>
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+      <c r="E36" t="s">
+        <v>66</v>
+      </c>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="H36" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H35"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2300-000000000000}">
+  <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="3" t="s">
@@ -38737,6 +39067,26 @@
         <v>67</v>
       </c>
       <c r="H35" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36" s="3">
+        <v>97</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>323</v>
+      </c>
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+      <c r="E36" t="s">
+        <v>66</v>
+      </c>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="H36" s="3" t="s">
         <v>69</v>
       </c>
     </row>
@@ -38746,14 +39096,14 @@
 </file>
 
 <file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H35"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2400-000000000000}">
+  <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="3" t="s">
@@ -39482,6 +39832,26 @@
         <v>67</v>
       </c>
       <c r="H35" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36" s="3">
+        <v>97</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>323</v>
+      </c>
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+      <c r="E36" t="s">
+        <v>66</v>
+      </c>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="H36" s="3" t="s">
         <v>70</v>
       </c>
     </row>
@@ -39491,14 +39861,14 @@
 </file>
 
 <file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H35"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2500-000000000000}">
+  <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="3" t="s">
@@ -40227,6 +40597,26 @@
         <v>67</v>
       </c>
       <c r="H35" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36" s="3">
+        <v>97</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>323</v>
+      </c>
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+      <c r="E36" t="s">
+        <v>66</v>
+      </c>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="H36" s="3" t="s">
         <v>72</v>
       </c>
     </row>
@@ -40236,14 +40626,14 @@
 </file>
 
 <file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I35"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2600-000000000000}">
+  <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
     <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
@@ -40994,20 +41384,40 @@
         <v>73</v>
       </c>
     </row>
+    <row r="36" spans="1:8">
+      <c r="A36" s="3">
+        <v>97</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>323</v>
+      </c>
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+      <c r="E36" t="s">
+        <v>66</v>
+      </c>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="H36" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C60"/>
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
     <col min="2" max="2" width="96.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
@@ -41678,14 +42088,14 @@
 </file>
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J35"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2700-000000000000}">
+  <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="4" t="s">
@@ -42394,6 +42804,26 @@
         <v>67</v>
       </c>
       <c r="H35" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36" s="3">
+        <v>97</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>323</v>
+      </c>
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+      <c r="E36" t="s">
+        <v>66</v>
+      </c>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="H36" s="3" t="s">
         <v>74</v>
       </c>
     </row>
@@ -42403,19 +42833,20 @@
 </file>
 
 <file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2800-000000000000}">
+  <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E18" sqref="E1:G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
     <col min="1" max="2" width="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>449</v>
       </c>
@@ -42429,7 +42860,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" customHeight="1">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>454</v>
       </c>
@@ -42440,10 +42871,11 @@
         <v>3.56</v>
       </c>
       <c r="D2">
-        <v>6.9000000000000006E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>0.09</v>
+      </c>
+      <c r="G2" s="17"/>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>451</v>
       </c>
@@ -42451,13 +42883,14 @@
         <v>451</v>
       </c>
       <c r="C3">
-        <v>3.8787878787878789</v>
+        <v>4</v>
       </c>
       <c r="D3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>0.03</v>
+      </c>
+      <c r="G3" s="17"/>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>456</v>
       </c>
@@ -42465,13 +42898,14 @@
         <v>456</v>
       </c>
       <c r="C4">
-        <v>2.7941176470588234</v>
+        <v>2.5</v>
       </c>
       <c r="D4">
-        <v>0.14117647058823529</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="G4" s="17"/>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>452</v>
       </c>
@@ -42479,13 +42913,15 @@
         <v>452</v>
       </c>
       <c r="C5">
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="D5">
-        <v>0.22777777777777775</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+        <v>0.1</v>
+      </c>
+      <c r="F5" s="16"/>
+      <c r="G5" s="17"/>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>458</v>
       </c>
@@ -42496,10 +42932,12 @@
         <v>1</v>
       </c>
       <c r="D6">
-        <v>0.17903225806451611</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+        <v>0.22</v>
+      </c>
+      <c r="F6" s="16"/>
+      <c r="G6" s="17"/>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>465</v>
       </c>
@@ -42507,13 +42945,14 @@
         <v>465</v>
       </c>
       <c r="C7">
-        <v>3.625</v>
+        <v>3.6</v>
       </c>
       <c r="D7">
-        <v>0.125</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+        <v>6.4285714285714293E-2</v>
+      </c>
+      <c r="G7" s="17"/>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>460</v>
       </c>
@@ -42524,10 +42963,12 @@
         <v>1.2</v>
       </c>
       <c r="D8">
-        <v>5.2105263157894738E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+        <v>0.04</v>
+      </c>
+      <c r="F8" s="16"/>
+      <c r="G8" s="17"/>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>463</v>
       </c>
@@ -42535,13 +42976,15 @@
         <v>463</v>
       </c>
       <c r="C9">
-        <v>0.50471698113207553</v>
+        <v>0.5</v>
       </c>
       <c r="D9">
-        <v>5.1886792452830195E-3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
+        <v>0</v>
+      </c>
+      <c r="F9" s="16"/>
+      <c r="G9" s="17"/>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>457</v>
       </c>
@@ -42552,10 +42995,13 @@
         <v>2</v>
       </c>
       <c r="D10">
-        <v>0.17903225806451611</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
+        <v>0.22</v>
+      </c>
+      <c r="F10" s="16"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="8"/>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
         <v>455</v>
       </c>
@@ -42563,13 +43009,15 @@
         <v>455</v>
       </c>
       <c r="C11">
-        <v>2.8343750000000001</v>
+        <v>2.5</v>
       </c>
       <c r="D11">
-        <v>8.9062500000000003E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
+        <v>0.10124999999999999</v>
+      </c>
+      <c r="G11" s="17"/>
+      <c r="H11" s="8"/>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12" t="s">
         <v>461</v>
       </c>
@@ -42580,10 +43028,13 @@
         <v>2.5</v>
       </c>
       <c r="D12">
-        <v>5.2105263157894738E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F12" s="16"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="8"/>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" t="s">
         <v>453</v>
       </c>
@@ -42591,13 +43042,15 @@
         <v>453</v>
       </c>
       <c r="C13">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="F13" s="16"/>
+      <c r="G13" s="17"/>
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14" t="s">
         <v>464</v>
       </c>
@@ -42605,13 +43058,15 @@
         <v>464</v>
       </c>
       <c r="C14">
-        <v>0.2807017543859649</v>
+        <v>0.5</v>
       </c>
       <c r="D14">
-        <v>1.4035087719298246E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
+        <v>0.04</v>
+      </c>
+      <c r="F14" s="16"/>
+      <c r="G14" s="17"/>
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15" t="s">
         <v>459</v>
       </c>
@@ -42622,10 +43077,12 @@
         <v>0.6</v>
       </c>
       <c r="D15">
-        <v>5.2105263157894738E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
+        <v>3.214285714285714E-2</v>
+      </c>
+      <c r="F15" s="16"/>
+      <c r="G15" s="17"/>
+    </row>
+    <row r="16" spans="1:8">
       <c r="A16" t="s">
         <v>466</v>
       </c>
@@ -42633,13 +43090,15 @@
         <v>466</v>
       </c>
       <c r="C16">
-        <v>0.80882352941176472</v>
+        <v>0.9</v>
       </c>
       <c r="D16">
-        <v>2.3529411764705882E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
+        <v>0.03</v>
+      </c>
+      <c r="F16" s="16"/>
+      <c r="G16" s="17"/>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" t="s">
         <v>462</v>
       </c>
@@ -42647,13 +43106,14 @@
         <v>462</v>
       </c>
       <c r="C17">
-        <v>1.28</v>
+        <v>1.4</v>
       </c>
       <c r="D17">
-        <v>0.10400000000000001</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
+        <v>8.8235294117647051E-2</v>
+      </c>
+      <c r="G17" s="17"/>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18" t="s">
         <v>593</v>
       </c>
@@ -42677,20 +43137,20 @@
 </file>
 
 <file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2900-000000000000}">
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
     <col min="1" max="2" width="14" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>449</v>
       </c>
@@ -42703,20 +43163,9 @@
       <c r="D1" t="s">
         <v>600</v>
       </c>
-      <c r="E1" t="s">
-        <v>655</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>656</v>
-      </c>
-      <c r="G1" s="16" t="s">
-        <v>657</v>
-      </c>
-      <c r="H1" t="s">
-        <v>658</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11">
+      <c r="F1" s="8"/>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>454</v>
       </c>
@@ -42739,11 +43188,8 @@
         <f>E2/F2</f>
         <v>3.56</v>
       </c>
-      <c r="H2">
-        <v>0.09</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>451</v>
       </c>
@@ -42766,21 +43212,8 @@
         <f t="shared" ref="G3:G17" si="0">E3/F3</f>
         <v>3.8787878787878789</v>
       </c>
-      <c r="H3">
-        <v>0.03</v>
-      </c>
-      <c r="I3">
-        <v>6.9</v>
-      </c>
-      <c r="J3">
-        <v>100</v>
-      </c>
-      <c r="K3">
-        <f>I3/J3</f>
-        <v>6.9000000000000006E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>456</v>
       </c>
@@ -42803,21 +43236,8 @@
         <f t="shared" si="0"/>
         <v>2.7941176470588234</v>
       </c>
-      <c r="H4">
-        <v>0.22500000000000001</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4">
-        <v>66</v>
-      </c>
-      <c r="K4">
-        <f t="shared" ref="K4:K18" si="1">I4/J4</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>452</v>
       </c>
@@ -42840,21 +43260,8 @@
         <f t="shared" si="0"/>
         <v>3.5</v>
       </c>
-      <c r="H5">
-        <v>0.1</v>
-      </c>
-      <c r="I5">
-        <v>4.8</v>
-      </c>
-      <c r="J5">
-        <v>34</v>
-      </c>
-      <c r="K5">
-        <f t="shared" si="1"/>
-        <v>0.14117647058823529</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>458</v>
       </c>
@@ -42877,21 +43284,8 @@
         <f t="shared" si="0"/>
         <v>1.2741935483870968</v>
       </c>
-      <c r="H6">
-        <v>0.22</v>
-      </c>
-      <c r="I6">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="J6">
-        <v>18</v>
-      </c>
-      <c r="K6">
-        <f t="shared" si="1"/>
-        <v>0.22777777777777775</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>465</v>
       </c>
@@ -42914,21 +43308,8 @@
         <f t="shared" si="0"/>
         <v>3.625</v>
       </c>
-      <c r="H7">
-        <v>6.4285714285714293E-2</v>
-      </c>
-      <c r="I7">
-        <v>11.1</v>
-      </c>
-      <c r="J7">
-        <v>62</v>
-      </c>
-      <c r="K7">
-        <f t="shared" si="1"/>
-        <v>0.17903225806451611</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>460</v>
       </c>
@@ -42942,30 +43323,17 @@
         <v>0.04</v>
       </c>
       <c r="E8">
-        <v>140</v>
+        <v>158</v>
       </c>
       <c r="F8" s="16">
-        <v>245</v>
+        <v>190</v>
       </c>
       <c r="G8" s="17">
         <f t="shared" si="0"/>
-        <v>0.5714285714285714</v>
-      </c>
-      <c r="H8">
-        <v>0.04</v>
-      </c>
-      <c r="I8">
-        <v>2</v>
-      </c>
-      <c r="J8">
-        <v>16</v>
-      </c>
-      <c r="K8">
-        <f t="shared" si="1"/>
-        <v>0.125</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
+        <v>0.83157894736842108</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>463</v>
       </c>
@@ -42988,21 +43356,8 @@
         <f t="shared" si="0"/>
         <v>0.50471698113207553</v>
       </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-      <c r="I9">
-        <v>9.9</v>
-      </c>
-      <c r="J9">
-        <v>190</v>
-      </c>
-      <c r="K9">
-        <f t="shared" si="1"/>
-        <v>5.2105263157894738E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11">
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
         <v>457</v>
       </c>
@@ -43025,21 +43380,8 @@
         <f t="shared" si="0"/>
         <v>1.2741935483870968</v>
       </c>
-      <c r="H10">
-        <v>0.22</v>
-      </c>
-      <c r="I10">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="J10">
-        <v>212</v>
-      </c>
-      <c r="K10">
-        <f t="shared" si="1"/>
-        <v>5.1886792452830195E-3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11">
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>455</v>
       </c>
@@ -43062,21 +43404,8 @@
         <f t="shared" si="0"/>
         <v>2.8343750000000001</v>
       </c>
-      <c r="H11">
-        <v>0.10124999999999999</v>
-      </c>
-      <c r="I11">
-        <v>11.1</v>
-      </c>
-      <c r="J11">
-        <v>62</v>
-      </c>
-      <c r="K11">
-        <f t="shared" si="1"/>
-        <v>0.17903225806451611</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11">
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
         <v>461</v>
       </c>
@@ -43099,21 +43428,8 @@
         <f t="shared" si="0"/>
         <v>0.83157894736842108</v>
       </c>
-      <c r="H12">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="I12">
-        <v>28.5</v>
-      </c>
-      <c r="J12">
-        <v>320</v>
-      </c>
-      <c r="K12">
-        <f t="shared" si="1"/>
-        <v>8.9062500000000003E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11">
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" t="s">
         <v>453</v>
       </c>
@@ -43136,21 +43452,8 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="H13">
-        <v>0</v>
-      </c>
-      <c r="I13">
-        <v>9.9</v>
-      </c>
-      <c r="J13">
-        <v>190</v>
-      </c>
-      <c r="K13">
-        <f t="shared" si="1"/>
-        <v>5.2105263157894738E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11">
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" t="s">
         <v>464</v>
       </c>
@@ -43173,21 +43476,8 @@
         <f t="shared" si="0"/>
         <v>0.2807017543859649</v>
       </c>
-      <c r="H14">
-        <v>0.04</v>
-      </c>
-      <c r="I14">
-        <v>0</v>
-      </c>
-      <c r="J14">
-        <v>46</v>
-      </c>
-      <c r="K14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11">
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15" t="s">
         <v>459</v>
       </c>
@@ -43210,21 +43500,8 @@
         <f t="shared" si="0"/>
         <v>0.83157894736842108</v>
       </c>
-      <c r="H15">
-        <v>3.214285714285714E-2</v>
-      </c>
-      <c r="I15">
-        <v>3.2</v>
-      </c>
-      <c r="J15">
-        <v>228</v>
-      </c>
-      <c r="K15">
-        <f t="shared" si="1"/>
-        <v>1.4035087719298246E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11">
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16" t="s">
         <v>466</v>
       </c>
@@ -43247,21 +43524,8 @@
         <f t="shared" si="0"/>
         <v>0.80882352941176472</v>
       </c>
-      <c r="H16">
-        <v>0.03</v>
-      </c>
-      <c r="I16">
-        <v>9.9</v>
-      </c>
-      <c r="J16">
-        <v>190</v>
-      </c>
-      <c r="K16">
-        <f t="shared" si="1"/>
-        <v>5.2105263157894738E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11">
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" t="s">
         <v>462</v>
       </c>
@@ -43284,21 +43548,8 @@
         <f t="shared" si="0"/>
         <v>1.28</v>
       </c>
-      <c r="H17">
-        <v>8.8235294117647051E-2</v>
-      </c>
-      <c r="I17">
-        <v>1.6</v>
-      </c>
-      <c r="J17">
-        <v>68</v>
-      </c>
-      <c r="K17">
-        <f t="shared" si="1"/>
-        <v>2.3529411764705882E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11">
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18" t="s">
         <v>593</v>
       </c>
@@ -43312,22 +43563,6 @@
         <v>0.2</v>
       </c>
       <c r="F18" s="8"/>
-      <c r="G18">
-        <v>6</v>
-      </c>
-      <c r="H18">
-        <v>0.2</v>
-      </c>
-      <c r="I18">
-        <v>2.6</v>
-      </c>
-      <c r="J18">
-        <v>25</v>
-      </c>
-      <c r="K18">
-        <f t="shared" si="1"/>
-        <v>0.10400000000000001</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -43335,14 +43570,14 @@
 </file>
 
 <file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2A00-000000000000}">
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
     <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
@@ -43350,7 +43585,7 @@
     <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" thickBot="1">
+    <row r="1" spans="1:10" ht="14.6" thickBot="1">
       <c r="A1" s="15"/>
       <c r="B1" s="3" t="s">
         <v>620</v>
@@ -43368,7 +43603,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.75" thickBot="1">
+    <row r="2" spans="1:10" ht="14.6" thickBot="1">
       <c r="A2" s="10" t="s">
         <v>601</v>
       </c>
@@ -43397,7 +43632,7 @@
         <v>0.10124999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.75" thickBot="1">
+    <row r="3" spans="1:10" ht="14.6" thickBot="1">
       <c r="A3" s="11" t="s">
         <v>602</v>
       </c>
@@ -43426,7 +43661,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15.75" thickBot="1">
+    <row r="4" spans="1:10" ht="14.6" thickBot="1">
       <c r="A4" s="11" t="s">
         <v>603</v>
       </c>
@@ -43455,7 +43690,7 @@
         <v>6.4285714285714293E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15.75" thickBot="1">
+    <row r="5" spans="1:10" ht="14.6" thickBot="1">
       <c r="A5" s="11" t="s">
         <v>615</v>
       </c>
@@ -43484,7 +43719,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15.75" thickBot="1">
+    <row r="6" spans="1:10" ht="14.6" thickBot="1">
       <c r="A6" s="11" t="s">
         <v>604</v>
       </c>
@@ -43513,7 +43748,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15.75" thickBot="1">
+    <row r="7" spans="1:10" ht="14.6" thickBot="1">
       <c r="A7" s="11" t="s">
         <v>605</v>
       </c>
@@ -43542,7 +43777,7 @@
         <v>3.214285714285714E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15.75" thickBot="1">
+    <row r="8" spans="1:10" ht="14.6" thickBot="1">
       <c r="A8" s="11" t="s">
         <v>606</v>
       </c>
@@ -43571,7 +43806,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="29.25" thickBot="1">
+    <row r="9" spans="1:10" ht="14.6" thickBot="1">
       <c r="A9" s="11" t="s">
         <v>608</v>
       </c>
@@ -43600,7 +43835,7 @@
         <v>0.22500000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15.75" thickBot="1">
+    <row r="10" spans="1:10" ht="14.6" thickBot="1">
       <c r="A10" s="11" t="s">
         <v>616</v>
       </c>
@@ -43629,7 +43864,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="15.75" thickBot="1">
+    <row r="11" spans="1:10" ht="14.6" thickBot="1">
       <c r="A11" s="11" t="s">
         <v>609</v>
       </c>
@@ -43658,7 +43893,7 @@
         <v>8.8235294117647051E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="15.75" thickBot="1">
+    <row r="12" spans="1:10" ht="14.6" thickBot="1">
       <c r="A12" s="11" t="s">
         <v>607</v>
       </c>
@@ -43687,7 +43922,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="15.75" thickBot="1">
+    <row r="13" spans="1:10" ht="14.6" thickBot="1">
       <c r="A13" s="11" t="s">
         <v>617</v>
       </c>
@@ -43713,7 +43948,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="29.25" thickBot="1">
+    <row r="14" spans="1:10" ht="28.75" thickBot="1">
       <c r="A14" s="11" t="s">
         <v>611</v>
       </c>
@@ -43742,7 +43977,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="29.25" thickBot="1">
+    <row r="15" spans="1:10" ht="28.75" thickBot="1">
       <c r="A15" s="11" t="s">
         <v>612</v>
       </c>
@@ -43771,7 +44006,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15.75" thickBot="1">
+    <row r="16" spans="1:10" ht="14.6" thickBot="1">
       <c r="A16" s="11" t="s">
         <v>613</v>
       </c>
@@ -43797,7 +44032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="15.75" thickBot="1">
+    <row r="17" spans="1:10" ht="14.6" thickBot="1">
       <c r="A17" s="11" t="s">
         <v>614</v>
       </c>
@@ -43823,7 +44058,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="15.75" thickBot="1">
+    <row r="18" spans="1:10" ht="14.6" thickBot="1">
       <c r="A18" s="11"/>
       <c r="B18" s="12"/>
       <c r="C18" s="12"/>
@@ -43835,14 +44070,14 @@
 </file>
 
 <file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2B00-000000000000}">
   <dimension ref="A1:B235"/>
   <sheetViews>
     <sheetView topLeftCell="A219" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B229" sqref="B229"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
     <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -45733,14 +45968,14 @@
 </file>
 
 <file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2C00-000000000000}">
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
@@ -46708,14 +46943,14 @@
 </file>
 
 <file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2D00-000000000000}">
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="M32" sqref="M32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
@@ -47725,14 +47960,14 @@
 </file>
 
 <file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2E00-000000000000}">
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
@@ -48742,14 +48977,14 @@
 </file>
 
 <file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2F00-000000000000}">
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
@@ -49759,14 +49994,14 @@
 </file>
 
 <file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3000-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="A1:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
     <col min="1" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
@@ -49810,12 +50045,12 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D97"/>
   <sheetViews>
     <sheetView topLeftCell="A73" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
@@ -51043,14 +51278,14 @@
 </file>
 
 <file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3100-000000000000}">
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
     <col min="12" max="12" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
@@ -52255,14 +52490,14 @@
 </file>
 
 <file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3200-000000000000}">
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -53464,14 +53699,14 @@
 </file>
 
 <file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3300-000000000000}">
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -54673,14 +54908,14 @@
 </file>
 
 <file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3400-000000000000}">
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -55882,14 +56117,14 @@
 </file>
 
 <file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3500-000000000000}">
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
     <col min="12" max="12" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -57094,14 +57329,14 @@
 </file>
 
 <file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3600-000000000000}">
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -58303,14 +58538,14 @@
 </file>
 
 <file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3700-000000000000}">
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -59512,14 +59747,14 @@
 </file>
 
 <file path=xl/worksheets/sheet57.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3800-000000000000}">
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -60721,14 +60956,14 @@
 </file>
 
 <file path=xl/worksheets/sheet58.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3900-000000000000}">
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -61930,14 +62165,14 @@
 </file>
 
 <file path=xl/worksheets/sheet59.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3A00-000000000000}">
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -63139,14 +63374,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
     <col min="2" max="2" width="22.5703125" bestFit="1" customWidth="1"/>
   </cols>
@@ -63270,14 +63505,14 @@
 </file>
 
 <file path=xl/worksheets/sheet60.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3B00-000000000000}">
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -64479,14 +64714,14 @@
 </file>
 
 <file path=xl/worksheets/sheet61.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3C00-000000000000}">
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
     <col min="12" max="12" width="25.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
@@ -65691,14 +65926,14 @@
 </file>
 
 <file path=xl/worksheets/sheet62.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3D00-000000000000}">
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -66900,14 +67135,14 @@
 </file>
 
 <file path=xl/worksheets/sheet63.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3E00-000000000000}">
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -68109,14 +68344,14 @@
 </file>
 
 <file path=xl/worksheets/sheet64.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3F00-000000000000}">
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -69318,14 +69553,14 @@
 </file>
 
 <file path=xl/worksheets/sheet65.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4000-000000000000}">
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -70527,14 +70762,14 @@
 </file>
 
 <file path=xl/worksheets/sheet66.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4100-000000000000}">
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -71736,14 +71971,14 @@
 </file>
 
 <file path=xl/worksheets/sheet67.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4200-000000000000}">
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="O39" sqref="O39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -72945,14 +73180,14 @@
 </file>
 
 <file path=xl/worksheets/sheet68.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4300-000000000000}">
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -74154,14 +74389,14 @@
 </file>
 
 <file path=xl/worksheets/sheet69.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4400-000000000000}">
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
     <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.85546875" bestFit="1" customWidth="1"/>
@@ -75367,14 +75602,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
     <col min="2" max="2" width="22.5703125" bestFit="1" customWidth="1"/>
   </cols>
@@ -75498,14 +75733,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
     <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
@@ -76379,14 +76614,14 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G35"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
@@ -76983,6 +77218,23 @@
         <v>67</v>
       </c>
       <c r="E35" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36">
+        <v>97</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="C36" t="s">
+        <v>66</v>
+      </c>
+      <c r="D36" t="s">
+        <v>67</v>
+      </c>
+      <c r="E36" t="s">
         <v>277</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Include all house expenditures
</commit_message>
<xml_diff>
--- a/Data/MetaData.xlsx
+++ b/Data/MetaData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Majid\Documents\GitHub\IRHEIS\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAB0C945-4C3E-4962-A11A-54C82CD42DAA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9AB0018-9B46-4455-BD76-A3769EB2850D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2880" yWindow="2880" windowWidth="18043" windowHeight="12566" tabRatio="858" firstSheet="24" activeTab="24" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2948" yWindow="2070" windowWidth="15630" windowHeight="10995" tabRatio="858" firstSheet="22" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CompressedFileNames" sheetId="1" r:id="rId1"/>
@@ -3025,9 +3025,9 @@
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="20.875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -3331,18 +3331,18 @@
       <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="12" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12.6875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="12" max="13" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="16" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="19.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="16" width="13.4375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="19.6875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="18" max="18" width="19" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="19" max="19" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="15.3125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
@@ -5416,18 +5416,18 @@
       <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="9" max="9" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12.6875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="12.7109375" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12.6875" customWidth="1" collapsed="1"/>
     <col min="12" max="12" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="12.6875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="14" max="14" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="15.3125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="13.4375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="12.5625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="13.6875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
@@ -7513,10 +7513,10 @@
       <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="8" max="8" width="10.5703125" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="10.5625" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="13.6875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
@@ -8559,7 +8559,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="23" spans="1:19">
+    <row r="23" spans="1:19" ht="13.9">
       <c r="A23">
         <v>84</v>
       </c>
@@ -9356,10 +9356,10 @@
       <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="13.6875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
@@ -10384,7 +10384,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="23" spans="1:19">
+    <row r="23" spans="1:19" ht="13.9">
       <c r="A23">
         <v>84</v>
       </c>
@@ -11181,15 +11181,15 @@
       <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="4" width="9.140625" style="3" collapsed="1"/>
-    <col min="5" max="5" width="9.140625" style="3"/>
-    <col min="6" max="6" width="9.140625" style="3" collapsed="1"/>
-    <col min="7" max="7" width="10.7109375" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="10" width="9.140625" style="3" collapsed="1"/>
-    <col min="11" max="11" width="11.140625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="16384" width="9.140625" style="3" collapsed="1"/>
+    <col min="1" max="4" width="9.125" style="3" collapsed="1"/>
+    <col min="5" max="5" width="9.125" style="3"/>
+    <col min="6" max="6" width="9.125" style="3" collapsed="1"/>
+    <col min="7" max="7" width="10.6875" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="10" width="9.125" style="3" collapsed="1"/>
+    <col min="11" max="11" width="11.125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="16384" width="9.125" style="3" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -12342,9 +12342,9 @@
       <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10.4375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="15" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
@@ -12703,16 +12703,16 @@
       <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.6875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8.875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="10" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="8.6875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="10" width="8.6875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="16.4375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -13922,13 +13922,13 @@
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.3125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="10.6875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="10.3125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="10.5625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -14766,10 +14766,10 @@
       <selection activeCell="E125" sqref="E125"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="2" width="11.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="2" width="11.4375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.3125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -16652,11 +16652,11 @@
       <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.5625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="16.4375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -17632,7 +17632,7 @@
       <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData>
     <row r="1" spans="1:18">
       <c r="A1" t="s">
@@ -19000,11 +19000,11 @@
       <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.5625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="16.4375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -19980,9 +19980,9 @@
       <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="10" max="10" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="16.4375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -21135,11 +21135,11 @@
       <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="9" width="14.140625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="9" width="14.125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="12.125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -21901,15 +21901,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C36" sqref="C2:C36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22:D33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="8.6875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="10.5625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -22658,7 +22658,7 @@
         <v>41111</v>
       </c>
       <c r="D22">
-        <v>42212</v>
+        <v>42215</v>
       </c>
       <c r="E22" t="s">
         <v>51</v>
@@ -22693,7 +22693,7 @@
         <v>41111</v>
       </c>
       <c r="D23">
-        <v>42212</v>
+        <v>42215</v>
       </c>
       <c r="E23" t="s">
         <v>66</v>
@@ -22728,7 +22728,7 @@
         <v>41111</v>
       </c>
       <c r="D24">
-        <v>42212</v>
+        <v>42215</v>
       </c>
       <c r="E24" t="s">
         <v>51</v>
@@ -22763,7 +22763,7 @@
         <v>41111</v>
       </c>
       <c r="D25">
-        <v>42212</v>
+        <v>42215</v>
       </c>
       <c r="E25" t="s">
         <v>66</v>
@@ -22798,7 +22798,7 @@
         <v>41111</v>
       </c>
       <c r="D26">
-        <v>42212</v>
+        <v>42215</v>
       </c>
       <c r="E26" t="s">
         <v>66</v>
@@ -22833,7 +22833,7 @@
         <v>41111</v>
       </c>
       <c r="D27">
-        <v>42212</v>
+        <v>42215</v>
       </c>
       <c r="E27" t="s">
         <v>66</v>
@@ -22868,7 +22868,7 @@
         <v>41111</v>
       </c>
       <c r="D28">
-        <v>42212</v>
+        <v>42215</v>
       </c>
       <c r="E28" t="s">
         <v>284</v>
@@ -22903,7 +22903,7 @@
         <v>41111</v>
       </c>
       <c r="D29">
-        <v>42212</v>
+        <v>42215</v>
       </c>
       <c r="E29" t="s">
         <v>66</v>
@@ -22938,7 +22938,7 @@
         <v>41111</v>
       </c>
       <c r="D30">
-        <v>42212</v>
+        <v>42215</v>
       </c>
       <c r="E30" t="s">
         <v>66</v>
@@ -22973,7 +22973,7 @@
         <v>41111</v>
       </c>
       <c r="D31">
-        <v>42212</v>
+        <v>42215</v>
       </c>
       <c r="E31" t="s">
         <v>66</v>
@@ -23008,7 +23008,7 @@
         <v>41111</v>
       </c>
       <c r="D32">
-        <v>42212</v>
+        <v>42215</v>
       </c>
       <c r="E32" t="s">
         <v>66</v>
@@ -23043,7 +23043,7 @@
         <v>41111</v>
       </c>
       <c r="D33">
-        <v>42212</v>
+        <v>42215</v>
       </c>
       <c r="E33" t="s">
         <v>66</v>
@@ -23185,12 +23185,12 @@
       <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.140625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="12.125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12.125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="12.125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -24204,11 +24204,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
@@ -25225,10 +25225,10 @@
       <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="13.5625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -25994,10 +25994,10 @@
       <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="18.4375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -26883,10 +26883,10 @@
       <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="20.3125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -27772,10 +27772,10 @@
       <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="16.125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -28541,38 +28541,38 @@
       <selection activeCell="AR42" sqref="AR42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="31" max="32" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="12.42578125" customWidth="1"/>
-    <col min="49" max="49" width="10.42578125" customWidth="1"/>
-    <col min="50" max="50" width="16.85546875" customWidth="1"/>
-    <col min="51" max="51" width="14.85546875" customWidth="1"/>
-    <col min="52" max="52" width="19.7109375" customWidth="1"/>
-    <col min="53" max="53" width="17.7109375" customWidth="1"/>
-    <col min="54" max="54" width="12.85546875" customWidth="1"/>
-    <col min="55" max="55" width="10.85546875" customWidth="1"/>
-    <col min="56" max="56" width="12.42578125" customWidth="1"/>
-    <col min="57" max="57" width="10.42578125" customWidth="1"/>
-    <col min="58" max="58" width="16.7109375" customWidth="1"/>
-    <col min="59" max="60" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.5625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.3125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.3125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="21.875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="19.4375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="10.6875" bestFit="1" customWidth="1"/>
+    <col min="31" max="32" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="12.6875" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="10.4375" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="12.4375" customWidth="1"/>
+    <col min="49" max="49" width="10.4375" customWidth="1"/>
+    <col min="50" max="50" width="16.875" customWidth="1"/>
+    <col min="51" max="51" width="14.875" customWidth="1"/>
+    <col min="52" max="52" width="19.6875" customWidth="1"/>
+    <col min="53" max="53" width="17.6875" customWidth="1"/>
+    <col min="54" max="54" width="12.875" customWidth="1"/>
+    <col min="55" max="55" width="10.875" customWidth="1"/>
+    <col min="56" max="56" width="12.4375" customWidth="1"/>
+    <col min="57" max="57" width="10.4375" customWidth="1"/>
+    <col min="58" max="58" width="16.6875" customWidth="1"/>
+    <col min="59" max="60" width="16.6875" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="14.6875" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="10.6875" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="12.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:63">
@@ -32119,12 +32119,12 @@
       <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="8" max="8" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="16.5703125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="12" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="16.5625" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.5625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="12" width="9.875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
@@ -33883,9 +33883,9 @@
       <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="16.125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -34771,9 +34771,9 @@
       <selection activeCell="O29" sqref="O29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="16.125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -35659,10 +35659,10 @@
       <selection activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="16.125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -36605,10 +36605,10 @@
       <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="15.4375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -37443,16 +37443,16 @@
       <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="3" collapsed="1"/>
-    <col min="3" max="3" width="9.7109375" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="6" width="9.140625" style="3" collapsed="1"/>
-    <col min="7" max="7" width="14.140625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="9" width="9.140625" style="3" collapsed="1"/>
-    <col min="10" max="10" width="10.5703125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="17.5703125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="16384" width="9.140625" style="3" collapsed="1"/>
+    <col min="1" max="2" width="9.125" style="3" collapsed="1"/>
+    <col min="3" max="3" width="9.6875" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="6" width="9.125" style="3" collapsed="1"/>
+    <col min="7" max="7" width="14.125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="9" width="9.125" style="3" collapsed="1"/>
+    <col min="10" max="10" width="10.5625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="17.5625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="16384" width="9.125" style="3" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -38592,9 +38592,9 @@
       <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="10.6875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -39360,7 +39360,7 @@
       <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="3" t="s">
@@ -40125,7 +40125,7 @@
       <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="3" t="s">
@@ -40890,7 +40890,7 @@
       <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="3" t="s">
@@ -41655,9 +41655,9 @@
       <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="2" max="2" width="96.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="96.6875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -42333,9 +42333,9 @@
       <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11.125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -43117,7 +43117,7 @@
       <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="4" t="s">
@@ -43862,10 +43862,10 @@
       <selection activeCell="E18" sqref="E1:G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="8"/>
+    <col min="6" max="6" width="9.125" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -44166,10 +44166,10 @@
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.3125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -44599,15 +44599,15 @@
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.3125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="14.6" thickBot="1">
+    <row r="1" spans="1:10" ht="13.9" thickBot="1">
       <c r="A1" s="15"/>
       <c r="B1" s="3" t="s">
         <v>617</v>
@@ -44625,7 +44625,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="14.6" thickBot="1">
+    <row r="2" spans="1:10" ht="13.9" thickBot="1">
       <c r="A2" s="10" t="s">
         <v>598</v>
       </c>
@@ -44654,7 +44654,7 @@
         <v>0.10124999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="14.6" thickBot="1">
+    <row r="3" spans="1:10" ht="13.9" thickBot="1">
       <c r="A3" s="11" t="s">
         <v>599</v>
       </c>
@@ -44683,7 +44683,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="14.6" thickBot="1">
+    <row r="4" spans="1:10" ht="13.9" thickBot="1">
       <c r="A4" s="11" t="s">
         <v>600</v>
       </c>
@@ -44712,7 +44712,7 @@
         <v>6.4285714285714293E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="14.6" thickBot="1">
+    <row r="5" spans="1:10" ht="13.9" thickBot="1">
       <c r="A5" s="11" t="s">
         <v>612</v>
       </c>
@@ -44741,7 +44741,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="14.6" thickBot="1">
+    <row r="6" spans="1:10" ht="13.9" thickBot="1">
       <c r="A6" s="11" t="s">
         <v>601</v>
       </c>
@@ -44770,7 +44770,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="14.6" thickBot="1">
+    <row r="7" spans="1:10" ht="13.9" thickBot="1">
       <c r="A7" s="11" t="s">
         <v>602</v>
       </c>
@@ -44799,7 +44799,7 @@
         <v>3.214285714285714E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="14.6" thickBot="1">
+    <row r="8" spans="1:10" ht="13.9" thickBot="1">
       <c r="A8" s="11" t="s">
         <v>603</v>
       </c>
@@ -44828,7 +44828,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="14.6" thickBot="1">
+    <row r="9" spans="1:10" ht="13.9" thickBot="1">
       <c r="A9" s="11" t="s">
         <v>605</v>
       </c>
@@ -44857,7 +44857,7 @@
         <v>0.22500000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="14.6" thickBot="1">
+    <row r="10" spans="1:10" ht="13.9" thickBot="1">
       <c r="A10" s="11" t="s">
         <v>613</v>
       </c>
@@ -44886,7 +44886,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="14.6" thickBot="1">
+    <row r="11" spans="1:10" ht="13.9" thickBot="1">
       <c r="A11" s="11" t="s">
         <v>606</v>
       </c>
@@ -44915,7 +44915,7 @@
         <v>8.8235294117647051E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="14.6" thickBot="1">
+    <row r="12" spans="1:10" ht="13.9" thickBot="1">
       <c r="A12" s="11" t="s">
         <v>604</v>
       </c>
@@ -44944,7 +44944,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="14.6" thickBot="1">
+    <row r="13" spans="1:10" ht="13.9" thickBot="1">
       <c r="A13" s="11" t="s">
         <v>614</v>
       </c>
@@ -44970,7 +44970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="28.75" thickBot="1">
+    <row r="14" spans="1:10" ht="27.4" thickBot="1">
       <c r="A14" s="11" t="s">
         <v>608</v>
       </c>
@@ -44999,7 +44999,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="28.75" thickBot="1">
+    <row r="15" spans="1:10" ht="27.4" thickBot="1">
       <c r="A15" s="11" t="s">
         <v>609</v>
       </c>
@@ -45028,7 +45028,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="14.6" thickBot="1">
+    <row r="16" spans="1:10" ht="13.9" thickBot="1">
       <c r="A16" s="11" t="s">
         <v>610</v>
       </c>
@@ -45054,7 +45054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="14.6" thickBot="1">
+    <row r="17" spans="1:10" ht="13.9" thickBot="1">
       <c r="A17" s="11" t="s">
         <v>611</v>
       </c>
@@ -45080,7 +45080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="14.6" thickBot="1">
+    <row r="18" spans="1:10" ht="13.9" thickBot="1">
       <c r="A18" s="11"/>
       <c r="B18" s="12"/>
       <c r="C18" s="12"/>
@@ -45099,9 +45099,9 @@
       <selection activeCell="B229" sqref="B229"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -46997,7 +46997,7 @@
       <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
@@ -47972,7 +47972,7 @@
       <selection activeCell="M32" sqref="M32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
@@ -48989,7 +48989,7 @@
       <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
@@ -50006,7 +50006,7 @@
       <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
@@ -51021,7 +51021,7 @@
   <sheetViews>
     <sheetView topLeftCell="A73" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
@@ -52256,9 +52256,9 @@
       <selection activeCell="C3" sqref="A1:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="10.3125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -52307,9 +52307,9 @@
       <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="12" max="12" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="16.4375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -53519,7 +53519,7 @@
       <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -54728,7 +54728,7 @@
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -55937,7 +55937,7 @@
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -57146,9 +57146,9 @@
       <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="12" max="12" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -58358,7 +58358,7 @@
       <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -59567,7 +59567,7 @@
       <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -60776,7 +60776,7 @@
       <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -61985,7 +61985,7 @@
       <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -63194,9 +63194,9 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="2" max="2" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.5625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -63325,7 +63325,7 @@
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -64534,7 +64534,7 @@
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -65743,9 +65743,9 @@
       <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="12" max="12" width="25.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="25.125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -66955,7 +66955,7 @@
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -68164,7 +68164,7 @@
       <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -69373,7 +69373,7 @@
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -70582,7 +70582,7 @@
       <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -71791,7 +71791,7 @@
       <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -73000,7 +73000,7 @@
       <selection activeCell="O39" sqref="O39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -74209,7 +74209,7 @@
       <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -75418,9 +75418,9 @@
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="2" max="2" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.5625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -75549,10 +75549,10 @@
       <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -76762,12 +76762,12 @@
       <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="6" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="12.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.4375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="6" width="12.4375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="12.4375" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="9" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
@@ -77643,7 +77643,7 @@
       <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">

</xml_diff>

<commit_message>
Add tenure situation and edit past files
</commit_message>
<xml_diff>
--- a/Data/MetaData.xlsx
+++ b/Data/MetaData.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Majid\Documents\GitHub\IRHEIS\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\IRHEIS\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72B9D604-0B11-4A04-AE65-D8DB5C88C780}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12765" yWindow="4658" windowWidth="15630" windowHeight="10995" tabRatio="858" firstSheet="16" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12765" yWindow="4665" windowWidth="15630" windowHeight="10995" tabRatio="858" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="CompressedFileNames" sheetId="1" r:id="rId1"/>
@@ -2074,12 +2073,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -2087,7 +2086,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -2095,7 +2094,7 @@
     <font>
       <sz val="18"/>
       <color theme="3"/>
-      <name val="Times New Roman"/>
+      <name val="Calibri Light"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="major"/>
@@ -2104,7 +2103,7 @@
       <b/>
       <sz val="15"/>
       <color theme="3"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -2113,7 +2112,7 @@
       <b/>
       <sz val="13"/>
       <color theme="3"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -2122,7 +2121,7 @@
       <b/>
       <sz val="11"/>
       <color theme="3"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -2130,7 +2129,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -2138,7 +2137,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -2146,7 +2145,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -2154,7 +2153,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -2163,7 +2162,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -2172,7 +2171,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -2180,7 +2179,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -2189,7 +2188,7 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -2197,7 +2196,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -2206,7 +2205,7 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -2215,7 +2214,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -2223,7 +2222,7 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -2231,13 +2230,13 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -2246,7 +2245,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -2704,48 +2703,48 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="‏20% - تأکید1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="‏20% - تاکید2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="‏20% - تاکید3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="‏20% - تاکید4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="‏20% - تاکید5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="‏20% - تاکید6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - آکسان 1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="‏40% - تاکید2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="‏40% - تاکید3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="‏40% - تاکید4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="‏40% - تاکید5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="‏40% - تاکید6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="‏60% - تأکید1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="‏60% - تاکید2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="‏60% - تاکید3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="‏60% - تاکید4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="‏60% - تاکید5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="‏60% - تاکید6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="بد" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="بررسی سلول" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="تأکید1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="تاکید2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="تاکید3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="تاکید4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="تاکید5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="تاکید6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="خروجی" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="خنثی" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="خوب" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="سلول پیوندی" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="عنوان" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="عنوان 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="عنوان 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="عنوان 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="عنوان 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="متن توصیفی" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="متن هشدار" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="مجموع" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="محاسبه" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="معمولی" xfId="0" builtinId="0"/>
-    <cellStyle name="ورودی" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="یادداشت" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3022,16 +3021,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="20.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -3328,25 +3327,25 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T42"/>
   <sheetViews>
     <sheetView topLeftCell="A11" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="12" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="12.6875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="12" max="13" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="16" width="13.4375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="19.6875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="16" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="19.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="18" max="18" width="19" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="19" max="19" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="15.3125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
@@ -5413,25 +5412,25 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T42"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="9" max="9" width="12.6875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="12.6875" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12.7109375" customWidth="1" collapsed="1"/>
     <col min="12" max="12" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="12.6875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="14" max="14" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="15.3125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="13.4375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="12.5625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="13.6875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
@@ -7510,17 +7509,17 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S36"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="8" max="8" width="10.5625" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="13.6875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="10.5703125" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
@@ -8563,7 +8562,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="23" spans="1:19" ht="13.9">
+    <row r="23" spans="1:19">
       <c r="A23">
         <v>84</v>
       </c>
@@ -9353,17 +9352,17 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S36"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="13.6875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
@@ -10388,7 +10387,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="23" spans="1:19" ht="13.9">
+    <row r="23" spans="1:19">
       <c r="A23">
         <v>84</v>
       </c>
@@ -11178,22 +11177,22 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="4" width="9.125" style="3" collapsed="1"/>
-    <col min="5" max="5" width="9.125" style="3"/>
-    <col min="6" max="6" width="9.125" style="3" collapsed="1"/>
-    <col min="7" max="7" width="10.6875" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="10" width="9.125" style="3" collapsed="1"/>
-    <col min="11" max="11" width="11.125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="16384" width="9.125" style="3" collapsed="1"/>
+    <col min="1" max="4" width="9.140625" style="3" collapsed="1"/>
+    <col min="5" max="5" width="9.140625" style="3"/>
+    <col min="6" max="6" width="9.140625" style="3" collapsed="1"/>
+    <col min="7" max="7" width="10.7109375" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="10" width="9.140625" style="3" collapsed="1"/>
+    <col min="11" max="11" width="11.140625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="16384" width="9.140625" style="3" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -12339,16 +12338,16 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="5" max="5" width="10.4375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="15" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
@@ -12700,23 +12699,23 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView topLeftCell="A28" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="9.6875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="8.6875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="14.125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="11.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="10" width="8.6875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="16.4375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="10" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -13919,17 +13918,17 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6086E500-DB2D-4363-94DB-66DBBC92D95E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="7" max="7" width="14.125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="16.4375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -14388,20 +14387,20 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E23" sqref="E23:G36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="16.125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.3125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="10.6875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="10.3125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="10.5625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -15232,17 +15231,17 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E127"/>
   <sheetViews>
     <sheetView topLeftCell="A109" workbookViewId="0">
       <selection activeCell="A126" sqref="A126:B127"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="11.4375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.3125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="2" width="11.42578125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -17135,14 +17134,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R36"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:18">
       <c r="A1" t="s">
@@ -18503,18 +18502,18 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="7" max="7" width="14.125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.5625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="16.4375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -19483,18 +19482,18 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="7" max="7" width="14.125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.5625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="16.4375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -20463,16 +20462,16 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="10" max="10" width="16.4375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -21618,18 +21617,18 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="7" max="7" width="14.125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="9" width="14.125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12.125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="9" width="14.140625" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -22388,18 +22387,18 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D22" sqref="D22:D33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="8.6875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="10.5625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -23668,19 +23667,19 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView topLeftCell="A14" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
       <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="7" max="7" width="14.125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="12.125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12.125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12.140625" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -24691,14 +24690,14 @@
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
@@ -25708,17 +25707,17 @@
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="7" max="7" width="14.125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="13.5625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -26477,17 +26476,17 @@
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="7" max="7" width="14.125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="18.4375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -27366,17 +27365,17 @@
 </file>
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="7" max="7" width="14.125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="20.3125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -28255,45 +28254,45 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BL36"/>
   <sheetViews>
-    <sheetView topLeftCell="AN1" workbookViewId="0">
-      <selection activeCell="AR42" sqref="AR42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="4" width="12.125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.5625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.3125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.3125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="21.875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="19.4375" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="11.125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="10.6875" bestFit="1" customWidth="1"/>
-    <col min="31" max="32" width="10.125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="9.875" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="12.6875" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="11.125" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="10.4375" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="12.4375" customWidth="1"/>
-    <col min="49" max="49" width="10.4375" customWidth="1"/>
-    <col min="50" max="50" width="16.875" customWidth="1"/>
-    <col min="51" max="51" width="14.875" customWidth="1"/>
-    <col min="52" max="52" width="19.6875" customWidth="1"/>
-    <col min="53" max="53" width="17.6875" customWidth="1"/>
-    <col min="54" max="54" width="12.875" customWidth="1"/>
-    <col min="55" max="55" width="10.875" customWidth="1"/>
-    <col min="56" max="56" width="12.4375" customWidth="1"/>
-    <col min="57" max="57" width="10.4375" customWidth="1"/>
-    <col min="58" max="58" width="16.6875" customWidth="1"/>
-    <col min="59" max="60" width="16.6875" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="14.6875" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="10.6875" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="31" max="32" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="12.42578125" customWidth="1"/>
+    <col min="49" max="49" width="10.42578125" customWidth="1"/>
+    <col min="50" max="50" width="16.85546875" customWidth="1"/>
+    <col min="51" max="51" width="14.85546875" customWidth="1"/>
+    <col min="52" max="52" width="19.7109375" customWidth="1"/>
+    <col min="53" max="53" width="17.7109375" customWidth="1"/>
+    <col min="54" max="54" width="12.85546875" customWidth="1"/>
+    <col min="55" max="55" width="10.85546875" customWidth="1"/>
+    <col min="56" max="56" width="12.42578125" customWidth="1"/>
+    <col min="57" max="57" width="10.42578125" customWidth="1"/>
+    <col min="58" max="58" width="16.7109375" customWidth="1"/>
+    <col min="59" max="60" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:63">
@@ -29411,7 +29410,7 @@
       <c r="BG15" s="9"/>
       <c r="BH15" s="9"/>
     </row>
-    <row r="16" spans="1:63" hidden="1">
+    <row r="16" spans="1:63">
       <c r="A16" s="9">
         <v>77</v>
       </c>
@@ -29477,7 +29476,7 @@
       <c r="BG16" s="9"/>
       <c r="BH16" s="9"/>
     </row>
-    <row r="17" spans="1:64" hidden="1">
+    <row r="17" spans="1:64">
       <c r="A17" s="9">
         <v>78</v>
       </c>
@@ -29543,7 +29542,7 @@
       <c r="BG17" s="9"/>
       <c r="BH17" s="9"/>
     </row>
-    <row r="18" spans="1:64" hidden="1">
+    <row r="18" spans="1:64">
       <c r="A18" s="9">
         <v>79</v>
       </c>
@@ -29609,7 +29608,7 @@
       <c r="BG18" s="9"/>
       <c r="BH18" s="9"/>
     </row>
-    <row r="19" spans="1:64" hidden="1">
+    <row r="19" spans="1:64">
       <c r="A19" s="9">
         <v>80</v>
       </c>
@@ -29675,7 +29674,7 @@
       <c r="BG19" s="9"/>
       <c r="BH19" s="9"/>
     </row>
-    <row r="20" spans="1:64" hidden="1">
+    <row r="20" spans="1:64">
       <c r="A20" s="9">
         <v>81</v>
       </c>
@@ -29741,7 +29740,7 @@
       <c r="BG20" s="9"/>
       <c r="BH20" s="9"/>
     </row>
-    <row r="21" spans="1:64" hidden="1">
+    <row r="21" spans="1:64">
       <c r="A21" s="9">
         <v>82</v>
       </c>
@@ -29807,7 +29806,7 @@
       <c r="BG21" s="9"/>
       <c r="BH21" s="9"/>
     </row>
-    <row r="22" spans="1:64" hidden="1">
+    <row r="22" spans="1:64">
       <c r="A22" s="9">
         <v>83</v>
       </c>
@@ -29873,7 +29872,7 @@
       <c r="BG22" s="9"/>
       <c r="BH22" s="9"/>
     </row>
-    <row r="23" spans="1:64" hidden="1">
+    <row r="23" spans="1:64">
       <c r="A23" s="9">
         <v>84</v>
       </c>
@@ -29939,7 +29938,7 @@
       <c r="BG23" s="9"/>
       <c r="BH23" s="9"/>
     </row>
-    <row r="24" spans="1:64" hidden="1">
+    <row r="24" spans="1:64">
       <c r="A24" s="9">
         <v>85</v>
       </c>
@@ -30005,7 +30004,7 @@
       <c r="BG24" s="9"/>
       <c r="BH24" s="9"/>
     </row>
-    <row r="25" spans="1:64" hidden="1">
+    <row r="25" spans="1:64">
       <c r="A25" s="9">
         <v>86</v>
       </c>
@@ -30071,7 +30070,7 @@
       <c r="BG25" s="9"/>
       <c r="BH25" s="9"/>
     </row>
-    <row r="26" spans="1:64" hidden="1">
+    <row r="26" spans="1:64">
       <c r="A26" s="9">
         <v>87</v>
       </c>
@@ -30137,7 +30136,7 @@
       <c r="BG26" s="9"/>
       <c r="BH26" s="9"/>
     </row>
-    <row r="27" spans="1:64" hidden="1">
+    <row r="27" spans="1:64">
       <c r="A27" s="9">
         <v>88</v>
       </c>
@@ -31833,17 +31832,17 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="7" max="7" width="14.125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="16.125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -32602,19 +32601,19 @@
 </file>
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P36"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="8" max="8" width="13.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="16.5625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.5625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="12" width="9.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="16.5703125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="12" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
@@ -34366,16 +34365,16 @@
 </file>
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="10" max="10" width="16.125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -35254,16 +35253,16 @@
 </file>
 
 <file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="O29" sqref="O29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="10" max="10" width="16.125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -36142,17 +36141,17 @@
 </file>
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K36"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="7" max="7" width="14.125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="16.125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -37088,17 +37087,17 @@
 </file>
 
 <file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="7" max="7" width="14.125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="15.4375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -37926,23 +37925,23 @@
 </file>
 
 <file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K36"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="9.125" style="3" collapsed="1"/>
-    <col min="3" max="3" width="9.6875" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="6" width="9.125" style="3" collapsed="1"/>
-    <col min="7" max="7" width="14.125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="9" width="9.125" style="3" collapsed="1"/>
-    <col min="10" max="10" width="10.5625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="17.5625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="16384" width="9.125" style="3" collapsed="1"/>
+    <col min="1" max="2" width="9.140625" style="3" collapsed="1"/>
+    <col min="3" max="3" width="9.7109375" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="6" width="9.140625" style="3" collapsed="1"/>
+    <col min="7" max="7" width="14.140625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="9" width="9.140625" style="3" collapsed="1"/>
+    <col min="10" max="10" width="10.5703125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="17.5703125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="16384" width="9.140625" style="3" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -39075,16 +39074,16 @@
 </file>
 
 <file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="8" max="8" width="10.6875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -39843,14 +39842,14 @@
 </file>
 
 <file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="3" t="s">
@@ -40608,14 +40607,14 @@
 </file>
 
 <file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="3" t="s">
@@ -41373,16 +41372,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C60"/>
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="96.6875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="96.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -42051,14 +42050,14 @@
 </file>
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="3" t="s">
@@ -42816,16 +42815,16 @@
 </file>
 
 <file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="8" max="8" width="11.125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -43600,14 +43599,14 @@
 </file>
 
 <file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="4" t="s">
@@ -44345,17 +44344,17 @@
 </file>
 
 <file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="E18" sqref="E1:G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.125" style="8"/>
+    <col min="6" max="6" width="9.140625" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -44649,17 +44648,17 @@
 </file>
 
 <file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.3125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -45082,22 +45081,22 @@
 </file>
 
 <file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="16.5625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.6875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.3125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="13.9" thickBot="1">
+    <row r="1" spans="1:10" ht="15.75" thickBot="1">
       <c r="A1" s="15"/>
       <c r="B1" s="3" t="s">
         <v>617</v>
@@ -45115,7 +45114,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="13.9" thickBot="1">
+    <row r="2" spans="1:10" ht="15.75" thickBot="1">
       <c r="A2" s="10" t="s">
         <v>598</v>
       </c>
@@ -45144,7 +45143,7 @@
         <v>0.10124999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="13.9" thickBot="1">
+    <row r="3" spans="1:10" ht="15.75" thickBot="1">
       <c r="A3" s="11" t="s">
         <v>599</v>
       </c>
@@ -45173,7 +45172,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="13.9" thickBot="1">
+    <row r="4" spans="1:10" ht="15.75" thickBot="1">
       <c r="A4" s="11" t="s">
         <v>600</v>
       </c>
@@ -45202,7 +45201,7 @@
         <v>6.4285714285714293E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="13.9" thickBot="1">
+    <row r="5" spans="1:10" ht="15.75" thickBot="1">
       <c r="A5" s="11" t="s">
         <v>612</v>
       </c>
@@ -45231,7 +45230,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="13.9" thickBot="1">
+    <row r="6" spans="1:10" ht="15.75" thickBot="1">
       <c r="A6" s="11" t="s">
         <v>601</v>
       </c>
@@ -45260,7 +45259,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="13.9" thickBot="1">
+    <row r="7" spans="1:10" ht="15.75" thickBot="1">
       <c r="A7" s="11" t="s">
         <v>602</v>
       </c>
@@ -45289,7 +45288,7 @@
         <v>3.214285714285714E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="13.9" thickBot="1">
+    <row r="8" spans="1:10" ht="15.75" thickBot="1">
       <c r="A8" s="11" t="s">
         <v>603</v>
       </c>
@@ -45318,7 +45317,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="13.9" thickBot="1">
+    <row r="9" spans="1:10" ht="29.25" thickBot="1">
       <c r="A9" s="11" t="s">
         <v>605</v>
       </c>
@@ -45347,7 +45346,7 @@
         <v>0.22500000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="13.9" thickBot="1">
+    <row r="10" spans="1:10" ht="15.75" thickBot="1">
       <c r="A10" s="11" t="s">
         <v>613</v>
       </c>
@@ -45376,7 +45375,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="13.9" thickBot="1">
+    <row r="11" spans="1:10" ht="15.75" thickBot="1">
       <c r="A11" s="11" t="s">
         <v>606</v>
       </c>
@@ -45405,7 +45404,7 @@
         <v>8.8235294117647051E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="13.9" thickBot="1">
+    <row r="12" spans="1:10" ht="15.75" thickBot="1">
       <c r="A12" s="11" t="s">
         <v>604</v>
       </c>
@@ -45434,7 +45433,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="13.9" thickBot="1">
+    <row r="13" spans="1:10" ht="15.75" thickBot="1">
       <c r="A13" s="11" t="s">
         <v>614</v>
       </c>
@@ -45460,7 +45459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="27.4" thickBot="1">
+    <row r="14" spans="1:10" ht="29.25" thickBot="1">
       <c r="A14" s="11" t="s">
         <v>608</v>
       </c>
@@ -45489,7 +45488,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="27.4" thickBot="1">
+    <row r="15" spans="1:10" ht="29.25" thickBot="1">
       <c r="A15" s="11" t="s">
         <v>609</v>
       </c>
@@ -45518,7 +45517,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="13.9" thickBot="1">
+    <row r="16" spans="1:10" ht="15.75" thickBot="1">
       <c r="A16" s="11" t="s">
         <v>610</v>
       </c>
@@ -45544,7 +45543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="13.9" thickBot="1">
+    <row r="17" spans="1:10" ht="15.75" thickBot="1">
       <c r="A17" s="11" t="s">
         <v>611</v>
       </c>
@@ -45570,7 +45569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="13.9" thickBot="1">
+    <row r="18" spans="1:10" ht="15.75" thickBot="1">
       <c r="A18" s="11"/>
       <c r="B18" s="12"/>
       <c r="C18" s="12"/>
@@ -45582,16 +45581,16 @@
 </file>
 
 <file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B235"/>
   <sheetViews>
     <sheetView topLeftCell="A219" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B229" sqref="B229"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="16.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -47480,14 +47479,14 @@
 </file>
 
 <file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
@@ -48455,14 +48454,14 @@
 </file>
 
 <file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="M32" sqref="M32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
@@ -49472,14 +49471,14 @@
 </file>
 
 <file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
@@ -50489,12 +50488,12 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D97"/>
   <sheetViews>
     <sheetView topLeftCell="A73" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
@@ -51722,14 +51721,14 @@
 </file>
 
 <file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
@@ -52739,16 +52738,16 @@
 </file>
 
 <file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="A1:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="10.3125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -52790,16 +52789,16 @@
 </file>
 
 <file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="12" max="12" width="16.4375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -54002,14 +54001,14 @@
 </file>
 
 <file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -55211,14 +55210,14 @@
 </file>
 
 <file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -56420,14 +56419,14 @@
 </file>
 
 <file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -57629,16 +57628,16 @@
 </file>
 
 <file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="12" max="12" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -58841,14 +58840,14 @@
 </file>
 
 <file path=xl/worksheets/sheet57.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -60050,14 +60049,14 @@
 </file>
 
 <file path=xl/worksheets/sheet58.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -61259,14 +61258,14 @@
 </file>
 
 <file path=xl/worksheets/sheet59.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -62468,16 +62467,16 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="22.5625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -62599,14 +62598,14 @@
 </file>
 
 <file path=xl/worksheets/sheet60.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -63808,14 +63807,14 @@
 </file>
 
 <file path=xl/worksheets/sheet61.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -65017,14 +65016,14 @@
 </file>
 
 <file path=xl/worksheets/sheet62.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -66226,16 +66225,16 @@
 </file>
 
 <file path=xl/worksheets/sheet63.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="12" max="12" width="25.125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="25.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -67438,14 +67437,14 @@
 </file>
 
 <file path=xl/worksheets/sheet64.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -68647,14 +68646,14 @@
 </file>
 
 <file path=xl/worksheets/sheet65.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -69856,14 +69855,14 @@
 </file>
 
 <file path=xl/worksheets/sheet66.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -71065,14 +71064,14 @@
 </file>
 
 <file path=xl/worksheets/sheet67.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -72274,14 +72273,14 @@
 </file>
 
 <file path=xl/worksheets/sheet68.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -73483,14 +73482,14 @@
 </file>
 
 <file path=xl/worksheets/sheet69.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="O39" sqref="O39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -74692,16 +74691,16 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="22.5625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -74823,14 +74822,14 @@
 </file>
 
 <file path=xl/worksheets/sheet70.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -76032,17 +76031,17 @@
 </file>
 
 <file path=xl/worksheets/sheet71.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="8" max="8" width="11.875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -77245,19 +77244,19 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="14.4375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="6" width="12.4375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="12.4375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="6" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="12.42578125" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="9" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
@@ -78126,14 +78125,14 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">

</xml_diff>

<commit_message>
Working in Durable Expenditures
</commit_message>
<xml_diff>
--- a/Data/MetaData.xlsx
+++ b/Data/MetaData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="12765" yWindow="4665" windowWidth="15630" windowHeight="10995" tabRatio="858" activeTab="2"/>
+    <workbookView xWindow="12765" yWindow="4665" windowWidth="15630" windowHeight="10995" tabRatio="858" firstSheet="29" activeTab="33"/>
   </bookViews>
   <sheets>
     <sheet name="CompressedFileNames" sheetId="1" r:id="rId1"/>
@@ -84,7 +84,7 @@
     <sheet name="Khoshkbar" sheetId="1027" r:id="rId70"/>
     <sheet name="Nooshabe" sheetId="1041" r:id="rId71"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -97,7 +97,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16059" uniqueCount="657">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16059" uniqueCount="658">
   <si>
     <t>Year</t>
   </si>
@@ -2069,6 +2069,9 @@
   <si>
     <t>FinServicesExp</t>
   </si>
+  <si>
+    <t>Durable_Sale</t>
+  </si>
 </sst>
 </file>
 
@@ -28257,8 +28260,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BL36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -35256,7 +35259,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O29" sqref="O29"/>
     </sheetView>
   </sheetViews>
@@ -36144,13 +36147,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F42" sqref="F42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
@@ -36174,19 +36178,19 @@
         <v>76</v>
       </c>
       <c r="G1" t="s">
+        <v>338</v>
+      </c>
+      <c r="H1" t="s">
+        <v>339</v>
+      </c>
+      <c r="I1" t="s">
         <v>300</v>
-      </c>
-      <c r="H1" t="s">
-        <v>338</v>
-      </c>
-      <c r="I1" t="s">
-        <v>339</v>
       </c>
       <c r="J1" t="s">
         <v>387</v>
       </c>
       <c r="K1" t="s">
-        <v>341</v>
+        <v>657</v>
       </c>
     </row>
     <row r="2" spans="1:11">

</xml_diff>

<commit_message>
Free and NonFree Durable Good
</commit_message>
<xml_diff>
--- a/Data/MetaData.xlsx
+++ b/Data/MetaData.xlsx
@@ -36148,7 +36148,7 @@
   <dimension ref="A1:K36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+      <selection activeCell="H11" sqref="H11:H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -36206,7 +36206,7 @@
       <c r="F2" t="s">
         <v>274</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>304</v>
       </c>
       <c r="J2" t="s">
@@ -36229,7 +36229,7 @@
       <c r="F3" t="s">
         <v>274</v>
       </c>
-      <c r="G3" t="s">
+      <c r="I3" t="s">
         <v>304</v>
       </c>
       <c r="J3" t="s">
@@ -36252,7 +36252,7 @@
       <c r="F4" t="s">
         <v>274</v>
       </c>
-      <c r="G4" t="s">
+      <c r="I4" t="s">
         <v>304</v>
       </c>
       <c r="J4" t="s">
@@ -36275,7 +36275,7 @@
       <c r="F5" t="s">
         <v>274</v>
       </c>
-      <c r="G5" t="s">
+      <c r="I5" t="s">
         <v>304</v>
       </c>
       <c r="J5" t="s">
@@ -36298,7 +36298,7 @@
       <c r="F6" t="s">
         <v>274</v>
       </c>
-      <c r="G6" t="s">
+      <c r="I6" t="s">
         <v>304</v>
       </c>
       <c r="J6" t="s">
@@ -36321,7 +36321,7 @@
       <c r="F7" t="s">
         <v>274</v>
       </c>
-      <c r="G7" t="s">
+      <c r="I7" t="s">
         <v>304</v>
       </c>
       <c r="J7" t="s">
@@ -36344,11 +36344,11 @@
       <c r="F8" t="s">
         <v>274</v>
       </c>
-      <c r="G8" t="s">
-        <v>304</v>
-      </c>
       <c r="H8" t="s">
         <v>275</v>
+      </c>
+      <c r="I8" t="s">
+        <v>304</v>
       </c>
       <c r="J8" t="s">
         <v>285</v>
@@ -36370,11 +36370,11 @@
       <c r="F9" t="s">
         <v>274</v>
       </c>
-      <c r="G9" t="s">
-        <v>304</v>
-      </c>
       <c r="H9" t="s">
         <v>275</v>
+      </c>
+      <c r="I9" t="s">
+        <v>304</v>
       </c>
       <c r="J9" t="s">
         <v>285</v>
@@ -36396,11 +36396,11 @@
       <c r="F10" t="s">
         <v>274</v>
       </c>
-      <c r="G10" t="s">
-        <v>304</v>
-      </c>
       <c r="H10" t="s">
         <v>275</v>
+      </c>
+      <c r="I10" t="s">
+        <v>304</v>
       </c>
       <c r="J10" t="s">
         <v>285</v>
@@ -36422,11 +36422,11 @@
       <c r="F11" t="s">
         <v>274</v>
       </c>
-      <c r="G11" t="s">
-        <v>304</v>
-      </c>
       <c r="H11" t="s">
         <v>275</v>
+      </c>
+      <c r="I11" t="s">
+        <v>304</v>
       </c>
       <c r="J11" t="s">
         <v>285</v>
@@ -36448,11 +36448,11 @@
       <c r="F12" t="s">
         <v>274</v>
       </c>
-      <c r="G12" t="s">
-        <v>304</v>
-      </c>
       <c r="H12" t="s">
         <v>275</v>
+      </c>
+      <c r="I12" t="s">
+        <v>304</v>
       </c>
       <c r="J12" t="s">
         <v>285</v>
@@ -36474,7 +36474,7 @@
       <c r="F13" t="s">
         <v>274</v>
       </c>
-      <c r="G13" t="s">
+      <c r="I13" t="s">
         <v>304</v>
       </c>
       <c r="J13" t="s">
@@ -36497,7 +36497,7 @@
       <c r="F14" t="s">
         <v>274</v>
       </c>
-      <c r="G14" t="s">
+      <c r="I14" t="s">
         <v>304</v>
       </c>
       <c r="J14" t="s">
@@ -36520,7 +36520,7 @@
       <c r="F15" t="s">
         <v>274</v>
       </c>
-      <c r="G15" t="s">
+      <c r="I15" t="s">
         <v>304</v>
       </c>
       <c r="J15" t="s">
@@ -36543,7 +36543,7 @@
       <c r="F16" t="s">
         <v>274</v>
       </c>
-      <c r="G16" t="s">
+      <c r="I16" t="s">
         <v>304</v>
       </c>
       <c r="J16" t="s">
@@ -36566,7 +36566,7 @@
       <c r="F17" t="s">
         <v>274</v>
       </c>
-      <c r="G17" t="s">
+      <c r="I17" t="s">
         <v>304</v>
       </c>
       <c r="J17" t="s">
@@ -36589,7 +36589,7 @@
       <c r="F18" t="s">
         <v>274</v>
       </c>
-      <c r="G18" t="s">
+      <c r="I18" t="s">
         <v>304</v>
       </c>
       <c r="J18" t="s">
@@ -36612,7 +36612,7 @@
       <c r="F19" t="s">
         <v>274</v>
       </c>
-      <c r="G19" t="s">
+      <c r="I19" t="s">
         <v>304</v>
       </c>
       <c r="J19" t="s">
@@ -36635,7 +36635,7 @@
       <c r="F20" t="s">
         <v>274</v>
       </c>
-      <c r="G20" t="s">
+      <c r="I20" t="s">
         <v>304</v>
       </c>
       <c r="J20" t="s">
@@ -36658,7 +36658,7 @@
       <c r="F21" t="s">
         <v>274</v>
       </c>
-      <c r="G21" t="s">
+      <c r="I21" t="s">
         <v>304</v>
       </c>
       <c r="J21" t="s">
@@ -36681,7 +36681,7 @@
       <c r="F22" t="s">
         <v>274</v>
       </c>
-      <c r="G22" t="s">
+      <c r="I22" t="s">
         <v>304</v>
       </c>
       <c r="J22" t="s">
@@ -36707,7 +36707,7 @@
       <c r="G23" t="s">
         <v>277</v>
       </c>
-      <c r="H23" t="s">
+      <c r="I23" t="s">
         <v>68</v>
       </c>
       <c r="J23" t="s">
@@ -36733,7 +36733,7 @@
       <c r="G24" t="s">
         <v>277</v>
       </c>
-      <c r="H24" t="s">
+      <c r="I24" t="s">
         <v>68</v>
       </c>
       <c r="J24" t="s">
@@ -36759,7 +36759,7 @@
       <c r="G25" t="s">
         <v>277</v>
       </c>
-      <c r="H25" t="s">
+      <c r="I25" t="s">
         <v>68</v>
       </c>
       <c r="J25" t="s">
@@ -36785,7 +36785,7 @@
       <c r="G26" t="s">
         <v>277</v>
       </c>
-      <c r="H26" t="s">
+      <c r="I26" t="s">
         <v>68</v>
       </c>
       <c r="J26" t="s">

</xml_diff>

<commit_message>
New breaking in durable goods
</commit_message>
<xml_diff>
--- a/Data/MetaData.xlsx
+++ b/Data/MetaData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="12765" yWindow="4665" windowWidth="15630" windowHeight="10995" tabRatio="858" firstSheet="23" activeTab="24"/>
+    <workbookView xWindow="12765" yWindow="4665" windowWidth="15630" windowHeight="10995" tabRatio="858" firstSheet="34" activeTab="40"/>
   </bookViews>
   <sheets>
     <sheet name="CompressedFileNames" sheetId="1" r:id="rId1"/>
@@ -23702,7 +23702,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
+    <sheetView zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
       <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
@@ -43663,8 +43663,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Update MetaData, P2Cols Sheet, Year:83-88
</commit_message>
<xml_diff>
--- a/Data/MetaData.xlsx
+++ b/Data/MetaData.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\IRHEIS\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhash\OneDrive\Documents\GitHub\IRHEIS\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3F50BBF-18C8-46CE-8FA4-F541B269741C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12765" yWindow="4665" windowWidth="15630" windowHeight="10995" tabRatio="858" firstSheet="31" activeTab="37"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" tabRatio="858" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CompressedFileNames" sheetId="1" r:id="rId1"/>
@@ -89,7 +90,7 @@
     <sheet name="Khoshkbar" sheetId="1027" r:id="rId75"/>
     <sheet name="Nooshabe" sheetId="1041" r:id="rId76"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -102,7 +103,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17129" uniqueCount="666">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17448" uniqueCount="682">
   <si>
     <t>Year</t>
   </si>
@@ -2101,11 +2102,59 @@
   <si>
     <t>Gazz_Exp</t>
   </si>
+  <si>
+    <t>DYCOL46</t>
+  </si>
+  <si>
+    <t>DYCOL47</t>
+  </si>
+  <si>
+    <t>DYCOL48</t>
+  </si>
+  <si>
+    <t>DYCOL49</t>
+  </si>
+  <si>
+    <t>DYCOL50</t>
+  </si>
+  <si>
+    <t>DYCOL51</t>
+  </si>
+  <si>
+    <t>other_month</t>
+  </si>
+  <si>
+    <t>DYCOL52</t>
+  </si>
+  <si>
+    <t>DYCOL53</t>
+  </si>
+  <si>
+    <t>DYCOL54</t>
+  </si>
+  <si>
+    <t>DYCOL55</t>
+  </si>
+  <si>
+    <t>noceremony_year</t>
+  </si>
+  <si>
+    <t>DYCOL56</t>
+  </si>
+  <si>
+    <t>DYCOL57</t>
+  </si>
+  <si>
+    <t>DYCOL58</t>
+  </si>
+  <si>
+    <t>other_name</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="22">
     <font>
       <sz val="11"/>
@@ -3053,16 +3102,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="20.86328125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -3359,25 +3408,25 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:T42"/>
   <sheetViews>
     <sheetView topLeftCell="A11" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="12" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12.73046875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="12" max="13" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="16" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="19.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="16" width="13.3984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="19.73046875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="18" max="18" width="19" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="19" max="19" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="15.265625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
@@ -5444,25 +5493,25 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:T42"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="9" max="9" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12.73046875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="12.7109375" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12.73046875" customWidth="1" collapsed="1"/>
     <col min="12" max="12" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="12.73046875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="14" max="14" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="15.265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="13.3984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="12.59765625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="13.73046875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
@@ -7541,17 +7590,17 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:S36"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="8" max="8" width="10.5703125" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="10.59765625" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="13.73046875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
@@ -9384,17 +9433,17 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:S36"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="13.73046875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
@@ -11209,22 +11258,22 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="4" width="9.140625" style="3" collapsed="1"/>
-    <col min="5" max="5" width="9.140625" style="3"/>
-    <col min="6" max="6" width="9.140625" style="3" collapsed="1"/>
-    <col min="7" max="7" width="10.7109375" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="10" width="9.140625" style="3" collapsed="1"/>
-    <col min="11" max="11" width="11.140625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="16384" width="9.140625" style="3" collapsed="1"/>
+    <col min="1" max="4" width="9.1328125" style="3" collapsed="1"/>
+    <col min="5" max="5" width="9.1328125" style="3"/>
+    <col min="6" max="6" width="9.1328125" style="3" collapsed="1"/>
+    <col min="7" max="7" width="10.73046875" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="10" width="9.1328125" style="3" collapsed="1"/>
+    <col min="11" max="11" width="11.1328125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="16384" width="9.1328125" style="3" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -12370,16 +12419,16 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10.3984375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="15" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
@@ -12731,23 +12780,23 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView topLeftCell="A28" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.73046875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8.86328125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="10" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="8.73046875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.1328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11.86328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="10" width="8.73046875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="16.3984375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -13950,17 +13999,17 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:K36"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.1328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="16.3984375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -14419,20 +14468,20 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E23" sqref="E23:G36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.1328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="10.73046875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="10.265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="10.59765625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -15263,17 +15312,17 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:E127"/>
   <sheetViews>
     <sheetView topLeftCell="A109" workbookViewId="0">
       <selection activeCell="A126" sqref="A126:B127"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="2" width="11.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="2" width="11.3984375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.265625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -17166,14 +17215,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:R36"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="1:18">
       <c r="A1" t="s">
@@ -18534,18 +18583,18 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.1328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.59765625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="16.3984375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -19514,18 +19563,18 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.1328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.59765625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="16.3984375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -20494,16 +20543,16 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:K36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="10" max="10" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="16.3984375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -21649,18 +21698,18 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="9" width="14.140625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.1328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="9" width="14.1328125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="12.1328125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -22419,18 +22468,18 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <dimension ref="A1:K36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D22" sqref="D22:D33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="8.73046875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="10.59765625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -23699,19 +23748,19 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
       <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.140625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.1328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="12.1328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12.1328125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="12.1328125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -24722,14 +24771,14 @@
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
@@ -25739,14 +25788,14 @@
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
@@ -26756,14 +26805,14 @@
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="C21" sqref="C16:D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
@@ -27773,16 +27822,16 @@
 </file>
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="10" max="10" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -28793,48 +28842,51 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BL36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:BO36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" zoomScale="109" zoomScaleNormal="109" workbookViewId="0">
+      <selection activeCell="BK37" sqref="BK37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="31" max="32" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="12.42578125" customWidth="1"/>
-    <col min="49" max="49" width="10.42578125" customWidth="1"/>
-    <col min="50" max="50" width="16.85546875" customWidth="1"/>
-    <col min="51" max="51" width="14.85546875" customWidth="1"/>
-    <col min="52" max="52" width="19.7109375" customWidth="1"/>
-    <col min="53" max="53" width="17.7109375" customWidth="1"/>
-    <col min="54" max="54" width="12.85546875" customWidth="1"/>
-    <col min="55" max="55" width="10.85546875" customWidth="1"/>
-    <col min="56" max="56" width="12.42578125" customWidth="1"/>
-    <col min="57" max="57" width="10.42578125" customWidth="1"/>
-    <col min="58" max="58" width="16.7109375" customWidth="1"/>
-    <col min="59" max="60" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.1328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.86328125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.59765625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.86328125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.265625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.265625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="21.86328125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="19.3984375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="11.1328125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="10.73046875" bestFit="1" customWidth="1"/>
+    <col min="31" max="32" width="10.1328125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="9.86328125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="12.73046875" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="11.1328125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="10.3984375" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="12.3984375" customWidth="1"/>
+    <col min="49" max="49" width="10.3984375" customWidth="1"/>
+    <col min="50" max="50" width="16.86328125" customWidth="1"/>
+    <col min="51" max="51" width="14.86328125" customWidth="1"/>
+    <col min="52" max="52" width="19.73046875" customWidth="1"/>
+    <col min="53" max="53" width="17.73046875" customWidth="1"/>
+    <col min="54" max="54" width="12.86328125" customWidth="1"/>
+    <col min="55" max="55" width="10.86328125" customWidth="1"/>
+    <col min="56" max="56" width="12.3984375" customWidth="1"/>
+    <col min="57" max="57" width="10.3984375" customWidth="1"/>
+    <col min="58" max="58" width="16.73046875" customWidth="1"/>
+    <col min="59" max="60" width="16.73046875" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="14.73046875" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="14.73046875" customWidth="1"/>
+    <col min="63" max="63" width="10.73046875" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="14.73046875" customWidth="1"/>
+    <col min="65" max="65" width="10.73046875" customWidth="1"/>
+    <col min="66" max="66" width="12.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:63">
+    <row r="1" spans="1:66">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -29019,13 +29071,22 @@
         <v>584</v>
       </c>
       <c r="BJ1" s="9" t="s">
+        <v>672</v>
+      </c>
+      <c r="BK1" s="9" t="s">
         <v>565</v>
       </c>
-      <c r="BK1" s="9" t="s">
+      <c r="BL1" s="9" t="s">
+        <v>681</v>
+      </c>
+      <c r="BM1" s="9" t="s">
         <v>566</v>
       </c>
-    </row>
-    <row r="2" spans="1:63" hidden="1">
+      <c r="BN1" s="9" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="2" spans="1:66" hidden="1">
       <c r="A2" s="9">
         <v>63</v>
       </c>
@@ -29091,7 +29152,7 @@
       <c r="BG2" s="9"/>
       <c r="BH2" s="9"/>
     </row>
-    <row r="3" spans="1:63" hidden="1">
+    <row r="3" spans="1:66" hidden="1">
       <c r="A3" s="9">
         <v>64</v>
       </c>
@@ -29157,7 +29218,7 @@
       <c r="BG3" s="9"/>
       <c r="BH3" s="9"/>
     </row>
-    <row r="4" spans="1:63" hidden="1">
+    <row r="4" spans="1:66" hidden="1">
       <c r="A4" s="9">
         <v>65</v>
       </c>
@@ -29223,7 +29284,7 @@
       <c r="BG4" s="9"/>
       <c r="BH4" s="9"/>
     </row>
-    <row r="5" spans="1:63" hidden="1">
+    <row r="5" spans="1:66" hidden="1">
       <c r="A5" s="9">
         <v>66</v>
       </c>
@@ -29289,7 +29350,7 @@
       <c r="BG5" s="9"/>
       <c r="BH5" s="9"/>
     </row>
-    <row r="6" spans="1:63" hidden="1">
+    <row r="6" spans="1:66" hidden="1">
       <c r="A6" s="9">
         <v>67</v>
       </c>
@@ -29355,7 +29416,7 @@
       <c r="BG6" s="9"/>
       <c r="BH6" s="9"/>
     </row>
-    <row r="7" spans="1:63" hidden="1">
+    <row r="7" spans="1:66" hidden="1">
       <c r="A7" s="9">
         <v>68</v>
       </c>
@@ -29421,7 +29482,7 @@
       <c r="BG7" s="9"/>
       <c r="BH7" s="9"/>
     </row>
-    <row r="8" spans="1:63" hidden="1">
+    <row r="8" spans="1:66" hidden="1">
       <c r="A8" s="9">
         <v>69</v>
       </c>
@@ -29487,7 +29548,7 @@
       <c r="BG8" s="9"/>
       <c r="BH8" s="9"/>
     </row>
-    <row r="9" spans="1:63" hidden="1">
+    <row r="9" spans="1:66" hidden="1">
       <c r="A9" s="9">
         <v>70</v>
       </c>
@@ -29553,7 +29614,7 @@
       <c r="BG9" s="9"/>
       <c r="BH9" s="9"/>
     </row>
-    <row r="10" spans="1:63" hidden="1">
+    <row r="10" spans="1:66" hidden="1">
       <c r="A10" s="9">
         <v>71</v>
       </c>
@@ -29619,7 +29680,7 @@
       <c r="BG10" s="9"/>
       <c r="BH10" s="9"/>
     </row>
-    <row r="11" spans="1:63" hidden="1">
+    <row r="11" spans="1:66" hidden="1">
       <c r="A11" s="9">
         <v>72</v>
       </c>
@@ -29685,7 +29746,7 @@
       <c r="BG11" s="9"/>
       <c r="BH11" s="9"/>
     </row>
-    <row r="12" spans="1:63" hidden="1">
+    <row r="12" spans="1:66" hidden="1">
       <c r="A12" s="9">
         <v>73</v>
       </c>
@@ -29751,7 +29812,7 @@
       <c r="BG12" s="9"/>
       <c r="BH12" s="9"/>
     </row>
-    <row r="13" spans="1:63" hidden="1">
+    <row r="13" spans="1:66" hidden="1">
       <c r="A13" s="9">
         <v>74</v>
       </c>
@@ -29817,7 +29878,7 @@
       <c r="BG13" s="9"/>
       <c r="BH13" s="9"/>
     </row>
-    <row r="14" spans="1:63" hidden="1">
+    <row r="14" spans="1:66" hidden="1">
       <c r="A14" s="9">
         <v>75</v>
       </c>
@@ -29883,7 +29944,7 @@
       <c r="BG14" s="9"/>
       <c r="BH14" s="9"/>
     </row>
-    <row r="15" spans="1:63" hidden="1">
+    <row r="15" spans="1:66" hidden="1">
       <c r="A15" s="9">
         <v>76</v>
       </c>
@@ -29949,7 +30010,7 @@
       <c r="BG15" s="9"/>
       <c r="BH15" s="9"/>
     </row>
-    <row r="16" spans="1:63">
+    <row r="16" spans="1:66">
       <c r="A16" s="9">
         <v>77</v>
       </c>
@@ -30015,7 +30076,7 @@
       <c r="BG16" s="9"/>
       <c r="BH16" s="9"/>
     </row>
-    <row r="17" spans="1:64">
+    <row r="17" spans="1:67">
       <c r="A17" s="9">
         <v>78</v>
       </c>
@@ -30081,7 +30142,7 @@
       <c r="BG17" s="9"/>
       <c r="BH17" s="9"/>
     </row>
-    <row r="18" spans="1:64">
+    <row r="18" spans="1:67">
       <c r="A18" s="9">
         <v>79</v>
       </c>
@@ -30147,7 +30208,7 @@
       <c r="BG18" s="9"/>
       <c r="BH18" s="9"/>
     </row>
-    <row r="19" spans="1:64">
+    <row r="19" spans="1:67">
       <c r="A19" s="9">
         <v>80</v>
       </c>
@@ -30213,7 +30274,7 @@
       <c r="BG19" s="9"/>
       <c r="BH19" s="9"/>
     </row>
-    <row r="20" spans="1:64">
+    <row r="20" spans="1:67">
       <c r="A20" s="9">
         <v>81</v>
       </c>
@@ -30279,7 +30340,7 @@
       <c r="BG20" s="9"/>
       <c r="BH20" s="9"/>
     </row>
-    <row r="21" spans="1:64">
+    <row r="21" spans="1:67">
       <c r="A21" s="9">
         <v>82</v>
       </c>
@@ -30345,57 +30406,125 @@
       <c r="BG21" s="9"/>
       <c r="BH21" s="9"/>
     </row>
-    <row r="22" spans="1:64">
+    <row r="22" spans="1:67">
       <c r="A22" s="9">
         <v>83</v>
       </c>
       <c r="B22" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="C22" s="9"/>
+      <c r="C22" s="9" t="s">
+        <v>67</v>
+      </c>
       <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
-      <c r="H22" s="9"/>
-      <c r="I22" s="9"/>
-      <c r="J22" s="9"/>
-      <c r="K22" s="9"/>
-      <c r="L22" s="9"/>
-      <c r="M22" s="9"/>
-      <c r="N22" s="9"/>
-      <c r="O22" s="9"/>
-      <c r="P22" s="9"/>
-      <c r="Q22" s="9"/>
-      <c r="R22" s="9"/>
-      <c r="S22" s="9"/>
-      <c r="T22" s="9"/>
-      <c r="U22" s="9"/>
-      <c r="V22" s="9"/>
-      <c r="W22" s="9"/>
-      <c r="X22" s="9"/>
-      <c r="Y22" s="9"/>
-      <c r="Z22" s="9"/>
-      <c r="AA22" s="9"/>
-      <c r="AB22" s="9"/>
-      <c r="AC22" s="9"/>
-      <c r="AD22" s="9"/>
-      <c r="AE22" s="9"/>
-      <c r="AF22" s="9"/>
-      <c r="AG22" s="9"/>
-      <c r="AH22" s="9"/>
-      <c r="AI22" s="9"/>
-      <c r="AJ22" s="9"/>
-      <c r="AK22" s="9"/>
-      <c r="AL22" s="9"/>
-      <c r="AM22" s="9"/>
-      <c r="AN22" s="9"/>
-      <c r="AO22" s="9"/>
+      <c r="E22" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="G22" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="H22" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="I22" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="J22" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="K22" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="L22" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="M22" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="N22" s="9" t="s">
+        <v>325</v>
+      </c>
+      <c r="O22" s="9" t="s">
+        <v>326</v>
+      </c>
+      <c r="P22" s="9" t="s">
+        <v>327</v>
+      </c>
+      <c r="Q22" s="9" t="s">
+        <v>328</v>
+      </c>
+      <c r="R22" s="9" t="s">
+        <v>329</v>
+      </c>
+      <c r="S22" s="9" t="s">
+        <v>621</v>
+      </c>
+      <c r="T22" s="9" t="s">
+        <v>622</v>
+      </c>
+      <c r="V22" s="9" t="s">
+        <v>623</v>
+      </c>
+      <c r="W22" s="9" t="s">
+        <v>624</v>
+      </c>
+      <c r="X22" s="9" t="s">
+        <v>625</v>
+      </c>
+      <c r="Y22" s="9" t="s">
+        <v>626</v>
+      </c>
+      <c r="Z22" s="9" t="s">
+        <v>627</v>
+      </c>
+      <c r="AA22" s="9" t="s">
+        <v>628</v>
+      </c>
+      <c r="AE22" s="9" t="s">
+        <v>629</v>
+      </c>
+      <c r="AF22" s="9" t="s">
+        <v>630</v>
+      </c>
+      <c r="AG22" s="9" t="s">
+        <v>631</v>
+      </c>
+      <c r="AH22" s="9" t="s">
+        <v>632</v>
+      </c>
+      <c r="AI22" s="9" t="s">
+        <v>633</v>
+      </c>
+      <c r="AJ22" s="9" t="s">
+        <v>634</v>
+      </c>
+      <c r="AK22" s="9" t="s">
+        <v>635</v>
+      </c>
+      <c r="AL22" s="9" t="s">
+        <v>636</v>
+      </c>
+      <c r="AM22" s="9" t="s">
+        <v>637</v>
+      </c>
+      <c r="AN22" s="9" t="s">
+        <v>638</v>
+      </c>
+      <c r="AO22" s="3" t="s">
+        <v>639</v>
+      </c>
       <c r="AP22" s="9"/>
       <c r="AQ22" s="9"/>
       <c r="AR22" s="9"/>
-      <c r="AS22" s="9"/>
-      <c r="AT22" s="9"/>
+      <c r="AS22" s="9" t="s">
+        <v>640</v>
+      </c>
+      <c r="AT22" s="9" t="s">
+        <v>641</v>
+      </c>
       <c r="AU22" s="9"/>
       <c r="AV22" s="9"/>
       <c r="AW22" s="9"/>
@@ -30411,337 +30540,912 @@
       <c r="BG22" s="9"/>
       <c r="BH22" s="9"/>
     </row>
-    <row r="23" spans="1:64">
+    <row r="23" spans="1:67">
       <c r="A23" s="9">
         <v>84</v>
       </c>
       <c r="B23" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="C23" s="9"/>
+      <c r="C23" s="9" t="s">
+        <v>67</v>
+      </c>
       <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
-      <c r="H23" s="9"/>
-      <c r="I23" s="9"/>
-      <c r="J23" s="9"/>
-      <c r="K23" s="9"/>
-      <c r="L23" s="9"/>
-      <c r="M23" s="9"/>
-      <c r="N23" s="9"/>
-      <c r="O23" s="9"/>
-      <c r="P23" s="9"/>
-      <c r="Q23" s="9"/>
-      <c r="R23" s="9"/>
-      <c r="S23" s="9"/>
-      <c r="T23" s="9"/>
-      <c r="U23" s="9"/>
-      <c r="V23" s="9"/>
-      <c r="W23" s="9"/>
-      <c r="X23" s="9"/>
-      <c r="Y23" s="9"/>
-      <c r="Z23" s="9"/>
-      <c r="AA23" s="9"/>
+      <c r="E23" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="G23" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="H23" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="I23" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="J23" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="K23" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="L23" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="M23" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="N23" s="9" t="s">
+        <v>325</v>
+      </c>
+      <c r="O23" s="9" t="s">
+        <v>326</v>
+      </c>
+      <c r="P23" s="9" t="s">
+        <v>327</v>
+      </c>
+      <c r="Q23" s="9" t="s">
+        <v>328</v>
+      </c>
+      <c r="R23" s="9" t="s">
+        <v>329</v>
+      </c>
+      <c r="S23" s="9" t="s">
+        <v>621</v>
+      </c>
+      <c r="T23" s="9" t="s">
+        <v>622</v>
+      </c>
+      <c r="U23" s="9" t="s">
+        <v>623</v>
+      </c>
+      <c r="V23" s="9" t="s">
+        <v>624</v>
+      </c>
+      <c r="W23" s="9" t="s">
+        <v>625</v>
+      </c>
+      <c r="X23" s="9" t="s">
+        <v>626</v>
+      </c>
+      <c r="Y23" s="9" t="s">
+        <v>627</v>
+      </c>
+      <c r="Z23" s="9" t="s">
+        <v>628</v>
+      </c>
+      <c r="AA23" s="9" t="s">
+        <v>629</v>
+      </c>
       <c r="AB23" s="9"/>
       <c r="AC23" s="9"/>
       <c r="AD23" s="9"/>
-      <c r="AE23" s="9"/>
-      <c r="AF23" s="9"/>
-      <c r="AG23" s="9"/>
-      <c r="AH23" s="9"/>
-      <c r="AI23" s="9"/>
-      <c r="AJ23" s="9"/>
-      <c r="AK23" s="9"/>
-      <c r="AL23" s="9"/>
-      <c r="AM23" s="9"/>
-      <c r="AN23" s="9"/>
-      <c r="AO23" s="9"/>
+      <c r="AE23" s="9" t="s">
+        <v>630</v>
+      </c>
+      <c r="AF23" s="9" t="s">
+        <v>631</v>
+      </c>
+      <c r="AG23" s="9" t="s">
+        <v>632</v>
+      </c>
+      <c r="AH23" s="9" t="s">
+        <v>633</v>
+      </c>
+      <c r="AI23" s="9" t="s">
+        <v>634</v>
+      </c>
+      <c r="AJ23" s="9" t="s">
+        <v>635</v>
+      </c>
+      <c r="AK23" s="9" t="s">
+        <v>636</v>
+      </c>
+      <c r="AL23" s="9" t="s">
+        <v>637</v>
+      </c>
+      <c r="AM23" s="9" t="s">
+        <v>638</v>
+      </c>
+      <c r="AN23" s="3" t="s">
+        <v>639</v>
+      </c>
+      <c r="AO23" s="3" t="s">
+        <v>640</v>
+      </c>
       <c r="AP23" s="9"/>
       <c r="AQ23" s="9"/>
       <c r="AR23" s="9"/>
-      <c r="AS23" s="9"/>
-      <c r="AT23" s="9"/>
+      <c r="AS23" s="9" t="s">
+        <v>641</v>
+      </c>
+      <c r="AT23" s="9" t="s">
+        <v>642</v>
+      </c>
       <c r="AU23" s="9"/>
-      <c r="AV23" s="9"/>
-      <c r="AW23" s="9"/>
-      <c r="AX23" s="9"/>
-      <c r="AY23" s="9"/>
-      <c r="AZ23" s="9"/>
-      <c r="BA23" s="9"/>
-      <c r="BB23" s="9"/>
-      <c r="BC23" s="9"/>
-      <c r="BD23" s="9"/>
-      <c r="BE23" s="9"/>
-      <c r="BF23" s="9"/>
-      <c r="BG23" s="9"/>
-      <c r="BH23" s="9"/>
-    </row>
-    <row r="24" spans="1:64">
+      <c r="AV23" s="9" t="s">
+        <v>643</v>
+      </c>
+      <c r="AW23" s="9" t="s">
+        <v>644</v>
+      </c>
+      <c r="AX23" s="9" t="s">
+        <v>645</v>
+      </c>
+      <c r="AY23" s="9" t="s">
+        <v>646</v>
+      </c>
+      <c r="AZ23" s="9" t="s">
+        <v>647</v>
+      </c>
+      <c r="BA23" s="9" t="s">
+        <v>648</v>
+      </c>
+      <c r="BB23" s="9" t="s">
+        <v>649</v>
+      </c>
+      <c r="BC23" s="9" t="s">
+        <v>650</v>
+      </c>
+      <c r="BD23" s="9" t="s">
+        <v>666</v>
+      </c>
+      <c r="BE23" s="9" t="s">
+        <v>667</v>
+      </c>
+      <c r="BH23" s="9" t="s">
+        <v>668</v>
+      </c>
+      <c r="BI23" s="9"/>
+      <c r="BJ23" s="9" t="s">
+        <v>669</v>
+      </c>
+      <c r="BK23" s="9" t="s">
+        <v>670</v>
+      </c>
+      <c r="BL23" s="9"/>
+      <c r="BM23" s="9" t="s">
+        <v>671</v>
+      </c>
+      <c r="BN23" s="9" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="24" spans="1:67">
       <c r="A24" s="9">
         <v>85</v>
       </c>
       <c r="B24" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="C24" s="9"/>
+      <c r="C24" s="9" t="s">
+        <v>67</v>
+      </c>
       <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
-      <c r="H24" s="9"/>
-      <c r="I24" s="9"/>
-      <c r="J24" s="9"/>
-      <c r="K24" s="9"/>
-      <c r="L24" s="9"/>
-      <c r="M24" s="9"/>
-      <c r="N24" s="9"/>
-      <c r="O24" s="9"/>
-      <c r="P24" s="9"/>
-      <c r="Q24" s="9"/>
-      <c r="R24" s="9"/>
-      <c r="S24" s="9"/>
-      <c r="T24" s="9"/>
-      <c r="U24" s="9"/>
-      <c r="V24" s="9"/>
-      <c r="W24" s="9"/>
-      <c r="X24" s="9"/>
-      <c r="Y24" s="9"/>
-      <c r="Z24" s="9"/>
-      <c r="AA24" s="9"/>
-      <c r="AB24" s="9"/>
-      <c r="AC24" s="9"/>
+      <c r="E24" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="G24" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="H24" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="I24" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="J24" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="K24" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="L24" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="M24" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="N24" s="9" t="s">
+        <v>325</v>
+      </c>
+      <c r="O24" s="9" t="s">
+        <v>326</v>
+      </c>
+      <c r="P24" s="9" t="s">
+        <v>327</v>
+      </c>
+      <c r="Q24" s="9" t="s">
+        <v>328</v>
+      </c>
+      <c r="R24" s="9" t="s">
+        <v>329</v>
+      </c>
+      <c r="S24" s="9" t="s">
+        <v>621</v>
+      </c>
+      <c r="T24" s="9" t="s">
+        <v>622</v>
+      </c>
+      <c r="U24" s="9" t="s">
+        <v>623</v>
+      </c>
+      <c r="V24" s="9" t="s">
+        <v>624</v>
+      </c>
+      <c r="W24" s="9" t="s">
+        <v>625</v>
+      </c>
+      <c r="X24" s="9" t="s">
+        <v>626</v>
+      </c>
+      <c r="Y24" s="9" t="s">
+        <v>627</v>
+      </c>
+      <c r="Z24" s="9" t="s">
+        <v>628</v>
+      </c>
+      <c r="AA24" s="9" t="s">
+        <v>629</v>
+      </c>
+      <c r="AB24" s="9" t="s">
+        <v>630</v>
+      </c>
+      <c r="AC24" s="9" t="s">
+        <v>631</v>
+      </c>
       <c r="AD24" s="9"/>
-      <c r="AE24" s="9"/>
-      <c r="AF24" s="9"/>
-      <c r="AG24" s="9"/>
-      <c r="AH24" s="9"/>
-      <c r="AI24" s="9"/>
-      <c r="AJ24" s="9"/>
-      <c r="AK24" s="9"/>
-      <c r="AL24" s="9"/>
-      <c r="AM24" s="9"/>
-      <c r="AN24" s="9"/>
-      <c r="AO24" s="9"/>
-      <c r="AP24" s="9"/>
-      <c r="AQ24" s="9"/>
-      <c r="AR24" s="9"/>
-      <c r="AS24" s="9"/>
-      <c r="AT24" s="9"/>
+      <c r="AE24" s="9" t="s">
+        <v>632</v>
+      </c>
+      <c r="AF24" s="9" t="s">
+        <v>633</v>
+      </c>
+      <c r="AG24" s="9" t="s">
+        <v>634</v>
+      </c>
+      <c r="AH24" s="9" t="s">
+        <v>635</v>
+      </c>
+      <c r="AI24" s="9" t="s">
+        <v>636</v>
+      </c>
+      <c r="AJ24" s="9" t="s">
+        <v>637</v>
+      </c>
+      <c r="AK24" s="9" t="s">
+        <v>638</v>
+      </c>
+      <c r="AL24" s="3" t="s">
+        <v>639</v>
+      </c>
+      <c r="AM24" s="3" t="s">
+        <v>640</v>
+      </c>
+      <c r="AN24" s="3" t="s">
+        <v>641</v>
+      </c>
+      <c r="AO24" s="3" t="s">
+        <v>642</v>
+      </c>
+      <c r="AP24" s="3" t="s">
+        <v>643</v>
+      </c>
+      <c r="AQ24" s="3" t="s">
+        <v>644</v>
+      </c>
+      <c r="AS24" s="9" t="s">
+        <v>645</v>
+      </c>
+      <c r="AT24" s="9" t="s">
+        <v>646</v>
+      </c>
       <c r="AU24" s="9"/>
-      <c r="AV24" s="9"/>
-      <c r="AW24" s="9"/>
-      <c r="AX24" s="9"/>
-      <c r="AY24" s="9"/>
-      <c r="AZ24" s="9"/>
-      <c r="BA24" s="9"/>
-      <c r="BB24" s="9"/>
-      <c r="BC24" s="9"/>
-      <c r="BD24" s="9"/>
-      <c r="BE24" s="9"/>
-      <c r="BF24" s="9"/>
-      <c r="BG24" s="9"/>
-      <c r="BH24" s="9"/>
-    </row>
-    <row r="25" spans="1:64">
+      <c r="AV24" s="9" t="s">
+        <v>647</v>
+      </c>
+      <c r="AW24" s="9" t="s">
+        <v>648</v>
+      </c>
+      <c r="AX24" s="9" t="s">
+        <v>649</v>
+      </c>
+      <c r="AY24" s="9" t="s">
+        <v>650</v>
+      </c>
+      <c r="AZ24" s="9" t="s">
+        <v>666</v>
+      </c>
+      <c r="BA24" s="9" t="s">
+        <v>667</v>
+      </c>
+      <c r="BB24" s="9" t="s">
+        <v>668</v>
+      </c>
+      <c r="BC24" s="9" t="s">
+        <v>669</v>
+      </c>
+      <c r="BD24" s="9" t="s">
+        <v>670</v>
+      </c>
+      <c r="BE24" s="9" t="s">
+        <v>671</v>
+      </c>
+      <c r="BH24" s="9" t="s">
+        <v>673</v>
+      </c>
+      <c r="BI24" s="9"/>
+      <c r="BJ24" s="9" t="s">
+        <v>674</v>
+      </c>
+      <c r="BK24" s="9" t="s">
+        <v>675</v>
+      </c>
+      <c r="BL24" s="9"/>
+      <c r="BM24" s="9" t="s">
+        <v>676</v>
+      </c>
+      <c r="BN24" s="9"/>
+    </row>
+    <row r="25" spans="1:67">
       <c r="A25" s="9">
         <v>86</v>
       </c>
       <c r="B25" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="C25" s="9"/>
+      <c r="C25" s="9" t="s">
+        <v>67</v>
+      </c>
       <c r="D25" s="9"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="9"/>
-      <c r="G25" s="9"/>
-      <c r="H25" s="9"/>
-      <c r="I25" s="9"/>
-      <c r="J25" s="9"/>
-      <c r="K25" s="9"/>
-      <c r="L25" s="9"/>
-      <c r="M25" s="9"/>
-      <c r="N25" s="9"/>
-      <c r="O25" s="9"/>
-      <c r="P25" s="9"/>
-      <c r="Q25" s="9"/>
-      <c r="R25" s="9"/>
-      <c r="S25" s="9"/>
-      <c r="T25" s="9"/>
-      <c r="U25" s="9"/>
-      <c r="V25" s="9"/>
-      <c r="W25" s="9"/>
-      <c r="X25" s="9"/>
-      <c r="Y25" s="9"/>
-      <c r="Z25" s="9"/>
-      <c r="AA25" s="9"/>
-      <c r="AB25" s="9"/>
-      <c r="AC25" s="9"/>
+      <c r="E25" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="F25" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="G25" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="H25" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="I25" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="J25" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="K25" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="L25" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="M25" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="N25" s="9" t="s">
+        <v>325</v>
+      </c>
+      <c r="O25" s="9" t="s">
+        <v>326</v>
+      </c>
+      <c r="P25" s="9" t="s">
+        <v>327</v>
+      </c>
+      <c r="Q25" s="9" t="s">
+        <v>328</v>
+      </c>
+      <c r="R25" s="9" t="s">
+        <v>329</v>
+      </c>
+      <c r="S25" s="9" t="s">
+        <v>621</v>
+      </c>
+      <c r="T25" s="9" t="s">
+        <v>622</v>
+      </c>
+      <c r="U25" s="9" t="s">
+        <v>623</v>
+      </c>
+      <c r="V25" s="9" t="s">
+        <v>624</v>
+      </c>
+      <c r="W25" s="9" t="s">
+        <v>625</v>
+      </c>
+      <c r="X25" s="9" t="s">
+        <v>626</v>
+      </c>
+      <c r="Y25" s="9" t="s">
+        <v>627</v>
+      </c>
+      <c r="Z25" s="9" t="s">
+        <v>628</v>
+      </c>
+      <c r="AA25" s="9" t="s">
+        <v>629</v>
+      </c>
+      <c r="AB25" s="9" t="s">
+        <v>630</v>
+      </c>
+      <c r="AC25" s="9" t="s">
+        <v>631</v>
+      </c>
       <c r="AD25" s="9"/>
-      <c r="AE25" s="9"/>
-      <c r="AF25" s="9"/>
-      <c r="AG25" s="9"/>
-      <c r="AH25" s="9"/>
-      <c r="AI25" s="9"/>
-      <c r="AJ25" s="9"/>
-      <c r="AK25" s="9"/>
-      <c r="AL25" s="9"/>
-      <c r="AM25" s="9"/>
-      <c r="AN25" s="9"/>
-      <c r="AO25" s="9"/>
-      <c r="AP25" s="9"/>
-      <c r="AQ25" s="9"/>
-      <c r="AR25" s="9"/>
-      <c r="AS25" s="9"/>
-      <c r="AT25" s="9"/>
-      <c r="AU25" s="9"/>
-      <c r="AV25" s="9"/>
-      <c r="AW25" s="9"/>
-      <c r="AX25" s="9"/>
-      <c r="AY25" s="9"/>
-      <c r="AZ25" s="9"/>
-      <c r="BA25" s="9"/>
-      <c r="BB25" s="9"/>
-      <c r="BC25" s="9"/>
-      <c r="BD25" s="9"/>
-      <c r="BE25" s="9"/>
-      <c r="BF25" s="9"/>
-      <c r="BG25" s="9"/>
-      <c r="BH25" s="9"/>
-    </row>
-    <row r="26" spans="1:64">
+      <c r="AE25" s="9" t="s">
+        <v>632</v>
+      </c>
+      <c r="AF25" s="9" t="s">
+        <v>633</v>
+      </c>
+      <c r="AG25" s="9" t="s">
+        <v>634</v>
+      </c>
+      <c r="AH25" s="9" t="s">
+        <v>635</v>
+      </c>
+      <c r="AI25" s="9" t="s">
+        <v>636</v>
+      </c>
+      <c r="AJ25" s="9" t="s">
+        <v>637</v>
+      </c>
+      <c r="AK25" s="9" t="s">
+        <v>638</v>
+      </c>
+      <c r="AL25" s="3" t="s">
+        <v>639</v>
+      </c>
+      <c r="AM25" s="3" t="s">
+        <v>640</v>
+      </c>
+      <c r="AN25" s="3" t="s">
+        <v>641</v>
+      </c>
+      <c r="AO25" s="3" t="s">
+        <v>642</v>
+      </c>
+      <c r="AP25" s="3" t="s">
+        <v>643</v>
+      </c>
+      <c r="AQ25" s="3" t="s">
+        <v>644</v>
+      </c>
+      <c r="AR25" s="9" t="s">
+        <v>645</v>
+      </c>
+      <c r="AS25" s="9" t="s">
+        <v>646</v>
+      </c>
+      <c r="AT25" s="9" t="s">
+        <v>647</v>
+      </c>
+      <c r="AU25" s="9" t="s">
+        <v>648</v>
+      </c>
+      <c r="AV25" s="9" t="s">
+        <v>649</v>
+      </c>
+      <c r="AW25" s="9" t="s">
+        <v>650</v>
+      </c>
+      <c r="AX25" s="9" t="s">
+        <v>666</v>
+      </c>
+      <c r="AY25" s="9" t="s">
+        <v>667</v>
+      </c>
+      <c r="AZ25" s="9" t="s">
+        <v>668</v>
+      </c>
+      <c r="BA25" s="9" t="s">
+        <v>669</v>
+      </c>
+      <c r="BB25" s="9" t="s">
+        <v>670</v>
+      </c>
+      <c r="BC25" s="9" t="s">
+        <v>671</v>
+      </c>
+      <c r="BD25" s="9" t="s">
+        <v>673</v>
+      </c>
+      <c r="BE25" s="9" t="s">
+        <v>674</v>
+      </c>
+      <c r="BH25" s="9" t="s">
+        <v>675</v>
+      </c>
+      <c r="BI25" s="9"/>
+      <c r="BJ25" s="9" t="s">
+        <v>676</v>
+      </c>
+      <c r="BK25" s="9" t="s">
+        <v>678</v>
+      </c>
+      <c r="BL25" s="9"/>
+      <c r="BM25" s="9" t="s">
+        <v>679</v>
+      </c>
+      <c r="BN25" s="9"/>
+    </row>
+    <row r="26" spans="1:67">
       <c r="A26" s="9">
         <v>87</v>
       </c>
       <c r="B26" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="C26" s="9"/>
-      <c r="D26" s="9"/>
-      <c r="E26" s="9"/>
-      <c r="F26" s="9"/>
-      <c r="G26" s="9"/>
-      <c r="H26" s="9"/>
-      <c r="I26" s="9"/>
-      <c r="J26" s="9"/>
-      <c r="K26" s="9"/>
-      <c r="L26" s="9"/>
-      <c r="M26" s="9"/>
-      <c r="N26" s="9"/>
-      <c r="O26" s="9"/>
-      <c r="P26" s="9"/>
-      <c r="Q26" s="9"/>
-      <c r="R26" s="9"/>
-      <c r="S26" s="9"/>
-      <c r="T26" s="9"/>
-      <c r="U26" s="9"/>
-      <c r="V26" s="9"/>
-      <c r="W26" s="9"/>
-      <c r="X26" s="9"/>
-      <c r="Y26" s="9"/>
-      <c r="Z26" s="9"/>
-      <c r="AA26" s="9"/>
-      <c r="AB26" s="9"/>
-      <c r="AC26" s="9"/>
-      <c r="AD26" s="9"/>
-      <c r="AE26" s="9"/>
-      <c r="AF26" s="9"/>
-      <c r="AG26" s="9"/>
-      <c r="AH26" s="9"/>
-      <c r="AI26" s="9"/>
-      <c r="AJ26" s="9"/>
-      <c r="AK26" s="9"/>
-      <c r="AL26" s="9"/>
-      <c r="AM26" s="9"/>
-      <c r="AN26" s="9"/>
-      <c r="AO26" s="9"/>
-      <c r="AP26" s="9"/>
-      <c r="AQ26" s="9"/>
-      <c r="AR26" s="9"/>
-      <c r="AS26" s="9"/>
-      <c r="AT26" s="9"/>
-      <c r="AU26" s="9"/>
-      <c r="AV26" s="9"/>
-      <c r="AW26" s="9"/>
-      <c r="AX26" s="9"/>
-      <c r="AY26" s="9"/>
-      <c r="AZ26" s="9"/>
-      <c r="BA26" s="9"/>
-      <c r="BB26" s="9"/>
-      <c r="BC26" s="9"/>
-      <c r="BD26" s="9"/>
-      <c r="BE26" s="9"/>
-      <c r="BF26" s="9"/>
-      <c r="BG26" s="9"/>
-      <c r="BH26" s="9"/>
-    </row>
-    <row r="27" spans="1:64">
+      <c r="C26" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="F26" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="G26" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="H26" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="I26" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="J26" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="K26" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="L26" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="M26" s="9" t="s">
+        <v>325</v>
+      </c>
+      <c r="N26" s="9" t="s">
+        <v>326</v>
+      </c>
+      <c r="O26" s="9" t="s">
+        <v>327</v>
+      </c>
+      <c r="P26" s="9" t="s">
+        <v>328</v>
+      </c>
+      <c r="Q26" s="9" t="s">
+        <v>329</v>
+      </c>
+      <c r="R26" s="9" t="s">
+        <v>621</v>
+      </c>
+      <c r="S26" s="9" t="s">
+        <v>622</v>
+      </c>
+      <c r="T26" s="9" t="s">
+        <v>623</v>
+      </c>
+      <c r="U26" s="9" t="s">
+        <v>624</v>
+      </c>
+      <c r="V26" s="9" t="s">
+        <v>625</v>
+      </c>
+      <c r="W26" s="9" t="s">
+        <v>626</v>
+      </c>
+      <c r="X26" s="9" t="s">
+        <v>627</v>
+      </c>
+      <c r="Y26" s="9" t="s">
+        <v>628</v>
+      </c>
+      <c r="Z26" s="9" t="s">
+        <v>629</v>
+      </c>
+      <c r="AA26" s="9" t="s">
+        <v>630</v>
+      </c>
+      <c r="AB26" s="9" t="s">
+        <v>631</v>
+      </c>
+      <c r="AC26" s="9" t="s">
+        <v>632</v>
+      </c>
+      <c r="AE26" s="9" t="s">
+        <v>633</v>
+      </c>
+      <c r="AF26" s="9" t="s">
+        <v>634</v>
+      </c>
+      <c r="AG26" s="9" t="s">
+        <v>635</v>
+      </c>
+      <c r="AH26" s="9" t="s">
+        <v>636</v>
+      </c>
+      <c r="AI26" s="9" t="s">
+        <v>637</v>
+      </c>
+      <c r="AJ26" s="9" t="s">
+        <v>638</v>
+      </c>
+      <c r="AK26" s="3" t="s">
+        <v>639</v>
+      </c>
+      <c r="AL26" s="3" t="s">
+        <v>640</v>
+      </c>
+      <c r="AM26" s="3" t="s">
+        <v>641</v>
+      </c>
+      <c r="AN26" s="3" t="s">
+        <v>642</v>
+      </c>
+      <c r="AO26" s="3" t="s">
+        <v>643</v>
+      </c>
+      <c r="AP26" s="3" t="s">
+        <v>644</v>
+      </c>
+      <c r="AQ26" s="9" t="s">
+        <v>645</v>
+      </c>
+      <c r="AR26" s="9" t="s">
+        <v>646</v>
+      </c>
+      <c r="AS26" s="9" t="s">
+        <v>647</v>
+      </c>
+      <c r="AT26" s="9" t="s">
+        <v>648</v>
+      </c>
+      <c r="AU26" s="9" t="s">
+        <v>649</v>
+      </c>
+      <c r="AV26" s="9" t="s">
+        <v>650</v>
+      </c>
+      <c r="AW26" s="9" t="s">
+        <v>666</v>
+      </c>
+      <c r="AX26" s="9" t="s">
+        <v>667</v>
+      </c>
+      <c r="AY26" s="9" t="s">
+        <v>668</v>
+      </c>
+      <c r="AZ26" s="9" t="s">
+        <v>669</v>
+      </c>
+      <c r="BA26" s="9" t="s">
+        <v>670</v>
+      </c>
+      <c r="BB26" s="9" t="s">
+        <v>671</v>
+      </c>
+      <c r="BC26" s="9" t="s">
+        <v>673</v>
+      </c>
+      <c r="BD26" s="9" t="s">
+        <v>674</v>
+      </c>
+      <c r="BE26" s="9" t="s">
+        <v>675</v>
+      </c>
+      <c r="BH26" s="9" t="s">
+        <v>676</v>
+      </c>
+      <c r="BI26" s="9"/>
+      <c r="BJ26" s="9" t="s">
+        <v>678</v>
+      </c>
+      <c r="BK26" s="9" t="s">
+        <v>679</v>
+      </c>
+      <c r="BL26" s="9"/>
+      <c r="BM26" s="9" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="27" spans="1:67">
       <c r="A27" s="9">
         <v>88</v>
       </c>
       <c r="B27" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="C27" s="9"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="9"/>
-      <c r="F27" s="9"/>
-      <c r="G27" s="9"/>
-      <c r="H27" s="9"/>
-      <c r="I27" s="9"/>
-      <c r="J27" s="9"/>
-      <c r="K27" s="9"/>
-      <c r="L27" s="9"/>
-      <c r="M27" s="9"/>
-      <c r="N27" s="9"/>
-      <c r="O27" s="9"/>
-      <c r="P27" s="9"/>
-      <c r="Q27" s="9"/>
-      <c r="R27" s="9"/>
-      <c r="S27" s="9"/>
-      <c r="T27" s="9"/>
-      <c r="U27" s="9"/>
-      <c r="V27" s="9"/>
-      <c r="W27" s="9"/>
-      <c r="X27" s="9"/>
-      <c r="Y27" s="9"/>
-      <c r="Z27" s="9"/>
-      <c r="AA27" s="9"/>
-      <c r="AB27" s="9"/>
-      <c r="AC27" s="9"/>
-      <c r="AD27" s="9"/>
-      <c r="AE27" s="9"/>
-      <c r="AF27" s="9"/>
-      <c r="AG27" s="9"/>
-      <c r="AH27" s="9"/>
-      <c r="AI27" s="9"/>
-      <c r="AJ27" s="9"/>
-      <c r="AK27" s="9"/>
-      <c r="AL27" s="9"/>
-      <c r="AM27" s="9"/>
-      <c r="AN27" s="9"/>
-      <c r="AO27" s="9"/>
-      <c r="AP27" s="9"/>
-      <c r="AQ27" s="9"/>
-      <c r="AR27" s="9"/>
-      <c r="AS27" s="9"/>
-      <c r="AT27" s="9"/>
-      <c r="AU27" s="9"/>
-      <c r="AV27" s="9"/>
-      <c r="AW27" s="9"/>
-      <c r="AX27" s="9"/>
-      <c r="AY27" s="9"/>
-      <c r="AZ27" s="9"/>
-      <c r="BA27" s="9"/>
-      <c r="BB27" s="9"/>
-      <c r="BC27" s="9"/>
-      <c r="BD27" s="9"/>
-      <c r="BE27" s="9"/>
-      <c r="BF27" s="9"/>
-      <c r="BG27" s="9"/>
-      <c r="BH27" s="9"/>
-    </row>
-    <row r="28" spans="1:64">
+      <c r="C27" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="F27" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="G27" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="H27" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="I27" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="J27" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="K27" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="L27" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="M27" s="9" t="s">
+        <v>325</v>
+      </c>
+      <c r="N27" s="9" t="s">
+        <v>326</v>
+      </c>
+      <c r="O27" s="9" t="s">
+        <v>327</v>
+      </c>
+      <c r="P27" s="9" t="s">
+        <v>328</v>
+      </c>
+      <c r="Q27" s="9" t="s">
+        <v>329</v>
+      </c>
+      <c r="R27" s="9" t="s">
+        <v>621</v>
+      </c>
+      <c r="S27" s="9" t="s">
+        <v>622</v>
+      </c>
+      <c r="T27" s="9" t="s">
+        <v>623</v>
+      </c>
+      <c r="U27" s="9" t="s">
+        <v>624</v>
+      </c>
+      <c r="V27" s="9" t="s">
+        <v>625</v>
+      </c>
+      <c r="W27" s="9" t="s">
+        <v>626</v>
+      </c>
+      <c r="X27" s="9" t="s">
+        <v>627</v>
+      </c>
+      <c r="Y27" s="9" t="s">
+        <v>628</v>
+      </c>
+      <c r="Z27" s="9" t="s">
+        <v>629</v>
+      </c>
+      <c r="AA27" s="9" t="s">
+        <v>630</v>
+      </c>
+      <c r="AB27" s="9" t="s">
+        <v>631</v>
+      </c>
+      <c r="AC27" s="9" t="s">
+        <v>632</v>
+      </c>
+      <c r="AE27" s="9" t="s">
+        <v>633</v>
+      </c>
+      <c r="AF27" s="9" t="s">
+        <v>634</v>
+      </c>
+      <c r="AG27" s="9" t="s">
+        <v>635</v>
+      </c>
+      <c r="AH27" s="9" t="s">
+        <v>636</v>
+      </c>
+      <c r="AI27" s="9" t="s">
+        <v>637</v>
+      </c>
+      <c r="AJ27" s="9" t="s">
+        <v>638</v>
+      </c>
+      <c r="AK27" s="3" t="s">
+        <v>639</v>
+      </c>
+      <c r="AL27" s="3" t="s">
+        <v>640</v>
+      </c>
+      <c r="AM27" s="3" t="s">
+        <v>641</v>
+      </c>
+      <c r="AN27" s="3" t="s">
+        <v>642</v>
+      </c>
+      <c r="AO27" s="3" t="s">
+        <v>643</v>
+      </c>
+      <c r="AP27" s="3" t="s">
+        <v>644</v>
+      </c>
+      <c r="AQ27" s="9" t="s">
+        <v>645</v>
+      </c>
+      <c r="AR27" s="9" t="s">
+        <v>646</v>
+      </c>
+      <c r="AS27" s="9" t="s">
+        <v>647</v>
+      </c>
+      <c r="AT27" s="9" t="s">
+        <v>648</v>
+      </c>
+      <c r="AU27" s="9" t="s">
+        <v>649</v>
+      </c>
+      <c r="AV27" s="9" t="s">
+        <v>650</v>
+      </c>
+      <c r="AW27" s="9" t="s">
+        <v>666</v>
+      </c>
+      <c r="AX27" s="9" t="s">
+        <v>667</v>
+      </c>
+      <c r="AY27" s="9" t="s">
+        <v>668</v>
+      </c>
+      <c r="AZ27" s="9" t="s">
+        <v>669</v>
+      </c>
+      <c r="BA27" s="9" t="s">
+        <v>670</v>
+      </c>
+      <c r="BB27" s="9" t="s">
+        <v>671</v>
+      </c>
+      <c r="BC27" s="9" t="s">
+        <v>673</v>
+      </c>
+      <c r="BD27" s="9" t="s">
+        <v>674</v>
+      </c>
+      <c r="BE27" s="9" t="s">
+        <v>675</v>
+      </c>
+      <c r="BH27" s="9" t="s">
+        <v>676</v>
+      </c>
+      <c r="BI27" s="9"/>
+      <c r="BJ27" s="9" t="s">
+        <v>678</v>
+      </c>
+      <c r="BK27" s="9" t="s">
+        <v>679</v>
+      </c>
+      <c r="BL27" s="9"/>
+      <c r="BM27" s="9" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="28" spans="1:67">
       <c r="A28" s="9">
         <v>89</v>
       </c>
@@ -30919,15 +31623,15 @@
       <c r="BH28" s="9" t="s">
         <v>579</v>
       </c>
-      <c r="BJ28" s="9" t="s">
+      <c r="BL28" s="9" t="s">
         <v>581</v>
       </c>
-      <c r="BK28" s="9" t="s">
+      <c r="BM28" s="9" t="s">
         <v>580</v>
       </c>
-      <c r="BL28" s="9"/>
-    </row>
-    <row r="29" spans="1:64">
+      <c r="BO28" s="9"/>
+    </row>
+    <row r="29" spans="1:67">
       <c r="A29" s="9">
         <v>90</v>
       </c>
@@ -31105,14 +31809,14 @@
       <c r="BH29" s="9" t="s">
         <v>579</v>
       </c>
-      <c r="BJ29" s="9" t="s">
+      <c r="BL29" s="9" t="s">
         <v>581</v>
       </c>
-      <c r="BK29" s="9" t="s">
+      <c r="BM29" s="9" t="s">
         <v>580</v>
       </c>
     </row>
-    <row r="30" spans="1:64">
+    <row r="30" spans="1:67">
       <c r="A30" s="9">
         <v>91</v>
       </c>
@@ -31296,14 +32000,15 @@
       <c r="BI30" s="9" t="s">
         <v>581</v>
       </c>
-      <c r="BJ30" s="9" t="s">
+      <c r="BJ30" s="9"/>
+      <c r="BL30" s="9" t="s">
         <v>582</v>
       </c>
-      <c r="BK30" s="9" t="s">
+      <c r="BM30" s="9" t="s">
         <v>583</v>
       </c>
     </row>
-    <row r="31" spans="1:64">
+    <row r="31" spans="1:67">
       <c r="A31" s="9">
         <v>92</v>
       </c>
@@ -31487,14 +32192,15 @@
       <c r="BI31" s="9" t="s">
         <v>581</v>
       </c>
-      <c r="BJ31" s="9" t="s">
+      <c r="BJ31" s="9"/>
+      <c r="BL31" s="9" t="s">
         <v>582</v>
       </c>
-      <c r="BK31" s="9" t="s">
+      <c r="BM31" s="9" t="s">
         <v>583</v>
       </c>
     </row>
-    <row r="32" spans="1:64">
+    <row r="32" spans="1:67">
       <c r="A32" s="9">
         <v>93</v>
       </c>
@@ -31678,14 +32384,15 @@
       <c r="BI32" s="9" t="s">
         <v>581</v>
       </c>
-      <c r="BJ32" s="9" t="s">
+      <c r="BJ32" s="9"/>
+      <c r="BL32" s="9" t="s">
         <v>582</v>
       </c>
-      <c r="BK32" s="9" t="s">
+      <c r="BM32" s="9" t="s">
         <v>583</v>
       </c>
     </row>
-    <row r="33" spans="1:63">
+    <row r="33" spans="1:66">
       <c r="A33" s="9">
         <v>94</v>
       </c>
@@ -31869,14 +32576,15 @@
       <c r="BI33" s="9" t="s">
         <v>581</v>
       </c>
-      <c r="BJ33" s="9" t="s">
+      <c r="BJ33" s="9"/>
+      <c r="BL33" s="9" t="s">
         <v>582</v>
       </c>
-      <c r="BK33" s="9" t="s">
+      <c r="BM33" s="9" t="s">
         <v>583</v>
       </c>
     </row>
-    <row r="34" spans="1:63">
+    <row r="34" spans="1:66">
       <c r="A34" s="9">
         <v>95</v>
       </c>
@@ -32060,14 +32768,15 @@
       <c r="BI34" s="9" t="s">
         <v>581</v>
       </c>
-      <c r="BJ34" s="9" t="s">
+      <c r="BJ34" s="9"/>
+      <c r="BL34" s="9" t="s">
         <v>582</v>
       </c>
-      <c r="BK34" s="9" t="s">
+      <c r="BM34" s="9" t="s">
         <v>583</v>
       </c>
     </row>
-    <row r="35" spans="1:63">
+    <row r="35" spans="1:66">
       <c r="A35" s="9">
         <v>96</v>
       </c>
@@ -32223,8 +32932,11 @@
       <c r="BI35" s="9"/>
       <c r="BJ35" s="9"/>
       <c r="BK35" s="9"/>
-    </row>
-    <row r="36" spans="1:63">
+      <c r="BL35" s="9"/>
+      <c r="BM35" s="9"/>
+      <c r="BN35" s="9"/>
+    </row>
+    <row r="36" spans="1:66">
       <c r="A36" s="9">
         <v>97</v>
       </c>
@@ -32367,18 +33079,19 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1D00-000000000000}">
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
@@ -33388,17 +34101,17 @@
 </file>
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1E00-000000000000}">
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.1328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="13.59765625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -34157,17 +34870,17 @@
 </file>
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1F00-000000000000}">
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.1328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="18.3984375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -35046,17 +35759,17 @@
 </file>
 
 <file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2000-000000000000}">
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.1328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="20.265625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -35935,17 +36648,17 @@
 </file>
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2100-000000000000}">
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.1328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="16.1328125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -36704,19 +37417,19 @@
 </file>
 
 <file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2200-000000000000}">
   <dimension ref="A1:P36"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="8" max="8" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="16.5703125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="12" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.86328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="16.59765625" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.59765625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="12" width="9.86328125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
@@ -38468,16 +39181,16 @@
 </file>
 
 <file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2300-000000000000}">
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="16.1328125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -39356,16 +40069,16 @@
 </file>
 
 <file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2400-000000000000}">
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="O29" sqref="O29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="16.1328125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -40244,19 +40957,19 @@
 </file>
 
 <file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2500-000000000000}">
   <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="15.140625" customWidth="1"/>
+    <col min="7" max="7" width="14.1328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="14.1328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.1328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="15.1328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -41192,18 +41905,18 @@
 </file>
 
 <file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2600-000000000000}">
   <dimension ref="A1:K36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.1328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.1328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.73046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -42145,16 +42858,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C60"/>
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="96.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="96.73046875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -42823,17 +43536,17 @@
 </file>
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2700-000000000000}">
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.1328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="15.3984375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -43661,23 +44374,23 @@
 </file>
 
 <file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2800-000000000000}">
   <dimension ref="A1:K36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="3" collapsed="1"/>
-    <col min="3" max="3" width="9.7109375" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="6" width="9.140625" style="3" collapsed="1"/>
-    <col min="7" max="7" width="14.140625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="9" width="9.140625" style="3" collapsed="1"/>
-    <col min="10" max="10" width="10.5703125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="17.5703125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="16384" width="9.140625" style="3" collapsed="1"/>
+    <col min="1" max="2" width="9.1328125" style="3" collapsed="1"/>
+    <col min="3" max="3" width="9.73046875" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="6" width="9.1328125" style="3" collapsed="1"/>
+    <col min="7" max="7" width="14.1328125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="9" width="9.1328125" style="3" collapsed="1"/>
+    <col min="10" max="10" width="10.59765625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="17.59765625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="16384" width="9.1328125" style="3" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -44810,16 +45523,16 @@
 </file>
 
 <file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2900-000000000000}">
   <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="10.73046875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -45578,14 +46291,14 @@
 </file>
 
 <file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2A00-000000000000}">
   <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="3" t="s">
@@ -46343,14 +47056,14 @@
 </file>
 
 <file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2B00-000000000000}">
   <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="3" t="s">
@@ -47108,14 +47821,14 @@
 </file>
 
 <file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2C00-000000000000}">
   <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="3" t="s">
@@ -47873,16 +48586,16 @@
 </file>
 
 <file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2D00-000000000000}">
   <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11.1328125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -48657,14 +49370,14 @@
 </file>
 
 <file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2E00-000000000000}">
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="4" t="s">
@@ -49402,17 +50115,17 @@
 </file>
 
 <file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2F00-000000000000}">
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="E18" sqref="E1:G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="8"/>
+    <col min="6" max="6" width="9.1328125" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -49697,7 +50410,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:C20">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C20">
     <sortCondition ref="A2:A20"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -49706,17 +50419,17 @@
 </file>
 
 <file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3000-000000000000}">
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -50139,12 +50852,12 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D97"/>
   <sheetViews>
     <sheetView topLeftCell="A73" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
@@ -51372,22 +52085,22 @@
 </file>
 
 <file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3100-000000000000}">
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.73046875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" thickBot="1">
+    <row r="1" spans="1:10" ht="14.65" thickBot="1">
       <c r="A1" s="15"/>
       <c r="B1" s="3" t="s">
         <v>617</v>
@@ -51405,7 +52118,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.75" thickBot="1">
+    <row r="2" spans="1:10" ht="14.65" thickBot="1">
       <c r="A2" s="10" t="s">
         <v>598</v>
       </c>
@@ -51434,7 +52147,7 @@
         <v>0.10124999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.75" thickBot="1">
+    <row r="3" spans="1:10" ht="14.65" thickBot="1">
       <c r="A3" s="11" t="s">
         <v>599</v>
       </c>
@@ -51463,7 +52176,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15.75" thickBot="1">
+    <row r="4" spans="1:10" ht="14.65" thickBot="1">
       <c r="A4" s="11" t="s">
         <v>600</v>
       </c>
@@ -51492,7 +52205,7 @@
         <v>6.4285714285714293E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15.75" thickBot="1">
+    <row r="5" spans="1:10" ht="14.65" thickBot="1">
       <c r="A5" s="11" t="s">
         <v>612</v>
       </c>
@@ -51521,7 +52234,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15.75" thickBot="1">
+    <row r="6" spans="1:10" ht="14.65" thickBot="1">
       <c r="A6" s="11" t="s">
         <v>601</v>
       </c>
@@ -51550,7 +52263,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15.75" thickBot="1">
+    <row r="7" spans="1:10" ht="14.65" thickBot="1">
       <c r="A7" s="11" t="s">
         <v>602</v>
       </c>
@@ -51579,7 +52292,7 @@
         <v>3.214285714285714E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15.75" thickBot="1">
+    <row r="8" spans="1:10" ht="14.65" thickBot="1">
       <c r="A8" s="11" t="s">
         <v>603</v>
       </c>
@@ -51608,7 +52321,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="29.25" thickBot="1">
+    <row r="9" spans="1:10" ht="14.65" thickBot="1">
       <c r="A9" s="11" t="s">
         <v>605</v>
       </c>
@@ -51637,7 +52350,7 @@
         <v>0.22500000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15.75" thickBot="1">
+    <row r="10" spans="1:10" ht="14.65" thickBot="1">
       <c r="A10" s="11" t="s">
         <v>613</v>
       </c>
@@ -51666,7 +52379,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="15.75" thickBot="1">
+    <row r="11" spans="1:10" ht="14.65" thickBot="1">
       <c r="A11" s="11" t="s">
         <v>606</v>
       </c>
@@ -51695,7 +52408,7 @@
         <v>8.8235294117647051E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="15.75" thickBot="1">
+    <row r="12" spans="1:10" ht="14.65" thickBot="1">
       <c r="A12" s="11" t="s">
         <v>604</v>
       </c>
@@ -51724,7 +52437,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="15.75" thickBot="1">
+    <row r="13" spans="1:10" ht="14.65" thickBot="1">
       <c r="A13" s="11" t="s">
         <v>614</v>
       </c>
@@ -51750,7 +52463,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="29.25" thickBot="1">
+    <row r="14" spans="1:10" ht="27.4" thickBot="1">
       <c r="A14" s="11" t="s">
         <v>608</v>
       </c>
@@ -51779,7 +52492,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="29.25" thickBot="1">
+    <row r="15" spans="1:10" ht="27.4" thickBot="1">
       <c r="A15" s="11" t="s">
         <v>609</v>
       </c>
@@ -51808,7 +52521,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15.75" thickBot="1">
+    <row r="16" spans="1:10" ht="14.65" thickBot="1">
       <c r="A16" s="11" t="s">
         <v>610</v>
       </c>
@@ -51834,7 +52547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="15.75" thickBot="1">
+    <row r="17" spans="1:10" ht="14.65" thickBot="1">
       <c r="A17" s="11" t="s">
         <v>611</v>
       </c>
@@ -51860,7 +52573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="15.75" thickBot="1">
+    <row r="18" spans="1:10" ht="14.65" thickBot="1">
       <c r="A18" s="11"/>
       <c r="B18" s="12"/>
       <c r="C18" s="12"/>
@@ -51872,16 +52585,16 @@
 </file>
 
 <file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3200-000000000000}">
   <dimension ref="A1:B235"/>
   <sheetViews>
     <sheetView topLeftCell="A219" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B229" sqref="B229"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -53770,14 +54483,14 @@
 </file>
 
 <file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3300-000000000000}">
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
@@ -54745,14 +55458,14 @@
 </file>
 
 <file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3400-000000000000}">
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="M32" sqref="M32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
@@ -55762,14 +56475,14 @@
 </file>
 
 <file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3500-000000000000}">
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
@@ -56779,14 +57492,14 @@
 </file>
 
 <file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3600-000000000000}">
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
@@ -57796,16 +58509,16 @@
 </file>
 
 <file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3700-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="A1:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="10.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -57847,16 +58560,16 @@
 </file>
 
 <file path=xl/worksheets/sheet57.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3800-000000000000}">
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="12" max="12" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="16.3984375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -59059,14 +59772,14 @@
 </file>
 
 <file path=xl/worksheets/sheet58.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3900-000000000000}">
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -60268,14 +60981,14 @@
 </file>
 
 <file path=xl/worksheets/sheet59.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3A00-000000000000}">
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -61477,16 +62190,16 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -61608,14 +62321,14 @@
 </file>
 
 <file path=xl/worksheets/sheet60.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3B00-000000000000}">
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -62817,16 +63530,16 @@
 </file>
 
 <file path=xl/worksheets/sheet61.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3C00-000000000000}">
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="12" max="12" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -64029,14 +64742,14 @@
 </file>
 
 <file path=xl/worksheets/sheet62.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3D00-000000000000}">
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -65238,14 +65951,14 @@
 </file>
 
 <file path=xl/worksheets/sheet63.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3E00-000000000000}">
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -66447,14 +67160,14 @@
 </file>
 
 <file path=xl/worksheets/sheet64.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3F00-000000000000}">
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -67656,14 +68369,14 @@
 </file>
 
 <file path=xl/worksheets/sheet65.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4000-000000000000}">
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -68865,14 +69578,14 @@
 </file>
 
 <file path=xl/worksheets/sheet66.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4100-000000000000}">
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -70074,14 +70787,14 @@
 </file>
 
 <file path=xl/worksheets/sheet67.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4200-000000000000}">
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -71283,16 +71996,16 @@
 </file>
 
 <file path=xl/worksheets/sheet68.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4300-000000000000}">
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="12" max="12" width="25.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="25.1328125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -72495,14 +73208,14 @@
 </file>
 
 <file path=xl/worksheets/sheet69.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4400-000000000000}">
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -73704,16 +74417,16 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -73835,14 +74548,14 @@
 </file>
 
 <file path=xl/worksheets/sheet70.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4500-000000000000}">
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -75044,14 +75757,14 @@
 </file>
 
 <file path=xl/worksheets/sheet71.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4600-000000000000}">
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -76253,14 +76966,14 @@
 </file>
 
 <file path=xl/worksheets/sheet72.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4700-000000000000}">
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -77462,14 +78175,14 @@
 </file>
 
 <file path=xl/worksheets/sheet73.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4800-000000000000}">
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -78671,14 +79384,14 @@
 </file>
 
 <file path=xl/worksheets/sheet74.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4900-000000000000}">
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="O39" sqref="O39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -79880,14 +80593,14 @@
 </file>
 
 <file path=xl/worksheets/sheet75.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4A00-000000000000}">
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -81089,17 +81802,17 @@
 </file>
 
 <file path=xl/worksheets/sheet76.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4B00-000000000000}">
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.86328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -82302,19 +83015,19 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="6" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="12.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.3984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13.86328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="6" width="12.3984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="12.3984375" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="9" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
@@ -83183,14 +83896,14 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">

</xml_diff>

<commit_message>
including 83-89 Codes in HHHouseProperties
</commit_message>
<xml_diff>
--- a/Data/MetaData.xlsx
+++ b/Data/MetaData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhash\OneDrive\Documents\GitHub\IRHEIS\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55ED5E3D-3E4E-42E9-8828-6E357A2EF08A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5463E2F9-15C6-4573-8C6B-72EDD0A68FED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" tabRatio="858" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28845,8 +28845,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:BO36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BE1" zoomScale="109" zoomScaleNormal="109" workbookViewId="0">
-      <selection activeCell="BK37" sqref="BK37"/>
+    <sheetView tabSelected="1" topLeftCell="BB1" zoomScale="90" zoomScaleNormal="109" workbookViewId="0">
+      <selection activeCell="BP29" sqref="BP29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -31614,13 +31614,13 @@
       <c r="BE28" s="9" t="s">
         <v>576</v>
       </c>
-      <c r="BF28" s="9" t="s">
+      <c r="BH28" s="9" t="s">
         <v>577</v>
       </c>
-      <c r="BG28" s="9" t="s">
+      <c r="BJ28" s="9" t="s">
         <v>578</v>
       </c>
-      <c r="BH28" s="9" t="s">
+      <c r="BK28" s="9" t="s">
         <v>579</v>
       </c>
       <c r="BL28" s="9" t="s">
@@ -31800,13 +31800,13 @@
       <c r="BE29" s="9" t="s">
         <v>576</v>
       </c>
-      <c r="BF29" s="9" t="s">
+      <c r="BH29" s="9" t="s">
         <v>577</v>
       </c>
-      <c r="BG29" s="9" t="s">
+      <c r="BJ29" s="9" t="s">
         <v>578</v>
       </c>
-      <c r="BH29" s="9" t="s">
+      <c r="BK29" s="9" t="s">
         <v>579</v>
       </c>
       <c r="BL29" s="9" t="s">
@@ -31988,19 +31988,18 @@
       <c r="BE30" s="9" t="s">
         <v>577</v>
       </c>
-      <c r="BF30" s="9" t="s">
+      <c r="BH30" s="9" t="s">
         <v>578</v>
       </c>
-      <c r="BG30" s="9" t="s">
+      <c r="BI30" s="9" t="s">
         <v>579</v>
       </c>
-      <c r="BH30" s="9" t="s">
+      <c r="BJ30" s="9" t="s">
         <v>580</v>
       </c>
-      <c r="BI30" s="9" t="s">
+      <c r="BK30" s="9" t="s">
         <v>581</v>
       </c>
-      <c r="BJ30" s="9"/>
       <c r="BL30" s="9" t="s">
         <v>582</v>
       </c>
@@ -32180,19 +32179,18 @@
       <c r="BE31" s="9" t="s">
         <v>577</v>
       </c>
-      <c r="BF31" s="9" t="s">
+      <c r="BH31" s="9" t="s">
         <v>578</v>
       </c>
-      <c r="BG31" s="9" t="s">
+      <c r="BI31" s="9" t="s">
         <v>579</v>
       </c>
-      <c r="BH31" s="9" t="s">
+      <c r="BJ31" s="9" t="s">
         <v>580</v>
       </c>
-      <c r="BI31" s="9" t="s">
+      <c r="BK31" s="9" t="s">
         <v>581</v>
       </c>
-      <c r="BJ31" s="9"/>
       <c r="BL31" s="9" t="s">
         <v>582</v>
       </c>
@@ -32372,19 +32370,18 @@
       <c r="BE32" s="9" t="s">
         <v>577</v>
       </c>
-      <c r="BF32" s="9" t="s">
+      <c r="BH32" s="9" t="s">
         <v>578</v>
       </c>
-      <c r="BG32" s="9" t="s">
+      <c r="BI32" s="9" t="s">
         <v>579</v>
       </c>
-      <c r="BH32" s="9" t="s">
+      <c r="BJ32" s="9" t="s">
         <v>580</v>
       </c>
-      <c r="BI32" s="9" t="s">
+      <c r="BK32" s="9" t="s">
         <v>581</v>
       </c>
-      <c r="BJ32" s="9"/>
       <c r="BL32" s="9" t="s">
         <v>582</v>
       </c>
@@ -32564,19 +32561,18 @@
       <c r="BE33" s="9" t="s">
         <v>577</v>
       </c>
-      <c r="BF33" s="9" t="s">
+      <c r="BH33" s="9" t="s">
         <v>578</v>
       </c>
-      <c r="BG33" s="9" t="s">
+      <c r="BI33" s="9" t="s">
         <v>579</v>
       </c>
-      <c r="BH33" s="9" t="s">
+      <c r="BJ33" s="9" t="s">
         <v>580</v>
       </c>
-      <c r="BI33" s="9" t="s">
+      <c r="BK33" s="9" t="s">
         <v>581</v>
       </c>
-      <c r="BJ33" s="9"/>
       <c r="BL33" s="9" t="s">
         <v>582</v>
       </c>
@@ -32756,19 +32752,18 @@
       <c r="BE34" s="9" t="s">
         <v>577</v>
       </c>
-      <c r="BF34" s="9" t="s">
+      <c r="BH34" s="9" t="s">
         <v>578</v>
       </c>
-      <c r="BG34" s="9" t="s">
+      <c r="BI34" s="9" t="s">
         <v>579</v>
       </c>
-      <c r="BH34" s="9" t="s">
+      <c r="BJ34" s="9" t="s">
         <v>580</v>
       </c>
-      <c r="BI34" s="9" t="s">
+      <c r="BK34" s="9" t="s">
         <v>581</v>
       </c>
-      <c r="BJ34" s="9"/>
       <c r="BL34" s="9" t="s">
         <v>582</v>
       </c>

</xml_diff>

<commit_message>
UpdatingMetaData P2Cols Sheet for 77-83
</commit_message>
<xml_diff>
--- a/Data/MetaData.xlsx
+++ b/Data/MetaData.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\IRHEIS\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhash\OneDrive\Documents\GitHub\IRHEIS\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7A1B8F5-4C1F-45C2-9676-A2B3902F38F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="20715" windowHeight="13275" tabRatio="858" firstSheet="62" activeTab="75"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" tabRatio="858" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CompressedFileNames" sheetId="1" r:id="rId1"/>
@@ -89,7 +90,7 @@
     <sheet name="Khoshkbar" sheetId="1027" r:id="rId75"/>
     <sheet name="Nooshabe" sheetId="1041" r:id="rId76"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -102,7 +103,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17896" uniqueCount="720">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17998" uniqueCount="724">
   <si>
     <t>Year</t>
   </si>
@@ -2263,11 +2264,23 @@
   <si>
     <t>98.rar</t>
   </si>
+  <si>
+    <t>Q8_1</t>
+  </si>
+  <si>
+    <t>Q8_2_1</t>
+  </si>
+  <si>
+    <t>Q8_2_2</t>
+  </si>
+  <si>
+    <t>Q8_2_3</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="22">
     <font>
       <sz val="11"/>
@@ -3215,16 +3228,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B37"/>
   <sheetViews>
     <sheetView topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="20.86328125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -3529,25 +3542,25 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:T42"/>
   <sheetViews>
     <sheetView topLeftCell="A11" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="12" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12.73046875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="12" max="13" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="16" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="19.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="16" width="13.3984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="19.73046875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="18" max="18" width="19" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="19" max="19" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="15.265625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
@@ -5614,25 +5627,25 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:T42"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="9" max="9" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12.73046875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="12.7109375" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12.73046875" customWidth="1" collapsed="1"/>
     <col min="12" max="12" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="12.73046875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="14" max="14" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="15.265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="13.3984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="12.59765625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="13.73046875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
@@ -7711,17 +7724,17 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:S36"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="8" max="8" width="10.5703125" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="10.59765625" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="13.73046875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
@@ -9554,17 +9567,17 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:S36"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="13.73046875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
@@ -11379,22 +11392,22 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="4" width="9.140625" style="3" collapsed="1"/>
-    <col min="5" max="5" width="9.140625" style="3"/>
-    <col min="6" max="6" width="9.140625" style="3" collapsed="1"/>
-    <col min="7" max="7" width="10.7109375" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="10" width="9.140625" style="3" collapsed="1"/>
-    <col min="11" max="11" width="11.140625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="16384" width="9.140625" style="3" collapsed="1"/>
+    <col min="1" max="4" width="9.1328125" style="3" collapsed="1"/>
+    <col min="5" max="5" width="9.1328125" style="3"/>
+    <col min="6" max="6" width="9.1328125" style="3" collapsed="1"/>
+    <col min="7" max="7" width="10.73046875" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="10" width="9.1328125" style="3" collapsed="1"/>
+    <col min="11" max="11" width="11.1328125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="16384" width="9.1328125" style="3" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -12540,16 +12553,16 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10.3984375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="15" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
@@ -12901,23 +12914,23 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView topLeftCell="A28" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.73046875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8.86328125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="10" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="8.73046875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.1328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11.86328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="10" width="8.73046875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="16.3984375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -14155,17 +14168,17 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:K36"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.1328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="16.3984375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -14624,20 +14637,20 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E23" sqref="E23:G36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.1328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="10.73046875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="10.265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="10.59765625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -15468,17 +15481,17 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:E127"/>
   <sheetViews>
     <sheetView topLeftCell="A109" workbookViewId="0">
       <selection activeCell="B130" sqref="B130"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="2" width="11.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="2" width="11.3984375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.265625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -17371,14 +17384,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:R37"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A36" sqref="A36:N37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="1:18">
       <c r="A1" t="s">
@@ -18774,18 +18787,18 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.1328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.59765625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="16.3984375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -19780,18 +19793,18 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.1328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.59765625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="16.3984375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -20786,16 +20799,16 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:K37"/>
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="10" max="10" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="16.3984375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -21976,18 +21989,18 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="9" width="14.140625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.1328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="9" width="14.1328125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="12.1328125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -22766,18 +22779,18 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <dimension ref="A1:K37"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="I39" sqref="I39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="8.73046875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="10.59765625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -24081,19 +24094,19 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView topLeftCell="A22" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.140625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.1328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="12.1328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12.1328125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="12.1328125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -25133,14 +25146,14 @@
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
   <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
@@ -26179,14 +26192,14 @@
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
@@ -27196,14 +27209,14 @@
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="C21" sqref="C16:D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
@@ -28213,16 +28226,16 @@
 </file>
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="10" max="10" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -29233,52 +29246,52 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:BR37"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="109" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36:BN37"/>
+    <sheetView tabSelected="1" topLeftCell="Z1" zoomScale="90" zoomScaleNormal="109" workbookViewId="0">
+      <selection activeCell="AN20" sqref="AN20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="31" max="32" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="12.42578125" customWidth="1"/>
-    <col min="49" max="49" width="10.42578125" customWidth="1"/>
-    <col min="50" max="50" width="16.85546875" customWidth="1"/>
-    <col min="51" max="51" width="14.85546875" customWidth="1"/>
-    <col min="52" max="52" width="19.7109375" customWidth="1"/>
-    <col min="53" max="53" width="17.7109375" customWidth="1"/>
-    <col min="54" max="54" width="12.85546875" customWidth="1"/>
-    <col min="55" max="55" width="10.85546875" customWidth="1"/>
-    <col min="56" max="56" width="12.42578125" customWidth="1"/>
-    <col min="57" max="57" width="10.42578125" customWidth="1"/>
-    <col min="58" max="58" width="16.7109375" customWidth="1"/>
-    <col min="59" max="60" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="14.7109375" customWidth="1"/>
-    <col min="63" max="63" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="14.7109375" customWidth="1"/>
-    <col min="65" max="65" width="10.7109375" customWidth="1"/>
-    <col min="66" max="66" width="18.42578125" customWidth="1"/>
-    <col min="67" max="67" width="18.28515625" customWidth="1"/>
+    <col min="4" max="4" width="12.1328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.86328125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.59765625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.86328125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.265625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.265625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="21.86328125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="19.3984375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="11.1328125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="10.73046875" bestFit="1" customWidth="1"/>
+    <col min="31" max="32" width="10.1328125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="9.86328125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="12.73046875" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="11.1328125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="10.3984375" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="12.3984375" customWidth="1"/>
+    <col min="49" max="49" width="10.3984375" customWidth="1"/>
+    <col min="50" max="50" width="16.86328125" customWidth="1"/>
+    <col min="51" max="51" width="14.86328125" customWidth="1"/>
+    <col min="52" max="52" width="19.73046875" customWidth="1"/>
+    <col min="53" max="53" width="17.73046875" customWidth="1"/>
+    <col min="54" max="54" width="12.86328125" customWidth="1"/>
+    <col min="55" max="55" width="10.86328125" customWidth="1"/>
+    <col min="56" max="56" width="12.3984375" customWidth="1"/>
+    <col min="57" max="57" width="10.3984375" customWidth="1"/>
+    <col min="58" max="58" width="16.73046875" customWidth="1"/>
+    <col min="59" max="60" width="16.73046875" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="14.73046875" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="14.73046875" customWidth="1"/>
+    <col min="63" max="63" width="10.73046875" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="14.73046875" customWidth="1"/>
+    <col min="65" max="65" width="10.73046875" customWidth="1"/>
+    <col min="66" max="66" width="18.3984375" customWidth="1"/>
+    <col min="67" max="67" width="18.265625" customWidth="1"/>
     <col min="68" max="68" width="23" customWidth="1"/>
     <col min="69" max="69" width="22" customWidth="1"/>
-    <col min="70" max="70" width="20.7109375" customWidth="1"/>
+    <col min="70" max="70" width="20.73046875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:70">
@@ -30424,50 +30437,112 @@
       <c r="B16" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="C16" s="9"/>
+      <c r="C16" s="9" t="s">
+        <v>682</v>
+      </c>
       <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="9"/>
-      <c r="J16" s="9"/>
-      <c r="K16" s="9"/>
-      <c r="L16" s="9"/>
-      <c r="M16" s="9"/>
-      <c r="N16" s="9"/>
-      <c r="O16" s="9"/>
-      <c r="P16" s="9"/>
-      <c r="Q16" s="9"/>
-      <c r="R16" s="9"/>
-      <c r="S16" s="9"/>
-      <c r="T16" s="9"/>
+      <c r="E16" s="9" t="s">
+        <v>402</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>683</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>684</v>
+      </c>
+      <c r="I16" s="9" t="s">
+        <v>685</v>
+      </c>
+      <c r="J16" s="9" t="s">
+        <v>686</v>
+      </c>
+      <c r="K16" s="9" t="s">
+        <v>687</v>
+      </c>
+      <c r="L16" s="9" t="s">
+        <v>689</v>
+      </c>
+      <c r="M16" s="9" t="s">
+        <v>690</v>
+      </c>
+      <c r="N16" s="9" t="s">
+        <v>691</v>
+      </c>
+      <c r="O16" s="9" t="s">
+        <v>692</v>
+      </c>
+      <c r="P16" s="9" t="s">
+        <v>698</v>
+      </c>
+      <c r="Q16" s="9" t="s">
+        <v>699</v>
+      </c>
+      <c r="R16" s="9" t="s">
+        <v>700</v>
+      </c>
+      <c r="S16" s="9" t="s">
+        <v>693</v>
+      </c>
+      <c r="T16" s="9" t="s">
+        <v>694</v>
+      </c>
       <c r="U16" s="9"/>
-      <c r="V16" s="9"/>
-      <c r="W16" s="9"/>
-      <c r="X16" s="9"/>
-      <c r="Y16" s="9"/>
+      <c r="V16" s="9" t="s">
+        <v>695</v>
+      </c>
+      <c r="W16" s="9" t="s">
+        <v>696</v>
+      </c>
+      <c r="X16" s="9" t="s">
+        <v>697</v>
+      </c>
+      <c r="Y16" s="9" t="s">
+        <v>688</v>
+      </c>
       <c r="Z16" s="9"/>
       <c r="AA16" s="9"/>
       <c r="AB16" s="9"/>
       <c r="AC16" s="9"/>
       <c r="AD16" s="9"/>
       <c r="AE16" s="9"/>
-      <c r="AF16" s="9"/>
-      <c r="AG16" s="9"/>
-      <c r="AH16" s="9"/>
-      <c r="AI16" s="9"/>
+      <c r="AF16" s="9" t="s">
+        <v>703</v>
+      </c>
+      <c r="AG16" s="9" t="s">
+        <v>704</v>
+      </c>
+      <c r="AH16" s="9" t="s">
+        <v>705</v>
+      </c>
+      <c r="AI16" s="9" t="s">
+        <v>707</v>
+      </c>
       <c r="AJ16" s="9"/>
-      <c r="AK16" s="9"/>
-      <c r="AL16" s="9"/>
-      <c r="AM16" s="9"/>
+      <c r="AK16" s="9" t="s">
+        <v>706</v>
+      </c>
+      <c r="AL16" s="9" t="s">
+        <v>711</v>
+      </c>
+      <c r="AM16" s="9" t="s">
+        <v>708</v>
+      </c>
       <c r="AN16" s="9"/>
-      <c r="AO16" s="9"/>
+      <c r="AO16" s="9" t="s">
+        <v>710</v>
+      </c>
       <c r="AP16" s="9"/>
       <c r="AQ16" s="9"/>
       <c r="AR16" s="9"/>
-      <c r="AS16" s="9"/>
-      <c r="AT16" s="9"/>
+      <c r="AS16" s="9" t="s">
+        <v>713</v>
+      </c>
+      <c r="AT16" s="9" t="s">
+        <v>714</v>
+      </c>
       <c r="AU16" s="9"/>
       <c r="AV16" s="9"/>
       <c r="AW16" s="9"/>
@@ -30483,57 +30558,119 @@
       <c r="BG16" s="9"/>
       <c r="BH16" s="9"/>
     </row>
-    <row r="17" spans="1:67">
+    <row r="17" spans="1:70">
       <c r="A17" s="9">
         <v>78</v>
       </c>
       <c r="B17" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="C17" s="9"/>
+      <c r="C17" s="9" t="s">
+        <v>682</v>
+      </c>
       <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="9"/>
-      <c r="J17" s="9"/>
-      <c r="K17" s="9"/>
-      <c r="L17" s="9"/>
-      <c r="M17" s="9"/>
-      <c r="N17" s="9"/>
-      <c r="O17" s="9"/>
-      <c r="P17" s="9"/>
-      <c r="Q17" s="9"/>
-      <c r="R17" s="9"/>
-      <c r="S17" s="9"/>
-      <c r="T17" s="9"/>
+      <c r="E17" s="9" t="s">
+        <v>402</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>683</v>
+      </c>
+      <c r="H17" s="9" t="s">
+        <v>684</v>
+      </c>
+      <c r="I17" s="9" t="s">
+        <v>685</v>
+      </c>
+      <c r="J17" s="9" t="s">
+        <v>686</v>
+      </c>
+      <c r="K17" s="9" t="s">
+        <v>687</v>
+      </c>
+      <c r="L17" s="9" t="s">
+        <v>689</v>
+      </c>
+      <c r="M17" s="9" t="s">
+        <v>690</v>
+      </c>
+      <c r="N17" s="9" t="s">
+        <v>691</v>
+      </c>
+      <c r="O17" s="9" t="s">
+        <v>692</v>
+      </c>
+      <c r="P17" s="9" t="s">
+        <v>698</v>
+      </c>
+      <c r="Q17" s="9" t="s">
+        <v>699</v>
+      </c>
+      <c r="R17" s="9" t="s">
+        <v>700</v>
+      </c>
+      <c r="S17" s="9" t="s">
+        <v>693</v>
+      </c>
+      <c r="T17" s="9" t="s">
+        <v>694</v>
+      </c>
       <c r="U17" s="9"/>
-      <c r="V17" s="9"/>
-      <c r="W17" s="9"/>
-      <c r="X17" s="9"/>
-      <c r="Y17" s="9"/>
+      <c r="V17" s="9" t="s">
+        <v>695</v>
+      </c>
+      <c r="W17" s="9" t="s">
+        <v>696</v>
+      </c>
+      <c r="X17" s="9" t="s">
+        <v>697</v>
+      </c>
+      <c r="Y17" s="9" t="s">
+        <v>688</v>
+      </c>
       <c r="Z17" s="9"/>
       <c r="AA17" s="9"/>
       <c r="AB17" s="9"/>
       <c r="AC17" s="9"/>
       <c r="AD17" s="9"/>
       <c r="AE17" s="9"/>
-      <c r="AF17" s="9"/>
-      <c r="AG17" s="9"/>
-      <c r="AH17" s="9"/>
-      <c r="AI17" s="9"/>
+      <c r="AF17" s="9" t="s">
+        <v>703</v>
+      </c>
+      <c r="AG17" s="9" t="s">
+        <v>704</v>
+      </c>
+      <c r="AH17" s="9" t="s">
+        <v>705</v>
+      </c>
+      <c r="AI17" s="9" t="s">
+        <v>707</v>
+      </c>
       <c r="AJ17" s="9"/>
-      <c r="AK17" s="9"/>
-      <c r="AL17" s="9"/>
-      <c r="AM17" s="9"/>
+      <c r="AK17" s="9" t="s">
+        <v>706</v>
+      </c>
+      <c r="AL17" s="9" t="s">
+        <v>711</v>
+      </c>
+      <c r="AM17" s="9" t="s">
+        <v>708</v>
+      </c>
       <c r="AN17" s="9"/>
-      <c r="AO17" s="9"/>
+      <c r="AO17" s="9" t="s">
+        <v>710</v>
+      </c>
       <c r="AP17" s="9"/>
       <c r="AQ17" s="9"/>
       <c r="AR17" s="9"/>
-      <c r="AS17" s="9"/>
-      <c r="AT17" s="9"/>
+      <c r="AS17" s="9" t="s">
+        <v>713</v>
+      </c>
+      <c r="AT17" s="9" t="s">
+        <v>714</v>
+      </c>
       <c r="AU17" s="9"/>
       <c r="AV17" s="9"/>
       <c r="AW17" s="9"/>
@@ -30548,58 +30685,132 @@
       <c r="BF17" s="9"/>
       <c r="BG17" s="9"/>
       <c r="BH17" s="9"/>
-    </row>
-    <row r="18" spans="1:67">
+      <c r="BO17" t="s">
+        <v>720</v>
+      </c>
+      <c r="BP17" t="s">
+        <v>721</v>
+      </c>
+      <c r="BQ17" t="s">
+        <v>722</v>
+      </c>
+      <c r="BR17" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="18" spans="1:70">
       <c r="A18" s="9">
         <v>79</v>
       </c>
       <c r="B18" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="C18" s="9"/>
+      <c r="C18" s="9" t="s">
+        <v>682</v>
+      </c>
       <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9"/>
-      <c r="J18" s="9"/>
-      <c r="K18" s="9"/>
-      <c r="L18" s="9"/>
-      <c r="M18" s="9"/>
-      <c r="N18" s="9"/>
-      <c r="O18" s="9"/>
-      <c r="P18" s="9"/>
-      <c r="Q18" s="9"/>
-      <c r="R18" s="9"/>
-      <c r="S18" s="9"/>
-      <c r="T18" s="9"/>
+      <c r="E18" s="9" t="s">
+        <v>402</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>683</v>
+      </c>
+      <c r="H18" s="9" t="s">
+        <v>684</v>
+      </c>
+      <c r="I18" s="9" t="s">
+        <v>685</v>
+      </c>
+      <c r="J18" s="9" t="s">
+        <v>686</v>
+      </c>
+      <c r="K18" s="9" t="s">
+        <v>687</v>
+      </c>
+      <c r="L18" s="9" t="s">
+        <v>689</v>
+      </c>
+      <c r="M18" s="9" t="s">
+        <v>690</v>
+      </c>
+      <c r="N18" s="9" t="s">
+        <v>691</v>
+      </c>
+      <c r="O18" s="9" t="s">
+        <v>692</v>
+      </c>
+      <c r="P18" s="9" t="s">
+        <v>698</v>
+      </c>
+      <c r="Q18" s="9" t="s">
+        <v>699</v>
+      </c>
+      <c r="R18" s="9" t="s">
+        <v>700</v>
+      </c>
+      <c r="S18" s="9" t="s">
+        <v>693</v>
+      </c>
+      <c r="T18" s="9" t="s">
+        <v>694</v>
+      </c>
       <c r="U18" s="9"/>
-      <c r="V18" s="9"/>
-      <c r="W18" s="9"/>
-      <c r="X18" s="9"/>
-      <c r="Y18" s="9"/>
+      <c r="V18" s="9" t="s">
+        <v>695</v>
+      </c>
+      <c r="W18" s="9" t="s">
+        <v>696</v>
+      </c>
+      <c r="X18" s="9" t="s">
+        <v>697</v>
+      </c>
+      <c r="Y18" s="9" t="s">
+        <v>688</v>
+      </c>
       <c r="Z18" s="9"/>
       <c r="AA18" s="9"/>
       <c r="AB18" s="9"/>
       <c r="AC18" s="9"/>
       <c r="AD18" s="9"/>
       <c r="AE18" s="9"/>
-      <c r="AF18" s="9"/>
-      <c r="AG18" s="9"/>
-      <c r="AH18" s="9"/>
-      <c r="AI18" s="9"/>
+      <c r="AF18" s="9" t="s">
+        <v>703</v>
+      </c>
+      <c r="AG18" s="9" t="s">
+        <v>704</v>
+      </c>
+      <c r="AH18" s="9" t="s">
+        <v>705</v>
+      </c>
+      <c r="AI18" s="9" t="s">
+        <v>707</v>
+      </c>
       <c r="AJ18" s="9"/>
-      <c r="AK18" s="9"/>
-      <c r="AL18" s="9"/>
-      <c r="AM18" s="9"/>
+      <c r="AK18" s="9" t="s">
+        <v>706</v>
+      </c>
+      <c r="AL18" s="9" t="s">
+        <v>711</v>
+      </c>
+      <c r="AM18" s="9" t="s">
+        <v>708</v>
+      </c>
       <c r="AN18" s="9"/>
-      <c r="AO18" s="9"/>
+      <c r="AO18" s="9" t="s">
+        <v>710</v>
+      </c>
       <c r="AP18" s="9"/>
       <c r="AQ18" s="9"/>
       <c r="AR18" s="9"/>
-      <c r="AS18" s="9"/>
-      <c r="AT18" s="9"/>
+      <c r="AS18" s="9" t="s">
+        <v>713</v>
+      </c>
+      <c r="AT18" s="9" t="s">
+        <v>714</v>
+      </c>
       <c r="AU18" s="9"/>
       <c r="AV18" s="9"/>
       <c r="AW18" s="9"/>
@@ -30614,8 +30825,20 @@
       <c r="BF18" s="9"/>
       <c r="BG18" s="9"/>
       <c r="BH18" s="9"/>
-    </row>
-    <row r="19" spans="1:67">
+      <c r="BO18" t="s">
+        <v>720</v>
+      </c>
+      <c r="BP18" t="s">
+        <v>721</v>
+      </c>
+      <c r="BQ18" t="s">
+        <v>722</v>
+      </c>
+      <c r="BR18" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="19" spans="1:70">
       <c r="A19" s="9">
         <v>80</v>
       </c>
@@ -30687,12 +30910,8 @@
       <c r="Y19" s="9" t="s">
         <v>688</v>
       </c>
-      <c r="Z19" s="9" t="s">
-        <v>701</v>
-      </c>
-      <c r="AA19" s="9" t="s">
-        <v>702</v>
-      </c>
+      <c r="Z19" s="9"/>
+      <c r="AA19" s="9"/>
       <c r="AB19" s="9"/>
       <c r="AC19" s="9"/>
       <c r="AD19" s="9"/>
@@ -30709,9 +30928,7 @@
       <c r="AI19" s="9" t="s">
         <v>707</v>
       </c>
-      <c r="AJ19" s="9" t="s">
-        <v>712</v>
-      </c>
+      <c r="AJ19" s="9"/>
       <c r="AK19" s="9" t="s">
         <v>706</v>
       </c>
@@ -30748,8 +30965,20 @@
       <c r="BF19" s="9"/>
       <c r="BG19" s="9"/>
       <c r="BH19" s="9"/>
-    </row>
-    <row r="20" spans="1:67">
+      <c r="BO19" t="s">
+        <v>720</v>
+      </c>
+      <c r="BP19" t="s">
+        <v>721</v>
+      </c>
+      <c r="BQ19" t="s">
+        <v>722</v>
+      </c>
+      <c r="BR19" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="20" spans="1:70">
       <c r="A20" s="9">
         <v>81</v>
       </c>
@@ -30885,7 +31114,7 @@
       <c r="BG20" s="9"/>
       <c r="BH20" s="9"/>
     </row>
-    <row r="21" spans="1:67">
+    <row r="21" spans="1:70">
       <c r="A21" s="9">
         <v>82</v>
       </c>
@@ -31021,7 +31250,7 @@
       <c r="BG21" s="9"/>
       <c r="BH21" s="9"/>
     </row>
-    <row r="22" spans="1:67">
+    <row r="22" spans="1:70">
       <c r="A22" s="9">
         <v>83</v>
       </c>
@@ -31155,7 +31384,7 @@
       <c r="BG22" s="9"/>
       <c r="BH22" s="9"/>
     </row>
-    <row r="23" spans="1:67">
+    <row r="23" spans="1:70">
       <c r="A23" s="9">
         <v>84</v>
       </c>
@@ -31329,7 +31558,7 @@
         <v>673</v>
       </c>
     </row>
-    <row r="24" spans="1:67">
+    <row r="24" spans="1:70">
       <c r="A24" s="9">
         <v>85</v>
       </c>
@@ -31508,7 +31737,7 @@
       </c>
       <c r="BN24" s="9"/>
     </row>
-    <row r="25" spans="1:67">
+    <row r="25" spans="1:70">
       <c r="A25" s="9">
         <v>86</v>
       </c>
@@ -31692,7 +31921,7 @@
       </c>
       <c r="BN25" s="9"/>
     </row>
-    <row r="26" spans="1:67">
+    <row r="26" spans="1:70">
       <c r="A26" s="9">
         <v>87</v>
       </c>
@@ -31876,7 +32105,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="27" spans="1:67">
+    <row r="27" spans="1:70">
       <c r="A27" s="9">
         <v>88</v>
       </c>
@@ -32060,7 +32289,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="28" spans="1:67">
+    <row r="28" spans="1:70">
       <c r="A28" s="9">
         <v>89</v>
       </c>
@@ -32246,7 +32475,7 @@
       </c>
       <c r="BO28" s="9"/>
     </row>
-    <row r="29" spans="1:67">
+    <row r="29" spans="1:70">
       <c r="A29" s="9">
         <v>90</v>
       </c>
@@ -32431,7 +32660,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="30" spans="1:67">
+    <row r="30" spans="1:70">
       <c r="A30" s="9">
         <v>91</v>
       </c>
@@ -32622,7 +32851,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="31" spans="1:67">
+    <row r="31" spans="1:70">
       <c r="A31" s="9">
         <v>92</v>
       </c>
@@ -32813,7 +33042,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="32" spans="1:67">
+    <row r="32" spans="1:70">
       <c r="A32" s="9">
         <v>93</v>
       </c>
@@ -33835,14 +34064,14 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1D00-000000000000}">
   <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
@@ -34881,17 +35110,17 @@
 </file>
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1E00-000000000000}">
   <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.1328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="13.59765625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -35670,17 +35899,17 @@
 </file>
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1F00-000000000000}">
   <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.1328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="18.3984375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -36579,17 +36808,17 @@
 </file>
 
 <file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2000-000000000000}">
   <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.1328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="20.265625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -37488,17 +37717,17 @@
 </file>
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2100-000000000000}">
   <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.1328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="16.1328125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -38277,19 +38506,19 @@
 </file>
 
 <file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2200-000000000000}">
   <dimension ref="A1:P37"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="A36" sqref="A36:P37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="8" max="8" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="16.5703125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="12" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.86328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="16.59765625" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.59765625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="12" width="9.86328125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
@@ -40091,16 +40320,16 @@
 </file>
 
 <file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2300-000000000000}">
   <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="16.1328125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -40999,16 +41228,16 @@
 </file>
 
 <file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2400-000000000000}">
   <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="16.1328125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -41907,19 +42136,19 @@
 </file>
 
 <file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2500-000000000000}">
   <dimension ref="A1:K37"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="C26" sqref="C26:D39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="15.140625" customWidth="1"/>
+    <col min="7" max="7" width="14.1328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="14.1328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.1328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="15.1328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -42906,18 +43135,18 @@
 </file>
 
 <file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2600-000000000000}">
   <dimension ref="A1:K36"/>
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.1328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.1328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.73046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -43859,16 +44088,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C60"/>
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="96.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="96.73046875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -44537,17 +44766,17 @@
 </file>
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2700-000000000000}">
   <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.1328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="15.3984375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -45398,23 +45627,23 @@
 </file>
 
 <file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2800-000000000000}">
   <dimension ref="A1:K37"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="3" collapsed="1"/>
-    <col min="3" max="3" width="9.7109375" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="6" width="9.140625" style="3" collapsed="1"/>
-    <col min="7" max="7" width="14.140625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="9" width="9.140625" style="3" collapsed="1"/>
-    <col min="10" max="10" width="10.5703125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="17.5703125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="16384" width="9.140625" style="3" collapsed="1"/>
+    <col min="1" max="2" width="9.1328125" style="3" collapsed="1"/>
+    <col min="3" max="3" width="9.73046875" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="6" width="9.1328125" style="3" collapsed="1"/>
+    <col min="7" max="7" width="14.1328125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="9" width="9.1328125" style="3" collapsed="1"/>
+    <col min="10" max="10" width="10.59765625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="17.59765625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="16384" width="9.1328125" style="3" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -46576,16 +46805,16 @@
 </file>
 
 <file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2900-000000000000}">
   <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="10.73046875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -47344,14 +47573,14 @@
 </file>
 
 <file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2A00-000000000000}">
   <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="3" t="s">
@@ -48109,14 +48338,14 @@
 </file>
 
 <file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2B00-000000000000}">
   <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="3" t="s">
@@ -48874,14 +49103,14 @@
 </file>
 
 <file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2C00-000000000000}">
   <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="3" t="s">
@@ -49639,16 +49868,16 @@
 </file>
 
 <file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2D00-000000000000}">
   <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11.1328125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -50423,14 +50652,14 @@
 </file>
 
 <file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2E00-000000000000}">
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="4" t="s">
@@ -51168,17 +51397,17 @@
 </file>
 
 <file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2F00-000000000000}">
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="E18" sqref="E1:G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="8"/>
+    <col min="6" max="6" width="9.1328125" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -51463,7 +51692,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:C20">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C20">
     <sortCondition ref="A2:A20"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -51472,17 +51701,17 @@
 </file>
 
 <file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3000-000000000000}">
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -51905,12 +52134,12 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D97"/>
   <sheetViews>
     <sheetView topLeftCell="A73" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
@@ -53138,22 +53367,22 @@
 </file>
 
 <file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3100-000000000000}">
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.73046875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" thickBot="1">
+    <row r="1" spans="1:10" ht="14.65" thickBot="1">
       <c r="A1" s="15"/>
       <c r="B1" s="3" t="s">
         <v>617</v>
@@ -53171,7 +53400,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.75" thickBot="1">
+    <row r="2" spans="1:10" ht="14.65" thickBot="1">
       <c r="A2" s="10" t="s">
         <v>598</v>
       </c>
@@ -53200,7 +53429,7 @@
         <v>0.10124999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.75" thickBot="1">
+    <row r="3" spans="1:10" ht="14.65" thickBot="1">
       <c r="A3" s="11" t="s">
         <v>599</v>
       </c>
@@ -53229,7 +53458,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15.75" thickBot="1">
+    <row r="4" spans="1:10" ht="14.65" thickBot="1">
       <c r="A4" s="11" t="s">
         <v>600</v>
       </c>
@@ -53258,7 +53487,7 @@
         <v>6.4285714285714293E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15.75" thickBot="1">
+    <row r="5" spans="1:10" ht="14.65" thickBot="1">
       <c r="A5" s="11" t="s">
         <v>612</v>
       </c>
@@ -53287,7 +53516,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15.75" thickBot="1">
+    <row r="6" spans="1:10" ht="14.65" thickBot="1">
       <c r="A6" s="11" t="s">
         <v>601</v>
       </c>
@@ -53316,7 +53545,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15.75" thickBot="1">
+    <row r="7" spans="1:10" ht="14.65" thickBot="1">
       <c r="A7" s="11" t="s">
         <v>602</v>
       </c>
@@ -53345,7 +53574,7 @@
         <v>3.214285714285714E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15.75" thickBot="1">
+    <row r="8" spans="1:10" ht="14.65" thickBot="1">
       <c r="A8" s="11" t="s">
         <v>603</v>
       </c>
@@ -53374,7 +53603,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="29.25" thickBot="1">
+    <row r="9" spans="1:10" ht="14.65" thickBot="1">
       <c r="A9" s="11" t="s">
         <v>605</v>
       </c>
@@ -53403,7 +53632,7 @@
         <v>0.22500000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15.75" thickBot="1">
+    <row r="10" spans="1:10" ht="14.65" thickBot="1">
       <c r="A10" s="11" t="s">
         <v>613</v>
       </c>
@@ -53432,7 +53661,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="15.75" thickBot="1">
+    <row r="11" spans="1:10" ht="14.65" thickBot="1">
       <c r="A11" s="11" t="s">
         <v>606</v>
       </c>
@@ -53461,7 +53690,7 @@
         <v>8.8235294117647051E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="15.75" thickBot="1">
+    <row r="12" spans="1:10" ht="14.65" thickBot="1">
       <c r="A12" s="11" t="s">
         <v>604</v>
       </c>
@@ -53490,7 +53719,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="15.75" thickBot="1">
+    <row r="13" spans="1:10" ht="14.65" thickBot="1">
       <c r="A13" s="11" t="s">
         <v>614</v>
       </c>
@@ -53516,7 +53745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="29.25" thickBot="1">
+    <row r="14" spans="1:10" ht="27.4" thickBot="1">
       <c r="A14" s="11" t="s">
         <v>608</v>
       </c>
@@ -53545,7 +53774,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="29.25" thickBot="1">
+    <row r="15" spans="1:10" ht="27.4" thickBot="1">
       <c r="A15" s="11" t="s">
         <v>609</v>
       </c>
@@ -53574,7 +53803,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15.75" thickBot="1">
+    <row r="16" spans="1:10" ht="14.65" thickBot="1">
       <c r="A16" s="11" t="s">
         <v>610</v>
       </c>
@@ -53600,7 +53829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="15.75" thickBot="1">
+    <row r="17" spans="1:10" ht="14.65" thickBot="1">
       <c r="A17" s="11" t="s">
         <v>611</v>
       </c>
@@ -53626,7 +53855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="15.75" thickBot="1">
+    <row r="18" spans="1:10" ht="14.65" thickBot="1">
       <c r="A18" s="11"/>
       <c r="B18" s="12"/>
       <c r="C18" s="12"/>
@@ -53638,16 +53867,16 @@
 </file>
 
 <file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3200-000000000000}">
   <dimension ref="A1:B235"/>
   <sheetViews>
     <sheetView topLeftCell="A219" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B229" sqref="B229"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -55536,14 +55765,14 @@
 </file>
 
 <file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3300-000000000000}">
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
@@ -56511,14 +56740,14 @@
 </file>
 
 <file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3400-000000000000}">
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="M32" sqref="M32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
@@ -57528,14 +57757,14 @@
 </file>
 
 <file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3500-000000000000}">
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
@@ -58545,14 +58774,14 @@
 </file>
 
 <file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3600-000000000000}">
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
@@ -59562,16 +59791,16 @@
 </file>
 
 <file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3700-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="A1:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="10.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -59613,16 +59842,16 @@
 </file>
 
 <file path=xl/worksheets/sheet57.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3800-000000000000}">
   <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="12" max="12" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="16.3984375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -60860,14 +61089,14 @@
 </file>
 
 <file path=xl/worksheets/sheet58.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3900-000000000000}">
   <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -62104,14 +62333,14 @@
 </file>
 
 <file path=xl/worksheets/sheet59.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3A00-000000000000}">
   <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -63348,16 +63577,16 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -63479,14 +63708,14 @@
 </file>
 
 <file path=xl/worksheets/sheet60.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3B00-000000000000}">
   <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -64723,16 +64952,16 @@
 </file>
 
 <file path=xl/worksheets/sheet61.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3C00-000000000000}">
   <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="12" max="12" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -65970,14 +66199,14 @@
 </file>
 
 <file path=xl/worksheets/sheet62.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3D00-000000000000}">
   <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -67214,14 +67443,14 @@
 </file>
 
 <file path=xl/worksheets/sheet63.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3E00-000000000000}">
   <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -68458,14 +68687,14 @@
 </file>
 
 <file path=xl/worksheets/sheet64.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3F00-000000000000}">
   <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -69702,14 +69931,14 @@
 </file>
 
 <file path=xl/worksheets/sheet65.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4000-000000000000}">
   <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -70946,14 +71175,14 @@
 </file>
 
 <file path=xl/worksheets/sheet66.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4100-000000000000}">
   <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -72190,14 +72419,14 @@
 </file>
 
 <file path=xl/worksheets/sheet67.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4200-000000000000}">
   <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -73434,16 +73663,16 @@
 </file>
 
 <file path=xl/worksheets/sheet68.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4300-000000000000}">
   <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="12" max="12" width="25.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="25.1328125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -74681,14 +74910,14 @@
 </file>
 
 <file path=xl/worksheets/sheet69.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4400-000000000000}">
   <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -75925,16 +76154,16 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -76056,14 +76285,14 @@
 </file>
 
 <file path=xl/worksheets/sheet70.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4500-000000000000}">
   <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -77300,14 +77529,14 @@
 </file>
 
 <file path=xl/worksheets/sheet71.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4600-000000000000}">
   <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -78544,14 +78773,14 @@
 </file>
 
 <file path=xl/worksheets/sheet72.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4700-000000000000}">
   <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -79788,14 +80017,14 @@
 </file>
 
 <file path=xl/worksheets/sheet73.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4800-000000000000}">
   <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -81032,14 +81261,14 @@
 </file>
 
 <file path=xl/worksheets/sheet74.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4900-000000000000}">
   <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -82276,14 +82505,14 @@
 </file>
 
 <file path=xl/worksheets/sheet75.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4A00-000000000000}">
   <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -83520,17 +83749,17 @@
 </file>
 
 <file path=xl/worksheets/sheet76.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4B00-000000000000}">
   <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q15" sqref="Q15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.86328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -84768,19 +84997,19 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="6" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="12.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.3984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13.86328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="6" width="12.3984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="12.3984375" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="9" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
@@ -85649,14 +85878,14 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">

</xml_diff>

<commit_message>
Minor update in sabad95 and metadata.xlsx
</commit_message>
<xml_diff>
--- a/Data/MetaData.xlsx
+++ b/Data/MetaData.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhash\OneDrive\Documents\GitHub\IRHEIS\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\IRHEIS\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E47BCC61-87F0-4631-BA71-A2FC3F39A0AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" tabRatio="858" firstSheet="38" activeTab="42" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="20715" windowHeight="13275" tabRatio="858" firstSheet="36" activeTab="37"/>
   </bookViews>
   <sheets>
     <sheet name="CompressedFileNames" sheetId="1" r:id="rId1"/>
@@ -2280,7 +2279,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="22">
     <font>
       <sz val="11"/>
@@ -3228,16 +3227,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B37"/>
   <sheetViews>
     <sheetView topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="20.86328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -3542,25 +3541,25 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T43"/>
   <sheetViews>
     <sheetView topLeftCell="A6" zoomScale="68" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="X39" sqref="X39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="12" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="12.73046875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="12" max="13" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="16" width="13.3984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="19.73046875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="16" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="19.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="18" max="18" width="19" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="19" max="19" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="15.265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
@@ -5686,25 +5685,25 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T43"/>
   <sheetViews>
     <sheetView zoomScale="54" workbookViewId="0">
       <selection activeCell="L49" sqref="L49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="9" max="9" width="12.73046875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="12.73046875" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12.7109375" customWidth="1" collapsed="1"/>
     <col min="12" max="12" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="12.73046875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="14" max="14" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="15.265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="13.3984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="12.59765625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="13.73046875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
@@ -7842,17 +7841,17 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S37"/>
   <sheetViews>
     <sheetView zoomScale="54" workbookViewId="0">
       <selection activeCell="K44" sqref="K44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="8" max="8" width="10.59765625" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="13.73046875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="10.5703125" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
@@ -9741,17 +9740,17 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S37"/>
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScale="84" workbookViewId="0">
       <selection activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="13.73046875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
@@ -11622,22 +11621,22 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView zoomScale="50" workbookViewId="0">
       <selection activeCell="H49" sqref="H49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="4" width="9.1328125" style="3" collapsed="1"/>
-    <col min="5" max="5" width="9.1328125" style="3"/>
-    <col min="6" max="6" width="9.1328125" style="3" collapsed="1"/>
-    <col min="7" max="7" width="10.73046875" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="10" width="9.1328125" style="3" collapsed="1"/>
-    <col min="11" max="11" width="11.1328125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="16384" width="9.1328125" style="3" collapsed="1"/>
+    <col min="1" max="4" width="9.140625" style="3" collapsed="1"/>
+    <col min="5" max="5" width="9.140625" style="3"/>
+    <col min="6" max="6" width="9.140625" style="3" collapsed="1"/>
+    <col min="7" max="7" width="10.7109375" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="10" width="9.140625" style="3" collapsed="1"/>
+    <col min="11" max="11" width="11.140625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="16384" width="9.140625" style="3" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -12815,16 +12814,16 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="5" max="5" width="10.3984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="15" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
@@ -13199,23 +13198,23 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView topLeftCell="A28" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="9.73046875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8.86328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="8.73046875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="14.1328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="11.86328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="10" width="8.73046875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="16.3984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="10" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -14453,17 +14452,17 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K36"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="7" max="7" width="14.1328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="16.3984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -14922,20 +14921,20 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E23" sqref="E23:G36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="16.1328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="10.73046875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="10.265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="10.59765625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -15766,17 +15765,17 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E127"/>
   <sheetViews>
     <sheetView topLeftCell="A109" workbookViewId="0">
       <selection activeCell="B130" sqref="B130"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="11.3984375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="2" width="11.42578125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -17669,14 +17668,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A36" sqref="A36:N37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:18">
       <c r="A1" t="s">
@@ -19072,18 +19071,18 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="7" max="7" width="14.1328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.59765625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="16.3984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -20078,18 +20077,18 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="7" max="7" width="14.1328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.59765625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="16.3984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -21084,16 +21083,16 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K37"/>
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="10" max="10" width="16.3984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -22274,18 +22273,18 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="7" max="7" width="14.1328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="9" width="14.1328125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12.1328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="9" width="14.140625" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -23064,18 +23063,18 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K37"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="I39" sqref="I39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="8.73046875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="10.59765625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -24379,19 +24378,19 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView topLeftCell="A22" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="7" max="7" width="14.1328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="12.1328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.1328125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12.1328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12.140625" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -25431,14 +25430,14 @@
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
@@ -26477,14 +26476,14 @@
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
@@ -27494,14 +27493,14 @@
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="C21" sqref="C16:D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
@@ -28511,16 +28510,16 @@
 </file>
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="10" max="10" width="11.1328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -29531,52 +29530,52 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BR37"/>
   <sheetViews>
     <sheetView topLeftCell="Z1" zoomScale="90" zoomScaleNormal="109" workbookViewId="0">
       <selection activeCell="AN20" sqref="AN20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="4" width="12.1328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.86328125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.59765625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.86328125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.265625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.265625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="21.86328125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="19.3984375" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="11.1328125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="10.73046875" bestFit="1" customWidth="1"/>
-    <col min="31" max="32" width="10.1328125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="9.86328125" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="12.73046875" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="11.1328125" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="10.3984375" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="12.3984375" customWidth="1"/>
-    <col min="49" max="49" width="10.3984375" customWidth="1"/>
-    <col min="50" max="50" width="16.86328125" customWidth="1"/>
-    <col min="51" max="51" width="14.86328125" customWidth="1"/>
-    <col min="52" max="52" width="19.73046875" customWidth="1"/>
-    <col min="53" max="53" width="17.73046875" customWidth="1"/>
-    <col min="54" max="54" width="12.86328125" customWidth="1"/>
-    <col min="55" max="55" width="10.86328125" customWidth="1"/>
-    <col min="56" max="56" width="12.3984375" customWidth="1"/>
-    <col min="57" max="57" width="10.3984375" customWidth="1"/>
-    <col min="58" max="58" width="16.73046875" customWidth="1"/>
-    <col min="59" max="60" width="16.73046875" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="14.73046875" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="14.73046875" customWidth="1"/>
-    <col min="63" max="63" width="10.73046875" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="14.73046875" customWidth="1"/>
-    <col min="65" max="65" width="10.73046875" customWidth="1"/>
-    <col min="66" max="66" width="18.3984375" customWidth="1"/>
-    <col min="67" max="67" width="18.265625" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="31" max="32" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="12.42578125" customWidth="1"/>
+    <col min="49" max="49" width="10.42578125" customWidth="1"/>
+    <col min="50" max="50" width="16.85546875" customWidth="1"/>
+    <col min="51" max="51" width="14.85546875" customWidth="1"/>
+    <col min="52" max="52" width="19.7109375" customWidth="1"/>
+    <col min="53" max="53" width="17.7109375" customWidth="1"/>
+    <col min="54" max="54" width="12.85546875" customWidth="1"/>
+    <col min="55" max="55" width="10.85546875" customWidth="1"/>
+    <col min="56" max="56" width="12.42578125" customWidth="1"/>
+    <col min="57" max="57" width="10.42578125" customWidth="1"/>
+    <col min="58" max="58" width="16.7109375" customWidth="1"/>
+    <col min="59" max="60" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="14.7109375" customWidth="1"/>
+    <col min="63" max="63" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="14.7109375" customWidth="1"/>
+    <col min="65" max="65" width="10.7109375" customWidth="1"/>
+    <col min="66" max="66" width="18.42578125" customWidth="1"/>
+    <col min="67" max="67" width="18.28515625" customWidth="1"/>
     <col min="68" max="68" width="23" customWidth="1"/>
     <col min="69" max="69" width="22" customWidth="1"/>
-    <col min="70" max="70" width="20.73046875" customWidth="1"/>
+    <col min="70" max="70" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:70">
@@ -34349,14 +34348,14 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
@@ -35395,17 +35394,17 @@
 </file>
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="7" max="7" width="14.1328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="13.59765625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -36184,17 +36183,17 @@
 </file>
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="7" max="7" width="14.1328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="18.3984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -37093,17 +37092,17 @@
 </file>
 
 <file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="7" max="7" width="14.1328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="20.265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -38002,17 +38001,17 @@
 </file>
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="7" max="7" width="14.1328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="16.1328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -38791,19 +38790,19 @@
 </file>
 
 <file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P37"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="A36" sqref="A36:P37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="8" max="8" width="13.86328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="16.59765625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.59765625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="12" width="9.86328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="16.5703125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="12" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
@@ -40605,16 +40604,16 @@
 </file>
 
 <file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="10" max="10" width="16.1328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -41513,16 +41512,16 @@
 </file>
 
 <file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="10" max="10" width="16.1328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -42421,19 +42420,19 @@
 </file>
 
 <file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C38" sqref="C26:D38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="7" max="7" width="14.1328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14.1328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.1328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="15.1328125" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -43080,12 +43079,8 @@
       <c r="B27" t="s">
         <v>276</v>
       </c>
-      <c r="C27" s="9">
-        <v>123111</v>
-      </c>
-      <c r="D27" s="9">
-        <v>123134</v>
-      </c>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
       <c r="E27" t="s">
         <v>66</v>
       </c>
@@ -43115,12 +43110,8 @@
       <c r="B28" t="s">
         <v>276</v>
       </c>
-      <c r="C28" s="9">
-        <v>123111</v>
-      </c>
-      <c r="D28" s="9">
-        <v>123134</v>
-      </c>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
       <c r="E28" t="s">
         <v>284</v>
       </c>
@@ -43150,12 +43141,8 @@
       <c r="B29" t="s">
         <v>276</v>
       </c>
-      <c r="C29" s="9">
-        <v>123111</v>
-      </c>
-      <c r="D29" s="9">
-        <v>123134</v>
-      </c>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
       <c r="E29" t="s">
         <v>66</v>
       </c>
@@ -43185,12 +43172,8 @@
       <c r="B30" t="s">
         <v>276</v>
       </c>
-      <c r="C30" s="9">
-        <v>123111</v>
-      </c>
-      <c r="D30" s="9">
-        <v>123134</v>
-      </c>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
       <c r="E30" t="s">
         <v>66</v>
       </c>
@@ -43220,12 +43203,8 @@
       <c r="B31" t="s">
         <v>276</v>
       </c>
-      <c r="C31" s="9">
-        <v>123111</v>
-      </c>
-      <c r="D31" s="9">
-        <v>123134</v>
-      </c>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
       <c r="E31" t="s">
         <v>66</v>
       </c>
@@ -43255,12 +43234,8 @@
       <c r="B32" t="s">
         <v>276</v>
       </c>
-      <c r="C32" s="9">
-        <v>123111</v>
-      </c>
-      <c r="D32" s="9">
-        <v>123134</v>
-      </c>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
       <c r="E32" t="s">
         <v>66</v>
       </c>
@@ -43290,12 +43265,8 @@
       <c r="B33" t="s">
         <v>276</v>
       </c>
-      <c r="C33" s="9">
-        <v>123111</v>
-      </c>
-      <c r="D33" s="9">
-        <v>123134</v>
-      </c>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
       <c r="E33" t="s">
         <v>66</v>
       </c>
@@ -43325,12 +43296,8 @@
       <c r="B34" t="s">
         <v>276</v>
       </c>
-      <c r="C34" s="9">
-        <v>123111</v>
-      </c>
-      <c r="D34" s="9">
-        <v>123134</v>
-      </c>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
       <c r="E34" t="s">
         <v>66</v>
       </c>
@@ -43360,12 +43327,8 @@
       <c r="B35" t="s">
         <v>276</v>
       </c>
-      <c r="C35" s="9">
-        <v>123111</v>
-      </c>
-      <c r="D35" s="9">
-        <v>123134</v>
-      </c>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
       <c r="E35" t="s">
         <v>66</v>
       </c>
@@ -43395,12 +43358,8 @@
       <c r="B36" t="s">
         <v>276</v>
       </c>
-      <c r="C36" s="9">
-        <v>123111</v>
-      </c>
-      <c r="D36" s="9">
-        <v>123134</v>
-      </c>
+      <c r="C36" s="9"/>
+      <c r="D36" s="9"/>
       <c r="E36" t="s">
         <v>66</v>
       </c>
@@ -43430,12 +43389,8 @@
       <c r="B37" t="s">
         <v>276</v>
       </c>
-      <c r="C37" s="9">
-        <v>123111</v>
-      </c>
-      <c r="D37" s="9">
-        <v>123134</v>
-      </c>
+      <c r="C37" s="9"/>
+      <c r="D37" s="9"/>
       <c r="E37" t="s">
         <v>66</v>
       </c>
@@ -43468,18 +43423,18 @@
 </file>
 
 <file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K36"/>
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="9" max="9" width="14.1328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.1328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.73046875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -44421,16 +44376,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C60"/>
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="96.73046875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="96.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -45099,17 +45054,17 @@
 </file>
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="7" max="7" width="14.1328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="15.3984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -45960,23 +45915,23 @@
 </file>
 
 <file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K37"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="9.1328125" style="3" collapsed="1"/>
-    <col min="3" max="3" width="9.73046875" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="6" width="9.1328125" style="3" collapsed="1"/>
-    <col min="7" max="7" width="14.1328125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="9" width="9.1328125" style="3" collapsed="1"/>
-    <col min="10" max="10" width="10.59765625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="17.59765625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="16384" width="9.1328125" style="3" collapsed="1"/>
+    <col min="1" max="2" width="9.140625" style="3" collapsed="1"/>
+    <col min="3" max="3" width="9.7109375" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="6" width="9.140625" style="3" collapsed="1"/>
+    <col min="7" max="7" width="14.140625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="9" width="9.140625" style="3" collapsed="1"/>
+    <col min="10" max="10" width="10.5703125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="17.5703125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="16384" width="9.140625" style="3" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -47138,16 +47093,16 @@
 </file>
 
 <file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H37"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="N27" sqref="N27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="8" max="8" width="10.73046875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -47926,14 +47881,14 @@
 </file>
 
 <file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="O30" sqref="O30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="3" t="s">
@@ -48711,14 +48666,14 @@
 </file>
 
 <file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H37"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="O31" sqref="O31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="3" t="s">
@@ -49496,14 +49451,14 @@
 </file>
 
 <file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H37"/>
   <sheetViews>
     <sheetView zoomScale="55" workbookViewId="0">
       <selection activeCell="K45" sqref="K45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="3" t="s">
@@ -50281,16 +50236,16 @@
 </file>
 
 <file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="Q28" sqref="Q28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="8" max="8" width="11.1328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -51085,14 +51040,14 @@
 </file>
 
 <file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="Q33" sqref="Q33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="4" t="s">
@@ -51851,17 +51806,17 @@
 </file>
 
 <file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="E18" sqref="E1:G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.1328125" style="8"/>
+    <col min="6" max="6" width="9.140625" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -52146,7 +52101,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C20">
+  <sortState ref="A2:C20">
     <sortCondition ref="A2:A20"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -52155,17 +52110,17 @@
 </file>
 
 <file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -52588,12 +52543,12 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D97"/>
   <sheetViews>
     <sheetView topLeftCell="A73" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
@@ -53821,22 +53776,22 @@
 </file>
 
 <file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="16.59765625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.73046875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.86328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="14.65" thickBot="1">
+    <row r="1" spans="1:10" ht="15.75" thickBot="1">
       <c r="A1" s="15"/>
       <c r="B1" s="3" t="s">
         <v>617</v>
@@ -53854,7 +53809,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="14.65" thickBot="1">
+    <row r="2" spans="1:10" ht="15.75" thickBot="1">
       <c r="A2" s="10" t="s">
         <v>598</v>
       </c>
@@ -53883,7 +53838,7 @@
         <v>0.10124999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="14.65" thickBot="1">
+    <row r="3" spans="1:10" ht="15.75" thickBot="1">
       <c r="A3" s="11" t="s">
         <v>599</v>
       </c>
@@ -53912,7 +53867,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="14.65" thickBot="1">
+    <row r="4" spans="1:10" ht="15.75" thickBot="1">
       <c r="A4" s="11" t="s">
         <v>600</v>
       </c>
@@ -53941,7 +53896,7 @@
         <v>6.4285714285714293E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="14.65" thickBot="1">
+    <row r="5" spans="1:10" ht="15.75" thickBot="1">
       <c r="A5" s="11" t="s">
         <v>612</v>
       </c>
@@ -53970,7 +53925,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="14.65" thickBot="1">
+    <row r="6" spans="1:10" ht="15.75" thickBot="1">
       <c r="A6" s="11" t="s">
         <v>601</v>
       </c>
@@ -53999,7 +53954,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="14.65" thickBot="1">
+    <row r="7" spans="1:10" ht="15.75" thickBot="1">
       <c r="A7" s="11" t="s">
         <v>602</v>
       </c>
@@ -54028,7 +53983,7 @@
         <v>3.214285714285714E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="14.65" thickBot="1">
+    <row r="8" spans="1:10" ht="15.75" thickBot="1">
       <c r="A8" s="11" t="s">
         <v>603</v>
       </c>
@@ -54057,7 +54012,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="14.65" thickBot="1">
+    <row r="9" spans="1:10" ht="29.25" thickBot="1">
       <c r="A9" s="11" t="s">
         <v>605</v>
       </c>
@@ -54086,7 +54041,7 @@
         <v>0.22500000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="14.65" thickBot="1">
+    <row r="10" spans="1:10" ht="15.75" thickBot="1">
       <c r="A10" s="11" t="s">
         <v>613</v>
       </c>
@@ -54115,7 +54070,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="14.65" thickBot="1">
+    <row r="11" spans="1:10" ht="15.75" thickBot="1">
       <c r="A11" s="11" t="s">
         <v>606</v>
       </c>
@@ -54144,7 +54099,7 @@
         <v>8.8235294117647051E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="14.65" thickBot="1">
+    <row r="12" spans="1:10" ht="15.75" thickBot="1">
       <c r="A12" s="11" t="s">
         <v>604</v>
       </c>
@@ -54173,7 +54128,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="14.65" thickBot="1">
+    <row r="13" spans="1:10" ht="15.75" thickBot="1">
       <c r="A13" s="11" t="s">
         <v>614</v>
       </c>
@@ -54199,7 +54154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="27.4" thickBot="1">
+    <row r="14" spans="1:10" ht="29.25" thickBot="1">
       <c r="A14" s="11" t="s">
         <v>608</v>
       </c>
@@ -54228,7 +54183,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="27.4" thickBot="1">
+    <row r="15" spans="1:10" ht="29.25" thickBot="1">
       <c r="A15" s="11" t="s">
         <v>609</v>
       </c>
@@ -54257,7 +54212,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="14.65" thickBot="1">
+    <row r="16" spans="1:10" ht="15.75" thickBot="1">
       <c r="A16" s="11" t="s">
         <v>610</v>
       </c>
@@ -54283,7 +54238,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="14.65" thickBot="1">
+    <row r="17" spans="1:10" ht="15.75" thickBot="1">
       <c r="A17" s="11" t="s">
         <v>611</v>
       </c>
@@ -54309,7 +54264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="14.65" thickBot="1">
+    <row r="18" spans="1:10" ht="15.75" thickBot="1">
       <c r="A18" s="11"/>
       <c r="B18" s="12"/>
       <c r="C18" s="12"/>
@@ -54321,16 +54276,16 @@
 </file>
 
 <file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B235"/>
   <sheetViews>
     <sheetView topLeftCell="A219" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B229" sqref="B229"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="16.86328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -56219,14 +56174,14 @@
 </file>
 
 <file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
@@ -57194,14 +57149,14 @@
 </file>
 
 <file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="M32" sqref="M32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
@@ -58211,14 +58166,14 @@
 </file>
 
 <file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
@@ -59228,14 +59183,14 @@
 </file>
 
 <file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
@@ -60245,16 +60200,16 @@
 </file>
 
 <file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="A1:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="10.265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -60296,16 +60251,16 @@
 </file>
 
 <file path=xl/worksheets/sheet57.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="12" max="12" width="16.3984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -61543,14 +61498,14 @@
 </file>
 
 <file path=xl/worksheets/sheet58.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -62787,14 +62742,14 @@
 </file>
 
 <file path=xl/worksheets/sheet59.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -64031,16 +63986,16 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="22.59765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -64162,14 +64117,14 @@
 </file>
 
 <file path=xl/worksheets/sheet60.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -65406,16 +65361,16 @@
 </file>
 
 <file path=xl/worksheets/sheet61.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="12" max="12" width="11.86328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -66653,14 +66608,14 @@
 </file>
 
 <file path=xl/worksheets/sheet62.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -67897,14 +67852,14 @@
 </file>
 
 <file path=xl/worksheets/sheet63.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -69141,14 +69096,14 @@
 </file>
 
 <file path=xl/worksheets/sheet64.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -70385,14 +70340,14 @@
 </file>
 
 <file path=xl/worksheets/sheet65.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -71629,14 +71584,14 @@
 </file>
 
 <file path=xl/worksheets/sheet66.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -72873,14 +72828,14 @@
 </file>
 
 <file path=xl/worksheets/sheet67.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -74117,16 +74072,16 @@
 </file>
 
 <file path=xl/worksheets/sheet68.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="12" max="12" width="25.1328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="25.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -75364,14 +75319,14 @@
 </file>
 
 <file path=xl/worksheets/sheet69.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -76608,16 +76563,16 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="22.59765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -76739,14 +76694,14 @@
 </file>
 
 <file path=xl/worksheets/sheet70.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -77983,14 +77938,14 @@
 </file>
 
 <file path=xl/worksheets/sheet71.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -79227,14 +79182,14 @@
 </file>
 
 <file path=xl/worksheets/sheet72.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -80471,14 +80426,14 @@
 </file>
 
 <file path=xl/worksheets/sheet73.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -81715,14 +81670,14 @@
 </file>
 
 <file path=xl/worksheets/sheet74.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -82959,14 +82914,14 @@
 </file>
 
 <file path=xl/worksheets/sheet75.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -84203,17 +84158,17 @@
 </file>
 
 <file path=xl/worksheets/sheet76.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="Q15" sqref="Q15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="8" max="8" width="11.86328125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.86328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -85451,19 +85406,19 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H37"/>
   <sheetViews>
     <sheetView topLeftCell="A30" workbookViewId="0">
       <selection activeCell="L40" sqref="L40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="14.3984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.86328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="6" width="12.3984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="12.3984375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="6" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="12.42578125" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="9" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
@@ -86384,14 +86339,14 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="R42" sqref="R42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">

</xml_diff>